<commit_message>
#900 Added generated property constants for i18n strings and validations
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3178" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3178" uniqueCount="1117">
   <si>
     <t>Field</t>
   </si>
@@ -341,7 +341,7 @@
     <t>DEAD</t>
   </si>
   <si>
-    <t xml:space="preserve">Dead </t>
+    <t>Dead</t>
   </si>
   <si>
     <t>BURIED</t>
@@ -491,7 +491,7 @@
     <t>RELIGIOUS_LEADER</t>
   </si>
   <si>
-    <t xml:space="preserve">Religious leader </t>
+    <t>Religious leader</t>
   </si>
   <si>
     <t>HOUSEWIFE</t>
@@ -1007,7 +1007,7 @@
     <t>admittedToHealthFacility</t>
   </si>
   <si>
-    <t>Was patient admitted at the health facility?</t>
+    <t>Was patient admitted at the health facility as an inpatient?</t>
   </si>
   <si>
     <t>admissionDate</t>
@@ -1451,7 +1451,7 @@
     <t>Pain behind eyes/Sensitivity to light</t>
   </si>
   <si>
-    <t>Pain behind eyes or eyes sensitive to light</t>
+    <t>ain behind eyes or eyes sensitive to light</t>
   </si>
   <si>
     <t>EVD, Lassa, New flu, CSM, Measles, Dengue, Monkeypox, Other</t>
@@ -1736,9 +1736,6 @@
     <t>patientIllLocation</t>
   </si>
   <si>
-    <t>Name of the village (and country) where the patient got ill</t>
-  </si>
-  <si>
     <t>AXILLARY</t>
   </si>
   <si>
@@ -1757,9 +1754,6 @@
     <t>rectal</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes </t>
-  </si>
-  <si>
     <t>burialAttended</t>
   </si>
   <si>
@@ -2102,9 +2096,6 @@
     <t>Stream</t>
   </si>
   <si>
-    <t>Dead</t>
-  </si>
-  <si>
     <t>PROCESSED</t>
   </si>
   <si>
@@ -3389,7 +3380,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.10.0-SNAPSHOT</t>
+    <t>1.11.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -5830,10 +5821,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -5851,13 +5842,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C3" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>17</v>
@@ -5872,13 +5863,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>17</v>
@@ -5891,16 +5882,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -5912,13 +5903,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>17</v>
@@ -5933,13 +5924,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>17</v>
@@ -5952,7 +5943,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>206</v>
@@ -5973,13 +5964,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="C9" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>17</v>
@@ -5994,13 +5985,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>17</v>
@@ -6015,13 +6006,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>17</v>
@@ -6034,16 +6025,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>341</v>
       </c>
       <c r="C12" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="E12"/>
       <c r="F12" s="10" t="s">
@@ -6070,13 +6061,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="B15" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="C15" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -6088,10 +6079,10 @@
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="C16" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -6103,10 +6094,10 @@
     <row r="17">
       <c r="A17"/>
       <c r="B17" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="C17" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -6118,10 +6109,10 @@
     <row r="18">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="C18" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -6133,10 +6124,10 @@
     <row r="19">
       <c r="A19"/>
       <c r="B19" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="C19" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
@@ -6148,10 +6139,10 @@
     <row r="20">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="C20" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
@@ -6163,7 +6154,7 @@
     <row r="21">
       <c r="A21"/>
       <c r="B21" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="C21" t="s">
         <v>332</v>
@@ -6178,10 +6169,10 @@
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="C22" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -6193,10 +6184,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="C23" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -6208,10 +6199,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="C24" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -6223,10 +6214,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="C25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -6238,10 +6229,10 @@
     <row r="26">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="C26" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
@@ -6253,10 +6244,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C27" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -6268,10 +6259,10 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="C28" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -6283,10 +6274,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="C29" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
@@ -6298,10 +6289,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C30" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -6313,10 +6304,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C31" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -6359,13 +6350,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="B35" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="C35" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -6392,10 +6383,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="C37" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
@@ -6407,10 +6398,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="C38" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
@@ -6471,13 +6462,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C2" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>17</v>
@@ -6492,13 +6483,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C3" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>17</v>
@@ -6511,13 +6502,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="C4" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>17</v>
@@ -6530,13 +6521,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="C5" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>17</v>
@@ -6549,16 +6540,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>940</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>941</v>
+      </c>
+      <c r="C6" t="s">
+        <v>942</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>943</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>944</v>
-      </c>
-      <c r="C6" t="s">
-        <v>945</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>946</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -6570,13 +6561,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="C7" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>17</v>
@@ -6589,13 +6580,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>17</v>
@@ -6610,13 +6601,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>17</v>
@@ -6629,13 +6620,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="C10" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>17</v>
@@ -6648,13 +6639,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>17</v>
@@ -6667,13 +6658,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>17</v>
@@ -6686,13 +6677,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>206</v>
       </c>
       <c r="C13" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>17</v>
@@ -6705,13 +6696,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>17</v>
@@ -6724,13 +6715,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>17</v>
@@ -6745,13 +6736,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>17</v>
@@ -6764,7 +6755,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>25</v>
@@ -6783,7 +6774,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>25</v>
@@ -6802,7 +6793,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>25</v>
@@ -6838,13 +6829,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B22" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="C22" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -6856,10 +6847,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="C23" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -6871,10 +6862,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="C24" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -6886,10 +6877,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="C25" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -6917,13 +6908,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="B28" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C28" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -6935,10 +6926,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="C29" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
@@ -6950,10 +6941,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="C30" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -6965,10 +6956,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C31" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -6980,10 +6971,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="C32" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -6995,10 +6986,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="C33" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -7010,10 +7001,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="C34" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
@@ -7025,10 +7016,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="C35" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -7040,10 +7031,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C36" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
@@ -7055,10 +7046,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="C37" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
@@ -7070,10 +7061,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="C38" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
@@ -7085,10 +7076,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C39" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -7100,10 +7091,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="C40" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
@@ -7115,10 +7106,10 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="C41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -7130,10 +7121,10 @@
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="C42" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -7145,10 +7136,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="C43" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="D43" t="s">
         <v>17</v>
@@ -7160,10 +7151,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="C44" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -7178,7 +7169,7 @@
         <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -7190,10 +7181,10 @@
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="C46" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
@@ -7205,10 +7196,10 @@
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="C47" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
@@ -7220,10 +7211,10 @@
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C48" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
@@ -7251,13 +7242,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="B51" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="C51" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -7269,10 +7260,10 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="C52" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
@@ -7284,10 +7275,10 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="C53" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -7315,13 +7306,13 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="B56" t="s">
         <v>295</v>
       </c>
       <c r="C56" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="D56" t="s">
         <v>17</v>
@@ -7336,7 +7327,7 @@
         <v>298</v>
       </c>
       <c r="C57" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
@@ -7348,10 +7339,10 @@
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="C58" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="D58" t="s">
         <v>17</v>
@@ -7363,10 +7354,10 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="C59" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
@@ -7429,13 +7420,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C2" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -7450,16 +7441,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>1036</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1038</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>1039</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -7471,16 +7462,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -7492,16 +7483,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="E5"/>
       <c r="F5" s="12" t="s">
@@ -7511,7 +7502,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>39</v>
@@ -7553,13 +7544,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
@@ -7572,16 +7563,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>1048</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1050</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>1051</v>
       </c>
       <c r="E9"/>
       <c r="F9" s="12" t="s">
@@ -7591,16 +7582,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="E10"/>
       <c r="F10" s="12" t="s">
@@ -7610,16 +7601,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="E11"/>
       <c r="F11" s="12" t="s">
@@ -7629,16 +7620,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="E12"/>
       <c r="F12" s="12" t="s">
@@ -7648,16 +7639,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="E13"/>
       <c r="F13" s="12" t="s">
@@ -7724,13 +7715,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>17</v>
@@ -7817,13 +7808,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="B23" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="C23" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -7835,10 +7826,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="C24" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -7866,19 +7857,19 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="B27" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="C27" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="28">
@@ -7887,7 +7878,7 @@
         <v>289</v>
       </c>
       <c r="C28" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -7899,16 +7890,16 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="C29" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="31">
@@ -7930,13 +7921,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="B32" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="C32" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -7948,10 +7939,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="C33" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -7978,10 +7969,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C35" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -7993,10 +7984,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="C36" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
@@ -8273,13 +8264,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="C2" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>17</v>
@@ -8297,10 +8288,10 @@
         <v>198</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="C3" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>17</v>
@@ -8315,13 +8306,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>17</v>
@@ -8334,10 +8325,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -8401,13 +8392,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>17</v>
@@ -8502,7 +8493,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>17</v>
@@ -8521,7 +8512,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>17</v>
@@ -8534,10 +8525,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -8553,7 +8544,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>341</v>
@@ -8589,13 +8580,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C13" t="s">
         <v>1093</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1095</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1096</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -8607,10 +8598,10 @@
     <row r="14">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="C14" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -8622,10 +8613,10 @@
     <row r="15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="C15" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -8637,10 +8628,10 @@
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="C16" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -8700,13 +8691,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>17</v>
@@ -8719,13 +8710,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>17</v>
@@ -8738,13 +8729,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>17</v>
@@ -8757,13 +8748,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>17</v>
@@ -8824,13 +8815,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>17</v>
@@ -8843,13 +8834,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>17</v>
@@ -8862,13 +8853,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>17</v>
@@ -8881,13 +8872,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>17</v>
@@ -8967,13 +8958,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>17</v>
@@ -9053,13 +9044,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>341</v>
       </c>
       <c r="C2" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>17</v>
@@ -9072,13 +9063,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>17</v>
@@ -9129,13 +9120,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>17</v>
@@ -9186,11 +9177,11 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>17</v>
@@ -9279,13 +9270,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>17</v>
@@ -9298,13 +9289,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>17</v>
@@ -9333,12 +9324,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
   </sheetData>
@@ -13141,7 +13132,7 @@
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>568</v>
+        <v>17</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>17</v>
@@ -13174,10 +13165,10 @@
         <v>355</v>
       </c>
       <c r="B93" t="s">
+        <v>568</v>
+      </c>
+      <c r="C93" t="s">
         <v>569</v>
-      </c>
-      <c r="C93" t="s">
-        <v>570</v>
       </c>
       <c r="D93" t="s">
         <v>17</v>
@@ -13189,10 +13180,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
+        <v>570</v>
+      </c>
+      <c r="C94" t="s">
         <v>571</v>
-      </c>
-      <c r="C94" t="s">
-        <v>572</v>
       </c>
       <c r="D94" t="s">
         <v>17</v>
@@ -13204,10 +13195,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
+        <v>572</v>
+      </c>
+      <c r="C95" t="s">
         <v>573</v>
-      </c>
-      <c r="C95" t="s">
-        <v>574</v>
       </c>
       <c r="D95" t="s">
         <v>17</v>
@@ -13241,7 +13232,7 @@
         <v>312</v>
       </c>
       <c r="C98" t="s">
-        <v>575</v>
+        <v>313</v>
       </c>
       <c r="D98" t="s">
         <v>17</v>
@@ -13332,16 +13323,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E2"/>
       <c r="F2" s="6" t="s">
@@ -13351,35 +13342,35 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C3" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E3"/>
       <c r="F3" s="6" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E4"/>
       <c r="F4" s="6" t="s">
@@ -13389,11 +13380,11 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -13406,11 +13397,11 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
@@ -13423,11 +13414,11 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -13440,89 +13431,89 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E8"/>
       <c r="F8" s="6" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C9" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E9"/>
       <c r="F9" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C10" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E10"/>
       <c r="F10" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C11" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E11"/>
       <c r="F11" s="6" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="G11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C12" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
@@ -13535,13 +13526,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C13" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -13554,13 +13545,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C14" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -13573,206 +13564,206 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C15" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E15"/>
       <c r="F15" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C16" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E16"/>
       <c r="F16" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C17" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E17"/>
       <c r="F17" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E18"/>
       <c r="F18" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E19"/>
       <c r="F19" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E20"/>
       <c r="F20" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C21" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E21"/>
       <c r="F21" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C22" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E22"/>
       <c r="F22" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E23"/>
       <c r="F23" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C24" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E24"/>
       <c r="F24" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="G24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C25" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E25"/>
       <c r="F25" s="6" t="s">
@@ -13782,35 +13773,35 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C26" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E26"/>
       <c r="F26" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C27" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E27"/>
       <c r="F27" s="6" t="s">
@@ -13820,35 +13811,35 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C28" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E28"/>
       <c r="F28" s="6" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="G28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C29" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E29"/>
       <c r="F29" s="6" t="s">
@@ -13858,130 +13849,130 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C30" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E30"/>
       <c r="F30" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E31"/>
       <c r="F31" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>653</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="C32" t="s">
         <v>655</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>656</v>
-      </c>
-      <c r="C32" t="s">
-        <v>657</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>658</v>
       </c>
       <c r="E32"/>
       <c r="F32" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E33"/>
       <c r="F33" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C34" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="E34"/>
       <c r="F34" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E35"/>
       <c r="F35" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C36" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="E36"/>
       <c r="F36" s="6" t="s">
@@ -13991,16 +13982,16 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C37" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E37"/>
       <c r="F37" s="6" t="s">
@@ -14010,13 +14001,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>17</v>
@@ -14029,13 +14020,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>17</v>
@@ -14048,13 +14039,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>677</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="C40" t="s">
         <v>679</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>680</v>
-      </c>
-      <c r="C40" t="s">
-        <v>681</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>17</v>
@@ -14148,13 +14139,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B48" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C48" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
@@ -14166,10 +14157,10 @@
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C49" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
@@ -14181,10 +14172,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C50" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
@@ -14196,10 +14187,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C51" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -14242,7 +14233,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B55" t="s">
         <v>100</v>
@@ -14263,7 +14254,7 @@
         <v>102</v>
       </c>
       <c r="C56" t="s">
-        <v>690</v>
+        <v>103</v>
       </c>
       <c r="D56" t="s">
         <v>17</v>
@@ -14275,10 +14266,10 @@
     <row r="57">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="C57" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
@@ -14355,13 +14346,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>17</v>
@@ -14460,7 +14451,7 @@
         <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>17</v>
@@ -14475,13 +14466,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C8" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>17</v>
@@ -14496,13 +14487,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>17</v>
@@ -14515,13 +14506,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>17</v>
@@ -14534,16 +14525,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>700</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="C11" t="s">
+        <v>702</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>703</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>704</v>
-      </c>
-      <c r="C11" t="s">
-        <v>705</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>706</v>
       </c>
       <c r="E11"/>
       <c r="F11" s="7" t="s">
@@ -14553,13 +14544,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="C12" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>17</v>
@@ -14572,13 +14563,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="C13" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>17</v>
@@ -14591,89 +14582,89 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>710</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="C14" t="s">
+        <v>712</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>713</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>714</v>
-      </c>
-      <c r="C14" t="s">
-        <v>715</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>716</v>
       </c>
       <c r="E14"/>
       <c r="F14" s="7" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="G14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E15"/>
       <c r="F15" s="7" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="G15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E16"/>
       <c r="F16" s="7" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="G16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>206</v>
       </c>
       <c r="C17" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E17"/>
       <c r="F17" s="7" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="G17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>17</v>
@@ -14686,16 +14677,16 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="C19" t="s">
+        <v>725</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>726</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>727</v>
-      </c>
-      <c r="C19" t="s">
-        <v>728</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>729</v>
       </c>
       <c r="E19"/>
       <c r="F19" s="7" t="s">
@@ -14705,13 +14696,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C20" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>17</v>
@@ -14724,13 +14715,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>17</v>
@@ -14944,13 +14935,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="B37" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C37" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
@@ -14962,10 +14953,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C38" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
@@ -14977,10 +14968,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="C39" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -14992,10 +14983,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C40" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
@@ -15007,10 +14998,10 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="C41" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -15038,19 +15029,19 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B44" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="C44" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="45">
@@ -15059,7 +15050,7 @@
         <v>289</v>
       </c>
       <c r="C45" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -15071,16 +15062,16 @@
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="C46" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="48">
@@ -15102,13 +15093,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B49" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C49" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
@@ -15120,10 +15111,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="C50" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
@@ -15135,10 +15126,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="C51" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -15166,76 +15157,76 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="B54" t="s">
+        <v>754</v>
+      </c>
+      <c r="C54" t="s">
+        <v>755</v>
+      </c>
+      <c r="D54" t="s">
+        <v>756</v>
+      </c>
+      <c r="E54" t="s">
         <v>757</v>
-      </c>
-      <c r="C54" t="s">
-        <v>758</v>
-      </c>
-      <c r="D54" t="s">
-        <v>759</v>
-      </c>
-      <c r="E54" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="55">
       <c r="A55"/>
       <c r="B55" t="s">
+        <v>758</v>
+      </c>
+      <c r="C55" t="s">
+        <v>759</v>
+      </c>
+      <c r="D55" t="s">
+        <v>760</v>
+      </c>
+      <c r="E55" t="s">
         <v>761</v>
-      </c>
-      <c r="C55" t="s">
-        <v>762</v>
-      </c>
-      <c r="D55" t="s">
-        <v>763</v>
-      </c>
-      <c r="E55" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
+        <v>762</v>
+      </c>
+      <c r="C56" t="s">
+        <v>763</v>
+      </c>
+      <c r="D56" t="s">
+        <v>764</v>
+      </c>
+      <c r="E56" t="s">
         <v>765</v>
-      </c>
-      <c r="C56" t="s">
-        <v>766</v>
-      </c>
-      <c r="D56" t="s">
-        <v>767</v>
-      </c>
-      <c r="E56" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="57">
       <c r="A57"/>
       <c r="B57" t="s">
+        <v>766</v>
+      </c>
+      <c r="C57" t="s">
+        <v>767</v>
+      </c>
+      <c r="D57" t="s">
+        <v>768</v>
+      </c>
+      <c r="E57" t="s">
         <v>769</v>
-      </c>
-      <c r="C57" t="s">
-        <v>770</v>
-      </c>
-      <c r="D57" t="s">
-        <v>771</v>
-      </c>
-      <c r="E57" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="C58" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D58" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E58" t="s">
         <v>17</v>
@@ -15260,13 +15251,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B61" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C61" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
@@ -15278,10 +15269,10 @@
     <row r="62">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="C62" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
@@ -15293,10 +15284,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="C63" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
@@ -15308,10 +15299,10 @@
     <row r="64">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C64" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
@@ -15397,7 +15388,7 @@
         <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>17</v>
@@ -15431,16 +15422,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -15452,13 +15443,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>17</v>
@@ -15473,16 +15464,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>787</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="C6" t="s">
+        <v>789</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>790</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>791</v>
-      </c>
-      <c r="C6" t="s">
-        <v>792</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>793</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -15494,16 +15485,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E7"/>
       <c r="F7" s="8" t="s">
@@ -15790,13 +15781,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="B27" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C27" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -15808,31 +15799,31 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="C28" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
     </row>
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="C29" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -15887,13 +15878,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C2" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>17</v>
@@ -15908,13 +15899,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>17</v>
@@ -15927,13 +15918,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>17</v>
@@ -15946,16 +15937,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -15967,7 +15958,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>39</v>
@@ -16066,13 +16057,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C11" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>17</v>
@@ -16087,13 +16078,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>17</v>
@@ -16106,13 +16097,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>17</v>
@@ -16127,13 +16118,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>17</v>
@@ -16146,13 +16137,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>17</v>
@@ -16165,13 +16156,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>17</v>
@@ -16184,13 +16175,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>17</v>
@@ -16203,13 +16194,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C18" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>17</v>
@@ -16222,13 +16213,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>17</v>
@@ -16241,13 +16232,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>17</v>
@@ -16260,13 +16251,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C21" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>17</v>
@@ -16279,13 +16270,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C22" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>17</v>
@@ -16298,10 +16289,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -16317,13 +16308,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>341</v>
       </c>
       <c r="C24" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>17</v>
@@ -16336,13 +16327,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>341</v>
       </c>
       <c r="C25" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>17</v>
@@ -16372,13 +16363,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="B28" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="C28" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -16390,10 +16381,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="C29" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
@@ -16405,10 +16396,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="C30" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -16420,10 +16411,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="C31" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -16435,10 +16426,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="C32" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -16450,10 +16441,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="C33" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -16465,10 +16456,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="C34" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
@@ -16480,10 +16471,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="C35" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -16495,10 +16486,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="C36" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
@@ -16541,13 +16532,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="B40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C40" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
@@ -16559,10 +16550,10 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="C41" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -16590,13 +16581,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="B44" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="C44" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -16608,10 +16599,10 @@
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="C45" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -16623,10 +16614,10 @@
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="C46" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
@@ -16654,13 +16645,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="B49" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="C49" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
@@ -16672,10 +16663,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="C50" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
@@ -16687,10 +16678,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="C51" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -16702,10 +16693,10 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="C52" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
@@ -16717,10 +16708,10 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="C53" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -16732,10 +16723,10 @@
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="C54" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
@@ -16747,7 +16738,7 @@
     <row r="55">
       <c r="A55"/>
       <c r="B55" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="C55" t="s">
         <v>332</v>
@@ -16762,10 +16753,10 @@
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="C56" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="D56" t="s">
         <v>17</v>
@@ -16777,10 +16768,10 @@
     <row r="57">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="C57" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
@@ -16792,10 +16783,10 @@
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="C58" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="D58" t="s">
         <v>17</v>
@@ -16807,10 +16798,10 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="C59" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
@@ -16822,10 +16813,10 @@
     <row r="60">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="C60" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
@@ -16837,10 +16828,10 @@
     <row r="61">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C61" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
@@ -16852,10 +16843,10 @@
     <row r="62">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="C62" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
@@ -16867,10 +16858,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="C63" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
@@ -16882,10 +16873,10 @@
     <row r="64">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C64" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
@@ -16897,10 +16888,10 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C65" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
#1774 Separated address fields on Case and Contact detailed export
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -3787,6 +3787,30 @@
     <t>Attending clinician</t>
   </si>
   <si>
+    <t>caze</t>
+  </si>
+  <si>
+    <t>CaseReference</t>
+  </si>
+  <si>
+    <t>Source case</t>
+  </si>
+  <si>
+    <t>caseIdExternalSystem</t>
+  </si>
+  <si>
+    <t>Case ID in external system</t>
+  </si>
+  <si>
+    <t>caseOrEventInformation</t>
+  </si>
+  <si>
+    <t>Case or event information</t>
+  </si>
+  <si>
+    <t>Disease of source case</t>
+  </si>
+  <si>
     <t>reportDateTime</t>
   </si>
   <si>
@@ -3802,117 +3826,141 @@
     <t>Responsible district</t>
   </si>
   <si>
+    <t>lastContactDate</t>
+  </si>
+  <si>
+    <t>Date of last contact</t>
+  </si>
+  <si>
+    <t>contactProximity</t>
+  </si>
+  <si>
+    <t>ContactProximity</t>
+  </si>
+  <si>
+    <t>Type of contact - if multiple pick the closest contact proximity</t>
+  </si>
+  <si>
+    <t>Select the type of contact with the case</t>
+  </si>
+  <si>
+    <t>contactProximityDetails</t>
+  </si>
+  <si>
+    <t>Additional information on the type of contact</t>
+  </si>
+  <si>
+    <t>contactCategory</t>
+  </si>
+  <si>
+    <t>ContactCategory</t>
+  </si>
+  <si>
+    <t>Contact Category</t>
+  </si>
+  <si>
+    <t>contactClassification</t>
+  </si>
+  <si>
+    <t>ContactClassification</t>
+  </si>
+  <si>
+    <t>Contact classification</t>
+  </si>
+  <si>
+    <t>contactStatus</t>
+  </si>
+  <si>
+    <t>ContactStatus</t>
+  </si>
+  <si>
+    <t>Contact status</t>
+  </si>
+  <si>
+    <t>followUpStatus</t>
+  </si>
+  <si>
+    <t>FollowUpStatus</t>
+  </si>
+  <si>
+    <t>Follow-up status</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Under follow-up: The follow-up process is running.&lt;/li&gt;&lt;li&gt;Follow-up completed: The follow-up has been completed.&lt;/li&gt;&lt;li&gt;Follow-up canceled: The follow-up process has been canceled, e.g. because the person died or the contact became irrelevant.&lt;/li&gt;&lt;li&gt;Lost to follow-up: The follow-up process could not be continued, e.g. because the person could not be found.&lt;/li&gt;&lt;li&gt;No follow-up: No contact follow-up is being done.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>followUpComment</t>
+  </si>
+  <si>
+    <t>Follow-up status comment</t>
+  </si>
+  <si>
+    <t>followUpUntil</t>
+  </si>
+  <si>
+    <t>Follow-up until</t>
+  </si>
+  <si>
+    <t>overwriteFollowUpUntil</t>
+  </si>
+  <si>
+    <t>Overwrite follow-up until date</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Description of how contact took place</t>
+  </si>
+  <si>
+    <t>relationToCase</t>
+  </si>
+  <si>
+    <t>ContactRelation</t>
+  </si>
+  <si>
+    <t>Relationship with case</t>
+  </si>
+  <si>
+    <t>Select the person's relation to the case</t>
+  </si>
+  <si>
+    <t>relationDescription</t>
+  </si>
+  <si>
+    <t>Relationship description</t>
+  </si>
+  <si>
+    <t>highPriority</t>
+  </si>
+  <si>
+    <t>High priority contact</t>
+  </si>
+  <si>
+    <t>immunosuppressiveTherapyBasicDisease</t>
+  </si>
+  <si>
+    <t>Immunosuppressive therapy or basic disease is present</t>
+  </si>
+  <si>
+    <t>immunosuppressiveTherapyBasicDiseaseDetails</t>
+  </si>
+  <si>
+    <t>careForPeopleOver60</t>
+  </si>
+  <si>
+    <t>Is the person medically/nursingly active in the care of patients or people over 60 years of age?</t>
+  </si>
+  <si>
     <t>Contact person</t>
   </si>
   <si>
-    <t>caze</t>
-  </si>
-  <si>
-    <t>CaseReference</t>
-  </si>
-  <si>
-    <t>Source case</t>
-  </si>
-  <si>
-    <t>Disease of source case</t>
-  </si>
-  <si>
-    <t>lastContactDate</t>
-  </si>
-  <si>
-    <t>Date of last contact</t>
-  </si>
-  <si>
-    <t>contactProximity</t>
-  </si>
-  <si>
-    <t>ContactProximity</t>
-  </si>
-  <si>
-    <t>Type of contact - if multiple pick the closest contact proximity</t>
-  </si>
-  <si>
-    <t>Select the type of contact with the case</t>
-  </si>
-  <si>
-    <t>contactClassification</t>
-  </si>
-  <si>
-    <t>ContactClassification</t>
-  </si>
-  <si>
-    <t>Contact classification</t>
-  </si>
-  <si>
-    <t>contactStatus</t>
-  </si>
-  <si>
-    <t>ContactStatus</t>
-  </si>
-  <si>
-    <t>Contact status</t>
-  </si>
-  <si>
-    <t>followUpStatus</t>
-  </si>
-  <si>
-    <t>FollowUpStatus</t>
-  </si>
-  <si>
-    <t>Follow-up status</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Under follow-up: The follow-up process is running.&lt;/li&gt;&lt;li&gt;Follow-up completed: The follow-up has been completed.&lt;/li&gt;&lt;li&gt;Follow-up canceled: The follow-up process has been canceled, e.g. because the person died or the contact became irrelevant.&lt;/li&gt;&lt;li&gt;Lost to follow-up: The follow-up process could not be continued, e.g. because the person could not be found.&lt;/li&gt;&lt;li&gt;No follow-up: No contact follow-up is being done.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>followUpComment</t>
-  </si>
-  <si>
-    <t>Follow-up status comment</t>
-  </si>
-  <si>
-    <t>followUpUntil</t>
-  </si>
-  <si>
-    <t>Follow-up until</t>
-  </si>
-  <si>
-    <t>overwriteFollowUpUntil</t>
-  </si>
-  <si>
-    <t>Overwrite follow-up until date</t>
-  </si>
-  <si>
     <t>contactOfficer</t>
   </si>
   <si>
     <t>Responsible contact officer</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Description of how contact took place</t>
-  </si>
-  <si>
-    <t>relationToCase</t>
-  </si>
-  <si>
-    <t>ContactRelation</t>
-  </si>
-  <si>
-    <t>Relationship with case</t>
-  </si>
-  <si>
-    <t>Select the person's relation to the case</t>
-  </si>
-  <si>
-    <t>relationDescription</t>
-  </si>
-  <si>
-    <t>Relationship description</t>
-  </si>
-  <si>
     <t>resultingCase</t>
   </si>
   <si>
@@ -3925,54 +3973,6 @@
     <t>Resulting case assigned by</t>
   </si>
   <si>
-    <t>highPriority</t>
-  </si>
-  <si>
-    <t>High priority contact</t>
-  </si>
-  <si>
-    <t>immunosuppressiveTherapyBasicDisease</t>
-  </si>
-  <si>
-    <t>Immunosuppressive therapy or basic disease is present</t>
-  </si>
-  <si>
-    <t>immunosuppressiveTherapyBasicDiseaseDetails</t>
-  </si>
-  <si>
-    <t>careForPeopleOver60</t>
-  </si>
-  <si>
-    <t>Is the person medically/nursingly active in the care of patients or people over 60 years of age?</t>
-  </si>
-  <si>
-    <t>caseIdExternalSystem</t>
-  </si>
-  <si>
-    <t>Case ID in external system</t>
-  </si>
-  <si>
-    <t>caseOrEventInformation</t>
-  </si>
-  <si>
-    <t>Case or event information</t>
-  </si>
-  <si>
-    <t>contactProximityDetails</t>
-  </si>
-  <si>
-    <t>Additional information on the type of contact</t>
-  </si>
-  <si>
-    <t>contactCategory</t>
-  </si>
-  <si>
-    <t>ContactCategory</t>
-  </si>
-  <si>
-    <t>Contact Category</t>
-  </si>
-  <si>
     <t>TOUCHED_FLUID</t>
   </si>
   <si>
@@ -4051,6 +4051,24 @@
     <t>Medical personnel at save proximity (&gt; 2 meter), without direct contact with secretions or excretions of the patient and without aerosol exposure</t>
   </si>
   <si>
+    <t>HIGH_RISK</t>
+  </si>
+  <si>
+    <t>High risk contact</t>
+  </si>
+  <si>
+    <t>LOW_RISK</t>
+  </si>
+  <si>
+    <t>Low risk contact</t>
+  </si>
+  <si>
+    <t>NO_RISK</t>
+  </si>
+  <si>
+    <t>No risk contact</t>
+  </si>
+  <si>
     <t>UNCONFIRMED</t>
   </si>
   <si>
@@ -4171,24 +4189,6 @@
     <t>Provided medical care for the case</t>
   </si>
   <si>
-    <t>HIGH_RISK</t>
-  </si>
-  <si>
-    <t>High risk contact</t>
-  </si>
-  <si>
-    <t>LOW_RISK</t>
-  </si>
-  <si>
-    <t>Low risk contact</t>
-  </si>
-  <si>
-    <t>NO_RISK</t>
-  </si>
-  <si>
-    <t>No risk contact</t>
-  </si>
-  <si>
     <t>Visited person</t>
   </si>
   <si>
@@ -5473,7 +5473,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.37.0-SNAPSHOT</t>
+    <t>1.38.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -6319,7 +6319,7 @@
 </file>
 
 <file path=xl/tables/table55.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="55" name="ContactContactClassification" displayName="ContactContactClassification" ref="A113:E116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="55" name="ContactContactCategory" displayName="ContactContactCategory" ref="A113:E116">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6333,7 +6333,7 @@
 </file>
 
 <file path=xl/tables/table56.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="56" name="ContactContactStatus" displayName="ContactContactStatus" ref="A118:E121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="56" name="ContactContactClassification" displayName="ContactContactClassification" ref="A118:E121">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6347,7 +6347,7 @@
 </file>
 
 <file path=xl/tables/table57.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="ContactFollowUpStatus" displayName="ContactFollowUpStatus" ref="A123:E128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="ContactContactStatus" displayName="ContactContactStatus" ref="A123:E126">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6361,7 +6361,7 @@
 </file>
 
 <file path=xl/tables/table58.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="ContactContactRelation" displayName="ContactContactRelation" ref="A130:E135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="ContactFollowUpStatus" displayName="ContactFollowUpStatus" ref="A128:E133">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6375,7 +6375,7 @@
 </file>
 
 <file path=xl/tables/table59.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="59" name="ContactYesNoUnknown" displayName="ContactYesNoUnknown" ref="A137:E140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="59" name="ContactContactRelation" displayName="ContactContactRelation" ref="A135:E140">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6403,7 +6403,7 @@
 </file>
 
 <file path=xl/tables/table60.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="60" name="ContactQuarantineType" displayName="ContactQuarantineType" ref="A142:E146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="60" name="ContactYesNoUnknown" displayName="ContactYesNoUnknown" ref="A142:E145">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6417,7 +6417,7 @@
 </file>
 
 <file path=xl/tables/table61.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="61" name="ContactContactCategory" displayName="ContactContactCategory" ref="A148:E151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="61" name="ContactQuarantineType" displayName="ContactQuarantineType" ref="A147:E151">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -10555,17 +10555,15 @@
         <v>1250</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>39</v>
+        <v>1251</v>
       </c>
       <c r="C2" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E2"/>
       <c r="G2" s="11" t="s">
         <v>12</v>
       </c>
@@ -10573,20 +10571,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>363</v>
+        <v>1253</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>364</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>365</v>
+        <v>1254</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
+      <c r="E3"/>
       <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
@@ -10594,13 +10590,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>439</v>
+        <v>1255</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>1256</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>18</v>
@@ -10613,13 +10609,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>442</v>
+        <v>343</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>1257</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>18</v>
@@ -10632,13 +10628,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>445</v>
+        <v>345</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>346</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>18</v>
@@ -10651,18 +10647,20 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>1258</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>1252</v>
+        <v>1259</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>1253</v>
-      </c>
-      <c r="E7"/>
+        <v>18</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
       <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
@@ -10670,18 +10668,20 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>314</v>
+        <v>363</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>46</v>
+        <v>364</v>
       </c>
       <c r="C8" t="s">
-        <v>1254</v>
+        <v>365</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>1253</v>
-      </c>
-      <c r="E8"/>
+        <v>18</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
       <c r="G8" s="11" t="s">
         <v>12</v>
       </c>
@@ -10689,20 +10689,18 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>356</v>
+        <v>439</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>357</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>1255</v>
+        <v>18</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
+      <c r="E9"/>
       <c r="G9" s="11" t="s">
         <v>12</v>
       </c>
@@ -10710,20 +10708,18 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1256</v>
+        <v>442</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>1257</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>1258</v>
+        <v>18</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
+      <c r="E10"/>
       <c r="G10" s="11" t="s">
         <v>12</v>
       </c>
@@ -10731,13 +10727,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>343</v>
+        <v>445</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>1259</v>
+        <v>18</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>18</v>
@@ -10750,16 +10746,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>345</v>
+        <v>312</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>346</v>
+        <v>1260</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>18</v>
+        <v>1261</v>
       </c>
       <c r="E12"/>
       <c r="G12" s="11" t="s">
@@ -10769,16 +10765,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1260</v>
+        <v>314</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>1261</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="E13"/>
       <c r="G13" s="11" t="s">
@@ -10788,18 +10784,20 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>1263</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>1264</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>1265</v>
-      </c>
-      <c r="E14"/>
+        <v>18</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
       <c r="G14" s="11" t="s">
         <v>12</v>
       </c>
@@ -10807,16 +10805,16 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>1266</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="11" t="s">
         <v>1268</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="E15"/>
       <c r="G15" s="11" t="s">
@@ -10829,10 +10827,10 @@
         <v>1269</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
         <v>1270</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1271</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>18</v>
@@ -10845,16 +10843,16 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>1272</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" t="s">
         <v>1273</v>
       </c>
-      <c r="C17" t="s">
-        <v>1274</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>1275</v>
+        <v>18</v>
       </c>
       <c r="E17"/>
       <c r="G17" s="11" t="s">
@@ -10864,13 +10862,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C18" t="s">
         <v>1276</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1277</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>18</v>
@@ -10883,10 +10881,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>1278</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>1279</v>
@@ -10905,13 +10903,13 @@
         <v>1280</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>480</v>
+        <v>1281</v>
       </c>
       <c r="C20" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>18</v>
+        <v>1283</v>
       </c>
       <c r="E20"/>
       <c r="G20" s="11" t="s">
@@ -10921,13 +10919,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>364</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>18</v>
@@ -10940,13 +10938,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>18</v>
@@ -10959,16 +10957,16 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1287</v>
+        <v>480</v>
       </c>
       <c r="C23" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>1289</v>
+        <v>18</v>
       </c>
       <c r="E23"/>
       <c r="G23" s="11" t="s">
@@ -10997,16 +10995,16 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>477</v>
+        <v>1292</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>9</v>
+        <v>1293</v>
       </c>
       <c r="C25" t="s">
-        <v>478</v>
+        <v>1294</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>18</v>
+        <v>1295</v>
       </c>
       <c r="E25"/>
       <c r="G25" s="11" t="s">
@@ -11016,13 +11014,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>1292</v>
+        <v>1296</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>1257</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>1293</v>
+        <v>1297</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>18</v>
@@ -11035,13 +11033,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1294</v>
+        <v>477</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>364</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>1295</v>
+        <v>478</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>18</v>
@@ -11054,13 +11052,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>480</v>
       </c>
       <c r="C28" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>18</v>
@@ -11073,13 +11071,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C29" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>18</v>
@@ -11092,7 +11090,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>9</v>
@@ -11111,13 +11109,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C31" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>18</v>
@@ -11187,18 +11185,20 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>1303</v>
+        <v>356</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>9</v>
+        <v>357</v>
       </c>
       <c r="C35" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E35"/>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
       <c r="G35" s="11" t="s">
         <v>12</v>
       </c>
@@ -11206,13 +11206,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>9</v>
+        <v>364</v>
       </c>
       <c r="C36" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>18</v>
@@ -11225,13 +11225,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>9</v>
+        <v>1251</v>
       </c>
       <c r="C37" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>18</v>
@@ -11244,10 +11244,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>1310</v>
+        <v>364</v>
       </c>
       <c r="C38" t="s">
         <v>1311</v>
@@ -12139,7 +12139,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="B99" t="s">
         <v>1312</v>
@@ -12353,7 +12353,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>1267</v>
+        <v>1272</v>
       </c>
       <c r="B114" t="s">
         <v>1338</v>
@@ -12365,13 +12365,13 @@
         <v>18</v>
       </c>
       <c r="E114" t="s">
-        <v>1340</v>
+        <v>18</v>
       </c>
     </row>
     <row r="115">
       <c r="A115"/>
       <c r="B115" t="s">
-        <v>513</v>
+        <v>1340</v>
       </c>
       <c r="C115" t="s">
         <v>1341</v>
@@ -12380,7 +12380,7 @@
         <v>18</v>
       </c>
       <c r="E115" t="s">
-        <v>515</v>
+        <v>18</v>
       </c>
     </row>
     <row r="116">
@@ -12395,7 +12395,7 @@
         <v>18</v>
       </c>
       <c r="E116" t="s">
-        <v>1344</v>
+        <v>18</v>
       </c>
     </row>
     <row r="118">
@@ -12417,49 +12417,49 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>1270</v>
+        <v>1275</v>
       </c>
       <c r="B119" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C119" t="s">
         <v>1345</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
+        <v>18</v>
+      </c>
+      <c r="E119" t="s">
         <v>1346</v>
-      </c>
-      <c r="D119" t="s">
-        <v>18</v>
-      </c>
-      <c r="E119" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="120">
       <c r="A120"/>
       <c r="B120" t="s">
+        <v>513</v>
+      </c>
+      <c r="C120" t="s">
         <v>1347</v>
       </c>
-      <c r="C120" t="s">
-        <v>1348</v>
-      </c>
       <c r="D120" t="s">
         <v>18</v>
       </c>
       <c r="E120" t="s">
-        <v>18</v>
+        <v>515</v>
       </c>
     </row>
     <row r="121">
       <c r="A121"/>
       <c r="B121" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C121" t="s">
         <v>1349</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
+        <v>18</v>
+      </c>
+      <c r="E121" t="s">
         <v>1350</v>
-      </c>
-      <c r="D121" t="s">
-        <v>18</v>
-      </c>
-      <c r="E121" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="123">
@@ -12481,7 +12481,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>1273</v>
+        <v>1278</v>
       </c>
       <c r="B124" t="s">
         <v>1351</v>
@@ -12490,192 +12490,192 @@
         <v>1352</v>
       </c>
       <c r="D124" t="s">
-        <v>1353</v>
+        <v>18</v>
       </c>
       <c r="E124" t="s">
-        <v>1354</v>
+        <v>18</v>
       </c>
     </row>
     <row r="125">
       <c r="A125"/>
       <c r="B125" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C125" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="D125" t="s">
-        <v>1357</v>
+        <v>18</v>
       </c>
       <c r="E125" t="s">
-        <v>1358</v>
+        <v>18</v>
       </c>
     </row>
     <row r="126">
       <c r="A126"/>
       <c r="B126" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E126" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>1</v>
+      </c>
+      <c r="B128" t="s">
+        <v>123</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+      <c r="D128" t="s">
+        <v>3</v>
+      </c>
+      <c r="E128" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D129" t="s">
         <v>1359</v>
       </c>
-      <c r="C126" t="s">
+      <c r="E129" t="s">
         <v>1360</v>
       </c>
-      <c r="D126" t="s">
+    </row>
+    <row r="130">
+      <c r="A130"/>
+      <c r="B130" t="s">
         <v>1361</v>
       </c>
-      <c r="E126" t="s">
+      <c r="C130" t="s">
         <v>1362</v>
       </c>
-    </row>
-    <row r="127">
-      <c r="A127"/>
-      <c r="B127" t="s">
+      <c r="D130" t="s">
         <v>1363</v>
       </c>
-      <c r="C127" t="s">
+      <c r="E130" t="s">
         <v>1364</v>
       </c>
-      <c r="D127" t="s">
+    </row>
+    <row r="131">
+      <c r="A131"/>
+      <c r="B131" t="s">
         <v>1365</v>
       </c>
-      <c r="E127" t="s">
+      <c r="C131" t="s">
         <v>1366</v>
       </c>
-    </row>
-    <row r="128">
-      <c r="A128"/>
-      <c r="B128" t="s">
+      <c r="D131" t="s">
         <v>1367</v>
       </c>
-      <c r="C128" t="s">
+      <c r="E131" t="s">
         <v>1368</v>
-      </c>
-      <c r="D128" t="s">
-        <v>1369</v>
-      </c>
-      <c r="E128" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="s">
-        <v>1</v>
-      </c>
-      <c r="B130" t="s">
-        <v>123</v>
-      </c>
-      <c r="C130" t="s">
-        <v>2</v>
-      </c>
-      <c r="D130" t="s">
-        <v>3</v>
-      </c>
-      <c r="E130" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="s">
-        <v>1287</v>
-      </c>
-      <c r="B131" t="s">
-        <v>1370</v>
-      </c>
-      <c r="C131" t="s">
-        <v>1371</v>
-      </c>
-      <c r="D131" t="s">
-        <v>18</v>
-      </c>
-      <c r="E131" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="132">
       <c r="A132"/>
       <c r="B132" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D132" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E132" t="s">
         <v>1372</v>
-      </c>
-      <c r="C132" t="s">
-        <v>1373</v>
-      </c>
-      <c r="D132" t="s">
-        <v>18</v>
-      </c>
-      <c r="E132" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="133">
       <c r="A133"/>
       <c r="B133" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C133" t="s">
         <v>1374</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>1375</v>
       </c>
-      <c r="D133" t="s">
-        <v>18</v>
-      </c>
       <c r="E133" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134"/>
-      <c r="B134" t="s">
+    <row r="135">
+      <c r="A135" t="s">
+        <v>1</v>
+      </c>
+      <c r="B135" t="s">
+        <v>123</v>
+      </c>
+      <c r="C135" t="s">
+        <v>2</v>
+      </c>
+      <c r="D135" t="s">
+        <v>3</v>
+      </c>
+      <c r="E135" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B136" t="s">
         <v>1376</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C136" t="s">
         <v>1377</v>
       </c>
-      <c r="D134" t="s">
-        <v>18</v>
-      </c>
-      <c r="E134" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135"/>
-      <c r="B135" t="s">
-        <v>260</v>
-      </c>
-      <c r="C135" t="s">
-        <v>262</v>
-      </c>
-      <c r="D135" t="s">
-        <v>18</v>
-      </c>
-      <c r="E135" t="s">
+      <c r="D136" t="s">
+        <v>18</v>
+      </c>
+      <c r="E136" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="s">
-        <v>1</v>
-      </c>
+      <c r="A137"/>
       <c r="B137" t="s">
-        <v>123</v>
+        <v>1378</v>
       </c>
       <c r="C137" t="s">
-        <v>2</v>
+        <v>1379</v>
       </c>
       <c r="D137" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E137" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="s">
-        <v>393</v>
-      </c>
+      <c r="A138"/>
       <c r="B138" t="s">
-        <v>534</v>
+        <v>1380</v>
       </c>
       <c r="C138" t="s">
-        <v>535</v>
+        <v>1381</v>
       </c>
       <c r="D138" t="s">
         <v>18</v>
@@ -12687,10 +12687,10 @@
     <row r="139">
       <c r="A139"/>
       <c r="B139" t="s">
-        <v>536</v>
+        <v>1382</v>
       </c>
       <c r="C139" t="s">
-        <v>537</v>
+        <v>1383</v>
       </c>
       <c r="D139" t="s">
         <v>18</v>
@@ -12702,10 +12702,10 @@
     <row r="140">
       <c r="A140"/>
       <c r="B140" t="s">
-        <v>341</v>
+        <v>260</v>
       </c>
       <c r="C140" t="s">
-        <v>342</v>
+        <v>262</v>
       </c>
       <c r="D140" t="s">
         <v>18</v>
@@ -12733,13 +12733,13 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>483</v>
+        <v>393</v>
       </c>
       <c r="B143" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
       <c r="C143" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
       <c r="D143" t="s">
         <v>18</v>
@@ -12751,10 +12751,10 @@
     <row r="144">
       <c r="A144"/>
       <c r="B144" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
       <c r="C144" t="s">
-        <v>563</v>
+        <v>537</v>
       </c>
       <c r="D144" t="s">
         <v>18</v>
@@ -12766,10 +12766,10 @@
     <row r="145">
       <c r="A145"/>
       <c r="B145" t="s">
-        <v>274</v>
+        <v>341</v>
       </c>
       <c r="C145" t="s">
-        <v>564</v>
+        <v>342</v>
       </c>
       <c r="D145" t="s">
         <v>18</v>
@@ -12778,47 +12778,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146"/>
-      <c r="B146" t="s">
-        <v>341</v>
-      </c>
-      <c r="C146" t="s">
-        <v>342</v>
-      </c>
-      <c r="D146" t="s">
-        <v>18</v>
-      </c>
-      <c r="E146" t="s">
-        <v>18</v>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>1</v>
+      </c>
+      <c r="B147" t="s">
+        <v>123</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+      <c r="D147" t="s">
+        <v>3</v>
+      </c>
+      <c r="E147" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>1</v>
+        <v>483</v>
       </c>
       <c r="B148" t="s">
-        <v>123</v>
+        <v>560</v>
       </c>
       <c r="C148" t="s">
-        <v>2</v>
+        <v>561</v>
       </c>
       <c r="D148" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E148" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="s">
-        <v>1310</v>
-      </c>
+      <c r="A149"/>
       <c r="B149" t="s">
-        <v>1378</v>
+        <v>562</v>
       </c>
       <c r="C149" t="s">
-        <v>1379</v>
+        <v>563</v>
       </c>
       <c r="D149" t="s">
         <v>18</v>
@@ -12830,10 +12830,10 @@
     <row r="150">
       <c r="A150"/>
       <c r="B150" t="s">
-        <v>1380</v>
+        <v>274</v>
       </c>
       <c r="C150" t="s">
-        <v>1381</v>
+        <v>564</v>
       </c>
       <c r="D150" t="s">
         <v>18</v>
@@ -12845,10 +12845,10 @@
     <row r="151">
       <c r="A151"/>
       <c r="B151" t="s">
-        <v>1382</v>
+        <v>341</v>
       </c>
       <c r="C151" t="s">
-        <v>1383</v>
+        <v>342</v>
       </c>
       <c r="D151" t="s">
         <v>18</v>
@@ -14098,7 +14098,7 @@
         <v>1402</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="C2" t="s">
         <v>1403</v>
@@ -14156,7 +14156,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1250</v>
+        <v>1258</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>39</v>
@@ -17446,10 +17446,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="C3" t="s">
         <v>1403</v>
@@ -18448,7 +18448,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1250</v>
+        <v>1258</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>39</v>
@@ -19900,10 +19900,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1292</v>
+        <v>1308</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
#2206: Code formatting with Eclipse 2020-03: sormas-api
- Added some missing serialVersionUID
- Added sometimes blank lines after method declaration
- @formatter:off for formatted query DTO constructors
- @formatter:off for HTML definitions
- Removed some empty blocks (usually from enum toString methods)
- Tests: throws Exception removed, method names changed to pattern
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6812" uniqueCount="1906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6824" uniqueCount="1912">
   <si>
     <t>Field</t>
   </si>
@@ -4264,10 +4264,10 @@
     <t>Face-to-face contact of at least 15 minutes</t>
   </si>
   <si>
-    <t>MEDICAL_UNSAVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical personal at close proximity (2 meter) without protective equipment		</t>
+    <t>MEDICAL_UNSAFE</t>
+  </si>
+  <si>
+    <t>Medical personnel with a high risk of exposure, e.g. unprotected relevant exposure to secretions, exposure to aerosols from COVID-19 cases</t>
   </si>
   <si>
     <t>SAME_ROOM</t>
@@ -4288,16 +4288,16 @@
     <t>Face-to-face contact of less than 15 minutes</t>
   </si>
   <si>
-    <t>MEDICAL_SAVE</t>
-  </si>
-  <si>
-    <t>Medical personal at save proximity (&gt; 2 meter) or with protective equipment</t>
+    <t>MEDICAL_SAFE</t>
+  </si>
+  <si>
+    <t>Medical personnel at save proximity (&gt; 2 meter) or with protective equipment</t>
   </si>
   <si>
     <t>MEDICAL_SAME_ROOM</t>
   </si>
   <si>
-    <t>Medical personal that was in same room or house with source case</t>
+    <t>Medical personnel that was in same room or house with source case</t>
   </si>
   <si>
     <t>AEROSOL</t>
@@ -4312,12 +4312,30 @@
     <t>Medical personnel at save proximity (&gt; 2 meter), without direct contact with secretions or excretions of the patient and without aerosol exposure</t>
   </si>
   <si>
+    <t>MEDICAL_LIMITED</t>
+  </si>
+  <si>
+    <t>Medical personnel with limited exposure, e.g. with contact &lt; 2m to COVID-19 cases without protective equipment, ≥ 15min face-to-face contact (without exposure as described under Ia)</t>
+  </si>
+  <si>
     <t>HIGH_RISK</t>
   </si>
   <si>
     <t>High risk contact</t>
   </si>
   <si>
+    <t>HIGH_RISK_MED</t>
+  </si>
+  <si>
+    <t>High risk medical contact</t>
+  </si>
+  <si>
+    <t>MEDIUM_RISK_MED</t>
+  </si>
+  <si>
+    <t>Medium risk medical contact</t>
+  </si>
+  <si>
     <t>LOW_RISK</t>
   </si>
   <si>
@@ -5752,7 +5770,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.41.0-SNAPSHOT</t>
+    <t>1.42.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -6598,7 +6616,7 @@
 </file>
 
 <file path=xl/tables/table55.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="55" name="ContactContactProximity" displayName="ContactContactProximity" ref="A108:E121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="55" name="ContactContactProximity" displayName="ContactContactProximity" ref="A108:E122">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6612,7 +6630,7 @@
 </file>
 
 <file path=xl/tables/table56.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="56" name="ContactContactCategory" displayName="ContactContactCategory" ref="A123:E126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="56" name="ContactContactCategory" displayName="ContactContactCategory" ref="A124:E129">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6626,7 +6644,7 @@
 </file>
 
 <file path=xl/tables/table57.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="ContactContactClassification" displayName="ContactContactClassification" ref="A128:E131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="ContactContactClassification" displayName="ContactContactClassification" ref="A131:E134">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6640,7 +6658,7 @@
 </file>
 
 <file path=xl/tables/table58.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="ContactContactStatus" displayName="ContactContactStatus" ref="A133:E136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="ContactContactStatus" displayName="ContactContactStatus" ref="A136:E139">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6654,7 +6672,7 @@
 </file>
 
 <file path=xl/tables/table59.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="59" name="ContactFollowUpStatus" displayName="ContactFollowUpStatus" ref="A138:E143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="59" name="ContactFollowUpStatus" displayName="ContactFollowUpStatus" ref="A141:E146">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6682,7 +6700,7 @@
 </file>
 
 <file path=xl/tables/table60.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="60" name="ContactContactRelation" displayName="ContactContactRelation" ref="A145:E150">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="60" name="ContactContactRelation" displayName="ContactContactRelation" ref="A148:E153">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6696,7 +6714,7 @@
 </file>
 
 <file path=xl/tables/table61.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="61" name="ContactYesNoUnknown" displayName="ContactYesNoUnknown" ref="A152:E155">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="61" name="ContactYesNoUnknown" displayName="ContactYesNoUnknown" ref="A155:E158">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6710,7 +6728,7 @@
 </file>
 
 <file path=xl/tables/table62.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="62" name="ContactQuarantineType" displayName="ContactQuarantineType" ref="A157:E161">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="62" name="ContactQuarantineType" displayName="ContactQuarantineType" ref="A160:E164">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -10801,7 +10819,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -12817,42 +12835,42 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" t="s">
-        <v>1</v>
-      </c>
-      <c r="B123" t="s">
-        <v>123</v>
-      </c>
-      <c r="C123" t="s">
-        <v>2</v>
-      </c>
-      <c r="D123" t="s">
-        <v>3</v>
-      </c>
-      <c r="E123" t="s">
-        <v>124</v>
+    <row r="122">
+      <c r="A122"/>
+      <c r="B122" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C122" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D122" t="s">
+        <v>18</v>
+      </c>
+      <c r="E122" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
+        <v>1</v>
+      </c>
+      <c r="B124" t="s">
+        <v>123</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" t="s">
+        <v>3</v>
+      </c>
+      <c r="E124" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
         <v>1359</v>
       </c>
-      <c r="B124" t="s">
-        <v>1425</v>
-      </c>
-      <c r="C124" t="s">
-        <v>1426</v>
-      </c>
-      <c r="D124" t="s">
-        <v>18</v>
-      </c>
-      <c r="E124" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125"/>
       <c r="B125" t="s">
         <v>1427</v>
       </c>
@@ -12881,294 +12899,294 @@
         <v>18</v>
       </c>
     </row>
+    <row r="127">
+      <c r="A127"/>
+      <c r="B127" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D127" t="s">
+        <v>18</v>
+      </c>
+      <c r="E127" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="128">
-      <c r="A128" t="s">
+      <c r="A128"/>
+      <c r="B128" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D128" t="s">
+        <v>18</v>
+      </c>
+      <c r="E128" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129"/>
+      <c r="B129" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D129" t="s">
+        <v>18</v>
+      </c>
+      <c r="E129" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
         <v>1</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B131" t="s">
         <v>123</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C131" t="s">
         <v>2</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D131" t="s">
         <v>3</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E131" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" t="s">
+    <row r="132">
+      <c r="A132" t="s">
         <v>1362</v>
       </c>
-      <c r="B129" t="s">
-        <v>1431</v>
-      </c>
-      <c r="C129" t="s">
-        <v>1432</v>
-      </c>
-      <c r="D129" t="s">
-        <v>18</v>
-      </c>
-      <c r="E129" t="s">
-        <v>1433</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130"/>
-      <c r="B130" t="s">
+      <c r="B132" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D132" t="s">
+        <v>18</v>
+      </c>
+      <c r="E132" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133"/>
+      <c r="B133" t="s">
         <v>536</v>
       </c>
-      <c r="C130" t="s">
-        <v>1434</v>
-      </c>
-      <c r="D130" t="s">
-        <v>18</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="C133" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D133" t="s">
+        <v>18</v>
+      </c>
+      <c r="E133" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131"/>
-      <c r="B131" t="s">
-        <v>1435</v>
-      </c>
-      <c r="C131" t="s">
-        <v>1436</v>
-      </c>
-      <c r="D131" t="s">
-        <v>18</v>
-      </c>
-      <c r="E131" t="s">
-        <v>1437</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="s">
+    <row r="134">
+      <c r="A134"/>
+      <c r="B134" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D134" t="s">
+        <v>18</v>
+      </c>
+      <c r="E134" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
         <v>1</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B136" t="s">
         <v>123</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C136" t="s">
         <v>2</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D136" t="s">
         <v>3</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E136" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" t="s">
+    <row r="137">
+      <c r="A137" t="s">
         <v>1365</v>
       </c>
-      <c r="B134" t="s">
-        <v>1438</v>
-      </c>
-      <c r="C134" t="s">
-        <v>1439</v>
-      </c>
-      <c r="D134" t="s">
-        <v>18</v>
-      </c>
-      <c r="E134" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135"/>
-      <c r="B135" t="s">
-        <v>1440</v>
-      </c>
-      <c r="C135" t="s">
-        <v>1441</v>
-      </c>
-      <c r="D135" t="s">
-        <v>18</v>
-      </c>
-      <c r="E135" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136"/>
-      <c r="B136" t="s">
-        <v>1442</v>
-      </c>
-      <c r="C136" t="s">
-        <v>1443</v>
-      </c>
-      <c r="D136" t="s">
-        <v>18</v>
-      </c>
-      <c r="E136" t="s">
+      <c r="B137" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D137" t="s">
+        <v>18</v>
+      </c>
+      <c r="E137" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="s">
+      <c r="A138"/>
+      <c r="B138" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D138" t="s">
+        <v>18</v>
+      </c>
+      <c r="E138" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139"/>
+      <c r="B139" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C139" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D139" t="s">
+        <v>18</v>
+      </c>
+      <c r="E139" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
         <v>1</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B141" t="s">
         <v>123</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C141" t="s">
         <v>2</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D141" t="s">
         <v>3</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E141" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" t="s">
+    <row r="142">
+      <c r="A142" t="s">
         <v>1368</v>
       </c>
-      <c r="B139" t="s">
-        <v>1444</v>
-      </c>
-      <c r="C139" t="s">
-        <v>1445</v>
-      </c>
-      <c r="D139" t="s">
-        <v>1446</v>
-      </c>
-      <c r="E139" t="s">
-        <v>1447</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140"/>
-      <c r="B140" t="s">
-        <v>1448</v>
-      </c>
-      <c r="C140" t="s">
-        <v>1449</v>
-      </c>
-      <c r="D140" t="s">
+      <c r="B142" t="s">
         <v>1450</v>
       </c>
-      <c r="E140" t="s">
+      <c r="C142" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="141">
-      <c r="A141"/>
-      <c r="B141" t="s">
+      <c r="D142" t="s">
         <v>1452</v>
       </c>
-      <c r="C141" t="s">
+      <c r="E142" t="s">
         <v>1453</v>
-      </c>
-      <c r="D141" t="s">
-        <v>1454</v>
-      </c>
-      <c r="E141" t="s">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142"/>
-      <c r="B142" t="s">
-        <v>1456</v>
-      </c>
-      <c r="C142" t="s">
-        <v>1457</v>
-      </c>
-      <c r="D142" t="s">
-        <v>1458</v>
-      </c>
-      <c r="E142" t="s">
-        <v>1459</v>
       </c>
     </row>
     <row r="143">
       <c r="A143"/>
       <c r="B143" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E143" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144"/>
+      <c r="B144" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D144" t="s">
         <v>1460</v>
       </c>
-      <c r="C143" t="s">
+      <c r="E144" t="s">
         <v>1461</v>
       </c>
-      <c r="D143" t="s">
+    </row>
+    <row r="145">
+      <c r="A145"/>
+      <c r="B145" t="s">
         <v>1462</v>
       </c>
-      <c r="E143" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="s">
+      <c r="C145" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D145" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E145" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146"/>
+      <c r="B146" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C146" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D146" t="s">
+        <v>1468</v>
+      </c>
+      <c r="E146" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
         <v>1</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B148" t="s">
         <v>123</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C148" t="s">
         <v>2</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D148" t="s">
         <v>3</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E148" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" t="s">
+    <row r="149">
+      <c r="A149" t="s">
         <v>1380</v>
       </c>
-      <c r="B146" t="s">
-        <v>1463</v>
-      </c>
-      <c r="C146" t="s">
-        <v>1464</v>
-      </c>
-      <c r="D146" t="s">
-        <v>18</v>
-      </c>
-      <c r="E146" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147"/>
-      <c r="B147" t="s">
-        <v>1465</v>
-      </c>
-      <c r="C147" t="s">
-        <v>1466</v>
-      </c>
-      <c r="D147" t="s">
-        <v>18</v>
-      </c>
-      <c r="E147" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148"/>
-      <c r="B148" t="s">
-        <v>1467</v>
-      </c>
-      <c r="C148" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D148" t="s">
-        <v>18</v>
-      </c>
-      <c r="E148" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149"/>
       <c r="B149" t="s">
         <v>1469</v>
       </c>
@@ -13185,158 +13203,203 @@
     <row r="150">
       <c r="A150"/>
       <c r="B150" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D150" t="s">
+        <v>18</v>
+      </c>
+      <c r="E150" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151"/>
+      <c r="B151" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D151" t="s">
+        <v>18</v>
+      </c>
+      <c r="E151" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152"/>
+      <c r="B152" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D152" t="s">
+        <v>18</v>
+      </c>
+      <c r="E152" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153"/>
+      <c r="B153" t="s">
         <v>260</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C153" t="s">
         <v>262</v>
       </c>
-      <c r="D150" t="s">
-        <v>18</v>
-      </c>
-      <c r="E150" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="s">
+      <c r="D153" t="s">
+        <v>18</v>
+      </c>
+      <c r="E153" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
         <v>1</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B155" t="s">
         <v>123</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C155" t="s">
         <v>2</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D155" t="s">
         <v>3</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E155" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" t="s">
+    <row r="156">
+      <c r="A156" t="s">
         <v>393</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B156" t="s">
         <v>557</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C156" t="s">
         <v>558</v>
       </c>
-      <c r="D153" t="s">
-        <v>18</v>
-      </c>
-      <c r="E153" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154"/>
-      <c r="B154" t="s">
+      <c r="D156" t="s">
+        <v>18</v>
+      </c>
+      <c r="E156" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157"/>
+      <c r="B157" t="s">
         <v>559</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C157" t="s">
         <v>560</v>
       </c>
-      <c r="D154" t="s">
-        <v>18</v>
-      </c>
-      <c r="E154" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155"/>
-      <c r="B155" t="s">
+      <c r="D157" t="s">
+        <v>18</v>
+      </c>
+      <c r="E157" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158"/>
+      <c r="B158" t="s">
         <v>341</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C158" t="s">
         <v>342</v>
       </c>
-      <c r="D155" t="s">
-        <v>18</v>
-      </c>
-      <c r="E155" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="s">
+      <c r="D158" t="s">
+        <v>18</v>
+      </c>
+      <c r="E158" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
         <v>1</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B160" t="s">
         <v>123</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C160" t="s">
         <v>2</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D160" t="s">
         <v>3</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E160" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" t="s">
+    <row r="161">
+      <c r="A161" t="s">
         <v>483</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B161" t="s">
         <v>583</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C161" t="s">
         <v>584</v>
       </c>
-      <c r="D158" t="s">
-        <v>18</v>
-      </c>
-      <c r="E158" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159"/>
-      <c r="B159" t="s">
+      <c r="D161" t="s">
+        <v>18</v>
+      </c>
+      <c r="E161" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162"/>
+      <c r="B162" t="s">
         <v>585</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C162" t="s">
         <v>586</v>
       </c>
-      <c r="D159" t="s">
-        <v>18</v>
-      </c>
-      <c r="E159" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160"/>
-      <c r="B160" t="s">
+      <c r="D162" t="s">
+        <v>18</v>
+      </c>
+      <c r="E162" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163"/>
+      <c r="B163" t="s">
         <v>274</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C163" t="s">
         <v>587</v>
       </c>
-      <c r="D160" t="s">
-        <v>18</v>
-      </c>
-      <c r="E160" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161"/>
-      <c r="B161" t="s">
+      <c r="D163" t="s">
+        <v>18</v>
+      </c>
+      <c r="E163" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164"/>
+      <c r="B164" t="s">
         <v>341</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C164" t="s">
         <v>342</v>
       </c>
-      <c r="D161" t="s">
-        <v>18</v>
-      </c>
-      <c r="E161" t="s">
+      <c r="D164" t="s">
+        <v>18</v>
+      </c>
+      <c r="E164" t="s">
         <v>18</v>
       </c>
     </row>
@@ -13409,7 +13472,7 @@
         <v>357</v>
       </c>
       <c r="C2" t="s">
-        <v>1471</v>
+        <v>1477</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>18</v>
@@ -13452,7 +13515,7 @@
         <v>1332</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>1472</v>
+        <v>1478</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -13464,13 +13527,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1473</v>
+        <v>1479</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>364</v>
       </c>
       <c r="C5" t="s">
-        <v>1474</v>
+        <v>1480</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>18</v>
@@ -13485,16 +13548,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1475</v>
+        <v>1481</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>1476</v>
+        <v>1482</v>
       </c>
       <c r="C6" t="s">
-        <v>1477</v>
+        <v>1483</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>1478</v>
+        <v>1484</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -13512,10 +13575,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>1479</v>
+        <v>1485</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>1480</v>
+        <v>1486</v>
       </c>
       <c r="E7"/>
       <c r="G7" s="12" t="s">
@@ -13550,7 +13613,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>1481</v>
+        <v>1487</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -13569,7 +13632,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>1482</v>
+        <v>1488</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>18</v>
@@ -14477,13 +14540,13 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>1476</v>
+        <v>1482</v>
       </c>
       <c r="B72" t="s">
-        <v>1483</v>
+        <v>1489</v>
       </c>
       <c r="C72" t="s">
-        <v>1484</v>
+        <v>1490</v>
       </c>
       <c r="D72" t="s">
         <v>18</v>
@@ -14495,31 +14558,31 @@
     <row r="73">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>1485</v>
+        <v>1491</v>
       </c>
       <c r="C73" t="s">
-        <v>1486</v>
+        <v>1492</v>
       </c>
       <c r="D73" t="s">
         <v>18</v>
       </c>
       <c r="E73" t="s">
-        <v>1487</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="74">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>1488</v>
+        <v>1494</v>
       </c>
       <c r="C74" t="s">
-        <v>1489</v>
+        <v>1495</v>
       </c>
       <c r="D74" t="s">
         <v>18</v>
       </c>
       <c r="E74" t="s">
-        <v>1490</v>
+        <v>1496</v>
       </c>
     </row>
   </sheetData>
@@ -14578,13 +14641,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1491</v>
+        <v>1497</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>1338</v>
       </c>
       <c r="C2" t="s">
-        <v>1492</v>
+        <v>1498</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>18</v>
@@ -14597,10 +14660,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1493</v>
+        <v>1499</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>1494</v>
+        <v>1500</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -14616,13 +14679,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1495</v>
+        <v>1501</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>1496</v>
+        <v>1502</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>18</v>
@@ -14635,13 +14698,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1497</v>
+        <v>1503</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>1498</v>
+        <v>1504</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>18</v>
@@ -14654,16 +14717,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1499</v>
+        <v>1505</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>1500</v>
+        <v>1506</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>1501</v>
+        <v>1507</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -14774,13 +14837,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1502</v>
+        <v>1508</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>1503</v>
+        <v>1509</v>
       </c>
       <c r="C12" t="s">
-        <v>1504</v>
+        <v>1510</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>18</v>
@@ -14795,13 +14858,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1505</v>
+        <v>1511</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>1506</v>
+        <v>1512</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>18</v>
@@ -14814,13 +14877,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1507</v>
+        <v>1513</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>1508</v>
+        <v>1514</v>
       </c>
       <c r="C14" t="s">
-        <v>1509</v>
+        <v>1515</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>18</v>
@@ -14835,7 +14898,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1510</v>
+        <v>1516</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>52</v>
@@ -14856,13 +14919,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1511</v>
+        <v>1517</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>1512</v>
+        <v>1518</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>18</v>
@@ -14875,13 +14938,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1513</v>
+        <v>1519</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>1514</v>
+        <v>1520</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>18</v>
@@ -14894,13 +14957,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1515</v>
+        <v>1521</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>1516</v>
+        <v>1522</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>18</v>
@@ -14913,13 +14976,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>1517</v>
+        <v>1523</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>1518</v>
+        <v>1524</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>18</v>
@@ -14932,13 +14995,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>1519</v>
+        <v>1525</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>1520</v>
+        <v>1526</v>
       </c>
       <c r="C20" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>18</v>
@@ -14951,13 +15014,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>1522</v>
+        <v>1528</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>1523</v>
+        <v>1529</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>18</v>
@@ -14970,7 +15033,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1524</v>
+        <v>1530</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>9</v>
@@ -14989,13 +15052,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1525</v>
+        <v>1531</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>1526</v>
+        <v>1532</v>
       </c>
       <c r="C23" t="s">
-        <v>1527</v>
+        <v>1533</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>18</v>
@@ -15008,10 +15071,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>1528</v>
+        <v>1534</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>1529</v>
+        <v>1535</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -15027,13 +15090,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>1530</v>
+        <v>1536</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>480</v>
       </c>
       <c r="C25" t="s">
-        <v>1531</v>
+        <v>1537</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>18</v>
@@ -15046,13 +15109,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>1532</v>
+        <v>1538</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>480</v>
       </c>
       <c r="C26" t="s">
-        <v>1533</v>
+        <v>1539</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>18</v>
@@ -15065,13 +15128,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1534</v>
+        <v>1540</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>1535</v>
+        <v>1541</v>
       </c>
       <c r="C27" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>18</v>
@@ -15084,13 +15147,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>1537</v>
+        <v>1543</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>480</v>
       </c>
       <c r="C28" t="s">
-        <v>1538</v>
+        <v>1544</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>18</v>
@@ -15103,13 +15166,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>1539</v>
+        <v>1545</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>480</v>
       </c>
       <c r="C29" t="s">
-        <v>1540</v>
+        <v>1546</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>18</v>
@@ -15122,11 +15185,11 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>1541</v>
+        <v>1547</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" t="s">
-        <v>1542</v>
+        <v>1548</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>18</v>
@@ -15139,11 +15202,11 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>1543</v>
+        <v>1549</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" t="s">
-        <v>1544</v>
+        <v>1550</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>18</v>
@@ -15156,13 +15219,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>1545</v>
+        <v>1551</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>1546</v>
+        <v>1552</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>18</v>
@@ -15175,13 +15238,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>1547</v>
+        <v>1553</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>1548</v>
+        <v>1554</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>18</v>
@@ -15211,13 +15274,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>1503</v>
+        <v>1509</v>
       </c>
       <c r="B36" t="s">
-        <v>1549</v>
+        <v>1555</v>
       </c>
       <c r="C36" t="s">
-        <v>1550</v>
+        <v>1556</v>
       </c>
       <c r="D36" t="s">
         <v>18</v>
@@ -15229,10 +15292,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>1551</v>
+        <v>1557</v>
       </c>
       <c r="C37" t="s">
-        <v>1552</v>
+        <v>1558</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
@@ -15244,10 +15307,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>1553</v>
+        <v>1559</v>
       </c>
       <c r="C38" t="s">
-        <v>1554</v>
+        <v>1560</v>
       </c>
       <c r="D38" t="s">
         <v>18</v>
@@ -15259,10 +15322,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>1555</v>
+        <v>1561</v>
       </c>
       <c r="C39" t="s">
-        <v>1556</v>
+        <v>1562</v>
       </c>
       <c r="D39" t="s">
         <v>18</v>
@@ -15274,10 +15337,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>1557</v>
+        <v>1563</v>
       </c>
       <c r="C40" t="s">
-        <v>1558</v>
+        <v>1564</v>
       </c>
       <c r="D40" t="s">
         <v>18</v>
@@ -15289,10 +15352,10 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>1559</v>
+        <v>1565</v>
       </c>
       <c r="C41" t="s">
-        <v>1560</v>
+        <v>1566</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -15304,10 +15367,10 @@
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>1561</v>
+        <v>1567</v>
       </c>
       <c r="C42" t="s">
-        <v>1562</v>
+        <v>1568</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
@@ -15319,10 +15382,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>1563</v>
+        <v>1569</v>
       </c>
       <c r="C43" t="s">
-        <v>1564</v>
+        <v>1570</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -15334,10 +15397,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>1565</v>
+        <v>1571</v>
       </c>
       <c r="C44" t="s">
-        <v>1566</v>
+        <v>1572</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
@@ -15349,10 +15412,10 @@
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>1567</v>
+        <v>1573</v>
       </c>
       <c r="C45" t="s">
-        <v>1568</v>
+        <v>1574</v>
       </c>
       <c r="D45" t="s">
         <v>18</v>
@@ -15364,10 +15427,10 @@
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>1569</v>
+        <v>1575</v>
       </c>
       <c r="C46" t="s">
-        <v>1570</v>
+        <v>1576</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
@@ -15379,10 +15442,10 @@
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>1571</v>
+        <v>1577</v>
       </c>
       <c r="C47" t="s">
-        <v>1572</v>
+        <v>1578</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
@@ -15394,10 +15457,10 @@
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>1573</v>
+        <v>1579</v>
       </c>
       <c r="C48" t="s">
-        <v>1574</v>
+        <v>1580</v>
       </c>
       <c r="D48" t="s">
         <v>18</v>
@@ -15409,10 +15472,10 @@
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>1575</v>
+        <v>1581</v>
       </c>
       <c r="C49" t="s">
-        <v>1576</v>
+        <v>1582</v>
       </c>
       <c r="D49" t="s">
         <v>18</v>
@@ -15424,10 +15487,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>1577</v>
+        <v>1583</v>
       </c>
       <c r="C50" t="s">
-        <v>1578</v>
+        <v>1584</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
@@ -15439,10 +15502,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>1579</v>
+        <v>1585</v>
       </c>
       <c r="C51" t="s">
-        <v>1580</v>
+        <v>1586</v>
       </c>
       <c r="D51" t="s">
         <v>18</v>
@@ -15454,10 +15517,10 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>1581</v>
+        <v>1587</v>
       </c>
       <c r="C52" t="s">
-        <v>1582</v>
+        <v>1588</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
@@ -15469,10 +15532,10 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>1583</v>
+        <v>1589</v>
       </c>
       <c r="C53" t="s">
-        <v>1584</v>
+        <v>1590</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -15484,10 +15547,10 @@
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>1585</v>
+        <v>1591</v>
       </c>
       <c r="C54" t="s">
-        <v>1586</v>
+        <v>1592</v>
       </c>
       <c r="D54" t="s">
         <v>18</v>
@@ -15530,13 +15593,13 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>1508</v>
+        <v>1514</v>
       </c>
       <c r="B58" t="s">
-        <v>1587</v>
+        <v>1593</v>
       </c>
       <c r="C58" t="s">
-        <v>1588</v>
+        <v>1594</v>
       </c>
       <c r="D58" t="s">
         <v>18</v>
@@ -15548,10 +15611,10 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>1589</v>
+        <v>1595</v>
       </c>
       <c r="C59" t="s">
-        <v>1590</v>
+        <v>1596</v>
       </c>
       <c r="D59" t="s">
         <v>18</v>
@@ -15579,13 +15642,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>1520</v>
+        <v>1526</v>
       </c>
       <c r="B62" t="s">
-        <v>1591</v>
+        <v>1597</v>
       </c>
       <c r="C62" t="s">
-        <v>1592</v>
+        <v>1598</v>
       </c>
       <c r="D62" t="s">
         <v>18</v>
@@ -15597,10 +15660,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>1593</v>
+        <v>1599</v>
       </c>
       <c r="C63" t="s">
-        <v>1594</v>
+        <v>1600</v>
       </c>
       <c r="D63" t="s">
         <v>18</v>
@@ -15628,13 +15691,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>1526</v>
+        <v>1532</v>
       </c>
       <c r="B66" t="s">
-        <v>1595</v>
+        <v>1601</v>
       </c>
       <c r="C66" t="s">
-        <v>1596</v>
+        <v>1602</v>
       </c>
       <c r="D66" t="s">
         <v>18</v>
@@ -15646,10 +15709,10 @@
     <row r="67">
       <c r="A67"/>
       <c r="B67" t="s">
-        <v>1597</v>
+        <v>1603</v>
       </c>
       <c r="C67" t="s">
-        <v>1598</v>
+        <v>1604</v>
       </c>
       <c r="D67" t="s">
         <v>18</v>
@@ -15661,10 +15724,10 @@
     <row r="68">
       <c r="A68"/>
       <c r="B68" t="s">
-        <v>1599</v>
+        <v>1605</v>
       </c>
       <c r="C68" t="s">
-        <v>1600</v>
+        <v>1606</v>
       </c>
       <c r="D68" t="s">
         <v>18</v>
@@ -15692,13 +15755,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>1535</v>
+        <v>1541</v>
       </c>
       <c r="B71" t="s">
-        <v>1601</v>
+        <v>1607</v>
       </c>
       <c r="C71" t="s">
-        <v>1602</v>
+        <v>1608</v>
       </c>
       <c r="D71" t="s">
         <v>18</v>
@@ -15725,10 +15788,10 @@
     <row r="73">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>1603</v>
+        <v>1609</v>
       </c>
       <c r="C73" t="s">
-        <v>1604</v>
+        <v>1610</v>
       </c>
       <c r="D73" t="s">
         <v>18</v>
@@ -15740,10 +15803,10 @@
     <row r="74">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>1605</v>
+        <v>1611</v>
       </c>
       <c r="C74" t="s">
-        <v>1606</v>
+        <v>1612</v>
       </c>
       <c r="D74" t="s">
         <v>18</v>
@@ -15811,10 +15874,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1607</v>
+        <v>1613</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>1529</v>
+        <v>1535</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -15832,16 +15895,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1608</v>
+        <v>1614</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>1609</v>
+        <v>1615</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1610</v>
+        <v>1616</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -15853,16 +15916,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1611</v>
+        <v>1617</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>1612</v>
+        <v>1618</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>1613</v>
+        <v>1619</v>
       </c>
       <c r="E4"/>
       <c r="G4" s="14" t="s">
@@ -15872,16 +15935,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1614</v>
+        <v>1620</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>1615</v>
+        <v>1621</v>
       </c>
       <c r="C5" t="s">
-        <v>1616</v>
+        <v>1622</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>1617</v>
+        <v>1623</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -15893,16 +15956,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1618</v>
+        <v>1624</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>1619</v>
+        <v>1625</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>1620</v>
+        <v>1626</v>
       </c>
       <c r="E6"/>
       <c r="G6" s="14" t="s">
@@ -15912,16 +15975,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>1621</v>
+        <v>1627</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>1622</v>
+        <v>1628</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>1623</v>
+        <v>1629</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -15933,7 +15996,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1510</v>
+        <v>1516</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>52</v>
@@ -15942,7 +16005,7 @@
         <v>597</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>1624</v>
+        <v>1630</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -15954,16 +16017,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1511</v>
+        <v>1517</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>1512</v>
+        <v>1518</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>1625</v>
+        <v>1631</v>
       </c>
       <c r="E9"/>
       <c r="G9" s="14" t="s">
@@ -15973,7 +16036,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1626</v>
+        <v>1632</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>364</v>
@@ -15994,16 +16057,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1627</v>
+        <v>1633</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>1535</v>
+        <v>1541</v>
       </c>
       <c r="C11" t="s">
-        <v>1628</v>
+        <v>1634</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>1629</v>
+        <v>1635</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -16015,16 +16078,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1630</v>
+        <v>1636</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>1631</v>
+        <v>1637</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>1632</v>
+        <v>1638</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -16036,16 +16099,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1633</v>
+        <v>1639</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>480</v>
       </c>
       <c r="C13" t="s">
-        <v>1634</v>
+        <v>1640</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>1635</v>
+        <v>1641</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -16057,16 +16120,16 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1636</v>
+        <v>1642</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>480</v>
       </c>
       <c r="C14" t="s">
-        <v>1637</v>
+        <v>1643</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>1638</v>
+        <v>1644</v>
       </c>
       <c r="E14"/>
       <c r="G14" s="14" t="s">
@@ -16076,16 +16139,16 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1639</v>
+        <v>1645</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>1640</v>
+        <v>1646</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>1641</v>
+        <v>1647</v>
       </c>
       <c r="E15"/>
       <c r="G15" s="14" t="s">
@@ -16095,13 +16158,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1642</v>
+        <v>1648</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>1643</v>
+        <v>1649</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>18</v>
@@ -16990,13 +17053,13 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>1615</v>
+        <v>1621</v>
       </c>
       <c r="B77" t="s">
-        <v>1644</v>
+        <v>1650</v>
       </c>
       <c r="C77" t="s">
-        <v>1645</v>
+        <v>1651</v>
       </c>
       <c r="D77" t="s">
         <v>18</v>
@@ -17008,10 +17071,10 @@
     <row r="78">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>1646</v>
+        <v>1652</v>
       </c>
       <c r="C78" t="s">
-        <v>1647</v>
+        <v>1653</v>
       </c>
       <c r="D78" t="s">
         <v>18</v>
@@ -17023,10 +17086,10 @@
     <row r="79">
       <c r="A79"/>
       <c r="B79" t="s">
-        <v>1648</v>
+        <v>1654</v>
       </c>
       <c r="C79" t="s">
-        <v>1649</v>
+        <v>1655</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
@@ -17038,10 +17101,10 @@
     <row r="80">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>1650</v>
+        <v>1656</v>
       </c>
       <c r="C80" t="s">
-        <v>1651</v>
+        <v>1657</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
@@ -17053,10 +17116,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>1652</v>
+        <v>1658</v>
       </c>
       <c r="C81" t="s">
-        <v>1653</v>
+        <v>1659</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -17068,7 +17131,7 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>1654</v>
+        <v>1660</v>
       </c>
       <c r="C82" t="s">
         <v>618</v>
@@ -17083,10 +17146,10 @@
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>1655</v>
+        <v>1661</v>
       </c>
       <c r="C83" t="s">
-        <v>1656</v>
+        <v>1662</v>
       </c>
       <c r="D83" t="s">
         <v>18</v>
@@ -17098,10 +17161,10 @@
     <row r="84">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>1657</v>
+        <v>1663</v>
       </c>
       <c r="C84" t="s">
-        <v>1658</v>
+        <v>1664</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
@@ -17113,10 +17176,10 @@
     <row r="85">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>1659</v>
+        <v>1665</v>
       </c>
       <c r="C85" t="s">
-        <v>1660</v>
+        <v>1666</v>
       </c>
       <c r="D85" t="s">
         <v>18</v>
@@ -17128,10 +17191,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>1661</v>
+        <v>1667</v>
       </c>
       <c r="C86" t="s">
-        <v>1662</v>
+        <v>1668</v>
       </c>
       <c r="D86" t="s">
         <v>18</v>
@@ -17143,10 +17206,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>1663</v>
+        <v>1669</v>
       </c>
       <c r="C87" t="s">
-        <v>1664</v>
+        <v>1670</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
@@ -17158,10 +17221,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>1665</v>
+        <v>1671</v>
       </c>
       <c r="C88" t="s">
-        <v>1666</v>
+        <v>1672</v>
       </c>
       <c r="D88" t="s">
         <v>18</v>
@@ -17173,10 +17236,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>1667</v>
+        <v>1673</v>
       </c>
       <c r="C89" t="s">
-        <v>1668</v>
+        <v>1674</v>
       </c>
       <c r="D89" t="s">
         <v>18</v>
@@ -17188,10 +17251,10 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
       <c r="C90" t="s">
-        <v>1670</v>
+        <v>1676</v>
       </c>
       <c r="D90" t="s">
         <v>18</v>
@@ -17203,10 +17266,10 @@
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>1671</v>
+        <v>1677</v>
       </c>
       <c r="C91" t="s">
-        <v>1672</v>
+        <v>1678</v>
       </c>
       <c r="D91" t="s">
         <v>18</v>
@@ -17218,10 +17281,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>1673</v>
+        <v>1679</v>
       </c>
       <c r="C92" t="s">
-        <v>1674</v>
+        <v>1680</v>
       </c>
       <c r="D92" t="s">
         <v>18</v>
@@ -17233,10 +17296,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>1675</v>
+        <v>1681</v>
       </c>
       <c r="C93" t="s">
-        <v>1676</v>
+        <v>1682</v>
       </c>
       <c r="D93" t="s">
         <v>18</v>
@@ -17248,10 +17311,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>1677</v>
+        <v>1683</v>
       </c>
       <c r="C94" t="s">
-        <v>1678</v>
+        <v>1684</v>
       </c>
       <c r="D94" t="s">
         <v>18</v>
@@ -17294,13 +17357,13 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>1535</v>
+        <v>1541</v>
       </c>
       <c r="B98" t="s">
-        <v>1601</v>
+        <v>1607</v>
       </c>
       <c r="C98" t="s">
-        <v>1602</v>
+        <v>1608</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
@@ -17327,10 +17390,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>1603</v>
+        <v>1609</v>
       </c>
       <c r="C100" t="s">
-        <v>1604</v>
+        <v>1610</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
@@ -17342,10 +17405,10 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
-        <v>1605</v>
+        <v>1611</v>
       </c>
       <c r="C101" t="s">
-        <v>1606</v>
+        <v>1612</v>
       </c>
       <c r="D101" t="s">
         <v>18</v>
@@ -17411,10 +17474,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1607</v>
+        <v>1613</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>1529</v>
+        <v>1535</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -17430,13 +17493,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1621</v>
+        <v>1627</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>1622</v>
+        <v>1628</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>18</v>
@@ -17449,13 +17512,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1679</v>
+        <v>1685</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>1680</v>
+        <v>1686</v>
       </c>
       <c r="C4" t="s">
-        <v>1681</v>
+        <v>1687</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>18</v>
@@ -17468,13 +17531,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1682</v>
+        <v>1688</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>1680</v>
+        <v>1686</v>
       </c>
       <c r="C5" t="s">
-        <v>1683</v>
+        <v>1689</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>18</v>
@@ -17487,13 +17550,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1684</v>
+        <v>1690</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>1680</v>
+        <v>1686</v>
       </c>
       <c r="C6" t="s">
-        <v>1685</v>
+        <v>1691</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>18</v>
@@ -17506,13 +17569,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>1686</v>
+        <v>1692</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>1687</v>
+        <v>1693</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>18</v>
@@ -17525,13 +17588,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1688</v>
+        <v>1694</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>1689</v>
+        <v>1695</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>18</v>
@@ -17544,13 +17607,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1690</v>
+        <v>1696</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>1691</v>
+        <v>1697</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>18</v>
@@ -17563,13 +17626,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1692</v>
+        <v>1698</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>1693</v>
+        <v>1699</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>18</v>
@@ -17582,13 +17645,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1694</v>
+        <v>1700</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>1695</v>
+        <v>1701</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>18</v>
@@ -17601,13 +17664,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1696</v>
+        <v>1702</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>1697</v>
+        <v>1703</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>18</v>
@@ -17620,13 +17683,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1698</v>
+        <v>1704</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>1699</v>
+        <v>1705</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>18</v>
@@ -17639,13 +17702,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1700</v>
+        <v>1706</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>1701</v>
+        <v>1707</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>18</v>
@@ -17658,13 +17721,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1702</v>
+        <v>1708</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>1703</v>
+        <v>1709</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>18</v>
@@ -17677,13 +17740,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1704</v>
+        <v>1710</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>1705</v>
+        <v>1711</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>18</v>
@@ -17696,13 +17759,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1706</v>
+        <v>1712</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>1707</v>
+        <v>1713</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>18</v>
@@ -17715,13 +17778,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1708</v>
+        <v>1714</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>1709</v>
+        <v>1715</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>18</v>
@@ -17734,13 +17797,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>1710</v>
+        <v>1716</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>1711</v>
+        <v>1717</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>18</v>
@@ -17753,13 +17816,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>1712</v>
+        <v>1718</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>1713</v>
+        <v>1719</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>18</v>
@@ -17772,13 +17835,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>1714</v>
+        <v>1720</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>1715</v>
+        <v>1721</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>18</v>
@@ -17791,13 +17854,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1716</v>
+        <v>1722</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>1717</v>
+        <v>1723</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>18</v>
@@ -17810,13 +17873,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1718</v>
+        <v>1724</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>1719</v>
+        <v>1725</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>18</v>
@@ -17846,13 +17909,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>1680</v>
+        <v>1686</v>
       </c>
       <c r="B26" t="s">
-        <v>1605</v>
+        <v>1611</v>
       </c>
       <c r="C26" t="s">
-        <v>1606</v>
+        <v>1612</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
@@ -17864,10 +17927,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>1603</v>
+        <v>1609</v>
       </c>
       <c r="C27" t="s">
-        <v>1604</v>
+        <v>1610</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
@@ -17879,10 +17942,10 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>1601</v>
+        <v>1607</v>
       </c>
       <c r="C28" t="s">
-        <v>1602</v>
+        <v>1608</v>
       </c>
       <c r="D28" t="s">
         <v>18</v>
@@ -17946,13 +18009,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1720</v>
+        <v>1726</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>1721</v>
+        <v>1727</v>
       </c>
       <c r="C2" t="s">
-        <v>1722</v>
+        <v>1728</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>18</v>
@@ -17973,7 +18036,7 @@
         <v>1338</v>
       </c>
       <c r="C3" t="s">
-        <v>1492</v>
+        <v>1498</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>18</v>
@@ -17986,13 +18049,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1723</v>
+        <v>1729</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>1724</v>
+        <v>1730</v>
       </c>
       <c r="C4" t="s">
-        <v>1725</v>
+        <v>1731</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>18</v>
@@ -18005,13 +18068,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1726</v>
+        <v>1732</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>1494</v>
+        <v>1500</v>
       </c>
       <c r="C5" t="s">
-        <v>1727</v>
+        <v>1733</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>18</v>
@@ -18024,16 +18087,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1728</v>
+        <v>1734</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1729</v>
+        <v>1735</v>
       </c>
       <c r="C6" t="s">
-        <v>1730</v>
+        <v>1736</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>1731</v>
+        <v>1737</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -18045,13 +18108,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>1732</v>
+        <v>1738</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>1733</v>
+        <v>1739</v>
       </c>
       <c r="C7" t="s">
-        <v>1734</v>
+        <v>1740</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>18</v>
@@ -18064,13 +18127,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1735</v>
+        <v>1741</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>1736</v>
+        <v>1742</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>18</v>
@@ -18085,13 +18148,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1737</v>
+        <v>1743</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>1738</v>
+        <v>1744</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>18</v>
@@ -18104,13 +18167,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1739</v>
+        <v>1745</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>1740</v>
+        <v>1746</v>
       </c>
       <c r="C10" t="s">
-        <v>1741</v>
+        <v>1747</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>18</v>
@@ -18123,13 +18186,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1742</v>
+        <v>1748</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>1743</v>
+        <v>1749</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>18</v>
@@ -18142,13 +18205,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1744</v>
+        <v>1750</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>1745</v>
+        <v>1751</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>18</v>
@@ -18161,13 +18224,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1746</v>
+        <v>1752</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>364</v>
       </c>
       <c r="C13" t="s">
-        <v>1747</v>
+        <v>1753</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>18</v>
@@ -18180,13 +18243,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1748</v>
+        <v>1754</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>1749</v>
+        <v>1755</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>18</v>
@@ -18199,13 +18262,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1750</v>
+        <v>1756</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>364</v>
       </c>
       <c r="C15" t="s">
-        <v>1751</v>
+        <v>1757</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>18</v>
@@ -18220,13 +18283,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1752</v>
+        <v>1758</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>1753</v>
+        <v>1759</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>18</v>
@@ -18239,7 +18302,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1754</v>
+        <v>1760</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
@@ -18258,7 +18321,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1755</v>
+        <v>1761</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>29</v>
@@ -18277,7 +18340,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>1756</v>
+        <v>1762</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>29</v>
@@ -18313,13 +18376,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1721</v>
+        <v>1727</v>
       </c>
       <c r="B22" t="s">
-        <v>1757</v>
+        <v>1763</v>
       </c>
       <c r="C22" t="s">
-        <v>1758</v>
+        <v>1764</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
@@ -18331,10 +18394,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>1759</v>
+        <v>1765</v>
       </c>
       <c r="C23" t="s">
-        <v>1760</v>
+        <v>1766</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
@@ -18346,10 +18409,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>1761</v>
+        <v>1767</v>
       </c>
       <c r="C24" t="s">
-        <v>1762</v>
+        <v>1768</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
@@ -18361,10 +18424,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>1763</v>
+        <v>1769</v>
       </c>
       <c r="C25" t="s">
-        <v>1764</v>
+        <v>1770</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -18392,13 +18455,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>1729</v>
+        <v>1735</v>
       </c>
       <c r="B28" t="s">
-        <v>1765</v>
+        <v>1771</v>
       </c>
       <c r="C28" t="s">
-        <v>1766</v>
+        <v>1772</v>
       </c>
       <c r="D28" t="s">
         <v>18</v>
@@ -18410,10 +18473,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>1767</v>
+        <v>1773</v>
       </c>
       <c r="C29" t="s">
-        <v>1768</v>
+        <v>1774</v>
       </c>
       <c r="D29" t="s">
         <v>18</v>
@@ -18425,10 +18488,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>1769</v>
+        <v>1775</v>
       </c>
       <c r="C30" t="s">
-        <v>1770</v>
+        <v>1776</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
@@ -18440,10 +18503,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>1771</v>
+        <v>1777</v>
       </c>
       <c r="C31" t="s">
-        <v>1772</v>
+        <v>1778</v>
       </c>
       <c r="D31" t="s">
         <v>18</v>
@@ -18455,10 +18518,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>1773</v>
+        <v>1779</v>
       </c>
       <c r="C32" t="s">
-        <v>1774</v>
+        <v>1780</v>
       </c>
       <c r="D32" t="s">
         <v>18</v>
@@ -18470,10 +18533,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>1775</v>
+        <v>1781</v>
       </c>
       <c r="C33" t="s">
-        <v>1776</v>
+        <v>1782</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>
@@ -18485,10 +18548,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>1777</v>
+        <v>1783</v>
       </c>
       <c r="C34" t="s">
-        <v>1778</v>
+        <v>1784</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>
@@ -18500,10 +18563,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>1779</v>
+        <v>1785</v>
       </c>
       <c r="C35" t="s">
-        <v>1780</v>
+        <v>1786</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
@@ -18515,10 +18578,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>1781</v>
+        <v>1787</v>
       </c>
       <c r="C36" t="s">
-        <v>1782</v>
+        <v>1788</v>
       </c>
       <c r="D36" t="s">
         <v>18</v>
@@ -18530,10 +18593,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>1783</v>
+        <v>1789</v>
       </c>
       <c r="C37" t="s">
-        <v>1784</v>
+        <v>1790</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
@@ -18545,10 +18608,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>1785</v>
+        <v>1791</v>
       </c>
       <c r="C38" t="s">
-        <v>1786</v>
+        <v>1792</v>
       </c>
       <c r="D38" t="s">
         <v>18</v>
@@ -18560,10 +18623,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>1787</v>
+        <v>1793</v>
       </c>
       <c r="C39" t="s">
-        <v>1788</v>
+        <v>1794</v>
       </c>
       <c r="D39" t="s">
         <v>18</v>
@@ -18575,10 +18638,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>1789</v>
+        <v>1795</v>
       </c>
       <c r="C40" t="s">
-        <v>1790</v>
+        <v>1796</v>
       </c>
       <c r="D40" t="s">
         <v>18</v>
@@ -18590,10 +18653,10 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>1791</v>
+        <v>1797</v>
       </c>
       <c r="C41" t="s">
-        <v>1792</v>
+        <v>1798</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -18605,10 +18668,10 @@
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>1793</v>
+        <v>1799</v>
       </c>
       <c r="C42" t="s">
-        <v>1794</v>
+        <v>1800</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
@@ -18620,10 +18683,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>1795</v>
+        <v>1801</v>
       </c>
       <c r="C43" t="s">
-        <v>1796</v>
+        <v>1802</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -18635,10 +18698,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>1797</v>
+        <v>1803</v>
       </c>
       <c r="C44" t="s">
-        <v>1798</v>
+        <v>1804</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
@@ -18653,7 +18716,7 @@
         <v>260</v>
       </c>
       <c r="C45" t="s">
-        <v>1799</v>
+        <v>1805</v>
       </c>
       <c r="D45" t="s">
         <v>18</v>
@@ -18665,10 +18728,10 @@
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>1800</v>
+        <v>1806</v>
       </c>
       <c r="C46" t="s">
-        <v>1801</v>
+        <v>1807</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
@@ -18680,10 +18743,10 @@
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>1802</v>
+        <v>1808</v>
       </c>
       <c r="C47" t="s">
-        <v>1803</v>
+        <v>1809</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
@@ -18695,10 +18758,10 @@
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>1804</v>
+        <v>1810</v>
       </c>
       <c r="C48" t="s">
-        <v>1805</v>
+        <v>1811</v>
       </c>
       <c r="D48" t="s">
         <v>18</v>
@@ -18726,13 +18789,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>1733</v>
+        <v>1739</v>
       </c>
       <c r="B51" t="s">
-        <v>1806</v>
+        <v>1812</v>
       </c>
       <c r="C51" t="s">
-        <v>1807</v>
+        <v>1813</v>
       </c>
       <c r="D51" t="s">
         <v>18</v>
@@ -18744,10 +18807,10 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>1808</v>
+        <v>1814</v>
       </c>
       <c r="C52" t="s">
-        <v>1809</v>
+        <v>1815</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
@@ -18759,10 +18822,10 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>1810</v>
+        <v>1816</v>
       </c>
       <c r="C53" t="s">
-        <v>1811</v>
+        <v>1817</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -18790,13 +18853,13 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>1740</v>
+        <v>1746</v>
       </c>
       <c r="B56" t="s">
         <v>542</v>
       </c>
       <c r="C56" t="s">
-        <v>1812</v>
+        <v>1818</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
@@ -18811,7 +18874,7 @@
         <v>545</v>
       </c>
       <c r="C57" t="s">
-        <v>1813</v>
+        <v>1819</v>
       </c>
       <c r="D57" t="s">
         <v>18</v>
@@ -18823,10 +18886,10 @@
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>1814</v>
+        <v>1820</v>
       </c>
       <c r="C58" t="s">
-        <v>1815</v>
+        <v>1821</v>
       </c>
       <c r="D58" t="s">
         <v>18</v>
@@ -18838,10 +18901,10 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>1816</v>
+        <v>1822</v>
       </c>
       <c r="C59" t="s">
-        <v>1817</v>
+        <v>1823</v>
       </c>
       <c r="D59" t="s">
         <v>18</v>
@@ -18908,16 +18971,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1818</v>
+        <v>1824</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>1819</v>
+        <v>1825</v>
       </c>
       <c r="C2" t="s">
-        <v>1820</v>
+        <v>1826</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>1821</v>
+        <v>1827</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -18929,16 +18992,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1822</v>
+        <v>1828</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>1823</v>
+        <v>1829</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>1824</v>
+        <v>1830</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -18950,16 +19013,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1825</v>
+        <v>1831</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>1826</v>
+        <v>1832</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>1827</v>
+        <v>1833</v>
       </c>
       <c r="E4"/>
       <c r="G4" s="17" t="s">
@@ -19011,13 +19074,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>1828</v>
+        <v>1834</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>1829</v>
+        <v>1835</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>18</v>
@@ -19030,16 +19093,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1830</v>
+        <v>1836</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>1831</v>
+        <v>1837</v>
       </c>
       <c r="C8" t="s">
-        <v>1832</v>
+        <v>1838</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>1833</v>
+        <v>1839</v>
       </c>
       <c r="E8"/>
       <c r="G8" s="17" t="s">
@@ -19049,16 +19112,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1834</v>
+        <v>1840</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>1835</v>
+        <v>1841</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>1836</v>
+        <v>1842</v>
       </c>
       <c r="E9"/>
       <c r="G9" s="17" t="s">
@@ -19068,16 +19131,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1837</v>
+        <v>1843</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>1838</v>
+        <v>1844</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>1839</v>
+        <v>1845</v>
       </c>
       <c r="E10"/>
       <c r="G10" s="17" t="s">
@@ -19087,16 +19150,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1840</v>
+        <v>1846</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>1841</v>
+        <v>1847</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>1842</v>
+        <v>1848</v>
       </c>
       <c r="E11"/>
       <c r="G11" s="17" t="s">
@@ -19106,16 +19169,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1843</v>
+        <v>1849</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>1844</v>
+        <v>1850</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>1845</v>
+        <v>1851</v>
       </c>
       <c r="E12"/>
       <c r="G12" s="17" t="s">
@@ -19182,13 +19245,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1846</v>
+        <v>1852</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>1847</v>
+        <v>1853</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>18</v>
@@ -19275,13 +19338,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1819</v>
+        <v>1825</v>
       </c>
       <c r="B22" t="s">
-        <v>1848</v>
+        <v>1854</v>
       </c>
       <c r="C22" t="s">
-        <v>1849</v>
+        <v>1855</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
@@ -19296,7 +19359,7 @@
         <v>536</v>
       </c>
       <c r="C23" t="s">
-        <v>1762</v>
+        <v>1768</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
@@ -19308,16 +19371,16 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>1850</v>
+        <v>1856</v>
       </c>
       <c r="C24" t="s">
-        <v>1851</v>
+        <v>1857</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>1852</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="26">
@@ -19339,13 +19402,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1831</v>
+        <v>1837</v>
       </c>
       <c r="B27" t="s">
-        <v>1853</v>
+        <v>1859</v>
       </c>
       <c r="C27" t="s">
-        <v>1854</v>
+        <v>1860</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
@@ -19387,10 +19450,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>1855</v>
+        <v>1861</v>
       </c>
       <c r="C30" t="s">
-        <v>1856</v>
+        <v>1862</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
@@ -19402,10 +19465,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>1857</v>
+        <v>1863</v>
       </c>
       <c r="C31" t="s">
-        <v>1858</v>
+        <v>1864</v>
       </c>
       <c r="D31" t="s">
         <v>18</v>
@@ -20360,13 +20423,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1723</v>
+        <v>1729</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>1724</v>
+        <v>1730</v>
       </c>
       <c r="C2" t="s">
-        <v>1762</v>
+        <v>1768</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>18</v>
@@ -20384,10 +20447,10 @@
         <v>356</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="C3" t="s">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>18</v>
@@ -20402,13 +20465,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1860</v>
+        <v>1866</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>1861</v>
+        <v>1867</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>18</v>
@@ -20492,13 +20555,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1862</v>
+        <v>1868</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>1863</v>
+        <v>1869</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>18</v>
@@ -20593,7 +20656,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>1864</v>
+        <v>1870</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>18</v>
@@ -20612,7 +20675,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>1865</v>
+        <v>1871</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>18</v>
@@ -20625,10 +20688,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1866</v>
+        <v>1872</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>1867</v>
+        <v>1873</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -20644,7 +20707,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1868</v>
+        <v>1874</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>480</v>
@@ -20663,7 +20726,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1869</v>
+        <v>1875</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>480</v>
@@ -20718,7 +20781,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1867</v>
+        <v>1873</v>
       </c>
       <c r="B15" t="s">
         <v>278</v>
@@ -21159,13 +21222,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1862</v>
+        <v>1868</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>1863</v>
+        <v>1869</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>18</v>
@@ -21178,13 +21241,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1870</v>
+        <v>1876</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>1871</v>
+        <v>1877</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>18</v>
@@ -21197,13 +21260,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1872</v>
+        <v>1878</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>1873</v>
+        <v>1879</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>18</v>
@@ -21216,7 +21279,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1869</v>
+        <v>1875</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>480</v>
@@ -21306,13 +21369,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1862</v>
+        <v>1868</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>1863</v>
+        <v>1869</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>18</v>
@@ -21325,13 +21388,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1870</v>
+        <v>1876</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>1871</v>
+        <v>1877</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>18</v>
@@ -21344,13 +21407,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1872</v>
+        <v>1878</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>1873</v>
+        <v>1879</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>18</v>
@@ -21382,7 +21445,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1869</v>
+        <v>1875</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>480</v>
@@ -21472,13 +21535,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1862</v>
+        <v>1868</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>1863</v>
+        <v>1869</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>18</v>
@@ -21529,7 +21592,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1869</v>
+        <v>1875</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>480</v>
@@ -21619,13 +21682,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1874</v>
+        <v>1880</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>480</v>
       </c>
       <c r="C2" t="s">
-        <v>1875</v>
+        <v>1881</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>18</v>
@@ -21638,13 +21701,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1876</v>
+        <v>1882</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>1877</v>
+        <v>1883</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>18</v>
@@ -21695,13 +21758,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1878</v>
+        <v>1884</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>1844</v>
+        <v>1850</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>18</v>
@@ -21752,11 +21815,11 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1879</v>
+        <v>1885</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" t="s">
-        <v>1880</v>
+        <v>1886</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>18</v>
@@ -21845,7 +21908,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1881</v>
+        <v>1887</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>52</v>
@@ -21870,7 +21933,7 @@
         <v>471</v>
       </c>
       <c r="C15" t="s">
-        <v>1882</v>
+        <v>1888</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>18</v>
@@ -21883,13 +21946,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1883</v>
+        <v>1889</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>364</v>
       </c>
       <c r="C16" t="s">
-        <v>1884</v>
+        <v>1890</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>18</v>
@@ -21902,16 +21965,16 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1885</v>
+        <v>1891</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>1886</v>
+        <v>1892</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>1887</v>
+        <v>1893</v>
       </c>
       <c r="E17"/>
       <c r="G17" s="23" t="s">
@@ -21921,10 +21984,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1888</v>
+        <v>1894</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>1889</v>
+        <v>1895</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -22816,13 +22879,13 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>1889</v>
+        <v>1895</v>
       </c>
       <c r="B79" t="s">
-        <v>1890</v>
+        <v>1896</v>
       </c>
       <c r="C79" t="s">
-        <v>1891</v>
+        <v>1897</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
@@ -22834,10 +22897,10 @@
     <row r="80">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>1892</v>
+        <v>1898</v>
       </c>
       <c r="C80" t="s">
-        <v>1893</v>
+        <v>1899</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
@@ -22849,10 +22912,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>1894</v>
+        <v>1900</v>
       </c>
       <c r="C81" t="s">
-        <v>1895</v>
+        <v>1901</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -22864,10 +22927,10 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>1896</v>
+        <v>1902</v>
       </c>
       <c r="C82" t="s">
-        <v>1897</v>
+        <v>1903</v>
       </c>
       <c r="D82" t="s">
         <v>18</v>
@@ -22879,10 +22942,10 @@
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>1898</v>
+        <v>1904</v>
       </c>
       <c r="C83" t="s">
-        <v>1899</v>
+        <v>1905</v>
       </c>
       <c r="D83" t="s">
         <v>18</v>
@@ -22894,10 +22957,10 @@
     <row r="84">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>1900</v>
+        <v>1906</v>
       </c>
       <c r="C84" t="s">
-        <v>1901</v>
+        <v>1907</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
@@ -22909,10 +22972,10 @@
     <row r="85">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>1902</v>
+        <v>1908</v>
       </c>
       <c r="C85" t="s">
-        <v>1903</v>
+        <v>1909</v>
       </c>
       <c r="D85" t="s">
         <v>18</v>
@@ -22941,12 +23004,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1904</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1905</v>
+        <v>1911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1637: Consider the facility type during import
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -1228,6 +1228,12 @@
     <t>Describe sequelae</t>
   </si>
   <si>
+    <t>facilityType</t>
+  </si>
+  <si>
+    <t>FacilityType</t>
+  </si>
+  <si>
     <t>healthFacility</t>
   </si>
   <si>
@@ -1582,12 +1588,6 @@
     <t>Trimester</t>
   </si>
   <si>
-    <t>facilityType</t>
-  </si>
-  <si>
-    <t>FacilityType</t>
-  </si>
-  <si>
     <t>BUBONIC</t>
   </si>
   <si>
@@ -1735,6 +1735,246 @@
     <t>No</t>
   </si>
   <si>
+    <t>ASSOCIATION</t>
+  </si>
+  <si>
+    <t>Association, club</t>
+  </si>
+  <si>
+    <t>BUSINESS</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>CAMPSITE</t>
+  </si>
+  <si>
+    <t>Campsite</t>
+  </si>
+  <si>
+    <t>CANTINE</t>
+  </si>
+  <si>
+    <t>Cantine</t>
+  </si>
+  <si>
+    <t>CHILDRENS_DAY_CARE</t>
+  </si>
+  <si>
+    <t>Children's day care</t>
+  </si>
+  <si>
+    <t>CHILDRENS_HOME</t>
+  </si>
+  <si>
+    <t>Children's home</t>
+  </si>
+  <si>
+    <t>CORRECTIONAL_FACILITY</t>
+  </si>
+  <si>
+    <t>Correctional facility</t>
+  </si>
+  <si>
+    <t>CRUISE_SHIP</t>
+  </si>
+  <si>
+    <t>Cruise ship</t>
+  </si>
+  <si>
+    <t>ELDERLY_CARE</t>
+  </si>
+  <si>
+    <t>Elderly care</t>
+  </si>
+  <si>
+    <t>EVENT_VENUE</t>
+  </si>
+  <si>
+    <t>Event venue</t>
+  </si>
+  <si>
+    <t>FOOD_STALL</t>
+  </si>
+  <si>
+    <t>Food stall</t>
+  </si>
+  <si>
+    <t>HOLIDAY_CAMP</t>
+  </si>
+  <si>
+    <t>Holiday camp</t>
+  </si>
+  <si>
+    <t>HOMELESS_SHELTER</t>
+  </si>
+  <si>
+    <t>Homeless shelter</t>
+  </si>
+  <si>
+    <t>HOSTEL</t>
+  </si>
+  <si>
+    <t>Hostel, dormitory</t>
+  </si>
+  <si>
+    <t>HOTEL</t>
+  </si>
+  <si>
+    <t>Hotel, B&amp;B, inn, lodge</t>
+  </si>
+  <si>
+    <t>KINDERGARTEN</t>
+  </si>
+  <si>
+    <t>Kindergarten/After school care</t>
+  </si>
+  <si>
+    <t>LABORATORY</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>MASS_ACCOMMODATION</t>
+  </si>
+  <si>
+    <t>Mass accomodation (e.g. guest and harvest workers)</t>
+  </si>
+  <si>
+    <t>MILITARY_BARRACKS</t>
+  </si>
+  <si>
+    <t>Military barracks</t>
+  </si>
+  <si>
+    <t>MOBILE_NURSING_SERVICE</t>
+  </si>
+  <si>
+    <t>Mobile nursing service</t>
+  </si>
+  <si>
+    <t>OTHER_ACCOMMODATION</t>
+  </si>
+  <si>
+    <t>Other Accomodation</t>
+  </si>
+  <si>
+    <t>OTHER_CARE_FACILITY</t>
+  </si>
+  <si>
+    <t>Other Care facility</t>
+  </si>
+  <si>
+    <t>OTHER_CATERING_OUTLET</t>
+  </si>
+  <si>
+    <t>Other Catering outlet</t>
+  </si>
+  <si>
+    <t>OTHER_EDUCATIONAL_FACILITY</t>
+  </si>
+  <si>
+    <t>Other Educational facility</t>
+  </si>
+  <si>
+    <t>OTHER_LEISURE_FACILITY</t>
+  </si>
+  <si>
+    <t>Other Leisure facility</t>
+  </si>
+  <si>
+    <t>OTHER_MEDICAL_FACILITY</t>
+  </si>
+  <si>
+    <t>Other Medical facility</t>
+  </si>
+  <si>
+    <t>OTHER_RESIDENCE</t>
+  </si>
+  <si>
+    <t>Other Residence</t>
+  </si>
+  <si>
+    <t>OTHER_WORKING_PLACE</t>
+  </si>
+  <si>
+    <t>Other Working place/company</t>
+  </si>
+  <si>
+    <t>OUTPATIENT_TREATMENT_FACILITY</t>
+  </si>
+  <si>
+    <t>Outpatient treatment facility</t>
+  </si>
+  <si>
+    <t>PLACE_OF_WORSHIP</t>
+  </si>
+  <si>
+    <t>Place of worship</t>
+  </si>
+  <si>
+    <t>PUBLIC_PLACE</t>
+  </si>
+  <si>
+    <t>Public place/playground</t>
+  </si>
+  <si>
+    <t>REFUGEE_ACCOMMODATION</t>
+  </si>
+  <si>
+    <t>Refrugee accomodation/initial reception facility</t>
+  </si>
+  <si>
+    <t>REHAB_FACILITY</t>
+  </si>
+  <si>
+    <t>Rehab facility</t>
+  </si>
+  <si>
+    <t>RESTAURANT</t>
+  </si>
+  <si>
+    <t>Restaurant/tavern</t>
+  </si>
+  <si>
+    <t>RETIREMENT_HOME</t>
+  </si>
+  <si>
+    <t>Retirement home</t>
+  </si>
+  <si>
+    <t>SCHOOL</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>SWIMMING_POOL</t>
+  </si>
+  <si>
+    <t>Swimming pool</t>
+  </si>
+  <si>
+    <t>THEATER</t>
+  </si>
+  <si>
+    <t>Theater/cinema</t>
+  </si>
+  <si>
+    <t>UNIVERSITY</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>ZOO</t>
+  </si>
+  <si>
+    <t>Zoological garden, animal park</t>
+  </si>
+  <si>
     <t>VACCINATED</t>
   </si>
   <si>
@@ -1840,12 +2080,6 @@
     <t>Community facility</t>
   </si>
   <si>
-    <t>LABORATORY</t>
-  </si>
-  <si>
-    <t>Laboratory</t>
-  </si>
-  <si>
     <t>OWN_DETERMINATION</t>
   </si>
   <si>
@@ -1880,240 +2114,6 @@
   </si>
   <si>
     <t>Third</t>
-  </si>
-  <si>
-    <t>ASSOCIATION</t>
-  </si>
-  <si>
-    <t>Association, club</t>
-  </si>
-  <si>
-    <t>BUSINESS</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>CAMPSITE</t>
-  </si>
-  <si>
-    <t>Campsite</t>
-  </si>
-  <si>
-    <t>CANTINE</t>
-  </si>
-  <si>
-    <t>Cantine</t>
-  </si>
-  <si>
-    <t>CHILDRENS_DAY_CARE</t>
-  </si>
-  <si>
-    <t>Children's day care</t>
-  </si>
-  <si>
-    <t>CHILDRENS_HOME</t>
-  </si>
-  <si>
-    <t>Children's home</t>
-  </si>
-  <si>
-    <t>CORRECTIONAL_FACILITY</t>
-  </si>
-  <si>
-    <t>Correctional facility</t>
-  </si>
-  <si>
-    <t>CRUISE_SHIP</t>
-  </si>
-  <si>
-    <t>Cruise ship</t>
-  </si>
-  <si>
-    <t>ELDERLY_CARE</t>
-  </si>
-  <si>
-    <t>Elderly care</t>
-  </si>
-  <si>
-    <t>EVENT_VENUE</t>
-  </si>
-  <si>
-    <t>Event venue</t>
-  </si>
-  <si>
-    <t>FOOD_STALL</t>
-  </si>
-  <si>
-    <t>Food stall</t>
-  </si>
-  <si>
-    <t>HOLIDAY_CAMP</t>
-  </si>
-  <si>
-    <t>Holiday camp</t>
-  </si>
-  <si>
-    <t>HOMELESS_SHELTER</t>
-  </si>
-  <si>
-    <t>Homeless shelter</t>
-  </si>
-  <si>
-    <t>HOSTEL</t>
-  </si>
-  <si>
-    <t>Hostel, dormitory</t>
-  </si>
-  <si>
-    <t>HOTEL</t>
-  </si>
-  <si>
-    <t>Hotel, B&amp;B, inn, lodge</t>
-  </si>
-  <si>
-    <t>KINDERGARTEN</t>
-  </si>
-  <si>
-    <t>Kindergarten/After school care</t>
-  </si>
-  <si>
-    <t>MASS_ACCOMMODATION</t>
-  </si>
-  <si>
-    <t>Mass accomodation (e.g. guest and harvest workers)</t>
-  </si>
-  <si>
-    <t>MILITARY_BARRACKS</t>
-  </si>
-  <si>
-    <t>Military barracks</t>
-  </si>
-  <si>
-    <t>MOBILE_NURSING_SERVICE</t>
-  </si>
-  <si>
-    <t>Mobile nursing service</t>
-  </si>
-  <si>
-    <t>OTHER_ACCOMMODATION</t>
-  </si>
-  <si>
-    <t>Other Accomodation</t>
-  </si>
-  <si>
-    <t>OTHER_CARE_FACILITY</t>
-  </si>
-  <si>
-    <t>Other Care facility</t>
-  </si>
-  <si>
-    <t>OTHER_CATERING_OUTLET</t>
-  </si>
-  <si>
-    <t>Other Catering outlet</t>
-  </si>
-  <si>
-    <t>OTHER_EDUCATIONAL_FACILITY</t>
-  </si>
-  <si>
-    <t>Other Educational facility</t>
-  </si>
-  <si>
-    <t>OTHER_LEISURE_FACILITY</t>
-  </si>
-  <si>
-    <t>Other Leisure facility</t>
-  </si>
-  <si>
-    <t>OTHER_MEDICAL_FACILITY</t>
-  </si>
-  <si>
-    <t>Other Medical facility</t>
-  </si>
-  <si>
-    <t>OTHER_RESIDENCE</t>
-  </si>
-  <si>
-    <t>Other Residence</t>
-  </si>
-  <si>
-    <t>OTHER_WORKING_PLACE</t>
-  </si>
-  <si>
-    <t>Other Working place/company</t>
-  </si>
-  <si>
-    <t>OUTPATIENT_TREATMENT_FACILITY</t>
-  </si>
-  <si>
-    <t>Outpatient treatment facility</t>
-  </si>
-  <si>
-    <t>PLACE_OF_WORSHIP</t>
-  </si>
-  <si>
-    <t>Place of worship</t>
-  </si>
-  <si>
-    <t>PUBLIC_PLACE</t>
-  </si>
-  <si>
-    <t>Public place/playground</t>
-  </si>
-  <si>
-    <t>REFUGEE_ACCOMMODATION</t>
-  </si>
-  <si>
-    <t>Refrugee accomodation/initial reception facility</t>
-  </si>
-  <si>
-    <t>REHAB_FACILITY</t>
-  </si>
-  <si>
-    <t>Rehab facility</t>
-  </si>
-  <si>
-    <t>RESTAURANT</t>
-  </si>
-  <si>
-    <t>Restaurant/tavern</t>
-  </si>
-  <si>
-    <t>RETIREMENT_HOME</t>
-  </si>
-  <si>
-    <t>Retirement home</t>
-  </si>
-  <si>
-    <t>SCHOOL</t>
-  </si>
-  <si>
-    <t>School</t>
-  </si>
-  <si>
-    <t>SWIMMING_POOL</t>
-  </si>
-  <si>
-    <t>Swimming pool</t>
-  </si>
-  <si>
-    <t>THEATER</t>
-  </si>
-  <si>
-    <t>Theater/cinema</t>
-  </si>
-  <si>
-    <t>UNIVERSITY</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>ZOO</t>
-  </si>
-  <si>
-    <t>Zoological garden, animal park</t>
   </si>
   <si>
     <t>admittedToHealthFacility</t>
@@ -6457,7 +6457,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="CaseVaccination" displayName="CaseVaccination" ref="A174:E177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="CaseFacilityType" displayName="CaseFacilityType" ref="A174:E215">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6471,7 +6471,7 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="CaseVaccinationInfoSource" displayName="CaseVaccinationInfoSource" ref="A179:E181">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="CaseVaccination" displayName="CaseVaccination" ref="A217:E220">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6485,7 +6485,7 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="CaseHospitalWardType" displayName="CaseHospitalWardType" ref="A183:E192">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="CaseVaccinationInfoSource" displayName="CaseVaccinationInfoSource" ref="A222:E224">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6499,7 +6499,7 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="CaseCaseOrigin" displayName="CaseCaseOrigin" ref="A194:E196">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="CaseHospitalWardType" displayName="CaseHospitalWardType" ref="A226:E235">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6513,7 +6513,7 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="CaseQuarantineType" displayName="CaseQuarantineType" ref="A198:E203">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="CaseCaseOrigin" displayName="CaseCaseOrigin" ref="A237:E239">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6527,7 +6527,7 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="CaseReportingType" displayName="CaseReportingType" ref="A205:E214">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="CaseQuarantineType" displayName="CaseQuarantineType" ref="A241:E246">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6541,7 +6541,7 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="CaseTrimester" displayName="CaseTrimester" ref="A216:E220">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="CaseReportingType" displayName="CaseReportingType" ref="A248:E257">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -6555,7 +6555,7 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="CaseFacilityType" displayName="CaseFacilityType" ref="A222:E263">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="CaseTrimester" displayName="CaseTrimester" ref="A259:E263">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -10248,7 +10248,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>1413</v>
@@ -10267,10 +10267,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -11411,7 +11411,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>29</v>
@@ -11430,7 +11430,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>29</v>
@@ -11449,7 +11449,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>29</v>
@@ -11682,7 +11682,7 @@
         <v>1458</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C23" t="s">
         <v>1459</v>
@@ -11755,13 +11755,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>18</v>
@@ -11777,7 +11777,7 @@
         <v>1468</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C28" t="s">
         <v>1469</v>
@@ -11850,13 +11850,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C32" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>18</v>
@@ -11869,13 +11869,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>18</v>
@@ -11888,13 +11888,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>18</v>
@@ -11907,13 +11907,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>18</v>
@@ -12004,13 +12004,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>18</v>
@@ -12023,13 +12023,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C41" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>18</v>
@@ -12042,13 +12042,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C42" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>18</v>
@@ -12061,13 +12061,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>18</v>
@@ -12080,13 +12080,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>18</v>
@@ -12099,13 +12099,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C45" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>18</v>
@@ -12118,13 +12118,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>18</v>
@@ -12137,13 +12137,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C47" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>18</v>
@@ -12156,13 +12156,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>18</v>
@@ -12175,13 +12175,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>18</v>
@@ -12194,13 +12194,13 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C50" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>18</v>
@@ -13792,13 +13792,13 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B163" t="s">
-        <v>588</v>
+        <v>668</v>
       </c>
       <c r="C163" t="s">
-        <v>589</v>
+        <v>669</v>
       </c>
       <c r="D163" t="s">
         <v>18</v>
@@ -13810,10 +13810,10 @@
     <row r="164">
       <c r="A164"/>
       <c r="B164" t="s">
-        <v>590</v>
+        <v>670</v>
       </c>
       <c r="C164" t="s">
-        <v>591</v>
+        <v>671</v>
       </c>
       <c r="D164" t="s">
         <v>18</v>
@@ -13828,7 +13828,7 @@
         <v>274</v>
       </c>
       <c r="C165" t="s">
-        <v>592</v>
+        <v>672</v>
       </c>
       <c r="D165" t="s">
         <v>18</v>
@@ -14052,13 +14052,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C8" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>18</v>
@@ -14071,7 +14071,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>29</v>
@@ -14090,7 +14090,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>29</v>
@@ -14109,7 +14109,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>29</v>
@@ -15263,7 +15263,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>29</v>
@@ -15282,7 +15282,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>29</v>
@@ -15301,7 +15301,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>29</v>
@@ -15387,7 +15387,7 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>18</v>
@@ -15522,7 +15522,7 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>18</v>
@@ -15576,7 +15576,7 @@
         <v>1621</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C26" t="s">
         <v>1622</v>
@@ -15595,7 +15595,7 @@
         <v>1623</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C27" t="s">
         <v>1624</v>
@@ -15633,7 +15633,7 @@
         <v>1628</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C29" t="s">
         <v>1629</v>
@@ -15652,7 +15652,7 @@
         <v>1630</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C30" t="s">
         <v>1631</v>
@@ -16485,7 +16485,7 @@
         <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>1715</v>
@@ -16585,7 +16585,7 @@
         <v>1724</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C13" t="s">
         <v>1725</v>
@@ -16606,7 +16606,7 @@
         <v>1727</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C14" t="s">
         <v>1728</v>
@@ -19481,7 +19481,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>18</v>
@@ -19842,13 +19842,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>364</v>
       </c>
       <c r="C22" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>18</v>
@@ -19880,7 +19880,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>29</v>
@@ -19899,7 +19899,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>29</v>
@@ -19918,7 +19918,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>29</v>
@@ -20130,10 +20130,10 @@
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>590</v>
+        <v>670</v>
       </c>
       <c r="C42" t="s">
-        <v>591</v>
+        <v>671</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
@@ -20175,7 +20175,7 @@
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>673</v>
+        <v>626</v>
       </c>
       <c r="C45" t="s">
         <v>1966</v>
@@ -21482,7 +21482,7 @@
         <v>1982</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>516</v>
+        <v>398</v>
       </c>
       <c r="C9" t="s">
         <v>1983</v>
@@ -21501,7 +21501,7 @@
         <v>1984</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -21520,7 +21520,7 @@
         <v>1985</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -21536,13 +21536,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>18</v>
@@ -21572,13 +21572,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>516</v>
+        <v>398</v>
       </c>
       <c r="B15" t="s">
-        <v>615</v>
+        <v>566</v>
       </c>
       <c r="C15" t="s">
-        <v>616</v>
+        <v>567</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
@@ -21590,10 +21590,10 @@
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>617</v>
+        <v>568</v>
       </c>
       <c r="C16" t="s">
-        <v>618</v>
+        <v>569</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -21605,10 +21605,10 @@
     <row r="17">
       <c r="A17"/>
       <c r="B17" t="s">
-        <v>619</v>
+        <v>570</v>
       </c>
       <c r="C17" t="s">
-        <v>620</v>
+        <v>571</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
@@ -21620,10 +21620,10 @@
     <row r="18">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>621</v>
+        <v>572</v>
       </c>
       <c r="C18" t="s">
-        <v>622</v>
+        <v>573</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -21635,10 +21635,10 @@
     <row r="19">
       <c r="A19"/>
       <c r="B19" t="s">
-        <v>623</v>
+        <v>574</v>
       </c>
       <c r="C19" t="s">
-        <v>624</v>
+        <v>575</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
@@ -21650,10 +21650,10 @@
     <row r="20">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>625</v>
+        <v>576</v>
       </c>
       <c r="C20" t="s">
-        <v>626</v>
+        <v>577</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
@@ -21665,10 +21665,10 @@
     <row r="21">
       <c r="A21"/>
       <c r="B21" t="s">
-        <v>627</v>
+        <v>578</v>
       </c>
       <c r="C21" t="s">
-        <v>628</v>
+        <v>579</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -21680,10 +21680,10 @@
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>629</v>
+        <v>580</v>
       </c>
       <c r="C22" t="s">
-        <v>630</v>
+        <v>581</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
@@ -21695,10 +21695,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>631</v>
+        <v>582</v>
       </c>
       <c r="C23" t="s">
-        <v>632</v>
+        <v>583</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
@@ -21710,10 +21710,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>633</v>
+        <v>584</v>
       </c>
       <c r="C24" t="s">
-        <v>634</v>
+        <v>585</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
@@ -21725,10 +21725,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>635</v>
+        <v>586</v>
       </c>
       <c r="C25" t="s">
-        <v>636</v>
+        <v>587</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -21740,10 +21740,10 @@
     <row r="26">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>637</v>
+        <v>588</v>
       </c>
       <c r="C26" t="s">
-        <v>638</v>
+        <v>589</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
@@ -21755,10 +21755,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>639</v>
+        <v>590</v>
       </c>
       <c r="C27" t="s">
-        <v>640</v>
+        <v>591</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
@@ -21785,10 +21785,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>641</v>
+        <v>592</v>
       </c>
       <c r="C29" t="s">
-        <v>642</v>
+        <v>593</v>
       </c>
       <c r="D29" t="s">
         <v>18</v>
@@ -21800,10 +21800,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>643</v>
+        <v>594</v>
       </c>
       <c r="C30" t="s">
-        <v>644</v>
+        <v>595</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
@@ -21815,10 +21815,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>645</v>
+        <v>596</v>
       </c>
       <c r="C31" t="s">
-        <v>646</v>
+        <v>597</v>
       </c>
       <c r="D31" t="s">
         <v>18</v>
@@ -21830,10 +21830,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C32" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D32" t="s">
         <v>18</v>
@@ -21845,10 +21845,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>647</v>
+        <v>600</v>
       </c>
       <c r="C33" t="s">
-        <v>648</v>
+        <v>601</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>
@@ -21860,10 +21860,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>649</v>
+        <v>602</v>
       </c>
       <c r="C34" t="s">
-        <v>650</v>
+        <v>603</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>
@@ -21875,10 +21875,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>651</v>
+        <v>604</v>
       </c>
       <c r="C35" t="s">
-        <v>652</v>
+        <v>605</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
@@ -21890,10 +21890,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>653</v>
+        <v>606</v>
       </c>
       <c r="C36" t="s">
-        <v>654</v>
+        <v>607</v>
       </c>
       <c r="D36" t="s">
         <v>18</v>
@@ -21905,10 +21905,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>655</v>
+        <v>608</v>
       </c>
       <c r="C37" t="s">
-        <v>656</v>
+        <v>609</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
@@ -21920,10 +21920,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>657</v>
+        <v>610</v>
       </c>
       <c r="C38" t="s">
-        <v>658</v>
+        <v>611</v>
       </c>
       <c r="D38" t="s">
         <v>18</v>
@@ -21935,10 +21935,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>659</v>
+        <v>612</v>
       </c>
       <c r="C39" t="s">
-        <v>660</v>
+        <v>613</v>
       </c>
       <c r="D39" t="s">
         <v>18</v>
@@ -21950,10 +21950,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>661</v>
+        <v>614</v>
       </c>
       <c r="C40" t="s">
-        <v>662</v>
+        <v>615</v>
       </c>
       <c r="D40" t="s">
         <v>18</v>
@@ -21965,10 +21965,10 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>663</v>
+        <v>616</v>
       </c>
       <c r="C41" t="s">
-        <v>664</v>
+        <v>617</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -21980,10 +21980,10 @@
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>665</v>
+        <v>618</v>
       </c>
       <c r="C42" t="s">
-        <v>666</v>
+        <v>619</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
@@ -21995,10 +21995,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>667</v>
+        <v>620</v>
       </c>
       <c r="C43" t="s">
-        <v>668</v>
+        <v>621</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -22010,10 +22010,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>669</v>
+        <v>622</v>
       </c>
       <c r="C44" t="s">
-        <v>670</v>
+        <v>623</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
@@ -22025,10 +22025,10 @@
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>671</v>
+        <v>624</v>
       </c>
       <c r="C45" t="s">
-        <v>672</v>
+        <v>625</v>
       </c>
       <c r="D45" t="s">
         <v>18</v>
@@ -22040,10 +22040,10 @@
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>673</v>
+        <v>626</v>
       </c>
       <c r="C46" t="s">
-        <v>674</v>
+        <v>627</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
@@ -22055,10 +22055,10 @@
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>675</v>
+        <v>628</v>
       </c>
       <c r="C47" t="s">
-        <v>676</v>
+        <v>629</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
@@ -22070,10 +22070,10 @@
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>677</v>
+        <v>630</v>
       </c>
       <c r="C48" t="s">
-        <v>678</v>
+        <v>631</v>
       </c>
       <c r="D48" t="s">
         <v>18</v>
@@ -22085,10 +22085,10 @@
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>679</v>
+        <v>632</v>
       </c>
       <c r="C49" t="s">
-        <v>680</v>
+        <v>633</v>
       </c>
       <c r="D49" t="s">
         <v>18</v>
@@ -22100,10 +22100,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>681</v>
+        <v>634</v>
       </c>
       <c r="C50" t="s">
-        <v>682</v>
+        <v>635</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
@@ -22115,10 +22115,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>683</v>
+        <v>636</v>
       </c>
       <c r="C51" t="s">
-        <v>684</v>
+        <v>637</v>
       </c>
       <c r="D51" t="s">
         <v>18</v>
@@ -22130,10 +22130,10 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>685</v>
+        <v>638</v>
       </c>
       <c r="C52" t="s">
-        <v>686</v>
+        <v>639</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
@@ -22145,10 +22145,10 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>687</v>
+        <v>640</v>
       </c>
       <c r="C53" t="s">
-        <v>688</v>
+        <v>641</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -22160,10 +22160,10 @@
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>689</v>
+        <v>642</v>
       </c>
       <c r="C54" t="s">
-        <v>690</v>
+        <v>643</v>
       </c>
       <c r="D54" t="s">
         <v>18</v>
@@ -22175,10 +22175,10 @@
     <row r="55">
       <c r="A55"/>
       <c r="B55" t="s">
-        <v>691</v>
+        <v>644</v>
       </c>
       <c r="C55" t="s">
-        <v>692</v>
+        <v>645</v>
       </c>
       <c r="D55" t="s">
         <v>18</v>
@@ -22628,7 +22628,7 @@
         <v>1985</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -22644,13 +22644,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>18</v>
@@ -22813,7 +22813,7 @@
         <v>1985</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -22829,13 +22829,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>18</v>
@@ -22960,7 +22960,7 @@
         <v>1985</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -22976,13 +22976,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>18</v>
@@ -23050,7 +23050,7 @@
         <v>1992</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C2" t="s">
         <v>1993</v>
@@ -23254,13 +23254,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>18</v>
@@ -23279,7 +23279,7 @@
         <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>18</v>
@@ -23292,10 +23292,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C15" t="s">
         <v>2001</v>
@@ -25037,38 +25037,36 @@
         <v>397</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>398</v>
       </c>
       <c r="C27" t="s">
-        <v>398</v>
+        <v>18</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E27"/>
       <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H27" t="b">
-        <v>1</v>
-      </c>
+      <c r="H27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>399</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
         <v>400</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>55</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28"/>
+        <v>401</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
       <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
@@ -25078,60 +25076,60 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>393</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>402</v>
+        <v>55</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>403</v>
+        <v>18</v>
       </c>
       <c r="E29"/>
       <c r="G29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H29"/>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>403</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C30" t="s">
         <v>404</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="C30" t="s">
-        <v>406</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E30"/>
       <c r="G30" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="H30" t="b">
-        <v>1</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>406</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C31" t="s">
         <v>408</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" t="s">
-        <v>409</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E31"/>
       <c r="G31" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H31" t="b">
         <v>1</v>
@@ -25139,20 +25137,20 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
         <v>411</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" t="s">
-        <v>412</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E32"/>
       <c r="G32" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H32" t="b">
         <v>1</v>
@@ -25160,29 +25158,31 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>413</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
         <v>414</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="C33" t="s">
-        <v>416</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E33"/>
       <c r="G33" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="H33"/>
+        <v>415</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>416</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>417</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C34" t="s">
         <v>418</v>
@@ -25192,30 +25192,30 @@
       </c>
       <c r="E34"/>
       <c r="G34" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="H34" t="b">
-        <v>1</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="H34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>419</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
         <v>420</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="C35" t="s">
-        <v>421</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E35"/>
       <c r="G35" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="H35"/>
+        <v>421</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
@@ -25241,7 +25241,7 @@
         <v>424</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
       <c r="C37" t="s">
         <v>425</v>
@@ -25251,18 +25251,16 @@
       </c>
       <c r="E37"/>
       <c r="G37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" t="b">
-        <v>1</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="H37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
         <v>426</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>9</v>
+        <v>364</v>
       </c>
       <c r="C38" t="s">
         <v>427</v>
@@ -25274,7 +25272,9 @@
       <c r="G38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H38"/>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
@@ -25319,26 +25319,26 @@
         <v>432</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
         <v>433</v>
-      </c>
-      <c r="C41" t="s">
-        <v>434</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E41"/>
       <c r="G41" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="H41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>434</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C42" t="s">
         <v>436</v>
@@ -25357,7 +25357,7 @@
         <v>437</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>364</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
         <v>438</v>
@@ -25367,7 +25367,7 @@
       </c>
       <c r="E43"/>
       <c r="G43" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="H43"/>
     </row>
@@ -25376,13 +25376,13 @@
         <v>439</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>29</v>
+        <v>364</v>
       </c>
       <c r="C44" t="s">
         <v>440</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>441</v>
+        <v>18</v>
       </c>
       <c r="E44"/>
       <c r="G44" s="3" t="s">
@@ -25392,16 +25392,16 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C45" t="s">
+        <v>442</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>443</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>444</v>
       </c>
       <c r="E45"/>
       <c r="G45" s="3" t="s">
@@ -25411,16 +25411,16 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C46" t="s">
+        <v>445</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>446</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>447</v>
       </c>
       <c r="E46"/>
       <c r="G46" s="3" t="s">
@@ -25430,16 +25430,16 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>447</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
         <v>448</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>449</v>
-      </c>
-      <c r="C47" t="s">
-        <v>449</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E47"/>
       <c r="G47" s="3" t="s">
@@ -25474,7 +25474,7 @@
         <v>453</v>
       </c>
       <c r="C49" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>18</v>
@@ -25487,10 +25487,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>454</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="C50" t="s">
         <v>456</v>
@@ -25512,7 +25512,7 @@
         <v>458</v>
       </c>
       <c r="C51" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>18</v>
@@ -25525,13 +25525,13 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>459</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" t="s">
         <v>461</v>
-      </c>
-      <c r="C52" t="s">
-        <v>462</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>18</v>
@@ -25544,13 +25544,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>462</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>464</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>18</v>
@@ -25563,13 +25563,13 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>465</v>
+        <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>466</v>
+        <v>18</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>18</v>
@@ -25582,13 +25582,13 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>466</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" t="s">
         <v>468</v>
-      </c>
-      <c r="C55" t="s">
-        <v>469</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>18</v>
@@ -25601,13 +25601,13 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>469</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" t="s">
         <v>471</v>
-      </c>
-      <c r="C56" t="s">
-        <v>472</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>18</v>
@@ -25620,10 +25620,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>472</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>473</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C57" t="s">
         <v>474</v>
@@ -25680,10 +25680,10 @@
         <v>479</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
         <v>480</v>
-      </c>
-      <c r="C60" t="s">
-        <v>481</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>18</v>
@@ -25696,13 +25696,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>481</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" t="s">
         <v>483</v>
-      </c>
-      <c r="C61" t="s">
-        <v>484</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>18</v>
@@ -25715,10 +25715,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>484</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>485</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C62" t="s">
         <v>486</v>
@@ -25737,7 +25737,7 @@
         <v>487</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
         <v>488</v>
@@ -25775,7 +25775,7 @@
         <v>491</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C65" t="s">
         <v>492</v>
@@ -25794,7 +25794,7 @@
         <v>493</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>480</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
         <v>494</v>
@@ -25813,7 +25813,7 @@
         <v>495</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C67" t="s">
         <v>496</v>
@@ -25832,7 +25832,7 @@
         <v>497</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>39</v>
+        <v>482</v>
       </c>
       <c r="C68" t="s">
         <v>498</v>
@@ -25870,7 +25870,7 @@
         <v>501</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>393</v>
+        <v>39</v>
       </c>
       <c r="C70" t="s">
         <v>502</v>
@@ -25889,7 +25889,7 @@
         <v>503</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>9</v>
+        <v>393</v>
       </c>
       <c r="C71" t="s">
         <v>504</v>
@@ -25908,7 +25908,7 @@
         <v>505</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>393</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
         <v>506</v>
@@ -25927,10 +25927,10 @@
         <v>507</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>9</v>
+        <v>393</v>
       </c>
       <c r="C73" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>18</v>
@@ -25943,13 +25943,13 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>509</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>18</v>
@@ -25962,10 +25962,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>510</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>511</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="C75" t="s">
         <v>512</v>
@@ -25984,7 +25984,7 @@
         <v>513</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>514</v>
+        <v>393</v>
       </c>
       <c r="C76" t="s">
         <v>514</v>
@@ -26006,7 +26006,7 @@
         <v>516</v>
       </c>
       <c r="C77" t="s">
-        <v>18</v>
+        <v>516</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>18</v>
@@ -27373,7 +27373,7 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B175" t="s">
         <v>566</v>
@@ -27406,10 +27406,10 @@
     <row r="177">
       <c r="A177"/>
       <c r="B177" t="s">
-        <v>341</v>
+        <v>570</v>
       </c>
       <c r="C177" t="s">
-        <v>342</v>
+        <v>571</v>
       </c>
       <c r="D177" t="s">
         <v>18</v>
@@ -27418,32 +27418,43 @@
         <v>18</v>
       </c>
     </row>
+    <row r="178">
+      <c r="A178"/>
+      <c r="B178" t="s">
+        <v>572</v>
+      </c>
+      <c r="C178" t="s">
+        <v>573</v>
+      </c>
+      <c r="D178" t="s">
+        <v>18</v>
+      </c>
+      <c r="E178" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="179">
-      <c r="A179" t="s">
-        <v>1</v>
-      </c>
+      <c r="A179"/>
       <c r="B179" t="s">
-        <v>123</v>
+        <v>574</v>
       </c>
       <c r="C179" t="s">
-        <v>2</v>
+        <v>575</v>
       </c>
       <c r="D179" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E179" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="s">
-        <v>415</v>
-      </c>
+      <c r="A180"/>
       <c r="B180" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="C180" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="D180" t="s">
         <v>18</v>
@@ -27455,10 +27466,10 @@
     <row r="181">
       <c r="A181"/>
       <c r="B181" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="C181" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="D181" t="s">
         <v>18</v>
@@ -27467,32 +27478,43 @@
         <v>18</v>
       </c>
     </row>
+    <row r="182">
+      <c r="A182"/>
+      <c r="B182" t="s">
+        <v>580</v>
+      </c>
+      <c r="C182" t="s">
+        <v>581</v>
+      </c>
+      <c r="D182" t="s">
+        <v>18</v>
+      </c>
+      <c r="E182" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="183">
-      <c r="A183" t="s">
-        <v>1</v>
-      </c>
+      <c r="A183"/>
       <c r="B183" t="s">
-        <v>123</v>
+        <v>582</v>
       </c>
       <c r="C183" t="s">
-        <v>2</v>
+        <v>583</v>
       </c>
       <c r="D183" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E183" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="s">
-        <v>433</v>
-      </c>
+      <c r="A184"/>
       <c r="B184" t="s">
-        <v>574</v>
+        <v>584</v>
       </c>
       <c r="C184" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
       <c r="D184" t="s">
         <v>18</v>
@@ -27504,10 +27526,10 @@
     <row r="185">
       <c r="A185"/>
       <c r="B185" t="s">
-        <v>276</v>
+        <v>586</v>
       </c>
       <c r="C185" t="s">
-        <v>277</v>
+        <v>587</v>
       </c>
       <c r="D185" t="s">
         <v>18</v>
@@ -27519,10 +27541,10 @@
     <row r="186">
       <c r="A186"/>
       <c r="B186" t="s">
-        <v>576</v>
+        <v>588</v>
       </c>
       <c r="C186" t="s">
-        <v>576</v>
+        <v>589</v>
       </c>
       <c r="D186" t="s">
         <v>18</v>
@@ -27534,10 +27556,10 @@
     <row r="187">
       <c r="A187"/>
       <c r="B187" t="s">
-        <v>577</v>
+        <v>590</v>
       </c>
       <c r="C187" t="s">
-        <v>577</v>
+        <v>591</v>
       </c>
       <c r="D187" t="s">
         <v>18</v>
@@ -27549,10 +27571,10 @@
     <row r="188">
       <c r="A188"/>
       <c r="B188" t="s">
-        <v>578</v>
+        <v>268</v>
       </c>
       <c r="C188" t="s">
-        <v>578</v>
+        <v>269</v>
       </c>
       <c r="D188" t="s">
         <v>18</v>
@@ -27564,10 +27586,10 @@
     <row r="189">
       <c r="A189"/>
       <c r="B189" t="s">
-        <v>579</v>
+        <v>592</v>
       </c>
       <c r="C189" t="s">
-        <v>580</v>
+        <v>593</v>
       </c>
       <c r="D189" t="s">
         <v>18</v>
@@ -27579,10 +27601,10 @@
     <row r="190">
       <c r="A190"/>
       <c r="B190" t="s">
-        <v>581</v>
+        <v>594</v>
       </c>
       <c r="C190" t="s">
-        <v>581</v>
+        <v>595</v>
       </c>
       <c r="D190" t="s">
         <v>18</v>
@@ -27594,10 +27616,10 @@
     <row r="191">
       <c r="A191"/>
       <c r="B191" t="s">
-        <v>582</v>
+        <v>596</v>
       </c>
       <c r="C191" t="s">
-        <v>583</v>
+        <v>597</v>
       </c>
       <c r="D191" t="s">
         <v>18</v>
@@ -27609,10 +27631,10 @@
     <row r="192">
       <c r="A192"/>
       <c r="B192" t="s">
-        <v>260</v>
+        <v>598</v>
       </c>
       <c r="C192" t="s">
-        <v>262</v>
+        <v>599</v>
       </c>
       <c r="D192" t="s">
         <v>18</v>
@@ -27621,32 +27643,43 @@
         <v>18</v>
       </c>
     </row>
+    <row r="193">
+      <c r="A193"/>
+      <c r="B193" t="s">
+        <v>600</v>
+      </c>
+      <c r="C193" t="s">
+        <v>601</v>
+      </c>
+      <c r="D193" t="s">
+        <v>18</v>
+      </c>
+      <c r="E193" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="194">
-      <c r="A194" t="s">
-        <v>1</v>
-      </c>
+      <c r="A194"/>
       <c r="B194" t="s">
-        <v>123</v>
+        <v>602</v>
       </c>
       <c r="C194" t="s">
-        <v>2</v>
+        <v>603</v>
       </c>
       <c r="D194" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E194" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="s">
-        <v>468</v>
-      </c>
+      <c r="A195"/>
       <c r="B195" t="s">
-        <v>584</v>
+        <v>604</v>
       </c>
       <c r="C195" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
       <c r="D195" t="s">
         <v>18</v>
@@ -27658,10 +27691,10 @@
     <row r="196">
       <c r="A196"/>
       <c r="B196" t="s">
-        <v>586</v>
+        <v>606</v>
       </c>
       <c r="C196" t="s">
-        <v>587</v>
+        <v>607</v>
       </c>
       <c r="D196" t="s">
         <v>18</v>
@@ -27670,32 +27703,43 @@
         <v>18</v>
       </c>
     </row>
+    <row r="197">
+      <c r="A197"/>
+      <c r="B197" t="s">
+        <v>608</v>
+      </c>
+      <c r="C197" t="s">
+        <v>609</v>
+      </c>
+      <c r="D197" t="s">
+        <v>18</v>
+      </c>
+      <c r="E197" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="198">
-      <c r="A198" t="s">
-        <v>1</v>
-      </c>
+      <c r="A198"/>
       <c r="B198" t="s">
-        <v>123</v>
+        <v>610</v>
       </c>
       <c r="C198" t="s">
-        <v>2</v>
+        <v>611</v>
       </c>
       <c r="D198" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E198" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="s">
-        <v>483</v>
-      </c>
+      <c r="A199"/>
       <c r="B199" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="C199" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="D199" t="s">
         <v>18</v>
@@ -27707,10 +27751,10 @@
     <row r="200">
       <c r="A200"/>
       <c r="B200" t="s">
-        <v>590</v>
+        <v>614</v>
       </c>
       <c r="C200" t="s">
-        <v>591</v>
+        <v>615</v>
       </c>
       <c r="D200" t="s">
         <v>18</v>
@@ -27722,10 +27766,10 @@
     <row r="201">
       <c r="A201"/>
       <c r="B201" t="s">
-        <v>274</v>
+        <v>616</v>
       </c>
       <c r="C201" t="s">
-        <v>592</v>
+        <v>617</v>
       </c>
       <c r="D201" t="s">
         <v>18</v>
@@ -27737,10 +27781,10 @@
     <row r="202">
       <c r="A202"/>
       <c r="B202" t="s">
-        <v>341</v>
+        <v>618</v>
       </c>
       <c r="C202" t="s">
-        <v>342</v>
+        <v>619</v>
       </c>
       <c r="D202" t="s">
         <v>18</v>
@@ -27752,10 +27796,10 @@
     <row r="203">
       <c r="A203"/>
       <c r="B203" t="s">
-        <v>260</v>
+        <v>620</v>
       </c>
       <c r="C203" t="s">
-        <v>262</v>
+        <v>621</v>
       </c>
       <c r="D203" t="s">
         <v>18</v>
@@ -27764,32 +27808,43 @@
         <v>18</v>
       </c>
     </row>
+    <row r="204">
+      <c r="A204"/>
+      <c r="B204" t="s">
+        <v>622</v>
+      </c>
+      <c r="C204" t="s">
+        <v>623</v>
+      </c>
+      <c r="D204" t="s">
+        <v>18</v>
+      </c>
+      <c r="E204" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="205">
-      <c r="A205" t="s">
-        <v>1</v>
-      </c>
+      <c r="A205"/>
       <c r="B205" t="s">
-        <v>123</v>
+        <v>624</v>
       </c>
       <c r="C205" t="s">
-        <v>2</v>
+        <v>625</v>
       </c>
       <c r="D205" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E205" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="s">
-        <v>509</v>
-      </c>
+      <c r="A206"/>
       <c r="B206" t="s">
-        <v>593</v>
+        <v>626</v>
       </c>
       <c r="C206" t="s">
-        <v>594</v>
+        <v>627</v>
       </c>
       <c r="D206" t="s">
         <v>18</v>
@@ -27801,10 +27856,10 @@
     <row r="207">
       <c r="A207"/>
       <c r="B207" t="s">
-        <v>595</v>
+        <v>628</v>
       </c>
       <c r="C207" t="s">
-        <v>596</v>
+        <v>629</v>
       </c>
       <c r="D207" t="s">
         <v>18</v>
@@ -27816,10 +27871,10 @@
     <row r="208">
       <c r="A208"/>
       <c r="B208" t="s">
-        <v>597</v>
+        <v>630</v>
       </c>
       <c r="C208" t="s">
-        <v>598</v>
+        <v>631</v>
       </c>
       <c r="D208" t="s">
         <v>18</v>
@@ -27831,10 +27886,10 @@
     <row r="209">
       <c r="A209"/>
       <c r="B209" t="s">
-        <v>599</v>
+        <v>632</v>
       </c>
       <c r="C209" t="s">
-        <v>600</v>
+        <v>633</v>
       </c>
       <c r="D209" t="s">
         <v>18</v>
@@ -27846,10 +27901,10 @@
     <row r="210">
       <c r="A210"/>
       <c r="B210" t="s">
-        <v>601</v>
+        <v>634</v>
       </c>
       <c r="C210" t="s">
-        <v>602</v>
+        <v>635</v>
       </c>
       <c r="D210" t="s">
         <v>18</v>
@@ -27861,10 +27916,10 @@
     <row r="211">
       <c r="A211"/>
       <c r="B211" t="s">
-        <v>603</v>
+        <v>636</v>
       </c>
       <c r="C211" t="s">
-        <v>604</v>
+        <v>637</v>
       </c>
       <c r="D211" t="s">
         <v>18</v>
@@ -27876,10 +27931,10 @@
     <row r="212">
       <c r="A212"/>
       <c r="B212" t="s">
-        <v>605</v>
+        <v>638</v>
       </c>
       <c r="C212" t="s">
-        <v>606</v>
+        <v>639</v>
       </c>
       <c r="D212" t="s">
         <v>18</v>
@@ -27891,10 +27946,10 @@
     <row r="213">
       <c r="A213"/>
       <c r="B213" t="s">
-        <v>607</v>
+        <v>640</v>
       </c>
       <c r="C213" t="s">
-        <v>608</v>
+        <v>641</v>
       </c>
       <c r="D213" t="s">
         <v>18</v>
@@ -27906,10 +27961,10 @@
     <row r="214">
       <c r="A214"/>
       <c r="B214" t="s">
-        <v>260</v>
+        <v>642</v>
       </c>
       <c r="C214" t="s">
-        <v>262</v>
+        <v>643</v>
       </c>
       <c r="D214" t="s">
         <v>18</v>
@@ -27918,47 +27973,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216">
-      <c r="A216" t="s">
-        <v>1</v>
-      </c>
-      <c r="B216" t="s">
-        <v>123</v>
-      </c>
-      <c r="C216" t="s">
-        <v>2</v>
-      </c>
-      <c r="D216" t="s">
-        <v>3</v>
-      </c>
-      <c r="E216" t="s">
-        <v>124</v>
+    <row r="215">
+      <c r="A215"/>
+      <c r="B215" t="s">
+        <v>644</v>
+      </c>
+      <c r="C215" t="s">
+        <v>645</v>
+      </c>
+      <c r="D215" t="s">
+        <v>18</v>
+      </c>
+      <c r="E215" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>514</v>
+        <v>1</v>
       </c>
       <c r="B217" t="s">
-        <v>609</v>
+        <v>123</v>
       </c>
       <c r="C217" t="s">
-        <v>610</v>
+        <v>2</v>
       </c>
       <c r="D217" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E217" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
     </row>
     <row r="218">
-      <c r="A218"/>
+      <c r="A218" t="s">
+        <v>407</v>
+      </c>
       <c r="B218" t="s">
-        <v>611</v>
+        <v>646</v>
       </c>
       <c r="C218" t="s">
-        <v>612</v>
+        <v>647</v>
       </c>
       <c r="D218" t="s">
         <v>18</v>
@@ -27970,10 +28025,10 @@
     <row r="219">
       <c r="A219"/>
       <c r="B219" t="s">
-        <v>613</v>
+        <v>648</v>
       </c>
       <c r="C219" t="s">
-        <v>614</v>
+        <v>649</v>
       </c>
       <c r="D219" t="s">
         <v>18</v>
@@ -28016,13 +28071,13 @@
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>516</v>
+        <v>417</v>
       </c>
       <c r="B223" t="s">
-        <v>615</v>
+        <v>650</v>
       </c>
       <c r="C223" t="s">
-        <v>616</v>
+        <v>651</v>
       </c>
       <c r="D223" t="s">
         <v>18</v>
@@ -28034,10 +28089,10 @@
     <row r="224">
       <c r="A224"/>
       <c r="B224" t="s">
-        <v>617</v>
+        <v>652</v>
       </c>
       <c r="C224" t="s">
-        <v>618</v>
+        <v>653</v>
       </c>
       <c r="D224" t="s">
         <v>18</v>
@@ -28046,43 +28101,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225">
-      <c r="A225"/>
-      <c r="B225" t="s">
-        <v>619</v>
-      </c>
-      <c r="C225" t="s">
-        <v>620</v>
-      </c>
-      <c r="D225" t="s">
-        <v>18</v>
-      </c>
-      <c r="E225" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="226">
-      <c r="A226"/>
+      <c r="A226" t="s">
+        <v>1</v>
+      </c>
       <c r="B226" t="s">
-        <v>621</v>
+        <v>123</v>
       </c>
       <c r="C226" t="s">
-        <v>622</v>
+        <v>2</v>
       </c>
       <c r="D226" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E226" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
     </row>
     <row r="227">
-      <c r="A227"/>
+      <c r="A227" t="s">
+        <v>435</v>
+      </c>
       <c r="B227" t="s">
-        <v>623</v>
+        <v>654</v>
       </c>
       <c r="C227" t="s">
-        <v>624</v>
+        <v>655</v>
       </c>
       <c r="D227" t="s">
         <v>18</v>
@@ -28094,10 +28138,10 @@
     <row r="228">
       <c r="A228"/>
       <c r="B228" t="s">
-        <v>625</v>
+        <v>276</v>
       </c>
       <c r="C228" t="s">
-        <v>626</v>
+        <v>277</v>
       </c>
       <c r="D228" t="s">
         <v>18</v>
@@ -28109,10 +28153,10 @@
     <row r="229">
       <c r="A229"/>
       <c r="B229" t="s">
-        <v>627</v>
+        <v>656</v>
       </c>
       <c r="C229" t="s">
-        <v>628</v>
+        <v>656</v>
       </c>
       <c r="D229" t="s">
         <v>18</v>
@@ -28124,10 +28168,10 @@
     <row r="230">
       <c r="A230"/>
       <c r="B230" t="s">
-        <v>629</v>
+        <v>657</v>
       </c>
       <c r="C230" t="s">
-        <v>630</v>
+        <v>657</v>
       </c>
       <c r="D230" t="s">
         <v>18</v>
@@ -28139,10 +28183,10 @@
     <row r="231">
       <c r="A231"/>
       <c r="B231" t="s">
-        <v>631</v>
+        <v>658</v>
       </c>
       <c r="C231" t="s">
-        <v>632</v>
+        <v>658</v>
       </c>
       <c r="D231" t="s">
         <v>18</v>
@@ -28154,10 +28198,10 @@
     <row r="232">
       <c r="A232"/>
       <c r="B232" t="s">
-        <v>633</v>
+        <v>659</v>
       </c>
       <c r="C232" t="s">
-        <v>634</v>
+        <v>660</v>
       </c>
       <c r="D232" t="s">
         <v>18</v>
@@ -28169,10 +28213,10 @@
     <row r="233">
       <c r="A233"/>
       <c r="B233" t="s">
-        <v>635</v>
+        <v>661</v>
       </c>
       <c r="C233" t="s">
-        <v>636</v>
+        <v>661</v>
       </c>
       <c r="D233" t="s">
         <v>18</v>
@@ -28184,10 +28228,10 @@
     <row r="234">
       <c r="A234"/>
       <c r="B234" t="s">
-        <v>637</v>
+        <v>662</v>
       </c>
       <c r="C234" t="s">
-        <v>638</v>
+        <v>663</v>
       </c>
       <c r="D234" t="s">
         <v>18</v>
@@ -28199,10 +28243,10 @@
     <row r="235">
       <c r="A235"/>
       <c r="B235" t="s">
-        <v>639</v>
+        <v>260</v>
       </c>
       <c r="C235" t="s">
-        <v>640</v>
+        <v>262</v>
       </c>
       <c r="D235" t="s">
         <v>18</v>
@@ -28211,43 +28255,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236">
-      <c r="A236"/>
-      <c r="B236" t="s">
-        <v>268</v>
-      </c>
-      <c r="C236" t="s">
-        <v>269</v>
-      </c>
-      <c r="D236" t="s">
-        <v>18</v>
-      </c>
-      <c r="E236" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="237">
-      <c r="A237"/>
+      <c r="A237" t="s">
+        <v>1</v>
+      </c>
       <c r="B237" t="s">
-        <v>641</v>
+        <v>123</v>
       </c>
       <c r="C237" t="s">
-        <v>642</v>
+        <v>2</v>
       </c>
       <c r="D237" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E237" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
     </row>
     <row r="238">
-      <c r="A238"/>
+      <c r="A238" t="s">
+        <v>470</v>
+      </c>
       <c r="B238" t="s">
-        <v>643</v>
+        <v>664</v>
       </c>
       <c r="C238" t="s">
-        <v>644</v>
+        <v>665</v>
       </c>
       <c r="D238" t="s">
         <v>18</v>
@@ -28259,10 +28292,10 @@
     <row r="239">
       <c r="A239"/>
       <c r="B239" t="s">
-        <v>645</v>
+        <v>666</v>
       </c>
       <c r="C239" t="s">
-        <v>646</v>
+        <v>667</v>
       </c>
       <c r="D239" t="s">
         <v>18</v>
@@ -28271,43 +28304,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240">
-      <c r="A240"/>
-      <c r="B240" t="s">
-        <v>601</v>
-      </c>
-      <c r="C240" t="s">
-        <v>602</v>
-      </c>
-      <c r="D240" t="s">
-        <v>18</v>
-      </c>
-      <c r="E240" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="241">
-      <c r="A241"/>
+      <c r="A241" t="s">
+        <v>1</v>
+      </c>
       <c r="B241" t="s">
-        <v>647</v>
+        <v>123</v>
       </c>
       <c r="C241" t="s">
-        <v>648</v>
+        <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E241" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
     </row>
     <row r="242">
-      <c r="A242"/>
+      <c r="A242" t="s">
+        <v>485</v>
+      </c>
       <c r="B242" t="s">
-        <v>649</v>
+        <v>668</v>
       </c>
       <c r="C242" t="s">
-        <v>650</v>
+        <v>669</v>
       </c>
       <c r="D242" t="s">
         <v>18</v>
@@ -28319,10 +28341,10 @@
     <row r="243">
       <c r="A243"/>
       <c r="B243" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="C243" t="s">
-        <v>652</v>
+        <v>671</v>
       </c>
       <c r="D243" t="s">
         <v>18</v>
@@ -28334,10 +28356,10 @@
     <row r="244">
       <c r="A244"/>
       <c r="B244" t="s">
-        <v>653</v>
+        <v>274</v>
       </c>
       <c r="C244" t="s">
-        <v>654</v>
+        <v>672</v>
       </c>
       <c r="D244" t="s">
         <v>18</v>
@@ -28349,10 +28371,10 @@
     <row r="245">
       <c r="A245"/>
       <c r="B245" t="s">
-        <v>655</v>
+        <v>341</v>
       </c>
       <c r="C245" t="s">
-        <v>656</v>
+        <v>342</v>
       </c>
       <c r="D245" t="s">
         <v>18</v>
@@ -28364,10 +28386,10 @@
     <row r="246">
       <c r="A246"/>
       <c r="B246" t="s">
-        <v>657</v>
+        <v>260</v>
       </c>
       <c r="C246" t="s">
-        <v>658</v>
+        <v>262</v>
       </c>
       <c r="D246" t="s">
         <v>18</v>
@@ -28376,43 +28398,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="247">
-      <c r="A247"/>
-      <c r="B247" t="s">
-        <v>659</v>
-      </c>
-      <c r="C247" t="s">
-        <v>660</v>
-      </c>
-      <c r="D247" t="s">
-        <v>18</v>
-      </c>
-      <c r="E247" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="248">
-      <c r="A248"/>
+      <c r="A248" t="s">
+        <v>1</v>
+      </c>
       <c r="B248" t="s">
-        <v>661</v>
+        <v>123</v>
       </c>
       <c r="C248" t="s">
-        <v>662</v>
+        <v>2</v>
       </c>
       <c r="D248" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E248" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
     </row>
     <row r="249">
-      <c r="A249"/>
+      <c r="A249" t="s">
+        <v>511</v>
+      </c>
       <c r="B249" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="C249" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="D249" t="s">
         <v>18</v>
@@ -28424,10 +28435,10 @@
     <row r="250">
       <c r="A250"/>
       <c r="B250" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="C250" t="s">
-        <v>666</v>
+        <v>676</v>
       </c>
       <c r="D250" t="s">
         <v>18</v>
@@ -28439,10 +28450,10 @@
     <row r="251">
       <c r="A251"/>
       <c r="B251" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="C251" t="s">
-        <v>668</v>
+        <v>678</v>
       </c>
       <c r="D251" t="s">
         <v>18</v>
@@ -28454,10 +28465,10 @@
     <row r="252">
       <c r="A252"/>
       <c r="B252" t="s">
-        <v>669</v>
+        <v>679</v>
       </c>
       <c r="C252" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="D252" t="s">
         <v>18</v>
@@ -28469,10 +28480,10 @@
     <row r="253">
       <c r="A253"/>
       <c r="B253" t="s">
-        <v>671</v>
+        <v>598</v>
       </c>
       <c r="C253" t="s">
-        <v>672</v>
+        <v>599</v>
       </c>
       <c r="D253" t="s">
         <v>18</v>
@@ -28484,10 +28495,10 @@
     <row r="254">
       <c r="A254"/>
       <c r="B254" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="C254" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
       <c r="D254" t="s">
         <v>18</v>
@@ -28499,10 +28510,10 @@
     <row r="255">
       <c r="A255"/>
       <c r="B255" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="C255" t="s">
-        <v>676</v>
+        <v>684</v>
       </c>
       <c r="D255" t="s">
         <v>18</v>
@@ -28514,10 +28525,10 @@
     <row r="256">
       <c r="A256"/>
       <c r="B256" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="C256" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
       <c r="D256" t="s">
         <v>18</v>
@@ -28529,10 +28540,10 @@
     <row r="257">
       <c r="A257"/>
       <c r="B257" t="s">
-        <v>679</v>
+        <v>260</v>
       </c>
       <c r="C257" t="s">
-        <v>680</v>
+        <v>262</v>
       </c>
       <c r="D257" t="s">
         <v>18</v>
@@ -28541,43 +28552,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="258">
-      <c r="A258"/>
-      <c r="B258" t="s">
-        <v>681</v>
-      </c>
-      <c r="C258" t="s">
-        <v>682</v>
-      </c>
-      <c r="D258" t="s">
-        <v>18</v>
-      </c>
-      <c r="E258" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="259">
-      <c r="A259"/>
+      <c r="A259" t="s">
+        <v>1</v>
+      </c>
       <c r="B259" t="s">
-        <v>683</v>
+        <v>123</v>
       </c>
       <c r="C259" t="s">
-        <v>684</v>
+        <v>2</v>
       </c>
       <c r="D259" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E259" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
     </row>
     <row r="260">
-      <c r="A260"/>
+      <c r="A260" t="s">
+        <v>516</v>
+      </c>
       <c r="B260" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C260" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="D260" t="s">
         <v>18</v>
@@ -28589,10 +28589,10 @@
     <row r="261">
       <c r="A261"/>
       <c r="B261" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C261" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D261" t="s">
         <v>18</v>
@@ -28604,10 +28604,10 @@
     <row r="262">
       <c r="A262"/>
       <c r="B262" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="C262" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="D262" t="s">
         <v>18</v>
@@ -28619,10 +28619,10 @@
     <row r="263">
       <c r="A263"/>
       <c r="B263" t="s">
-        <v>691</v>
+        <v>341</v>
       </c>
       <c r="C263" t="s">
-        <v>692</v>
+        <v>342</v>
       </c>
       <c r="D263" t="s">
         <v>18</v>
@@ -29871,7 +29871,7 @@
         <v>839</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C45" t="s">
         <v>840</v>
@@ -29890,7 +29890,7 @@
         <v>841</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C46" t="s">
         <v>842</v>
@@ -29928,7 +29928,7 @@
         <v>845</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C48" t="s">
         <v>846</v>
@@ -29947,7 +29947,7 @@
         <v>847</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C49" t="s">
         <v>848</v>
@@ -29966,7 +29966,7 @@
         <v>849</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C50" t="s">
         <v>850</v>
@@ -30004,7 +30004,7 @@
         <v>854</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C52" t="s">
         <v>855</v>
@@ -30137,7 +30137,7 @@
         <v>865</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C59" t="s">
         <v>866</v>
@@ -30175,7 +30175,7 @@
         <v>869</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C61" t="s">
         <v>870</v>
@@ -30951,7 +30951,7 @@
         <v>969</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C101" t="s">
         <v>970</v>
@@ -33534,7 +33534,7 @@
         <v>1276</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C51" t="s">
         <v>1277</v>
@@ -33937,13 +33937,13 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B79" t="s">
-        <v>566</v>
+        <v>646</v>
       </c>
       <c r="C79" t="s">
-        <v>567</v>
+        <v>647</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
@@ -33955,10 +33955,10 @@
     <row r="80">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>568</v>
+        <v>648</v>
       </c>
       <c r="C80" t="s">
-        <v>569</v>
+        <v>649</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
@@ -34594,7 +34594,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>1350</v>
@@ -35208,7 +35208,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>1350</v>

</xml_diff>

<commit_message>
#2728 do not count deleted participants
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7849" uniqueCount="2150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7849" uniqueCount="2152">
   <si>
     <t>Field</t>
   </si>
@@ -6331,7 +6331,13 @@
     <t>publicOwnership</t>
   </si>
   <si>
+    <t>Public ownership</t>
+  </si>
+  <si>
     <t>archived</t>
+  </si>
+  <si>
+    <t>Archived</t>
   </si>
   <si>
     <t>epidCode</t>
@@ -12785,7 +12791,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>584</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>18</v>
@@ -12804,7 +12810,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>587</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>18</v>
@@ -12823,7 +12829,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>590</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>18</v>
@@ -23256,7 +23262,7 @@
         <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>2098</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>18</v>
@@ -23269,13 +23275,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>2100</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>18</v>
@@ -24525,13 +24531,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2099</v>
+        <v>2101</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>2100</v>
+        <v>2102</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>18</v>
@@ -24544,13 +24550,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2101</v>
+        <v>2103</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>2102</v>
+        <v>2104</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>18</v>
@@ -24563,13 +24569,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>2100</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>18</v>
@@ -24601,10 +24607,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2103</v>
+        <v>2105</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>2104</v>
+        <v>2106</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -24691,13 +24697,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2099</v>
+        <v>2101</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>2100</v>
+        <v>2102</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>18</v>
@@ -24710,13 +24716,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2101</v>
+        <v>2103</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>2102</v>
+        <v>2104</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>18</v>
@@ -24748,13 +24754,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>2100</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>18</v>
@@ -24895,13 +24901,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>2100</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>18</v>
@@ -24985,13 +24991,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2105</v>
+        <v>2107</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>2106</v>
+        <v>2108</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>18</v>
@@ -25004,13 +25010,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2107</v>
+        <v>2109</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>2108</v>
+        <v>2110</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>18</v>
@@ -25061,7 +25067,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2109</v>
+        <v>2111</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>9</v>
@@ -25105,7 +25111,7 @@
         <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>2110</v>
+        <v>2112</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>18</v>
@@ -25118,11 +25124,11 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2111</v>
+        <v>2113</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" t="s">
-        <v>2112</v>
+        <v>2114</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>18</v>
@@ -25135,10 +25141,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2103</v>
+        <v>2105</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>2104</v>
+        <v>2106</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -25230,7 +25236,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2113</v>
+        <v>2115</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>58</v>
@@ -25255,7 +25261,7 @@
         <v>615</v>
       </c>
       <c r="C16" t="s">
-        <v>2114</v>
+        <v>2116</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>18</v>
@@ -25268,13 +25274,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2115</v>
+        <v>2117</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>498</v>
       </c>
       <c r="C17" t="s">
-        <v>2116</v>
+        <v>2118</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>18</v>
@@ -25287,16 +25293,16 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2117</v>
+        <v>2119</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>2118</v>
+        <v>2120</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>2119</v>
+        <v>2121</v>
       </c>
       <c r="E18"/>
       <c r="G18" s="23" t="s">
@@ -25306,10 +25312,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2120</v>
+        <v>2122</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>2121</v>
+        <v>2123</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -26201,13 +26207,13 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>2121</v>
+        <v>2123</v>
       </c>
       <c r="B80" t="s">
-        <v>2122</v>
+        <v>2124</v>
       </c>
       <c r="C80" t="s">
-        <v>2123</v>
+        <v>2125</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
@@ -26219,10 +26225,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>2124</v>
+        <v>2126</v>
       </c>
       <c r="C81" t="s">
-        <v>2125</v>
+        <v>2127</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -26234,10 +26240,10 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>2126</v>
+        <v>2128</v>
       </c>
       <c r="C82" t="s">
-        <v>2127</v>
+        <v>2129</v>
       </c>
       <c r="D82" t="s">
         <v>18</v>
@@ -26249,10 +26255,10 @@
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>2128</v>
+        <v>2130</v>
       </c>
       <c r="C83" t="s">
-        <v>2129</v>
+        <v>2131</v>
       </c>
       <c r="D83" t="s">
         <v>18</v>
@@ -26264,10 +26270,10 @@
     <row r="84">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>2130</v>
+        <v>2132</v>
       </c>
       <c r="C84" t="s">
-        <v>2131</v>
+        <v>2133</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
@@ -26279,10 +26285,10 @@
     <row r="85">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>2132</v>
+        <v>2134</v>
       </c>
       <c r="C85" t="s">
-        <v>2133</v>
+        <v>2135</v>
       </c>
       <c r="D85" t="s">
         <v>18</v>
@@ -26294,10 +26300,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>2134</v>
+        <v>2136</v>
       </c>
       <c r="C86" t="s">
-        <v>2135</v>
+        <v>2137</v>
       </c>
       <c r="D86" t="s">
         <v>18</v>
@@ -26309,10 +26315,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>2136</v>
+        <v>2138</v>
       </c>
       <c r="C87" t="s">
-        <v>2137</v>
+        <v>2139</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
@@ -26324,10 +26330,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>2138</v>
+        <v>2140</v>
       </c>
       <c r="C88" t="s">
-        <v>2139</v>
+        <v>2141</v>
       </c>
       <c r="D88" t="s">
         <v>18</v>
@@ -26339,10 +26345,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>2140</v>
+        <v>2142</v>
       </c>
       <c r="C89" t="s">
-        <v>2141</v>
+        <v>2143</v>
       </c>
       <c r="D89" t="s">
         <v>18</v>
@@ -26354,10 +26360,10 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>2142</v>
+        <v>2144</v>
       </c>
       <c r="C90" t="s">
-        <v>2143</v>
+        <v>2145</v>
       </c>
       <c r="D90" t="s">
         <v>18</v>
@@ -26369,10 +26375,10 @@
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>2144</v>
+        <v>2146</v>
       </c>
       <c r="C91" t="s">
-        <v>2145</v>
+        <v>2147</v>
       </c>
       <c r="D91" t="s">
         <v>18</v>
@@ -26384,10 +26390,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>2146</v>
+        <v>2148</v>
       </c>
       <c r="C92" t="s">
-        <v>2147</v>
+        <v>2149</v>
       </c>
       <c r="D92" t="s">
         <v>18</v>
@@ -26416,12 +26422,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2148</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2149</v>
+        <v>2151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#4773 add missing sample material types
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11215" uniqueCount="2782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11235" uniqueCount="2792">
   <si>
     <t>Field</t>
   </si>
@@ -6789,6 +6789,36 @@
   </si>
   <si>
     <t>Brain tissue</t>
+  </si>
+  <si>
+    <t>ANTERIOR_NARES_SWAB</t>
+  </si>
+  <si>
+    <t>Anterior nares swab</t>
+  </si>
+  <si>
+    <t>OROPHARYNGEAL_ASPIRATE</t>
+  </si>
+  <si>
+    <t>Oropharyngeal aspirate</t>
+  </si>
+  <si>
+    <t>NASOPHARYNGEAL_ASPIRATE</t>
+  </si>
+  <si>
+    <t>Nasopharyngeal aspirate</t>
+  </si>
+  <si>
+    <t>LOWER_RESPIRATORY_SAMPLE</t>
+  </si>
+  <si>
+    <t>Lower respiratory sample</t>
+  </si>
+  <si>
+    <t>PLEURAL_FLUID_SPECIMEN</t>
+  </si>
+  <si>
+    <t>Pleural fluid specimen</t>
   </si>
   <si>
     <t>EXTERNAL</t>
@@ -8618,7 +8648,7 @@
 </file>
 
 <file path=xl/tables/table105.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="105" name="SampleSampleMaterial" displayName="SampleSampleMaterial" ref="A45:E65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="105" name="SampleSampleMaterial" displayName="SampleSampleMaterial" ref="A45:E70">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -8632,7 +8662,7 @@
 </file>
 
 <file path=xl/tables/table106.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="106" name="SampleSamplePurpose" displayName="SampleSamplePurpose" ref="A67:E69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="106" name="SampleSamplePurpose" displayName="SampleSamplePurpose" ref="A72:E74">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -8646,7 +8676,7 @@
 </file>
 
 <file path=xl/tables/table107.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="107" name="SampleSpecimenCondition" displayName="SampleSpecimenCondition" ref="A71:E73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="107" name="SampleSpecimenCondition" displayName="SampleSpecimenCondition" ref="A76:E78">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -8660,7 +8690,7 @@
 </file>
 
 <file path=xl/tables/table108.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="108" name="SampleSampleSource" displayName="SampleSampleSource" ref="A75:E78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="108" name="SampleSampleSource" displayName="SampleSampleSource" ref="A80:E83">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -8674,7 +8704,7 @@
 </file>
 
 <file path=xl/tables/table109.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="109" name="SamplePathogenTestResultType" displayName="SamplePathogenTestResultType" ref="A80:E85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="109" name="SamplePathogenTestResultType" displayName="SamplePathogenTestResultType" ref="A85:E90">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -8702,7 +8732,7 @@
 </file>
 
 <file path=xl/tables/table110.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="110" name="SampleSamplingReason" displayName="SampleSamplingReason" ref="A87:E101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="110" name="SampleSamplingReason" displayName="SampleSamplingReason" ref="A92:E106">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -22762,7 +22792,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -24011,10 +24041,10 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>179</v>
+        <v>2250</v>
       </c>
       <c r="C65" t="s">
-        <v>180</v>
+        <v>2251</v>
       </c>
       <c r="D65" t="s">
         <v>22</v>
@@ -24023,32 +24053,43 @@
         <v>22</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66"/>
+      <c r="B66" t="s">
+        <v>2252</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2253</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="67">
-      <c r="A67" t="s">
-        <v>1</v>
-      </c>
+      <c r="A67"/>
       <c r="B67" t="s">
-        <v>158</v>
+        <v>2254</v>
       </c>
       <c r="C67" t="s">
-        <v>3</v>
+        <v>2255</v>
       </c>
       <c r="D67" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E67" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s">
-        <v>2166</v>
-      </c>
+      <c r="A68"/>
       <c r="B68" t="s">
-        <v>2250</v>
+        <v>2256</v>
       </c>
       <c r="C68" t="s">
-        <v>2251</v>
+        <v>2257</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -24060,10 +24101,10 @@
     <row r="69">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>2252</v>
+        <v>2258</v>
       </c>
       <c r="C69" t="s">
-        <v>2253</v>
+        <v>2259</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -24072,47 +24113,47 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" t="s">
-        <v>158</v>
-      </c>
-      <c r="C71" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" t="s">
-        <v>4</v>
-      </c>
-      <c r="E71" t="s">
-        <v>168</v>
+    <row r="70">
+      <c r="A70"/>
+      <c r="B70" t="s">
+        <v>179</v>
+      </c>
+      <c r="C70" t="s">
+        <v>180</v>
+      </c>
+      <c r="D70" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>2178</v>
+        <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>2254</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
-        <v>2255</v>
+        <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E72" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73"/>
+      <c r="A73" t="s">
+        <v>2166</v>
+      </c>
       <c r="B73" t="s">
-        <v>2256</v>
+        <v>2260</v>
       </c>
       <c r="C73" t="s">
-        <v>2257</v>
+        <v>2261</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -24121,47 +24162,47 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>1</v>
-      </c>
-      <c r="B75" t="s">
-        <v>158</v>
-      </c>
-      <c r="C75" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" t="s">
-        <v>4</v>
-      </c>
-      <c r="E75" t="s">
-        <v>168</v>
+    <row r="74">
+      <c r="A74"/>
+      <c r="B74" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2263</v>
+      </c>
+      <c r="D74" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>2184</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>2258</v>
+        <v>158</v>
       </c>
       <c r="C76" t="s">
-        <v>2259</v>
+        <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77"/>
+      <c r="A77" t="s">
+        <v>2178</v>
+      </c>
       <c r="B77" t="s">
-        <v>2260</v>
+        <v>2264</v>
       </c>
       <c r="C77" t="s">
-        <v>2261</v>
+        <v>2265</v>
       </c>
       <c r="D77" t="s">
         <v>22</v>
@@ -24173,10 +24214,10 @@
     <row r="78">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>2262</v>
+        <v>2266</v>
       </c>
       <c r="C78" t="s">
-        <v>2263</v>
+        <v>2267</v>
       </c>
       <c r="D78" t="s">
         <v>22</v>
@@ -24204,13 +24245,13 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>2193</v>
+        <v>2184</v>
       </c>
       <c r="B81" t="s">
-        <v>2264</v>
+        <v>2268</v>
       </c>
       <c r="C81" t="s">
-        <v>2265</v>
+        <v>2269</v>
       </c>
       <c r="D81" t="s">
         <v>22</v>
@@ -24222,10 +24263,10 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>936</v>
+        <v>2270</v>
       </c>
       <c r="C82" t="s">
-        <v>938</v>
+        <v>2271</v>
       </c>
       <c r="D82" t="s">
         <v>22</v>
@@ -24237,10 +24278,10 @@
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>2266</v>
+        <v>2272</v>
       </c>
       <c r="C83" t="s">
-        <v>2267</v>
+        <v>2273</v>
       </c>
       <c r="D83" t="s">
         <v>22</v>
@@ -24249,62 +24290,62 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84"/>
-      <c r="B84" t="s">
-        <v>2268</v>
-      </c>
-      <c r="C84" t="s">
-        <v>2269</v>
-      </c>
-      <c r="D84" t="s">
-        <v>22</v>
-      </c>
-      <c r="E84" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="85">
-      <c r="A85"/>
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
       <c r="B85" t="s">
-        <v>2270</v>
+        <v>158</v>
       </c>
       <c r="C85" t="s">
-        <v>2271</v>
+        <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E85" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>2193</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2274</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2275</v>
+      </c>
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="s">
-        <v>1</v>
-      </c>
+      <c r="A87"/>
       <c r="B87" t="s">
-        <v>158</v>
+        <v>936</v>
       </c>
       <c r="C87" t="s">
-        <v>3</v>
+        <v>938</v>
       </c>
       <c r="D87" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E87" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="s">
-        <v>2208</v>
-      </c>
+      <c r="A88"/>
       <c r="B88" t="s">
-        <v>2272</v>
+        <v>2276</v>
       </c>
       <c r="C88" t="s">
-        <v>2273</v>
+        <v>2277</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -24316,10 +24357,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>2274</v>
+        <v>2278</v>
       </c>
       <c r="C89" t="s">
-        <v>2275</v>
+        <v>2279</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -24331,10 +24372,10 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>919</v>
+        <v>2280</v>
       </c>
       <c r="C90" t="s">
-        <v>643</v>
+        <v>2281</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -24343,43 +24384,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91"/>
-      <c r="B91" t="s">
-        <v>2276</v>
-      </c>
-      <c r="C91" t="s">
-        <v>2277</v>
-      </c>
-      <c r="D91" t="s">
-        <v>22</v>
-      </c>
-      <c r="E91" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="92">
-      <c r="A92"/>
+      <c r="A92" t="s">
+        <v>1</v>
+      </c>
       <c r="B92" t="s">
-        <v>2278</v>
+        <v>158</v>
       </c>
       <c r="C92" t="s">
-        <v>2279</v>
+        <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E92" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93"/>
+      <c r="A93" t="s">
+        <v>2208</v>
+      </c>
       <c r="B93" t="s">
-        <v>2280</v>
+        <v>2282</v>
       </c>
       <c r="C93" t="s">
-        <v>2281</v>
+        <v>2283</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -24391,10 +24421,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>2282</v>
+        <v>2284</v>
       </c>
       <c r="C94" t="s">
-        <v>2283</v>
+        <v>2285</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -24406,10 +24436,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>2284</v>
+        <v>919</v>
       </c>
       <c r="C95" t="s">
-        <v>2285</v>
+        <v>643</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -24451,10 +24481,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>1071</v>
+        <v>2290</v>
       </c>
       <c r="C98" t="s">
-        <v>2290</v>
+        <v>2291</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -24466,10 +24496,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>2291</v>
+        <v>2292</v>
       </c>
       <c r="C99" t="s">
-        <v>791</v>
+        <v>2293</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -24481,10 +24511,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>185</v>
+        <v>2294</v>
       </c>
       <c r="C100" t="s">
-        <v>186</v>
+        <v>2295</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
@@ -24496,15 +24526,90 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
+        <v>2296</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2297</v>
+      </c>
+      <c r="D101" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102"/>
+      <c r="B102" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2299</v>
+      </c>
+      <c r="D102" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103"/>
+      <c r="B103" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D103" t="s">
+        <v>22</v>
+      </c>
+      <c r="E103" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104"/>
+      <c r="B104" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C104" t="s">
+        <v>791</v>
+      </c>
+      <c r="D104" t="s">
+        <v>22</v>
+      </c>
+      <c r="E104" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105"/>
+      <c r="B105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C105" t="s">
+        <v>186</v>
+      </c>
+      <c r="D105" t="s">
+        <v>22</v>
+      </c>
+      <c r="E105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106"/>
+      <c r="B106" t="s">
         <v>1074</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C106" t="s">
         <v>847</v>
       </c>
-      <c r="D101" t="s">
-        <v>22</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" t="s">
         <v>22</v>
       </c>
     </row>
@@ -24581,7 +24686,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2292</v>
+        <v>2302</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2187</v>
@@ -24605,17 +24710,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2293</v>
+        <v>2303</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>91</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2294</v>
+        <v>2304</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>2295</v>
+        <v>2305</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -24629,17 +24734,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2296</v>
+        <v>2306</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2297</v>
+        <v>2307</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>2298</v>
+        <v>2308</v>
       </c>
       <c r="F4"/>
       <c r="H4" s="16" t="s">
@@ -24651,14 +24756,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2299</v>
+        <v>2309</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2300</v>
+        <v>2310</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>22</v>
@@ -24673,17 +24778,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2301</v>
+        <v>2311</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>2302</v>
+        <v>2312</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2303</v>
+        <v>2313</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>2304</v>
+        <v>2314</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -24697,7 +24802,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2305</v>
+        <v>2315</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>12</v>
@@ -24706,10 +24811,10 @@
         <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>2306</v>
+        <v>2316</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>2307</v>
+        <v>2317</v>
       </c>
       <c r="F7"/>
       <c r="H7" s="16" t="s">
@@ -24721,17 +24826,17 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2308</v>
+        <v>2318</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2309</v>
+        <v>2319</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>2310</v>
+        <v>2320</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -24755,7 +24860,7 @@
         <v>230</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>2311</v>
+        <v>2321</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -24781,7 +24886,7 @@
         <v>2170</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>2312</v>
+        <v>2322</v>
       </c>
       <c r="F10"/>
       <c r="H10" s="16" t="s">
@@ -24793,7 +24898,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2313</v>
+        <v>2323</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>626</v>
@@ -24819,17 +24924,17 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2314</v>
+        <v>2324</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>2193</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2315</v>
+        <v>2325</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>2316</v>
+        <v>2326</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -24843,7 +24948,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2317</v>
+        <v>2327</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>12</v>
@@ -24852,10 +24957,10 @@
         <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>2318</v>
+        <v>2328</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>2319</v>
+        <v>2329</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -24869,17 +24974,17 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2320</v>
+        <v>2330</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>140</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>2321</v>
+        <v>2331</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>2322</v>
+        <v>2332</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -24893,17 +24998,17 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2323</v>
+        <v>2333</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>140</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2324</v>
+        <v>2334</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>2325</v>
+        <v>2335</v>
       </c>
       <c r="F15"/>
       <c r="H15" s="16" t="s">
@@ -24915,7 +25020,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2326</v>
+        <v>2336</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>12</v>
@@ -24924,10 +25029,10 @@
         <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>2327</v>
+        <v>2337</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>2328</v>
+        <v>2338</v>
       </c>
       <c r="F16"/>
       <c r="H16" s="16" t="s">
@@ -24939,14 +25044,14 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2329</v>
+        <v>2339</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>2330</v>
+        <v>2340</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>22</v>
@@ -24985,14 +25090,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2331</v>
+        <v>2341</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>140</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2332</v>
+        <v>2342</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>22</v>
@@ -25937,13 +26042,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>2302</v>
+        <v>2312</v>
       </c>
       <c r="B85" t="s">
-        <v>2333</v>
+        <v>2343</v>
       </c>
       <c r="C85" t="s">
-        <v>2334</v>
+        <v>2344</v>
       </c>
       <c r="D85" t="s">
         <v>22</v>
@@ -25955,10 +26060,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>2335</v>
+        <v>2345</v>
       </c>
       <c r="C86" t="s">
-        <v>2336</v>
+        <v>2346</v>
       </c>
       <c r="D86" t="s">
         <v>22</v>
@@ -25970,10 +26075,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>2337</v>
+        <v>2347</v>
       </c>
       <c r="C87" t="s">
-        <v>2338</v>
+        <v>2348</v>
       </c>
       <c r="D87" t="s">
         <v>22</v>
@@ -25985,10 +26090,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>2339</v>
+        <v>2349</v>
       </c>
       <c r="C88" t="s">
-        <v>2340</v>
+        <v>2350</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -26000,10 +26105,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>2341</v>
+        <v>2351</v>
       </c>
       <c r="C89" t="s">
-        <v>2342</v>
+        <v>2352</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -26015,7 +26120,7 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>2343</v>
+        <v>2353</v>
       </c>
       <c r="C90" t="s">
         <v>1087</v>
@@ -26030,10 +26135,10 @@
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>2344</v>
+        <v>2354</v>
       </c>
       <c r="C91" t="s">
-        <v>2345</v>
+        <v>2355</v>
       </c>
       <c r="D91" t="s">
         <v>22</v>
@@ -26045,10 +26150,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>2346</v>
+        <v>2356</v>
       </c>
       <c r="C92" t="s">
-        <v>2347</v>
+        <v>2357</v>
       </c>
       <c r="D92" t="s">
         <v>22</v>
@@ -26060,10 +26165,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>2348</v>
+        <v>2358</v>
       </c>
       <c r="C93" t="s">
-        <v>2349</v>
+        <v>2359</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -26075,10 +26180,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>2350</v>
+        <v>2360</v>
       </c>
       <c r="C94" t="s">
-        <v>2351</v>
+        <v>2361</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -26090,10 +26195,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>2352</v>
+        <v>2362</v>
       </c>
       <c r="C95" t="s">
-        <v>2353</v>
+        <v>2363</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -26105,10 +26210,10 @@
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
-        <v>2354</v>
+        <v>2364</v>
       </c>
       <c r="C96" t="s">
-        <v>2355</v>
+        <v>2365</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -26120,10 +26225,10 @@
     <row r="97">
       <c r="A97"/>
       <c r="B97" t="s">
-        <v>2356</v>
+        <v>2366</v>
       </c>
       <c r="C97" t="s">
-        <v>2357</v>
+        <v>2367</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
@@ -26135,10 +26240,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>2358</v>
+        <v>2368</v>
       </c>
       <c r="C98" t="s">
-        <v>2359</v>
+        <v>2369</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -26150,10 +26255,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>2360</v>
+        <v>2370</v>
       </c>
       <c r="C99" t="s">
-        <v>2361</v>
+        <v>2371</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -26165,10 +26270,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>2362</v>
+        <v>2372</v>
       </c>
       <c r="C100" t="s">
-        <v>2363</v>
+        <v>2373</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
@@ -26180,10 +26285,10 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
-        <v>2364</v>
+        <v>2374</v>
       </c>
       <c r="C101" t="s">
-        <v>2365</v>
+        <v>2375</v>
       </c>
       <c r="D101" t="s">
         <v>22</v>
@@ -26195,10 +26300,10 @@
     <row r="102">
       <c r="A102"/>
       <c r="B102" t="s">
-        <v>2366</v>
+        <v>2376</v>
       </c>
       <c r="C102" t="s">
-        <v>2367</v>
+        <v>2377</v>
       </c>
       <c r="D102" t="s">
         <v>22</v>
@@ -26210,10 +26315,10 @@
     <row r="103">
       <c r="A103"/>
       <c r="B103" t="s">
-        <v>2368</v>
+        <v>2378</v>
       </c>
       <c r="C103" t="s">
-        <v>2369</v>
+        <v>2379</v>
       </c>
       <c r="D103" t="s">
         <v>22</v>
@@ -26225,10 +26330,10 @@
     <row r="104">
       <c r="A104"/>
       <c r="B104" t="s">
-        <v>2370</v>
+        <v>2380</v>
       </c>
       <c r="C104" t="s">
-        <v>2371</v>
+        <v>2381</v>
       </c>
       <c r="D104" t="s">
         <v>22</v>
@@ -26274,10 +26379,10 @@
         <v>2193</v>
       </c>
       <c r="B108" t="s">
-        <v>2264</v>
+        <v>2274</v>
       </c>
       <c r="C108" t="s">
-        <v>2265</v>
+        <v>2275</v>
       </c>
       <c r="D108" t="s">
         <v>22</v>
@@ -26304,10 +26409,10 @@
     <row r="110">
       <c r="A110"/>
       <c r="B110" t="s">
-        <v>2266</v>
+        <v>2276</v>
       </c>
       <c r="C110" t="s">
-        <v>2267</v>
+        <v>2277</v>
       </c>
       <c r="D110" t="s">
         <v>22</v>
@@ -26319,10 +26424,10 @@
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>2268</v>
+        <v>2278</v>
       </c>
       <c r="C111" t="s">
-        <v>2269</v>
+        <v>2279</v>
       </c>
       <c r="D111" t="s">
         <v>22</v>
@@ -26334,10 +26439,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>2270</v>
+        <v>2280</v>
       </c>
       <c r="C112" t="s">
-        <v>2271</v>
+        <v>2281</v>
       </c>
       <c r="D112" t="s">
         <v>22</v>
@@ -26416,7 +26521,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2292</v>
+        <v>2302</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>2187</v>
@@ -26438,14 +26543,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2308</v>
+        <v>2318</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>55</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2309</v>
+        <v>2319</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>22</v>
@@ -26460,14 +26565,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2372</v>
+        <v>2382</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>2373</v>
+        <v>2383</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2374</v>
+        <v>2384</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>22</v>
@@ -26482,14 +26587,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2375</v>
+        <v>2385</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>2373</v>
+        <v>2383</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2376</v>
+        <v>2386</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>22</v>
@@ -26504,14 +26609,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2377</v>
+        <v>2387</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>2373</v>
+        <v>2383</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2378</v>
+        <v>2388</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>22</v>
@@ -26526,14 +26631,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2379</v>
+        <v>2389</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2380</v>
+        <v>2390</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>22</v>
@@ -26548,14 +26653,14 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2381</v>
+        <v>2391</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2382</v>
+        <v>2392</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>22</v>
@@ -26570,14 +26675,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2383</v>
+        <v>2393</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2384</v>
+        <v>2394</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>22</v>
@@ -26592,14 +26697,14 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2385</v>
+        <v>2395</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>2386</v>
+        <v>2396</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>22</v>
@@ -26614,14 +26719,14 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2387</v>
+        <v>2397</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>2388</v>
+        <v>2398</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>22</v>
@@ -26636,14 +26741,14 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2389</v>
+        <v>2399</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2390</v>
+        <v>2400</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>22</v>
@@ -26658,14 +26763,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2391</v>
+        <v>2401</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2392</v>
+        <v>2402</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>22</v>
@@ -26680,14 +26785,14 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2393</v>
+        <v>2403</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>2394</v>
+        <v>2404</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>22</v>
@@ -26702,14 +26807,14 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2395</v>
+        <v>2405</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2396</v>
+        <v>2406</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>22</v>
@@ -26724,14 +26829,14 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2397</v>
+        <v>2407</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2398</v>
+        <v>2408</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>22</v>
@@ -26746,14 +26851,14 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2399</v>
+        <v>2409</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>2400</v>
+        <v>2410</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>22</v>
@@ -26768,14 +26873,14 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2401</v>
+        <v>2411</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
-        <v>2402</v>
+        <v>2412</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>22</v>
@@ -26790,14 +26895,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2403</v>
+        <v>2413</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2404</v>
+        <v>2414</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>22</v>
@@ -26812,14 +26917,14 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2405</v>
+        <v>2415</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>2406</v>
+        <v>2416</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>22</v>
@@ -26834,14 +26939,14 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>2407</v>
+        <v>2417</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>2408</v>
+        <v>2418</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>22</v>
@@ -26856,14 +26961,14 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>2409</v>
+        <v>2419</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>2410</v>
+        <v>2420</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>22</v>
@@ -26878,14 +26983,14 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>2411</v>
+        <v>2421</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C23"/>
       <c r="D23" t="s">
-        <v>2412</v>
+        <v>2422</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>22</v>
@@ -26917,13 +27022,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>2373</v>
+        <v>2383</v>
       </c>
       <c r="B26" t="s">
-        <v>2268</v>
+        <v>2278</v>
       </c>
       <c r="C26" t="s">
-        <v>2269</v>
+        <v>2279</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
@@ -26935,10 +27040,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>2266</v>
+        <v>2276</v>
       </c>
       <c r="C27" t="s">
-        <v>2267</v>
+        <v>2277</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
@@ -26950,10 +27055,10 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>2264</v>
+        <v>2274</v>
       </c>
       <c r="C28" t="s">
-        <v>2265</v>
+        <v>2275</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -27029,14 +27134,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2413</v>
+        <v>2423</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>2414</v>
+        <v>2424</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2415</v>
+        <v>2425</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>22</v>
@@ -27075,14 +27180,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2416</v>
+        <v>2426</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>2417</v>
+        <v>2427</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2418</v>
+        <v>2428</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>22</v>
@@ -27097,7 +27202,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2419</v>
+        <v>2429</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>1690</v>
@@ -27119,17 +27224,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2420</v>
+        <v>2430</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>2421</v>
+        <v>2431</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2422</v>
+        <v>2432</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>2423</v>
+        <v>2433</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -27143,14 +27248,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2424</v>
+        <v>2434</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>2425</v>
+        <v>2435</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2426</v>
+        <v>2436</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>22</v>
@@ -27165,14 +27270,14 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2427</v>
+        <v>2437</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2428</v>
+        <v>2438</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>22</v>
@@ -27189,14 +27294,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2429</v>
+        <v>2439</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2430</v>
+        <v>2440</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>22</v>
@@ -27211,14 +27316,14 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2431</v>
+        <v>2441</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>2432</v>
+        <v>2442</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>2433</v>
+        <v>2443</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>22</v>
@@ -27233,14 +27338,14 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2434</v>
+        <v>2444</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>2435</v>
+        <v>2445</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>22</v>
@@ -27255,14 +27360,14 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2436</v>
+        <v>2446</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2437</v>
+        <v>2447</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>22</v>
@@ -27277,14 +27382,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2438</v>
+        <v>2448</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>626</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2439</v>
+        <v>2449</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>22</v>
@@ -27299,14 +27404,14 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2440</v>
+        <v>2450</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>2441</v>
+        <v>2451</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>22</v>
@@ -27321,14 +27426,14 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2442</v>
+        <v>2452</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>626</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2443</v>
+        <v>2453</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>22</v>
@@ -27345,14 +27450,14 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2444</v>
+        <v>2454</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2445</v>
+        <v>2455</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>22</v>
@@ -27367,7 +27472,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2446</v>
+        <v>2456</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -27389,7 +27494,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2447</v>
+        <v>2457</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -27411,7 +27516,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2448</v>
+        <v>2458</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -27450,13 +27555,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>2414</v>
+        <v>2424</v>
       </c>
       <c r="B22" t="s">
-        <v>2449</v>
+        <v>2459</v>
       </c>
       <c r="C22" t="s">
-        <v>2450</v>
+        <v>2460</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -27468,10 +27573,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>2451</v>
+        <v>2461</v>
       </c>
       <c r="C23" t="s">
-        <v>2452</v>
+        <v>2462</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -27483,10 +27588,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>2453</v>
+        <v>2463</v>
       </c>
       <c r="C24" t="s">
-        <v>2454</v>
+        <v>2464</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -27498,10 +27603,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>2455</v>
+        <v>2465</v>
       </c>
       <c r="C25" t="s">
-        <v>2456</v>
+        <v>2466</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -27529,13 +27634,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>2421</v>
+        <v>2431</v>
       </c>
       <c r="B28" t="s">
-        <v>2457</v>
+        <v>2467</v>
       </c>
       <c r="C28" t="s">
-        <v>2458</v>
+        <v>2468</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -27547,10 +27652,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>2459</v>
+        <v>2469</v>
       </c>
       <c r="C29" t="s">
-        <v>2460</v>
+        <v>2470</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
@@ -27562,10 +27667,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>2461</v>
+        <v>2471</v>
       </c>
       <c r="C30" t="s">
-        <v>2462</v>
+        <v>2472</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -27577,10 +27682,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>2463</v>
+        <v>2473</v>
       </c>
       <c r="C31" t="s">
-        <v>2464</v>
+        <v>2474</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
@@ -27592,10 +27697,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>2465</v>
+        <v>2475</v>
       </c>
       <c r="C32" t="s">
-        <v>2466</v>
+        <v>2476</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
@@ -27610,7 +27715,7 @@
         <v>917</v>
       </c>
       <c r="C33" t="s">
-        <v>2467</v>
+        <v>2477</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -27622,10 +27727,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>2468</v>
+        <v>2478</v>
       </c>
       <c r="C34" t="s">
-        <v>2469</v>
+        <v>2479</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
@@ -27637,10 +27742,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>2470</v>
+        <v>2480</v>
       </c>
       <c r="C35" t="s">
-        <v>2471</v>
+        <v>2481</v>
       </c>
       <c r="D35" t="s">
         <v>22</v>
@@ -27652,10 +27757,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>2472</v>
+        <v>2482</v>
       </c>
       <c r="C36" t="s">
-        <v>2473</v>
+        <v>2483</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
@@ -27667,10 +27772,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>2474</v>
+        <v>2484</v>
       </c>
       <c r="C37" t="s">
-        <v>2475</v>
+        <v>2485</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -27682,10 +27787,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>2476</v>
+        <v>2486</v>
       </c>
       <c r="C38" t="s">
-        <v>2477</v>
+        <v>2487</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
@@ -27697,10 +27802,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>2478</v>
+        <v>2488</v>
       </c>
       <c r="C39" t="s">
-        <v>2479</v>
+        <v>2489</v>
       </c>
       <c r="D39" t="s">
         <v>22</v>
@@ -27712,10 +27817,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>2480</v>
+        <v>2490</v>
       </c>
       <c r="C40" t="s">
-        <v>2481</v>
+        <v>2491</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
@@ -27727,10 +27832,10 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>2482</v>
+        <v>2492</v>
       </c>
       <c r="C41" t="s">
-        <v>2483</v>
+        <v>2493</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -27742,10 +27847,10 @@
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>2484</v>
+        <v>2494</v>
       </c>
       <c r="C42" t="s">
-        <v>2485</v>
+        <v>2495</v>
       </c>
       <c r="D42" t="s">
         <v>22</v>
@@ -27757,10 +27862,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>2486</v>
+        <v>2496</v>
       </c>
       <c r="C43" t="s">
-        <v>2487</v>
+        <v>2497</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -27772,10 +27877,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>2488</v>
+        <v>2498</v>
       </c>
       <c r="C44" t="s">
-        <v>2489</v>
+        <v>2499</v>
       </c>
       <c r="D44" t="s">
         <v>22</v>
@@ -27787,10 +27892,10 @@
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>2490</v>
+        <v>2500</v>
       </c>
       <c r="C45" t="s">
-        <v>2491</v>
+        <v>2501</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -27802,10 +27907,10 @@
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>2492</v>
+        <v>2502</v>
       </c>
       <c r="C46" t="s">
-        <v>2493</v>
+        <v>2503</v>
       </c>
       <c r="D46" t="s">
         <v>22</v>
@@ -27820,7 +27925,7 @@
         <v>179</v>
       </c>
       <c r="C47" t="s">
-        <v>2494</v>
+        <v>2504</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -27832,10 +27937,10 @@
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>2495</v>
+        <v>2505</v>
       </c>
       <c r="C48" t="s">
-        <v>2496</v>
+        <v>2506</v>
       </c>
       <c r="D48" t="s">
         <v>22</v>
@@ -27847,10 +27952,10 @@
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>2497</v>
+        <v>2507</v>
       </c>
       <c r="C49" t="s">
-        <v>2498</v>
+        <v>2508</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -27862,10 +27967,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>2499</v>
+        <v>2509</v>
       </c>
       <c r="C50" t="s">
-        <v>2500</v>
+        <v>2510</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
@@ -27893,13 +27998,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>2425</v>
+        <v>2435</v>
       </c>
       <c r="B53" t="s">
-        <v>2501</v>
+        <v>2511</v>
       </c>
       <c r="C53" t="s">
-        <v>2502</v>
+        <v>2512</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -27911,10 +28016,10 @@
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>2503</v>
+        <v>2513</v>
       </c>
       <c r="C54" t="s">
-        <v>2504</v>
+        <v>2514</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -27926,10 +28031,10 @@
     <row r="55">
       <c r="A55"/>
       <c r="B55" t="s">
-        <v>2505</v>
+        <v>2515</v>
       </c>
       <c r="C55" t="s">
-        <v>2506</v>
+        <v>2516</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -27957,13 +28062,13 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>2432</v>
+        <v>2442</v>
       </c>
       <c r="B58" t="s">
         <v>936</v>
       </c>
       <c r="C58" t="s">
-        <v>2507</v>
+        <v>2517</v>
       </c>
       <c r="D58" t="s">
         <v>22</v>
@@ -27978,7 +28083,7 @@
         <v>939</v>
       </c>
       <c r="C59" t="s">
-        <v>2508</v>
+        <v>2518</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
@@ -27990,10 +28095,10 @@
     <row r="60">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>2509</v>
+        <v>2519</v>
       </c>
       <c r="C60" t="s">
-        <v>2510</v>
+        <v>2520</v>
       </c>
       <c r="D60" t="s">
         <v>22</v>
@@ -28005,10 +28110,10 @@
     <row r="61">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>2511</v>
+        <v>2521</v>
       </c>
       <c r="C61" t="s">
-        <v>2512</v>
+        <v>2522</v>
       </c>
       <c r="D61" t="s">
         <v>22</v>
@@ -28087,10 +28192,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2513</v>
+        <v>2523</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>2417</v>
+        <v>2427</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
@@ -28109,17 +28214,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2514</v>
+        <v>2524</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>2515</v>
+        <v>2525</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2516</v>
+        <v>2526</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>2517</v>
+        <v>2527</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -28133,14 +28238,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2518</v>
+        <v>2528</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>2519</v>
+        <v>2529</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2520</v>
+        <v>2530</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>22</v>
@@ -28155,10 +28260,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2521</v>
+        <v>2531</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>2522</v>
+        <v>2532</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
@@ -28177,14 +28282,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2523</v>
+        <v>2533</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2524</v>
+        <v>2534</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>22</v>
@@ -28199,14 +28304,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2525</v>
+        <v>2535</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2526</v>
+        <v>2536</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>22</v>
@@ -28221,14 +28326,14 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2527</v>
+        <v>2537</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>2528</v>
+        <v>2538</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2529</v>
+        <v>2539</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>22</v>
@@ -28287,14 +28392,14 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2530</v>
+        <v>2540</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>2531</v>
+        <v>2541</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>22</v>
@@ -28309,7 +28414,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2532</v>
+        <v>2542</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>12</v>
@@ -28319,7 +28424,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>2533</v>
+        <v>2543</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -28333,14 +28438,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2534</v>
+        <v>2544</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>651</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2535</v>
+        <v>2545</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>22</v>
@@ -28362,10 +28467,10 @@
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>2536</v>
+        <v>2546</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>2537</v>
+        <v>2547</v>
       </c>
       <c r="F14"/>
       <c r="H14" s="19" t="s">
@@ -28384,10 +28489,10 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2538</v>
+        <v>2548</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>2539</v>
+        <v>2549</v>
       </c>
       <c r="F15"/>
       <c r="H15" s="19" t="s">
@@ -28447,14 +28552,14 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2540</v>
+        <v>2550</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
-        <v>2541</v>
+        <v>2551</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>22</v>
@@ -28469,14 +28574,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2542</v>
+        <v>2552</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2543</v>
+        <v>2553</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>22</v>
@@ -28491,7 +28596,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2544</v>
+        <v>2554</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>115</v>
@@ -28523,7 +28628,7 @@
         <v>1625</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>2545</v>
+        <v>2555</v>
       </c>
       <c r="F21"/>
       <c r="H21" s="19" t="s">
@@ -28603,14 +28708,14 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>2546</v>
+        <v>2556</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>2547</v>
+        <v>2557</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>22</v>
@@ -28647,14 +28752,14 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>2548</v>
+        <v>2558</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>2549</v>
+        <v>2559</v>
       </c>
       <c r="C27"/>
       <c r="D27" t="s">
-        <v>2550</v>
+        <v>2560</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>22</v>
@@ -28669,14 +28774,14 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>2551</v>
+        <v>2561</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>2552</v>
+        <v>2562</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>2553</v>
+        <v>2563</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>22</v>
@@ -28691,14 +28796,14 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>2554</v>
+        <v>2564</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C29"/>
       <c r="D29" t="s">
-        <v>2555</v>
+        <v>2565</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>22</v>
@@ -28713,17 +28818,17 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>2556</v>
+        <v>2566</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C30"/>
       <c r="D30" t="s">
-        <v>2557</v>
+        <v>2567</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>2558</v>
+        <v>2568</v>
       </c>
       <c r="F30"/>
       <c r="H30" s="19" t="s">
@@ -28735,17 +28840,17 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>2559</v>
+        <v>2569</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C31"/>
       <c r="D31" t="s">
-        <v>2560</v>
+        <v>2570</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>2561</v>
+        <v>2571</v>
       </c>
       <c r="F31"/>
       <c r="H31" s="19" t="s">
@@ -28757,17 +28862,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>2562</v>
+        <v>2572</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C32"/>
       <c r="D32" t="s">
-        <v>2563</v>
+        <v>2573</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>2564</v>
+        <v>2574</v>
       </c>
       <c r="F32"/>
       <c r="H32" s="19" t="s">
@@ -28779,17 +28884,17 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>2565</v>
+        <v>2575</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C33"/>
       <c r="D33" t="s">
-        <v>2566</v>
+        <v>2576</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>2567</v>
+        <v>2577</v>
       </c>
       <c r="F33"/>
       <c r="H33" s="19" t="s">
@@ -28801,17 +28906,17 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>2568</v>
+        <v>2578</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C34"/>
       <c r="D34" t="s">
-        <v>2569</v>
+        <v>2579</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>2570</v>
+        <v>2580</v>
       </c>
       <c r="F34"/>
       <c r="H34" s="19" t="s">
@@ -28823,17 +28928,17 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>2571</v>
+        <v>2581</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C35"/>
       <c r="D35" t="s">
-        <v>2572</v>
+        <v>2582</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>2573</v>
+        <v>2583</v>
       </c>
       <c r="F35"/>
       <c r="H35" s="19" t="s">
@@ -28845,17 +28950,17 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>2574</v>
+        <v>2584</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C36"/>
       <c r="D36" t="s">
-        <v>2575</v>
+        <v>2585</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>2576</v>
+        <v>2586</v>
       </c>
       <c r="F36"/>
       <c r="H36" s="19" t="s">
@@ -28911,7 +29016,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>2577</v>
+        <v>2587</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>626</v>
@@ -28920,7 +29025,7 @@
         <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>2578</v>
+        <v>2588</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>22</v>
@@ -28935,14 +29040,14 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>2579</v>
+        <v>2589</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C40"/>
       <c r="D40" t="s">
-        <v>2580</v>
+        <v>2590</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>22</v>
@@ -29023,14 +29128,14 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>2581</v>
+        <v>2591</v>
       </c>
       <c r="B44" s="19" t="s">
         <v>651</v>
       </c>
       <c r="C44"/>
       <c r="D44" t="s">
-        <v>2582</v>
+        <v>2592</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>22</v>
@@ -29045,14 +29150,14 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>2583</v>
+        <v>2593</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>2584</v>
+        <v>2594</v>
       </c>
       <c r="C45"/>
       <c r="D45" t="s">
-        <v>2585</v>
+        <v>2595</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>22</v>
@@ -29067,17 +29172,17 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>2586</v>
+        <v>2596</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>2587</v>
+        <v>2597</v>
       </c>
       <c r="C46"/>
       <c r="D46" t="s">
-        <v>2588</v>
+        <v>2598</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>2589</v>
+        <v>2599</v>
       </c>
       <c r="F46"/>
       <c r="H46" s="19" t="s">
@@ -29091,14 +29196,14 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>2590</v>
+        <v>2600</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>2591</v>
+        <v>2601</v>
       </c>
       <c r="C47"/>
       <c r="D47" t="s">
-        <v>2592</v>
+        <v>2602</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>22</v>
@@ -29115,14 +29220,14 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>2593</v>
+        <v>2603</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>2594</v>
+        <v>2604</v>
       </c>
       <c r="C48"/>
       <c r="D48" t="s">
-        <v>2595</v>
+        <v>2605</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>22</v>
@@ -29139,14 +29244,14 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>2596</v>
+        <v>2606</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>2597</v>
+        <v>2607</v>
       </c>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>2598</v>
+        <v>2608</v>
       </c>
       <c r="E49" s="19" t="s">
         <v>22</v>
@@ -29207,14 +29312,14 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>2599</v>
+        <v>2609</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>2600</v>
+        <v>2610</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>22</v>
@@ -29248,13 +29353,13 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>2515</v>
+        <v>2525</v>
       </c>
       <c r="B55" t="s">
-        <v>2601</v>
+        <v>2611</v>
       </c>
       <c r="C55" t="s">
-        <v>2602</v>
+        <v>2612</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -29266,10 +29371,10 @@
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
-        <v>2453</v>
+        <v>2463</v>
       </c>
       <c r="C56" t="s">
-        <v>2454</v>
+        <v>2464</v>
       </c>
       <c r="D56" t="s">
         <v>22</v>
@@ -29296,10 +29401,10 @@
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>2603</v>
+        <v>2613</v>
       </c>
       <c r="C58" t="s">
-        <v>2604</v>
+        <v>2614</v>
       </c>
       <c r="D58" t="s">
         <v>22</v>
@@ -29342,13 +29447,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>2519</v>
+        <v>2529</v>
       </c>
       <c r="B62" t="s">
-        <v>2505</v>
+        <v>2515</v>
       </c>
       <c r="C62" t="s">
-        <v>2605</v>
+        <v>2615</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -29360,10 +29465,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>2606</v>
+        <v>2616</v>
       </c>
       <c r="C63" t="s">
-        <v>2607</v>
+        <v>2617</v>
       </c>
       <c r="D63" t="s">
         <v>22</v>
@@ -29375,10 +29480,10 @@
     <row r="64">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>2501</v>
+        <v>2511</v>
       </c>
       <c r="C64" t="s">
-        <v>2608</v>
+        <v>2618</v>
       </c>
       <c r="D64" t="s">
         <v>22</v>
@@ -29421,7 +29526,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>2522</v>
+        <v>2532</v>
       </c>
       <c r="B68" t="s">
         <v>936</v>
@@ -29439,10 +29544,10 @@
     <row r="69">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>2609</v>
+        <v>2619</v>
       </c>
       <c r="C69" t="s">
-        <v>2610</v>
+        <v>2620</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -29500,7 +29605,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>2528</v>
+        <v>2538</v>
       </c>
       <c r="B74" t="s">
         <v>936</v>
@@ -29518,7 +29623,7 @@
     <row r="75">
       <c r="A75"/>
       <c r="B75" t="s">
-        <v>2609</v>
+        <v>2619</v>
       </c>
       <c r="C75" t="s">
         <v>1046</v>
@@ -29548,10 +29653,10 @@
     <row r="77">
       <c r="A77"/>
       <c r="B77" t="s">
-        <v>2611</v>
+        <v>2621</v>
       </c>
       <c r="C77" t="s">
-        <v>2612</v>
+        <v>2622</v>
       </c>
       <c r="D77" t="s">
         <v>22</v>
@@ -30000,13 +30105,13 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>2549</v>
+        <v>2559</v>
       </c>
       <c r="B111" t="s">
-        <v>2613</v>
+        <v>2623</v>
       </c>
       <c r="C111" t="s">
-        <v>2614</v>
+        <v>2624</v>
       </c>
       <c r="D111" t="s">
         <v>22</v>
@@ -30018,10 +30123,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>2615</v>
+        <v>2625</v>
       </c>
       <c r="C112" t="s">
-        <v>2616</v>
+        <v>2626</v>
       </c>
       <c r="D112" t="s">
         <v>22</v>
@@ -30033,10 +30138,10 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>2617</v>
+        <v>2627</v>
       </c>
       <c r="C113" t="s">
-        <v>2618</v>
+        <v>2628</v>
       </c>
       <c r="D113" t="s">
         <v>22</v>
@@ -30048,10 +30153,10 @@
     <row r="114">
       <c r="A114"/>
       <c r="B114" t="s">
-        <v>2619</v>
+        <v>2629</v>
       </c>
       <c r="C114" t="s">
-        <v>2620</v>
+        <v>2630</v>
       </c>
       <c r="D114" t="s">
         <v>22</v>
@@ -30063,10 +30168,10 @@
     <row r="115">
       <c r="A115"/>
       <c r="B115" t="s">
-        <v>2621</v>
+        <v>2631</v>
       </c>
       <c r="C115" t="s">
-        <v>2622</v>
+        <v>2632</v>
       </c>
       <c r="D115" t="s">
         <v>22</v>
@@ -30094,13 +30199,13 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>2552</v>
+        <v>2562</v>
       </c>
       <c r="B118" t="s">
-        <v>2623</v>
+        <v>2633</v>
       </c>
       <c r="C118" t="s">
-        <v>2624</v>
+        <v>2634</v>
       </c>
       <c r="D118" t="s">
         <v>22</v>
@@ -30112,10 +30217,10 @@
     <row r="119">
       <c r="A119"/>
       <c r="B119" t="s">
-        <v>2625</v>
+        <v>2635</v>
       </c>
       <c r="C119" t="s">
-        <v>2626</v>
+        <v>2636</v>
       </c>
       <c r="D119" t="s">
         <v>22</v>
@@ -30127,10 +30232,10 @@
     <row r="120">
       <c r="A120"/>
       <c r="B120" t="s">
-        <v>2627</v>
+        <v>2637</v>
       </c>
       <c r="C120" t="s">
-        <v>2628</v>
+        <v>2638</v>
       </c>
       <c r="D120" t="s">
         <v>22</v>
@@ -30142,10 +30247,10 @@
     <row r="121">
       <c r="A121"/>
       <c r="B121" t="s">
-        <v>2629</v>
+        <v>2639</v>
       </c>
       <c r="C121" t="s">
-        <v>2630</v>
+        <v>2640</v>
       </c>
       <c r="D121" t="s">
         <v>22</v>
@@ -30157,10 +30262,10 @@
     <row r="122">
       <c r="A122"/>
       <c r="B122" t="s">
-        <v>2631</v>
+        <v>2641</v>
       </c>
       <c r="C122" t="s">
-        <v>2632</v>
+        <v>2642</v>
       </c>
       <c r="D122" t="s">
         <v>22</v>
@@ -31062,13 +31167,13 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>2584</v>
+        <v>2594</v>
       </c>
       <c r="B184" t="s">
-        <v>2633</v>
+        <v>2643</v>
       </c>
       <c r="C184" t="s">
-        <v>2634</v>
+        <v>2644</v>
       </c>
       <c r="D184" t="s">
         <v>22</v>
@@ -31080,10 +31185,10 @@
     <row r="185">
       <c r="A185"/>
       <c r="B185" t="s">
-        <v>2260</v>
+        <v>2270</v>
       </c>
       <c r="C185" t="s">
-        <v>2635</v>
+        <v>2645</v>
       </c>
       <c r="D185" t="s">
         <v>22</v>
@@ -31095,10 +31200,10 @@
     <row r="186">
       <c r="A186"/>
       <c r="B186" t="s">
-        <v>2262</v>
+        <v>2272</v>
       </c>
       <c r="C186" t="s">
-        <v>2636</v>
+        <v>2646</v>
       </c>
       <c r="D186" t="s">
         <v>22</v>
@@ -31110,10 +31215,10 @@
     <row r="187">
       <c r="A187"/>
       <c r="B187" t="s">
-        <v>2637</v>
+        <v>2647</v>
       </c>
       <c r="C187" t="s">
-        <v>2638</v>
+        <v>2648</v>
       </c>
       <c r="D187" t="s">
         <v>22</v>
@@ -31125,10 +31230,10 @@
     <row r="188">
       <c r="A188"/>
       <c r="B188" t="s">
-        <v>2639</v>
+        <v>2649</v>
       </c>
       <c r="C188" t="s">
-        <v>2640</v>
+        <v>2650</v>
       </c>
       <c r="D188" t="s">
         <v>22</v>
@@ -31171,7 +31276,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>2587</v>
+        <v>2597</v>
       </c>
       <c r="B192" t="s">
         <v>893</v>
@@ -31250,13 +31355,13 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>2591</v>
+        <v>2601</v>
       </c>
       <c r="B198" t="s">
-        <v>2641</v>
+        <v>2651</v>
       </c>
       <c r="C198" t="s">
-        <v>2642</v>
+        <v>2652</v>
       </c>
       <c r="D198" t="s">
         <v>22</v>
@@ -31268,10 +31373,10 @@
     <row r="199">
       <c r="A199"/>
       <c r="B199" t="s">
-        <v>2643</v>
+        <v>2653</v>
       </c>
       <c r="C199" t="s">
-        <v>2644</v>
+        <v>2654</v>
       </c>
       <c r="D199" t="s">
         <v>22</v>
@@ -31283,10 +31388,10 @@
     <row r="200">
       <c r="A200"/>
       <c r="B200" t="s">
-        <v>2645</v>
+        <v>2655</v>
       </c>
       <c r="C200" t="s">
-        <v>2646</v>
+        <v>2656</v>
       </c>
       <c r="D200" t="s">
         <v>22</v>
@@ -31298,10 +31403,10 @@
     <row r="201">
       <c r="A201"/>
       <c r="B201" t="s">
-        <v>2647</v>
+        <v>2657</v>
       </c>
       <c r="C201" t="s">
-        <v>2648</v>
+        <v>2658</v>
       </c>
       <c r="D201" t="s">
         <v>22</v>
@@ -31313,10 +31418,10 @@
     <row r="202">
       <c r="A202"/>
       <c r="B202" t="s">
-        <v>2649</v>
+        <v>2659</v>
       </c>
       <c r="C202" t="s">
-        <v>2650</v>
+        <v>2660</v>
       </c>
       <c r="D202" t="s">
         <v>22</v>
@@ -31328,10 +31433,10 @@
     <row r="203">
       <c r="A203"/>
       <c r="B203" t="s">
-        <v>2651</v>
+        <v>2661</v>
       </c>
       <c r="C203" t="s">
-        <v>2652</v>
+        <v>2662</v>
       </c>
       <c r="D203" t="s">
         <v>22</v>
@@ -31374,13 +31479,13 @@
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>2594</v>
+        <v>2604</v>
       </c>
       <c r="B207" t="s">
-        <v>2653</v>
+        <v>2663</v>
       </c>
       <c r="C207" t="s">
-        <v>2654</v>
+        <v>2664</v>
       </c>
       <c r="D207" t="s">
         <v>22</v>
@@ -31392,10 +31497,10 @@
     <row r="208">
       <c r="A208"/>
       <c r="B208" t="s">
-        <v>2655</v>
+        <v>2665</v>
       </c>
       <c r="C208" t="s">
-        <v>2656</v>
+        <v>2666</v>
       </c>
       <c r="D208" t="s">
         <v>22</v>
@@ -31407,10 +31512,10 @@
     <row r="209">
       <c r="A209"/>
       <c r="B209" t="s">
-        <v>2657</v>
+        <v>2667</v>
       </c>
       <c r="C209" t="s">
-        <v>2658</v>
+        <v>2668</v>
       </c>
       <c r="D209" t="s">
         <v>22</v>
@@ -31422,10 +31527,10 @@
     <row r="210">
       <c r="A210"/>
       <c r="B210" t="s">
-        <v>2659</v>
+        <v>2669</v>
       </c>
       <c r="C210" t="s">
-        <v>2660</v>
+        <v>2670</v>
       </c>
       <c r="D210" t="s">
         <v>22</v>
@@ -31437,10 +31542,10 @@
     <row r="211">
       <c r="A211"/>
       <c r="B211" t="s">
-        <v>2661</v>
+        <v>2671</v>
       </c>
       <c r="C211" t="s">
-        <v>2662</v>
+        <v>2672</v>
       </c>
       <c r="D211" t="s">
         <v>22</v>
@@ -31483,13 +31588,13 @@
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>2597</v>
+        <v>2607</v>
       </c>
       <c r="B215" t="s">
-        <v>2663</v>
+        <v>2673</v>
       </c>
       <c r="C215" t="s">
-        <v>2664</v>
+        <v>2674</v>
       </c>
       <c r="D215" t="s">
         <v>22</v>
@@ -31501,10 +31606,10 @@
     <row r="216">
       <c r="A216"/>
       <c r="B216" t="s">
-        <v>2665</v>
+        <v>2675</v>
       </c>
       <c r="C216" t="s">
-        <v>2666</v>
+        <v>2676</v>
       </c>
       <c r="D216" t="s">
         <v>22</v>
@@ -31516,10 +31621,10 @@
     <row r="217">
       <c r="A217"/>
       <c r="B217" t="s">
-        <v>2667</v>
+        <v>2677</v>
       </c>
       <c r="C217" t="s">
-        <v>2668</v>
+        <v>2678</v>
       </c>
       <c r="D217" t="s">
         <v>22</v>
@@ -31531,10 +31636,10 @@
     <row r="218">
       <c r="A218"/>
       <c r="B218" t="s">
-        <v>2669</v>
+        <v>2679</v>
       </c>
       <c r="C218" t="s">
-        <v>2670</v>
+        <v>2680</v>
       </c>
       <c r="D218" t="s">
         <v>22</v>
@@ -31546,10 +31651,10 @@
     <row r="219">
       <c r="A219"/>
       <c r="B219" t="s">
-        <v>2671</v>
+        <v>2681</v>
       </c>
       <c r="C219" t="s">
-        <v>2672</v>
+        <v>2682</v>
       </c>
       <c r="D219" t="s">
         <v>22</v>
@@ -33333,14 +33438,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2416</v>
+        <v>2426</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>2417</v>
+        <v>2427</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2454</v>
+        <v>2464</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>22</v>
@@ -33360,11 +33465,11 @@
         <v>617</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>2673</v>
+        <v>2683</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2673</v>
+        <v>2683</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>22</v>
@@ -33381,7 +33486,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2674</v>
+        <v>2684</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>12</v>
@@ -33390,7 +33495,7 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>2675</v>
+        <v>2685</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>22</v>
@@ -33515,7 +33620,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2676</v>
+        <v>2686</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>140</v>
@@ -33601,14 +33706,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2677</v>
+        <v>2687</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>2678</v>
+        <v>2688</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2679</v>
+        <v>2689</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>22</v>
@@ -33625,14 +33730,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2416</v>
+        <v>2426</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>2417</v>
+        <v>2427</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2418</v>
+        <v>2428</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>22</v>
@@ -33647,14 +33752,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2680</v>
+        <v>2690</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>2681</v>
+        <v>2691</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2682</v>
+        <v>2692</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>22</v>
@@ -33669,14 +33774,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2424</v>
+        <v>2434</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>2683</v>
+        <v>2693</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2426</v>
+        <v>2436</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>22</v>
@@ -33691,7 +33796,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2684</v>
+        <v>2694</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>55</v>
@@ -33715,14 +33820,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2685</v>
+        <v>2695</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>2686</v>
+        <v>2696</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2687</v>
+        <v>2697</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>22</v>
@@ -33737,7 +33842,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2434</v>
+        <v>2444</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>55</v>
@@ -33759,14 +33864,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2438</v>
+        <v>2448</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>626</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2439</v>
+        <v>2449</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>22</v>
@@ -33781,14 +33886,14 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2688</v>
+        <v>2698</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>2531</v>
+        <v>2541</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>22</v>
@@ -33825,14 +33930,14 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2689</v>
+        <v>2699</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2445</v>
+        <v>2455</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>22</v>
@@ -33847,14 +33952,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2690</v>
+        <v>2700</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>626</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2691</v>
+        <v>2701</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>22</v>
@@ -33886,13 +33991,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2678</v>
+        <v>2688</v>
       </c>
       <c r="B16" t="s">
-        <v>2453</v>
+        <v>2463</v>
       </c>
       <c r="C16" t="s">
-        <v>2454</v>
+        <v>2464</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -33920,13 +34025,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2681</v>
+        <v>2691</v>
       </c>
       <c r="B19" t="s">
-        <v>2692</v>
+        <v>2702</v>
       </c>
       <c r="C19" t="s">
-        <v>2693</v>
+        <v>2703</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -33938,10 +34043,10 @@
     <row r="20">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>2468</v>
+        <v>2478</v>
       </c>
       <c r="C20" t="s">
-        <v>2694</v>
+        <v>2704</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -33953,10 +34058,10 @@
     <row r="21">
       <c r="A21"/>
       <c r="B21" t="s">
-        <v>2695</v>
+        <v>2705</v>
       </c>
       <c r="C21" t="s">
-        <v>2696</v>
+        <v>2706</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -33968,10 +34073,10 @@
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>2472</v>
+        <v>2482</v>
       </c>
       <c r="C22" t="s">
-        <v>2697</v>
+        <v>2707</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -33983,10 +34088,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>2698</v>
+        <v>2708</v>
       </c>
       <c r="C23" t="s">
-        <v>2699</v>
+        <v>2709</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -33998,10 +34103,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>2700</v>
+        <v>2710</v>
       </c>
       <c r="C24" t="s">
-        <v>2701</v>
+        <v>2711</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -34013,10 +34118,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>2702</v>
+        <v>2712</v>
       </c>
       <c r="C25" t="s">
-        <v>2703</v>
+        <v>2713</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -34028,10 +34133,10 @@
     <row r="26">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>2704</v>
+        <v>2714</v>
       </c>
       <c r="C26" t="s">
-        <v>2705</v>
+        <v>2715</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
@@ -34043,10 +34148,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>2706</v>
+        <v>2716</v>
       </c>
       <c r="C27" t="s">
-        <v>2707</v>
+        <v>2717</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
@@ -34089,13 +34194,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>2683</v>
+        <v>2693</v>
       </c>
       <c r="B31" t="s">
-        <v>2501</v>
+        <v>2511</v>
       </c>
       <c r="C31" t="s">
-        <v>2502</v>
+        <v>2512</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
@@ -34107,10 +34212,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>2503</v>
+        <v>2513</v>
       </c>
       <c r="C32" t="s">
-        <v>2504</v>
+        <v>2514</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
@@ -34122,10 +34227,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>2505</v>
+        <v>2515</v>
       </c>
       <c r="C33" t="s">
-        <v>2506</v>
+        <v>2516</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -34153,7 +34258,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>2686</v>
+        <v>2696</v>
       </c>
       <c r="B36" t="s">
         <v>936</v>
@@ -34171,10 +34276,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>2708</v>
+        <v>2718</v>
       </c>
       <c r="C37" t="s">
-        <v>2709</v>
+        <v>2719</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -34268,14 +34373,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2710</v>
+        <v>2720</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2711</v>
+        <v>2721</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>22</v>
@@ -34495,7 +34600,7 @@
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2712</v>
+        <v>2722</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>22</v>
@@ -34517,7 +34622,7 @@
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2713</v>
+        <v>2723</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>22</v>
@@ -34532,7 +34637,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2714</v>
+        <v>2724</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>69</v>
@@ -34554,14 +34659,14 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2715</v>
+        <v>2725</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2716</v>
+        <v>2726</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>22</v>
@@ -34576,14 +34681,14 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2717</v>
+        <v>2727</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2718</v>
+        <v>2728</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>22</v>
@@ -35669,14 +35774,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2719</v>
+        <v>2729</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2720</v>
+        <v>2730</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>22</v>
@@ -35713,14 +35818,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2721</v>
+        <v>2731</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2722</v>
+        <v>2732</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>22</v>
@@ -35735,14 +35840,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2723</v>
+        <v>2733</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2724</v>
+        <v>2734</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>22</v>
@@ -35757,14 +35862,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2717</v>
+        <v>2727</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>140</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2718</v>
+        <v>2728</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>22</v>
@@ -35843,14 +35948,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2710</v>
+        <v>2720</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2711</v>
+        <v>2721</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>22</v>
@@ -35865,14 +35970,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2725</v>
+        <v>2735</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2726</v>
+        <v>2736</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>22</v>
@@ -35887,14 +35992,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2727</v>
+        <v>2737</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>42</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2728</v>
+        <v>2738</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>22</v>
@@ -35909,14 +36014,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2717</v>
+        <v>2727</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>140</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2718</v>
+        <v>2728</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>22</v>
@@ -35953,10 +36058,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2729</v>
+        <v>2739</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>2730</v>
+        <v>2740</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
@@ -36039,14 +36144,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2710</v>
+        <v>2720</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2711</v>
+        <v>2721</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>22</v>
@@ -36061,14 +36166,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2725</v>
+        <v>2735</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2726</v>
+        <v>2736</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>22</v>
@@ -36083,14 +36188,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2727</v>
+        <v>2737</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>42</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2728</v>
+        <v>2738</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>22</v>
@@ -36127,14 +36232,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2717</v>
+        <v>2727</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>140</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2718</v>
+        <v>2728</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>22</v>
@@ -36235,14 +36340,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2710</v>
+        <v>2720</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2711</v>
+        <v>2721</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>22</v>
@@ -36301,14 +36406,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2717</v>
+        <v>2727</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>140</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2718</v>
+        <v>2728</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>22</v>
@@ -36409,14 +36514,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2731</v>
+        <v>2741</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>140</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2732</v>
+        <v>2742</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>22</v>
@@ -36431,14 +36536,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2733</v>
+        <v>2743</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2734</v>
+        <v>2744</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>22</v>
@@ -36497,14 +36602,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2735</v>
+        <v>2745</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2566</v>
+        <v>2576</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>22</v>
@@ -36548,7 +36653,7 @@
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2736</v>
+        <v>2746</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>22</v>
@@ -36563,12 +36668,12 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2737</v>
+        <v>2747</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2738</v>
+        <v>2748</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>22</v>
@@ -36671,7 +36776,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2739</v>
+        <v>2749</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>72</v>
@@ -36700,7 +36805,7 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2740</v>
+        <v>2750</v>
       </c>
       <c r="E15" s="27" t="s">
         <v>22</v>
@@ -36715,14 +36820,14 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2741</v>
+        <v>2751</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>626</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2742</v>
+        <v>2752</v>
       </c>
       <c r="E16" s="27" t="s">
         <v>22</v>
@@ -36737,17 +36842,17 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2743</v>
+        <v>2753</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>91</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>2744</v>
+        <v>2754</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>2745</v>
+        <v>2755</v>
       </c>
       <c r="F17"/>
       <c r="H17" s="27" t="s">
@@ -36759,10 +36864,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2746</v>
+        <v>2756</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>2747</v>
+        <v>2757</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
@@ -36781,14 +36886,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2748</v>
+        <v>2758</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>140</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2749</v>
+        <v>2759</v>
       </c>
       <c r="E19" s="27" t="s">
         <v>22</v>
@@ -37731,13 +37836,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>2747</v>
+        <v>2757</v>
       </c>
       <c r="B85" t="s">
-        <v>2750</v>
+        <v>2760</v>
       </c>
       <c r="C85" t="s">
-        <v>2751</v>
+        <v>2761</v>
       </c>
       <c r="D85" t="s">
         <v>22</v>
@@ -37749,10 +37854,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>2752</v>
+        <v>2762</v>
       </c>
       <c r="C86" t="s">
-        <v>2753</v>
+        <v>2763</v>
       </c>
       <c r="D86" t="s">
         <v>22</v>
@@ -37764,10 +37869,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>2754</v>
+        <v>2764</v>
       </c>
       <c r="C87" t="s">
-        <v>2755</v>
+        <v>2765</v>
       </c>
       <c r="D87" t="s">
         <v>22</v>
@@ -37779,10 +37884,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>2756</v>
+        <v>2766</v>
       </c>
       <c r="C88" t="s">
-        <v>2757</v>
+        <v>2767</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -37794,10 +37899,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>2758</v>
+        <v>2768</v>
       </c>
       <c r="C89" t="s">
-        <v>2759</v>
+        <v>2769</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -37809,10 +37914,10 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>2760</v>
+        <v>2770</v>
       </c>
       <c r="C90" t="s">
-        <v>2761</v>
+        <v>2771</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -37824,10 +37929,10 @@
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>2762</v>
+        <v>2772</v>
       </c>
       <c r="C91" t="s">
-        <v>2763</v>
+        <v>2773</v>
       </c>
       <c r="D91" t="s">
         <v>22</v>
@@ -37839,10 +37944,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>2764</v>
+        <v>2774</v>
       </c>
       <c r="C92" t="s">
-        <v>2765</v>
+        <v>2775</v>
       </c>
       <c r="D92" t="s">
         <v>22</v>
@@ -37854,10 +37959,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>2766</v>
+        <v>2776</v>
       </c>
       <c r="C93" t="s">
-        <v>2767</v>
+        <v>2777</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -37869,10 +37974,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>2768</v>
+        <v>2778</v>
       </c>
       <c r="C94" t="s">
-        <v>2769</v>
+        <v>2779</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -37884,10 +37989,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>2770</v>
+        <v>2780</v>
       </c>
       <c r="C95" t="s">
-        <v>2771</v>
+        <v>2781</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -37899,10 +38004,10 @@
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
-        <v>2772</v>
+        <v>2782</v>
       </c>
       <c r="C96" t="s">
-        <v>2773</v>
+        <v>2783</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -37914,10 +38019,10 @@
     <row r="97">
       <c r="A97"/>
       <c r="B97" t="s">
-        <v>2774</v>
+        <v>2784</v>
       </c>
       <c r="C97" t="s">
-        <v>2775</v>
+        <v>2785</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
@@ -37929,10 +38034,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>2776</v>
+        <v>2786</v>
       </c>
       <c r="C98" t="s">
-        <v>2777</v>
+        <v>2787</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -37944,10 +38049,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>2778</v>
+        <v>2788</v>
       </c>
       <c r="C99" t="s">
-        <v>2779</v>
+        <v>2789</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -37977,12 +38082,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2780</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2781</v>
+        <v>2791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5644 / #4694 - move jurisdiction check to database for cases
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12051" uniqueCount="2866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12067" uniqueCount="2874">
   <si>
     <t>Field</t>
   </si>
@@ -7679,6 +7679,18 @@
     <t>contact tracing</t>
   </si>
   <si>
+    <t>CONTACT_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>contact management</t>
+  </si>
+  <si>
+    <t>SOURCECASE_TRACING</t>
+  </si>
+  <si>
+    <t>source case tracing</t>
+  </si>
+  <si>
     <t>SAMPLE_COLLECTION</t>
   </si>
   <si>
@@ -7745,6 +7757,18 @@
     <t>quarantine place</t>
   </si>
   <si>
+    <t>QUARANTINE_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>quarantine management</t>
+  </si>
+  <si>
+    <t>QUARANTINE_ORDER_SEND</t>
+  </si>
+  <si>
+    <t>send quarantine order</t>
+  </si>
+  <si>
     <t>VACCINATION_ACTIVITIES</t>
   </si>
   <si>
@@ -8639,7 +8663,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.60.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -9387,7 +9411,7 @@
 </file>
 
 <file path=xl/tables/table136.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="136" name="TaskTaskType" displayName="TaskTaskType" ref="A27:E50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="136" name="TaskTaskType" displayName="TaskTaskType" ref="A27:E54">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -9401,7 +9425,7 @@
 </file>
 
 <file path=xl/tables/table137.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="137" name="TaskTaskPriority" displayName="TaskTaskPriority" ref="A52:E55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="137" name="TaskTaskPriority" displayName="TaskTaskPriority" ref="A56:E59">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -9415,7 +9439,7 @@
 </file>
 
 <file path=xl/tables/table138.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="138" name="TaskTaskStatus" displayName="TaskTaskStatus" ref="A57:E61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="138" name="TaskTaskStatus" displayName="TaskTaskStatus" ref="A61:E65">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -31965,7 +31989,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -32809,10 +32833,10 @@
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>173</v>
+        <v>2571</v>
       </c>
       <c r="C47" t="s">
-        <v>2571</v>
+        <v>2572</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -32824,10 +32848,10 @@
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="C48" t="s">
-        <v>2573</v>
+        <v>2574</v>
       </c>
       <c r="D48" t="s">
         <v>22</v>
@@ -32839,10 +32863,10 @@
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>2574</v>
+        <v>2575</v>
       </c>
       <c r="C49" t="s">
-        <v>2575</v>
+        <v>2576</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -32854,10 +32878,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>2576</v>
+        <v>2577</v>
       </c>
       <c r="C50" t="s">
-        <v>2577</v>
+        <v>2578</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
@@ -32866,32 +32890,43 @@
         <v>22</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51"/>
+      <c r="B51" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2579</v>
+      </c>
+      <c r="D51" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>1</v>
-      </c>
+      <c r="A52"/>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>2580</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>2581</v>
       </c>
       <c r="D52" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s">
-        <v>2502</v>
-      </c>
+      <c r="A53"/>
       <c r="B53" t="s">
-        <v>2578</v>
+        <v>2582</v>
       </c>
       <c r="C53" t="s">
-        <v>2579</v>
+        <v>2583</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -32903,10 +32938,10 @@
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>2580</v>
+        <v>2584</v>
       </c>
       <c r="C54" t="s">
-        <v>2581</v>
+        <v>2585</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -32915,47 +32950,47 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55"/>
-      <c r="B55" t="s">
-        <v>2582</v>
-      </c>
-      <c r="C55" t="s">
-        <v>2583</v>
-      </c>
-      <c r="D55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E55" t="s">
-        <v>22</v>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>2502</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>2586</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2587</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s">
-        <v>2509</v>
-      </c>
+      <c r="A58"/>
       <c r="B58" t="s">
-        <v>981</v>
+        <v>2588</v>
       </c>
       <c r="C58" t="s">
-        <v>2584</v>
+        <v>2589</v>
       </c>
       <c r="D58" t="s">
         <v>22</v>
@@ -32967,45 +33002,94 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
+        <v>2590</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2591</v>
+      </c>
+      <c r="D59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B62" t="s">
+        <v>981</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2592</v>
+      </c>
+      <c r="D62" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63"/>
+      <c r="B63" t="s">
         <v>984</v>
       </c>
-      <c r="C59" t="s">
-        <v>2585</v>
-      </c>
-      <c r="D59" t="s">
-        <v>22</v>
-      </c>
-      <c r="E59" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60"/>
-      <c r="B60" t="s">
-        <v>2586</v>
-      </c>
-      <c r="C60" t="s">
-        <v>2587</v>
-      </c>
-      <c r="D60" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61"/>
-      <c r="B61" t="s">
-        <v>2588</v>
-      </c>
-      <c r="C61" t="s">
-        <v>2589</v>
-      </c>
-      <c r="D61" t="s">
-        <v>22</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="C63" t="s">
+        <v>2593</v>
+      </c>
+      <c r="D63" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64"/>
+      <c r="B64" t="s">
+        <v>2594</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D64" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65"/>
+      <c r="B65" t="s">
+        <v>2596</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2597</v>
+      </c>
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" t="s">
         <v>22</v>
       </c>
     </row>
@@ -33079,7 +33163,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2590</v>
+        <v>2598</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>2494</v>
@@ -33101,17 +33185,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2591</v>
+        <v>2599</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>2592</v>
+        <v>2600</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2593</v>
+        <v>2601</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>2594</v>
+        <v>2602</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -33125,14 +33209,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2595</v>
+        <v>2603</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>2596</v>
+        <v>2604</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2597</v>
+        <v>2605</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>22</v>
@@ -33147,10 +33231,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2598</v>
+        <v>2606</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>2599</v>
+        <v>2607</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
@@ -33169,14 +33253,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2600</v>
+        <v>2608</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2601</v>
+        <v>2609</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>22</v>
@@ -33191,14 +33275,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2602</v>
+        <v>2610</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2603</v>
+        <v>2611</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>22</v>
@@ -33213,14 +33297,14 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2604</v>
+        <v>2612</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>2605</v>
+        <v>2613</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2606</v>
+        <v>2614</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>22</v>
@@ -33279,14 +33363,14 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2607</v>
+        <v>2615</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>2608</v>
+        <v>2616</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>22</v>
@@ -33301,7 +33385,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2609</v>
+        <v>2617</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>12</v>
@@ -33311,7 +33395,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>2610</v>
+        <v>2618</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -33325,14 +33409,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2611</v>
+        <v>2619</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>687</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2612</v>
+        <v>2620</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>22</v>
@@ -33354,10 +33438,10 @@
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>2613</v>
+        <v>2621</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>2614</v>
+        <v>2622</v>
       </c>
       <c r="F14"/>
       <c r="H14" s="22" t="s">
@@ -33376,10 +33460,10 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2615</v>
+        <v>2623</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>2616</v>
+        <v>2624</v>
       </c>
       <c r="F15"/>
       <c r="H15" s="22" t="s">
@@ -33439,14 +33523,14 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2617</v>
+        <v>2625</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
-        <v>2618</v>
+        <v>2626</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>22</v>
@@ -33461,14 +33545,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2619</v>
+        <v>2627</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2620</v>
+        <v>2628</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>22</v>
@@ -33483,7 +33567,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2621</v>
+        <v>2629</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>110</v>
@@ -33515,7 +33599,7 @@
         <v>1139</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>2622</v>
+        <v>2630</v>
       </c>
       <c r="F21"/>
       <c r="H21" s="22" t="s">
@@ -33595,14 +33679,14 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>2623</v>
+        <v>2631</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>2624</v>
+        <v>2632</v>
       </c>
       <c r="E25" s="22" t="s">
         <v>22</v>
@@ -33639,14 +33723,14 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>2625</v>
+        <v>2633</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>2626</v>
+        <v>2634</v>
       </c>
       <c r="C27"/>
       <c r="D27" t="s">
-        <v>2627</v>
+        <v>2635</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>22</v>
@@ -33661,14 +33745,14 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>2628</v>
+        <v>2636</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>2629</v>
+        <v>2637</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>2630</v>
+        <v>2638</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>22</v>
@@ -33683,14 +33767,14 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>2631</v>
+        <v>2639</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C29"/>
       <c r="D29" t="s">
-        <v>2632</v>
+        <v>2640</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>22</v>
@@ -33705,17 +33789,17 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>2633</v>
+        <v>2641</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C30"/>
       <c r="D30" t="s">
-        <v>2634</v>
+        <v>2642</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>2635</v>
+        <v>2643</v>
       </c>
       <c r="F30"/>
       <c r="H30" s="22" t="s">
@@ -33727,17 +33811,17 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>2636</v>
+        <v>2644</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C31"/>
       <c r="D31" t="s">
-        <v>2637</v>
+        <v>2645</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>2638</v>
+        <v>2646</v>
       </c>
       <c r="F31"/>
       <c r="H31" s="22" t="s">
@@ -33749,17 +33833,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>2639</v>
+        <v>2647</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C32"/>
       <c r="D32" t="s">
-        <v>2640</v>
+        <v>2648</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>2641</v>
+        <v>2649</v>
       </c>
       <c r="F32"/>
       <c r="H32" s="22" t="s">
@@ -33771,7 +33855,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>2642</v>
+        <v>2650</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>12</v>
@@ -33781,7 +33865,7 @@
         <v>562</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>2643</v>
+        <v>2651</v>
       </c>
       <c r="F33"/>
       <c r="H33" s="22" t="s">
@@ -33793,17 +33877,17 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>2644</v>
+        <v>2652</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C34"/>
       <c r="D34" t="s">
-        <v>2645</v>
+        <v>2653</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>2646</v>
+        <v>2654</v>
       </c>
       <c r="F34"/>
       <c r="H34" s="22" t="s">
@@ -33815,17 +33899,17 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>2647</v>
+        <v>2655</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C35"/>
       <c r="D35" t="s">
-        <v>2648</v>
+        <v>2656</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>2649</v>
+        <v>2657</v>
       </c>
       <c r="F35"/>
       <c r="H35" s="22" t="s">
@@ -33837,17 +33921,17 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>2650</v>
+        <v>2658</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C36"/>
       <c r="D36" t="s">
-        <v>2651</v>
+        <v>2659</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>2652</v>
+        <v>2660</v>
       </c>
       <c r="F36"/>
       <c r="H36" s="22" t="s">
@@ -33903,7 +33987,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>2653</v>
+        <v>2661</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>662</v>
@@ -33927,14 +34011,14 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>2654</v>
+        <v>2662</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C40"/>
       <c r="D40" t="s">
-        <v>2655</v>
+        <v>2663</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>22</v>
@@ -34015,14 +34099,14 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>2656</v>
+        <v>2664</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>687</v>
       </c>
       <c r="C44"/>
       <c r="D44" t="s">
-        <v>2657</v>
+        <v>2665</v>
       </c>
       <c r="E44" s="22" t="s">
         <v>22</v>
@@ -34037,14 +34121,14 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>2658</v>
+        <v>2666</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>2659</v>
+        <v>2667</v>
       </c>
       <c r="C45"/>
       <c r="D45" t="s">
-        <v>2660</v>
+        <v>2668</v>
       </c>
       <c r="E45" s="22" t="s">
         <v>22</v>
@@ -34059,17 +34143,17 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>2661</v>
+        <v>2669</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>2662</v>
+        <v>2670</v>
       </c>
       <c r="C46"/>
       <c r="D46" t="s">
-        <v>2663</v>
+        <v>2671</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>2664</v>
+        <v>2672</v>
       </c>
       <c r="F46"/>
       <c r="H46" s="22" t="s">
@@ -34083,14 +34167,14 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>2665</v>
+        <v>2673</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>2666</v>
+        <v>2674</v>
       </c>
       <c r="C47"/>
       <c r="D47" t="s">
-        <v>2667</v>
+        <v>2675</v>
       </c>
       <c r="E47" s="22" t="s">
         <v>22</v>
@@ -34107,14 +34191,14 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>2668</v>
+        <v>2676</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>2669</v>
+        <v>2677</v>
       </c>
       <c r="C48"/>
       <c r="D48" t="s">
-        <v>2670</v>
+        <v>2678</v>
       </c>
       <c r="E48" s="22" t="s">
         <v>22</v>
@@ -34131,14 +34215,14 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>2671</v>
+        <v>2679</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>2672</v>
+        <v>2680</v>
       </c>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>2673</v>
+        <v>2681</v>
       </c>
       <c r="E49" s="22" t="s">
         <v>22</v>
@@ -34155,14 +34239,14 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>2674</v>
+        <v>2682</v>
       </c>
       <c r="B50" s="22" t="s">
         <v>687</v>
       </c>
       <c r="C50"/>
       <c r="D50" t="s">
-        <v>2675</v>
+        <v>2683</v>
       </c>
       <c r="E50" s="22" t="s">
         <v>22</v>
@@ -34179,7 +34263,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>2676</v>
+        <v>2684</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51"/>
@@ -34201,14 +34285,14 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>2677</v>
+        <v>2685</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>687</v>
       </c>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>2678</v>
+        <v>2686</v>
       </c>
       <c r="E52" s="22" t="s">
         <v>22</v>
@@ -34225,7 +34309,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>2679</v>
+        <v>2687</v>
       </c>
       <c r="B53" s="22"/>
       <c r="C53"/>
@@ -34291,14 +34375,14 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>2680</v>
+        <v>2688</v>
       </c>
       <c r="B56" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C56"/>
       <c r="D56" t="s">
-        <v>2681</v>
+        <v>2689</v>
       </c>
       <c r="E56" s="22" t="s">
         <v>22</v>
@@ -34332,13 +34416,13 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>2592</v>
+        <v>2600</v>
       </c>
       <c r="B59" t="s">
-        <v>2682</v>
+        <v>2690</v>
       </c>
       <c r="C59" t="s">
-        <v>2683</v>
+        <v>2691</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
@@ -34380,10 +34464,10 @@
     <row r="62">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>2684</v>
+        <v>2692</v>
       </c>
       <c r="C62" t="s">
-        <v>2685</v>
+        <v>2693</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -34426,13 +34510,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>2596</v>
+        <v>2604</v>
       </c>
       <c r="B66" t="s">
-        <v>2582</v>
+        <v>2590</v>
       </c>
       <c r="C66" t="s">
-        <v>2686</v>
+        <v>2694</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -34444,10 +34528,10 @@
     <row r="67">
       <c r="A67"/>
       <c r="B67" t="s">
-        <v>2687</v>
+        <v>2695</v>
       </c>
       <c r="C67" t="s">
-        <v>2688</v>
+        <v>2696</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -34459,10 +34543,10 @@
     <row r="68">
       <c r="A68"/>
       <c r="B68" t="s">
-        <v>2578</v>
+        <v>2586</v>
       </c>
       <c r="C68" t="s">
-        <v>2689</v>
+        <v>2697</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -34505,7 +34589,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>2599</v>
+        <v>2607</v>
       </c>
       <c r="B72" t="s">
         <v>981</v>
@@ -34523,10 +34607,10 @@
     <row r="73">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>2690</v>
+        <v>2698</v>
       </c>
       <c r="C73" t="s">
-        <v>2691</v>
+        <v>2699</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -34584,7 +34668,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>2605</v>
+        <v>2613</v>
       </c>
       <c r="B78" t="s">
         <v>981</v>
@@ -34602,7 +34686,7 @@
     <row r="79">
       <c r="A79"/>
       <c r="B79" t="s">
-        <v>2690</v>
+        <v>2698</v>
       </c>
       <c r="C79" t="s">
         <v>1091</v>
@@ -34632,10 +34716,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>2692</v>
+        <v>2700</v>
       </c>
       <c r="C81" t="s">
-        <v>2693</v>
+        <v>2701</v>
       </c>
       <c r="D81" t="s">
         <v>22</v>
@@ -35129,13 +35213,13 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>2626</v>
+        <v>2634</v>
       </c>
       <c r="B118" t="s">
-        <v>2694</v>
+        <v>2702</v>
       </c>
       <c r="C118" t="s">
-        <v>2695</v>
+        <v>2703</v>
       </c>
       <c r="D118" t="s">
         <v>22</v>
@@ -35147,10 +35231,10 @@
     <row r="119">
       <c r="A119"/>
       <c r="B119" t="s">
-        <v>2696</v>
+        <v>2704</v>
       </c>
       <c r="C119" t="s">
-        <v>2697</v>
+        <v>2705</v>
       </c>
       <c r="D119" t="s">
         <v>22</v>
@@ -35162,10 +35246,10 @@
     <row r="120">
       <c r="A120"/>
       <c r="B120" t="s">
-        <v>2698</v>
+        <v>2706</v>
       </c>
       <c r="C120" t="s">
-        <v>2699</v>
+        <v>2707</v>
       </c>
       <c r="D120" t="s">
         <v>22</v>
@@ -35177,10 +35261,10 @@
     <row r="121">
       <c r="A121"/>
       <c r="B121" t="s">
-        <v>2700</v>
+        <v>2708</v>
       </c>
       <c r="C121" t="s">
-        <v>2701</v>
+        <v>2709</v>
       </c>
       <c r="D121" t="s">
         <v>22</v>
@@ -35192,10 +35276,10 @@
     <row r="122">
       <c r="A122"/>
       <c r="B122" t="s">
-        <v>2702</v>
+        <v>2710</v>
       </c>
       <c r="C122" t="s">
-        <v>2703</v>
+        <v>2711</v>
       </c>
       <c r="D122" t="s">
         <v>22</v>
@@ -35223,13 +35307,13 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>2629</v>
+        <v>2637</v>
       </c>
       <c r="B125" t="s">
-        <v>2704</v>
+        <v>2712</v>
       </c>
       <c r="C125" t="s">
-        <v>2705</v>
+        <v>2713</v>
       </c>
       <c r="D125" t="s">
         <v>22</v>
@@ -35241,10 +35325,10 @@
     <row r="126">
       <c r="A126"/>
       <c r="B126" t="s">
-        <v>2706</v>
+        <v>2714</v>
       </c>
       <c r="C126" t="s">
-        <v>2707</v>
+        <v>2715</v>
       </c>
       <c r="D126" t="s">
         <v>22</v>
@@ -35256,10 +35340,10 @@
     <row r="127">
       <c r="A127"/>
       <c r="B127" t="s">
-        <v>2708</v>
+        <v>2716</v>
       </c>
       <c r="C127" t="s">
-        <v>2709</v>
+        <v>2717</v>
       </c>
       <c r="D127" t="s">
         <v>22</v>
@@ -35271,10 +35355,10 @@
     <row r="128">
       <c r="A128"/>
       <c r="B128" t="s">
-        <v>2710</v>
+        <v>2718</v>
       </c>
       <c r="C128" t="s">
-        <v>2711</v>
+        <v>2719</v>
       </c>
       <c r="D128" t="s">
         <v>22</v>
@@ -35286,10 +35370,10 @@
     <row r="129">
       <c r="A129"/>
       <c r="B129" t="s">
-        <v>2712</v>
+        <v>2720</v>
       </c>
       <c r="C129" t="s">
-        <v>2713</v>
+        <v>2721</v>
       </c>
       <c r="D129" t="s">
         <v>22</v>
@@ -36191,13 +36275,13 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>2659</v>
+        <v>2667</v>
       </c>
       <c r="B191" t="s">
-        <v>2714</v>
+        <v>2722</v>
       </c>
       <c r="C191" t="s">
-        <v>2715</v>
+        <v>2723</v>
       </c>
       <c r="D191" t="s">
         <v>22</v>
@@ -36212,7 +36296,7 @@
         <v>2328</v>
       </c>
       <c r="C192" t="s">
-        <v>2716</v>
+        <v>2724</v>
       </c>
       <c r="D192" t="s">
         <v>22</v>
@@ -36227,7 +36311,7 @@
         <v>2330</v>
       </c>
       <c r="C193" t="s">
-        <v>2717</v>
+        <v>2725</v>
       </c>
       <c r="D193" t="s">
         <v>22</v>
@@ -36239,10 +36323,10 @@
     <row r="194">
       <c r="A194"/>
       <c r="B194" t="s">
-        <v>2718</v>
+        <v>2726</v>
       </c>
       <c r="C194" t="s">
-        <v>2719</v>
+        <v>2727</v>
       </c>
       <c r="D194" t="s">
         <v>22</v>
@@ -36254,10 +36338,10 @@
     <row r="195">
       <c r="A195"/>
       <c r="B195" t="s">
-        <v>2720</v>
+        <v>2728</v>
       </c>
       <c r="C195" t="s">
-        <v>2721</v>
+        <v>2729</v>
       </c>
       <c r="D195" t="s">
         <v>22</v>
@@ -36300,7 +36384,7 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>2662</v>
+        <v>2670</v>
       </c>
       <c r="B199" t="s">
         <v>934</v>
@@ -36379,13 +36463,13 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>2666</v>
+        <v>2674</v>
       </c>
       <c r="B205" t="s">
-        <v>2722</v>
+        <v>2730</v>
       </c>
       <c r="C205" t="s">
-        <v>2723</v>
+        <v>2731</v>
       </c>
       <c r="D205" t="s">
         <v>22</v>
@@ -36397,10 +36481,10 @@
     <row r="206">
       <c r="A206"/>
       <c r="B206" t="s">
-        <v>2724</v>
+        <v>2732</v>
       </c>
       <c r="C206" t="s">
-        <v>2725</v>
+        <v>2733</v>
       </c>
       <c r="D206" t="s">
         <v>22</v>
@@ -36412,10 +36496,10 @@
     <row r="207">
       <c r="A207"/>
       <c r="B207" t="s">
-        <v>2726</v>
+        <v>2734</v>
       </c>
       <c r="C207" t="s">
-        <v>2727</v>
+        <v>2735</v>
       </c>
       <c r="D207" t="s">
         <v>22</v>
@@ -36427,10 +36511,10 @@
     <row r="208">
       <c r="A208"/>
       <c r="B208" t="s">
-        <v>2728</v>
+        <v>2736</v>
       </c>
       <c r="C208" t="s">
-        <v>2729</v>
+        <v>2737</v>
       </c>
       <c r="D208" t="s">
         <v>22</v>
@@ -36442,10 +36526,10 @@
     <row r="209">
       <c r="A209"/>
       <c r="B209" t="s">
-        <v>2730</v>
+        <v>2738</v>
       </c>
       <c r="C209" t="s">
-        <v>2731</v>
+        <v>2739</v>
       </c>
       <c r="D209" t="s">
         <v>22</v>
@@ -36457,10 +36541,10 @@
     <row r="210">
       <c r="A210"/>
       <c r="B210" t="s">
-        <v>2732</v>
+        <v>2740</v>
       </c>
       <c r="C210" t="s">
-        <v>2733</v>
+        <v>2741</v>
       </c>
       <c r="D210" t="s">
         <v>22</v>
@@ -36503,13 +36587,13 @@
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>2669</v>
+        <v>2677</v>
       </c>
       <c r="B214" t="s">
-        <v>2734</v>
+        <v>2742</v>
       </c>
       <c r="C214" t="s">
-        <v>2735</v>
+        <v>2743</v>
       </c>
       <c r="D214" t="s">
         <v>22</v>
@@ -36521,10 +36605,10 @@
     <row r="215">
       <c r="A215"/>
       <c r="B215" t="s">
-        <v>2736</v>
+        <v>2744</v>
       </c>
       <c r="C215" t="s">
-        <v>2737</v>
+        <v>2745</v>
       </c>
       <c r="D215" t="s">
         <v>22</v>
@@ -36536,10 +36620,10 @@
     <row r="216">
       <c r="A216"/>
       <c r="B216" t="s">
-        <v>2738</v>
+        <v>2746</v>
       </c>
       <c r="C216" t="s">
-        <v>2739</v>
+        <v>2747</v>
       </c>
       <c r="D216" t="s">
         <v>22</v>
@@ -36551,10 +36635,10 @@
     <row r="217">
       <c r="A217"/>
       <c r="B217" t="s">
-        <v>2740</v>
+        <v>2748</v>
       </c>
       <c r="C217" t="s">
-        <v>2741</v>
+        <v>2749</v>
       </c>
       <c r="D217" t="s">
         <v>22</v>
@@ -36566,10 +36650,10 @@
     <row r="218">
       <c r="A218"/>
       <c r="B218" t="s">
-        <v>2742</v>
+        <v>2750</v>
       </c>
       <c r="C218" t="s">
-        <v>2743</v>
+        <v>2751</v>
       </c>
       <c r="D218" t="s">
         <v>22</v>
@@ -36612,13 +36696,13 @@
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>2672</v>
+        <v>2680</v>
       </c>
       <c r="B222" t="s">
-        <v>2744</v>
+        <v>2752</v>
       </c>
       <c r="C222" t="s">
-        <v>2745</v>
+        <v>2753</v>
       </c>
       <c r="D222" t="s">
         <v>22</v>
@@ -36630,10 +36714,10 @@
     <row r="223">
       <c r="A223"/>
       <c r="B223" t="s">
-        <v>2746</v>
+        <v>2754</v>
       </c>
       <c r="C223" t="s">
-        <v>2747</v>
+        <v>2755</v>
       </c>
       <c r="D223" t="s">
         <v>22</v>
@@ -36645,10 +36729,10 @@
     <row r="224">
       <c r="A224"/>
       <c r="B224" t="s">
-        <v>2748</v>
+        <v>2756</v>
       </c>
       <c r="C224" t="s">
-        <v>2749</v>
+        <v>2757</v>
       </c>
       <c r="D224" t="s">
         <v>22</v>
@@ -36660,10 +36744,10 @@
     <row r="225">
       <c r="A225"/>
       <c r="B225" t="s">
-        <v>2750</v>
+        <v>2758</v>
       </c>
       <c r="C225" t="s">
-        <v>2751</v>
+        <v>2759</v>
       </c>
       <c r="D225" t="s">
         <v>22</v>
@@ -36675,10 +36759,10 @@
     <row r="226">
       <c r="A226"/>
       <c r="B226" t="s">
-        <v>2752</v>
+        <v>2760</v>
       </c>
       <c r="C226" t="s">
-        <v>2753</v>
+        <v>2761</v>
       </c>
       <c r="D226" t="s">
         <v>22</v>
@@ -36839,7 +36923,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2754</v>
+        <v>2762</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>12</v>
@@ -36848,7 +36932,7 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>2755</v>
+        <v>2763</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>22</v>
@@ -37059,14 +37143,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2756</v>
+        <v>2764</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>2757</v>
+        <v>2765</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2758</v>
+        <v>2766</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>22</v>
@@ -37105,14 +37189,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2759</v>
+        <v>2767</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>2760</v>
+        <v>2768</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2761</v>
+        <v>2769</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>22</v>
@@ -37130,7 +37214,7 @@
         <v>2501</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>2762</v>
+        <v>2770</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
@@ -37149,7 +37233,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2763</v>
+        <v>2771</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>55</v>
@@ -37173,14 +37257,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2764</v>
+        <v>2772</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>2765</v>
+        <v>2773</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2766</v>
+        <v>2774</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>22</v>
@@ -37239,14 +37323,14 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2767</v>
+        <v>2775</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>2608</v>
+        <v>2616</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>22</v>
@@ -37283,7 +37367,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2768</v>
+        <v>2776</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>12</v>
@@ -37305,14 +37389,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2769</v>
+        <v>2777</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>662</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2770</v>
+        <v>2778</v>
       </c>
       <c r="E13" s="24" t="s">
         <v>22</v>
@@ -37344,7 +37428,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2757</v>
+        <v>2765</v>
       </c>
       <c r="B16" t="s">
         <v>2530</v>
@@ -37378,13 +37462,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2760</v>
+        <v>2768</v>
       </c>
       <c r="B19" t="s">
-        <v>2771</v>
+        <v>2779</v>
       </c>
       <c r="C19" t="s">
-        <v>2772</v>
+        <v>2780</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -37396,10 +37480,10 @@
     <row r="20">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>2545</v>
+        <v>2549</v>
       </c>
       <c r="C20" t="s">
-        <v>2773</v>
+        <v>2781</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -37411,10 +37495,10 @@
     <row r="21">
       <c r="A21"/>
       <c r="B21" t="s">
-        <v>2774</v>
+        <v>2782</v>
       </c>
       <c r="C21" t="s">
-        <v>2775</v>
+        <v>2783</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -37426,10 +37510,10 @@
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>2549</v>
+        <v>2553</v>
       </c>
       <c r="C22" t="s">
-        <v>2776</v>
+        <v>2784</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -37441,10 +37525,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>2777</v>
+        <v>2785</v>
       </c>
       <c r="C23" t="s">
-        <v>2778</v>
+        <v>2786</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -37456,10 +37540,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>2779</v>
+        <v>2787</v>
       </c>
       <c r="C24" t="s">
-        <v>2780</v>
+        <v>2788</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -37471,10 +37555,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>2781</v>
+        <v>2789</v>
       </c>
       <c r="C25" t="s">
-        <v>2782</v>
+        <v>2790</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -37486,10 +37570,10 @@
     <row r="26">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>2783</v>
+        <v>2791</v>
       </c>
       <c r="C26" t="s">
-        <v>2784</v>
+        <v>2792</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
@@ -37501,10 +37585,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>2785</v>
+        <v>2793</v>
       </c>
       <c r="C27" t="s">
-        <v>2786</v>
+        <v>2794</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
@@ -37547,13 +37631,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>2762</v>
+        <v>2770</v>
       </c>
       <c r="B31" t="s">
-        <v>2578</v>
+        <v>2586</v>
       </c>
       <c r="C31" t="s">
-        <v>2579</v>
+        <v>2587</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
@@ -37565,10 +37649,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>2580</v>
+        <v>2588</v>
       </c>
       <c r="C32" t="s">
-        <v>2581</v>
+        <v>2589</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
@@ -37580,10 +37664,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>2582</v>
+        <v>2590</v>
       </c>
       <c r="C33" t="s">
-        <v>2583</v>
+        <v>2591</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -37611,7 +37695,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>2765</v>
+        <v>2773</v>
       </c>
       <c r="B36" t="s">
         <v>981</v>
@@ -37629,10 +37713,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>2787</v>
+        <v>2795</v>
       </c>
       <c r="C37" t="s">
-        <v>2788</v>
+        <v>2796</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -37726,14 +37810,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2789</v>
+        <v>2797</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2790</v>
+        <v>2798</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>22</v>
@@ -38041,7 +38125,7 @@
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2791</v>
+        <v>2799</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>22</v>
@@ -38063,7 +38147,7 @@
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>2792</v>
+        <v>2800</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>22</v>
@@ -38078,7 +38162,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2793</v>
+        <v>2801</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>69</v>
@@ -38100,14 +38184,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2794</v>
+        <v>2802</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>132</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2795</v>
+        <v>2803</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>22</v>
@@ -38122,14 +38206,14 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2796</v>
+        <v>2804</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>132</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>2797</v>
+        <v>2805</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>22</v>
@@ -39215,14 +39299,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2798</v>
+        <v>2806</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2799</v>
+        <v>2807</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>22</v>
@@ -39259,14 +39343,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2800</v>
+        <v>2808</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2801</v>
+        <v>2809</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>22</v>
@@ -39281,14 +39365,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2802</v>
+        <v>2810</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2803</v>
+        <v>2811</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>22</v>
@@ -39303,14 +39387,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2796</v>
+        <v>2804</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>132</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2797</v>
+        <v>2805</v>
       </c>
       <c r="E6" s="26" t="s">
         <v>22</v>
@@ -39411,14 +39495,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2789</v>
+        <v>2797</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2790</v>
+        <v>2798</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>22</v>
@@ -39433,14 +39517,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2804</v>
+        <v>2812</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2805</v>
+        <v>2813</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>22</v>
@@ -39455,14 +39539,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2806</v>
+        <v>2814</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2807</v>
+        <v>2815</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>22</v>
@@ -39477,14 +39561,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2796</v>
+        <v>2804</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>132</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2797</v>
+        <v>2805</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>22</v>
@@ -39521,14 +39605,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2808</v>
+        <v>2816</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>2809</v>
+        <v>2817</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2810</v>
+        <v>2818</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>22</v>
@@ -39629,14 +39713,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2789</v>
+        <v>2797</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2790</v>
+        <v>2798</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>22</v>
@@ -39651,14 +39735,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2804</v>
+        <v>2812</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2805</v>
+        <v>2813</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>22</v>
@@ -39673,14 +39757,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2806</v>
+        <v>2814</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2807</v>
+        <v>2815</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>22</v>
@@ -39717,14 +39801,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2796</v>
+        <v>2804</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>132</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2797</v>
+        <v>2805</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>22</v>
@@ -39825,14 +39909,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2789</v>
+        <v>2797</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2790</v>
+        <v>2798</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>22</v>
@@ -39847,7 +39931,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2806</v>
+        <v>2814</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>42</v>
@@ -39913,14 +39997,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2796</v>
+        <v>2804</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>132</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2797</v>
+        <v>2805</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>22</v>
@@ -41824,14 +41908,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2811</v>
+        <v>2819</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>132</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2812</v>
+        <v>2820</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>22</v>
@@ -41846,14 +41930,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2813</v>
+        <v>2821</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2814</v>
+        <v>2822</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>22</v>
@@ -41912,7 +41996,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2815</v>
+        <v>2823</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>12</v>
@@ -41934,14 +42018,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2816</v>
+        <v>2824</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2817</v>
+        <v>2825</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>22</v>
@@ -41963,7 +42047,7 @@
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2818</v>
+        <v>2826</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>22</v>
@@ -41978,12 +42062,12 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2819</v>
+        <v>2827</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2820</v>
+        <v>2828</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>22</v>
@@ -42086,7 +42170,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2821</v>
+        <v>2829</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>72</v>
@@ -42115,7 +42199,7 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2822</v>
+        <v>2830</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>22</v>
@@ -42130,14 +42214,14 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2823</v>
+        <v>2831</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>662</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2824</v>
+        <v>2832</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>22</v>
@@ -42152,17 +42236,17 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2825</v>
+        <v>2833</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>91</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>2826</v>
+        <v>2834</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>2827</v>
+        <v>2835</v>
       </c>
       <c r="F17"/>
       <c r="H17" s="30" t="s">
@@ -42174,10 +42258,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2828</v>
+        <v>2836</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>2829</v>
+        <v>2837</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
@@ -42196,14 +42280,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2830</v>
+        <v>2838</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>132</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2831</v>
+        <v>2839</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>22</v>
@@ -43146,13 +43230,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>2829</v>
+        <v>2837</v>
       </c>
       <c r="B85" t="s">
-        <v>2832</v>
+        <v>2840</v>
       </c>
       <c r="C85" t="s">
-        <v>2833</v>
+        <v>2841</v>
       </c>
       <c r="D85" t="s">
         <v>22</v>
@@ -43164,10 +43248,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>2834</v>
+        <v>2842</v>
       </c>
       <c r="C86" t="s">
-        <v>2835</v>
+        <v>2843</v>
       </c>
       <c r="D86" t="s">
         <v>22</v>
@@ -43179,10 +43263,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>2836</v>
+        <v>2844</v>
       </c>
       <c r="C87" t="s">
-        <v>2837</v>
+        <v>2845</v>
       </c>
       <c r="D87" t="s">
         <v>22</v>
@@ -43194,10 +43278,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>2838</v>
+        <v>2846</v>
       </c>
       <c r="C88" t="s">
-        <v>2839</v>
+        <v>2847</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -43209,10 +43293,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>2840</v>
+        <v>2848</v>
       </c>
       <c r="C89" t="s">
-        <v>2841</v>
+        <v>2849</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -43224,10 +43308,10 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>2842</v>
+        <v>2850</v>
       </c>
       <c r="C90" t="s">
-        <v>2843</v>
+        <v>2851</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -43239,10 +43323,10 @@
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>2844</v>
+        <v>2852</v>
       </c>
       <c r="C91" t="s">
-        <v>2845</v>
+        <v>2853</v>
       </c>
       <c r="D91" t="s">
         <v>22</v>
@@ -43254,10 +43338,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>2846</v>
+        <v>2854</v>
       </c>
       <c r="C92" t="s">
-        <v>2847</v>
+        <v>2855</v>
       </c>
       <c r="D92" t="s">
         <v>22</v>
@@ -43269,10 +43353,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>2848</v>
+        <v>2856</v>
       </c>
       <c r="C93" t="s">
-        <v>2849</v>
+        <v>2857</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -43284,10 +43368,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>2850</v>
+        <v>2858</v>
       </c>
       <c r="C94" t="s">
-        <v>2851</v>
+        <v>2859</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -43299,10 +43383,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>2852</v>
+        <v>2860</v>
       </c>
       <c r="C95" t="s">
-        <v>2853</v>
+        <v>2861</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -43314,10 +43398,10 @@
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
-        <v>2854</v>
+        <v>2862</v>
       </c>
       <c r="C96" t="s">
-        <v>2855</v>
+        <v>2863</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -43329,10 +43413,10 @@
     <row r="97">
       <c r="A97"/>
       <c r="B97" t="s">
-        <v>2856</v>
+        <v>2864</v>
       </c>
       <c r="C97" t="s">
-        <v>2857</v>
+        <v>2865</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
@@ -43344,10 +43428,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>2858</v>
+        <v>2866</v>
       </c>
       <c r="C98" t="s">
-        <v>2859</v>
+        <v>2867</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -43359,10 +43443,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>2860</v>
+        <v>2868</v>
       </c>
       <c r="C99" t="s">
-        <v>2861</v>
+        <v>2869</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -43374,10 +43458,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>2862</v>
+        <v>2870</v>
       </c>
       <c r="C100" t="s">
-        <v>2863</v>
+        <v>2871</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
@@ -43407,12 +43491,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2864</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2865</v>
+        <v>2873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#6688] extract etcd client and create producer
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12784" uniqueCount="2929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12793" uniqueCount="2933">
   <si>
     <t>Field</t>
   </si>
@@ -7617,6 +7617,15 @@
     <t>contact</t>
   </si>
   <si>
+    <t>travelEntry</t>
+  </si>
+  <si>
+    <t>TravelEntryReference</t>
+  </si>
+  <si>
+    <t>Travel entry</t>
+  </si>
+  <si>
     <t>taskType</t>
   </si>
   <si>
@@ -7726,6 +7735,9 @@
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>TRAVEL_ENTRY</t>
   </si>
   <si>
     <t>ACTIVE_SEARCH_FOR_OTHER_CASES</t>
@@ -9578,7 +9590,7 @@
 </file>
 
 <file path=xl/tables/table135.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="135" name="Task" displayName="Task" ref="A1:K19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="135" name="Task" displayName="Task" ref="A1:K20">
   <autoFilter/>
   <tableColumns count="11">
     <tableColumn id="1" name="Field"/>
@@ -9598,7 +9610,7 @@
 </file>
 
 <file path=xl/tables/table136.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="136" name="TaskTaskContext" displayName="TaskTaskContext" ref="A21:E25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="136" name="TaskTaskContext" displayName="TaskTaskContext" ref="A22:E27">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -9612,7 +9624,7 @@
 </file>
 
 <file path=xl/tables/table137.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="137" name="TaskTaskType" displayName="TaskTaskType" ref="A27:E54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="137" name="TaskTaskType" displayName="TaskTaskType" ref="A29:E56">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -9626,7 +9638,7 @@
 </file>
 
 <file path=xl/tables/table138.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="138" name="TaskTaskPriority" displayName="TaskTaskPriority" ref="A56:E59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="138" name="TaskTaskPriority" displayName="TaskTaskPriority" ref="A58:E61">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -9640,7 +9652,7 @@
 </file>
 
 <file path=xl/tables/table139.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="139" name="TaskTaskStatus" displayName="TaskTaskStatus" ref="A61:E65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="139" name="TaskTaskStatus" displayName="TaskTaskStatus" ref="A63:E67">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -32392,7 +32404,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -32548,11 +32560,9 @@
         <v>2525</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>2526</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F6"/>
       <c r="H6" s="21" t="s">
         <v>16</v>
       </c>
@@ -32562,19 +32572,21 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>2526</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>2527</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>2528</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
+        <v>2528</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>2529</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7"/>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
       <c r="H7" s="21" t="s">
         <v>16</v>
       </c>
@@ -32587,18 +32599,16 @@
         <v>2530</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>55</v>
+        <v>2531</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2531</v>
+        <v>2532</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
+      <c r="F8"/>
       <c r="H8" s="21" t="s">
         <v>16</v>
       </c>
@@ -32608,19 +32618,21 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2532</v>
+        <v>2533</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2533</v>
+        <v>2534</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F9"/>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
       <c r="H9" s="21" t="s">
         <v>16</v>
       </c>
@@ -32630,10 +32642,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2534</v>
+        <v>2535</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>2535</v>
+        <v>55</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
@@ -32655,11 +32667,11 @@
         <v>2537</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>55</v>
+        <v>2538</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>2538</v>
+        <v>2539</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>22</v>
@@ -32674,14 +32686,14 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2539</v>
+        <v>2540</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2540</v>
+        <v>2541</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>22</v>
@@ -32696,14 +32708,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2541</v>
+        <v>2542</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>666</v>
+        <v>55</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2542</v>
+        <v>2543</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>22</v>
@@ -32718,14 +32730,14 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2543</v>
+        <v>2544</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>12</v>
+        <v>666</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>2544</v>
+        <v>2545</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>22</v>
@@ -32740,21 +32752,19 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2545</v>
+        <v>2546</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>666</v>
+        <v>12</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2546</v>
+        <v>2547</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
+      <c r="F15"/>
       <c r="H15" s="21" t="s">
         <v>16</v>
       </c>
@@ -32764,19 +32774,21 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2547</v>
+        <v>2548</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>12</v>
+        <v>666</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2548</v>
+        <v>2549</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F16"/>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
       <c r="H16" s="21" t="s">
         <v>16</v>
       </c>
@@ -32786,14 +32798,14 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2549</v>
+        <v>2550</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>2551</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>22</v>
@@ -32808,7 +32820,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2550</v>
+        <v>2552</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>42</v>
@@ -32830,7 +32842,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2551</v>
+        <v>2553</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>42</v>
@@ -32850,47 +32862,54 @@
       <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>166</v>
-      </c>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>2554</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20"/>
+      <c r="H20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>2517</v>
       </c>
-      <c r="B22" t="s">
-        <v>2552</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2553</v>
-      </c>
-      <c r="D22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23"/>
       <c r="B23" t="s">
-        <v>2554</v>
+        <v>2555</v>
       </c>
       <c r="C23" t="s">
-        <v>2555</v>
+        <v>2556</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -32902,10 +32921,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>2556</v>
+        <v>2557</v>
       </c>
       <c r="C24" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -32917,10 +32936,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>2558</v>
+        <v>2559</v>
       </c>
       <c r="C25" t="s">
-        <v>2559</v>
+        <v>2560</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -32929,57 +32948,57 @@
         <v>22</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26"/>
+      <c r="B26" t="s">
+        <v>2561</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="27">
-      <c r="A27" t="s">
+      <c r="A27"/>
+      <c r="B27" t="s">
+        <v>2563</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2525</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>156</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>2524</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2560</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2561</v>
-      </c>
-      <c r="D28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29"/>
-      <c r="B29" t="s">
-        <v>2562</v>
-      </c>
-      <c r="C29" t="s">
-        <v>2563</v>
-      </c>
-      <c r="D29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="30">
-      <c r="A30"/>
+      <c r="A30" t="s">
+        <v>2527</v>
+      </c>
       <c r="B30" t="s">
         <v>2564</v>
       </c>
@@ -33026,10 +33045,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>965</v>
+        <v>2570</v>
       </c>
       <c r="C33" t="s">
-        <v>2570</v>
+        <v>2571</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -33041,10 +33060,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>2571</v>
+        <v>2572</v>
       </c>
       <c r="C34" t="s">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
@@ -33056,7 +33075,7 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>2573</v>
+        <v>965</v>
       </c>
       <c r="C35" t="s">
         <v>2574</v>
@@ -33296,10 +33315,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>177</v>
+        <v>2605</v>
       </c>
       <c r="C51" t="s">
-        <v>2605</v>
+        <v>2606</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -33311,10 +33330,10 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>2606</v>
+        <v>2607</v>
       </c>
       <c r="C52" t="s">
-        <v>2607</v>
+        <v>2608</v>
       </c>
       <c r="D52" t="s">
         <v>22</v>
@@ -33326,7 +33345,7 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>2608</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
         <v>2609</v>
@@ -33353,57 +33372,57 @@
         <v>22</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55"/>
+      <c r="B55" t="s">
+        <v>2612</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2613</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="56">
-      <c r="A56" t="s">
+      <c r="A56"/>
+      <c r="B56" t="s">
+        <v>2614</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2615</v>
+      </c>
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
         <v>1</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>156</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>3</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D58" t="s">
         <v>4</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E58" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>2528</v>
-      </c>
-      <c r="B57" t="s">
-        <v>2612</v>
-      </c>
-      <c r="C57" t="s">
-        <v>2613</v>
-      </c>
-      <c r="D57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E57" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58"/>
-      <c r="B58" t="s">
-        <v>2614</v>
-      </c>
-      <c r="C58" t="s">
-        <v>2615</v>
-      </c>
-      <c r="D58" t="s">
-        <v>22</v>
-      </c>
-      <c r="E58" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="59">
-      <c r="A59"/>
+      <c r="A59" t="s">
+        <v>2531</v>
+      </c>
       <c r="B59" t="s">
         <v>2616</v>
       </c>
@@ -33417,62 +33436,62 @@
         <v>22</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60"/>
+      <c r="B60" t="s">
+        <v>2618</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2619</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="61">
-      <c r="A61" t="s">
+      <c r="A61"/>
+      <c r="B61" t="s">
+        <v>2620</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2621</v>
+      </c>
+      <c r="D61" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
         <v>1</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>156</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>3</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D63" t="s">
         <v>4</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E63" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>2535</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="64">
+      <c r="A64" t="s">
+        <v>2538</v>
+      </c>
+      <c r="B64" t="s">
         <v>988</v>
       </c>
-      <c r="C62" t="s">
-        <v>2618</v>
-      </c>
-      <c r="D62" t="s">
-        <v>22</v>
-      </c>
-      <c r="E62" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63"/>
-      <c r="B63" t="s">
-        <v>991</v>
-      </c>
-      <c r="C63" t="s">
-        <v>2619</v>
-      </c>
-      <c r="D63" t="s">
-        <v>22</v>
-      </c>
-      <c r="E63" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64"/>
-      <c r="B64" t="s">
-        <v>2620</v>
-      </c>
       <c r="C64" t="s">
-        <v>2621</v>
+        <v>2622</v>
       </c>
       <c r="D64" t="s">
         <v>22</v>
@@ -33484,7 +33503,7 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>2622</v>
+        <v>991</v>
       </c>
       <c r="C65" t="s">
         <v>2623</v>
@@ -33493,6 +33512,36 @@
         <v>22</v>
       </c>
       <c r="E65" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66"/>
+      <c r="B66" t="s">
+        <v>2624</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67"/>
+      <c r="B67" t="s">
+        <v>2626</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D67" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" t="s">
         <v>22</v>
       </c>
     </row>
@@ -33566,7 +33615,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2624</v>
+        <v>2628</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>2520</v>
@@ -33588,17 +33637,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2625</v>
+        <v>2629</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>2626</v>
+        <v>2630</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2627</v>
+        <v>2631</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>2628</v>
+        <v>2632</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -33612,14 +33661,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2629</v>
+        <v>2633</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>2630</v>
+        <v>2634</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2631</v>
+        <v>2635</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>22</v>
@@ -33634,12 +33683,12 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2632</v>
+        <v>2636</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2633</v>
+        <v>2637</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>22</v>
@@ -33654,10 +33703,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2634</v>
+        <v>2638</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>2635</v>
+        <v>2639</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
@@ -33676,14 +33725,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2636</v>
+        <v>2640</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2637</v>
+        <v>2641</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>22</v>
@@ -33698,14 +33747,14 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2638</v>
+        <v>2642</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2639</v>
+        <v>2643</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>22</v>
@@ -33720,14 +33769,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2640</v>
+        <v>2644</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>2641</v>
+        <v>2645</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2642</v>
+        <v>2646</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>22</v>
@@ -33786,14 +33835,14 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2643</v>
+        <v>2647</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2644</v>
+        <v>2648</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>22</v>
@@ -33808,7 +33857,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2645</v>
+        <v>2649</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>12</v>
@@ -33818,7 +33867,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>2646</v>
+        <v>2650</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -33832,14 +33881,14 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2647</v>
+        <v>2651</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>691</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>2648</v>
+        <v>2652</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>22</v>
@@ -33861,10 +33910,10 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2649</v>
+        <v>2653</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>2650</v>
+        <v>2654</v>
       </c>
       <c r="F15"/>
       <c r="H15" s="22" t="s">
@@ -33883,10 +33932,10 @@
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2651</v>
+        <v>2655</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>2652</v>
+        <v>2656</v>
       </c>
       <c r="F16"/>
       <c r="H16" s="22" t="s">
@@ -33946,14 +33995,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2653</v>
+        <v>2657</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2654</v>
+        <v>2658</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>22</v>
@@ -33968,14 +34017,14 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2655</v>
+        <v>2659</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>2656</v>
+        <v>2660</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>22</v>
@@ -33990,7 +34039,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>2657</v>
+        <v>2661</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>110</v>
@@ -34022,7 +34071,7 @@
         <v>1158</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>2658</v>
+        <v>2662</v>
       </c>
       <c r="F22"/>
       <c r="H22" s="22" t="s">
@@ -34102,14 +34151,14 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>2659</v>
+        <v>2663</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>2660</v>
+        <v>2664</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>22</v>
@@ -34146,14 +34195,14 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>2661</v>
+        <v>2665</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>2662</v>
+        <v>2666</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>2663</v>
+        <v>2667</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>22</v>
@@ -34168,14 +34217,14 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>2664</v>
+        <v>2668</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>2665</v>
+        <v>2669</v>
       </c>
       <c r="C29"/>
       <c r="D29" t="s">
-        <v>2666</v>
+        <v>2670</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>22</v>
@@ -34190,14 +34239,14 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>2667</v>
+        <v>2671</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C30"/>
       <c r="D30" t="s">
-        <v>2668</v>
+        <v>2672</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>22</v>
@@ -34212,17 +34261,17 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>2669</v>
+        <v>2673</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C31"/>
       <c r="D31" t="s">
-        <v>2670</v>
+        <v>2674</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>2671</v>
+        <v>2675</v>
       </c>
       <c r="F31"/>
       <c r="H31" s="22" t="s">
@@ -34234,17 +34283,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>2672</v>
+        <v>2676</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C32"/>
       <c r="D32" t="s">
-        <v>2673</v>
+        <v>2677</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>2674</v>
+        <v>2678</v>
       </c>
       <c r="F32"/>
       <c r="H32" s="22" t="s">
@@ -34256,17 +34305,17 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>2675</v>
+        <v>2679</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C33"/>
       <c r="D33" t="s">
-        <v>2676</v>
+        <v>2680</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>2677</v>
+        <v>2681</v>
       </c>
       <c r="F33"/>
       <c r="H33" s="22" t="s">
@@ -34278,7 +34327,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>2678</v>
+        <v>2682</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>12</v>
@@ -34288,7 +34337,7 @@
         <v>566</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>2679</v>
+        <v>2683</v>
       </c>
       <c r="F34"/>
       <c r="H34" s="22" t="s">
@@ -34300,17 +34349,17 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>2680</v>
+        <v>2684</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C35"/>
       <c r="D35" t="s">
-        <v>2681</v>
+        <v>2685</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>2682</v>
+        <v>2686</v>
       </c>
       <c r="F35"/>
       <c r="H35" s="22" t="s">
@@ -34322,17 +34371,17 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>2683</v>
+        <v>2687</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C36"/>
       <c r="D36" t="s">
-        <v>2684</v>
+        <v>2688</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>2685</v>
+        <v>2689</v>
       </c>
       <c r="F36"/>
       <c r="H36" s="22" t="s">
@@ -34344,17 +34393,17 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>2686</v>
+        <v>2690</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C37"/>
       <c r="D37" t="s">
-        <v>2687</v>
+        <v>2691</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>2688</v>
+        <v>2692</v>
       </c>
       <c r="F37"/>
       <c r="H37" s="22" t="s">
@@ -34430,7 +34479,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>2689</v>
+        <v>2693</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>666</v>
@@ -34454,14 +34503,14 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>2690</v>
+        <v>2694</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C42"/>
       <c r="D42" t="s">
-        <v>2691</v>
+        <v>2695</v>
       </c>
       <c r="E42" s="22" t="s">
         <v>22</v>
@@ -34542,14 +34591,14 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>2692</v>
+        <v>2696</v>
       </c>
       <c r="B46" s="22" t="s">
         <v>691</v>
       </c>
       <c r="C46"/>
       <c r="D46" t="s">
-        <v>2693</v>
+        <v>2697</v>
       </c>
       <c r="E46" s="22" t="s">
         <v>22</v>
@@ -34564,14 +34613,14 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>2694</v>
+        <v>2698</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>2695</v>
+        <v>2699</v>
       </c>
       <c r="C47"/>
       <c r="D47" t="s">
-        <v>2696</v>
+        <v>2700</v>
       </c>
       <c r="E47" s="22" t="s">
         <v>22</v>
@@ -34586,17 +34635,17 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>2697</v>
+        <v>2701</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>2698</v>
+        <v>2702</v>
       </c>
       <c r="C48"/>
       <c r="D48" t="s">
-        <v>2699</v>
+        <v>2703</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>2700</v>
+        <v>2704</v>
       </c>
       <c r="F48"/>
       <c r="H48" s="22" t="s">
@@ -34610,14 +34659,14 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>2701</v>
+        <v>2705</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>2702</v>
+        <v>2706</v>
       </c>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>2703</v>
+        <v>2707</v>
       </c>
       <c r="E49" s="22" t="s">
         <v>22</v>
@@ -34634,14 +34683,14 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>2704</v>
+        <v>2708</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>2705</v>
+        <v>2709</v>
       </c>
       <c r="C50"/>
       <c r="D50" t="s">
-        <v>2706</v>
+        <v>2710</v>
       </c>
       <c r="E50" s="22" t="s">
         <v>22</v>
@@ -34658,14 +34707,14 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>2707</v>
+        <v>2711</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>2708</v>
+        <v>2712</v>
       </c>
       <c r="C51"/>
       <c r="D51" t="s">
-        <v>2709</v>
+        <v>2713</v>
       </c>
       <c r="E51" s="22" t="s">
         <v>22</v>
@@ -34682,14 +34731,14 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>2710</v>
+        <v>2714</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>691</v>
       </c>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>2711</v>
+        <v>2715</v>
       </c>
       <c r="E52" s="22" t="s">
         <v>22</v>
@@ -34706,7 +34755,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>2712</v>
+        <v>2716</v>
       </c>
       <c r="B53" s="22"/>
       <c r="C53"/>
@@ -34728,14 +34777,14 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>2713</v>
+        <v>2717</v>
       </c>
       <c r="B54" s="22" t="s">
         <v>691</v>
       </c>
       <c r="C54"/>
       <c r="D54" t="s">
-        <v>2714</v>
+        <v>2718</v>
       </c>
       <c r="E54" s="22" t="s">
         <v>22</v>
@@ -34752,7 +34801,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>2715</v>
+        <v>2719</v>
       </c>
       <c r="B55" s="22"/>
       <c r="C55"/>
@@ -34842,14 +34891,14 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>2716</v>
+        <v>2720</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>2717</v>
+        <v>2721</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
-        <v>2718</v>
+        <v>2722</v>
       </c>
       <c r="E59" s="22" t="s">
         <v>22</v>
@@ -34881,13 +34930,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>2626</v>
+        <v>2630</v>
       </c>
       <c r="B62" t="s">
-        <v>2719</v>
+        <v>2723</v>
       </c>
       <c r="C62" t="s">
-        <v>2720</v>
+        <v>2724</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -34899,10 +34948,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>2556</v>
+        <v>2559</v>
       </c>
       <c r="C63" t="s">
-        <v>2557</v>
+        <v>2560</v>
       </c>
       <c r="D63" t="s">
         <v>22</v>
@@ -34929,10 +34978,10 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>2721</v>
+        <v>2725</v>
       </c>
       <c r="C65" t="s">
-        <v>2722</v>
+        <v>2726</v>
       </c>
       <c r="D65" t="s">
         <v>22</v>
@@ -34975,13 +35024,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>2630</v>
+        <v>2634</v>
       </c>
       <c r="B69" t="s">
-        <v>2616</v>
+        <v>2620</v>
       </c>
       <c r="C69" t="s">
-        <v>2723</v>
+        <v>2727</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -34993,10 +35042,10 @@
     <row r="70">
       <c r="A70"/>
       <c r="B70" t="s">
-        <v>2724</v>
+        <v>2728</v>
       </c>
       <c r="C70" t="s">
-        <v>2725</v>
+        <v>2729</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -35008,10 +35057,10 @@
     <row r="71">
       <c r="A71"/>
       <c r="B71" t="s">
-        <v>2612</v>
+        <v>2616</v>
       </c>
       <c r="C71" t="s">
-        <v>2726</v>
+        <v>2730</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
@@ -35054,7 +35103,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>2635</v>
+        <v>2639</v>
       </c>
       <c r="B75" t="s">
         <v>988</v>
@@ -35072,10 +35121,10 @@
     <row r="76">
       <c r="A76"/>
       <c r="B76" t="s">
-        <v>2727</v>
+        <v>2731</v>
       </c>
       <c r="C76" t="s">
-        <v>2728</v>
+        <v>2732</v>
       </c>
       <c r="D76" t="s">
         <v>22</v>
@@ -35133,7 +35182,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>2641</v>
+        <v>2645</v>
       </c>
       <c r="B81" t="s">
         <v>988</v>
@@ -35151,7 +35200,7 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>2727</v>
+        <v>2731</v>
       </c>
       <c r="C82" t="s">
         <v>1106</v>
@@ -35181,10 +35230,10 @@
     <row r="84">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>2729</v>
+        <v>2733</v>
       </c>
       <c r="C84" t="s">
-        <v>2730</v>
+        <v>2734</v>
       </c>
       <c r="D84" t="s">
         <v>22</v>
@@ -35678,13 +35727,13 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>2662</v>
+        <v>2666</v>
       </c>
       <c r="B121" t="s">
-        <v>2731</v>
+        <v>2735</v>
       </c>
       <c r="C121" t="s">
-        <v>2732</v>
+        <v>2736</v>
       </c>
       <c r="D121" t="s">
         <v>22</v>
@@ -35696,10 +35745,10 @@
     <row r="122">
       <c r="A122"/>
       <c r="B122" t="s">
-        <v>2733</v>
+        <v>2737</v>
       </c>
       <c r="C122" t="s">
-        <v>2734</v>
+        <v>2738</v>
       </c>
       <c r="D122" t="s">
         <v>22</v>
@@ -35711,10 +35760,10 @@
     <row r="123">
       <c r="A123"/>
       <c r="B123" t="s">
-        <v>2735</v>
+        <v>2739</v>
       </c>
       <c r="C123" t="s">
-        <v>2736</v>
+        <v>2740</v>
       </c>
       <c r="D123" t="s">
         <v>22</v>
@@ -35726,10 +35775,10 @@
     <row r="124">
       <c r="A124"/>
       <c r="B124" t="s">
-        <v>2737</v>
+        <v>2741</v>
       </c>
       <c r="C124" t="s">
-        <v>2738</v>
+        <v>2742</v>
       </c>
       <c r="D124" t="s">
         <v>22</v>
@@ -35741,10 +35790,10 @@
     <row r="125">
       <c r="A125"/>
       <c r="B125" t="s">
-        <v>2739</v>
+        <v>2743</v>
       </c>
       <c r="C125" t="s">
-        <v>2740</v>
+        <v>2744</v>
       </c>
       <c r="D125" t="s">
         <v>22</v>
@@ -35772,13 +35821,13 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>2665</v>
+        <v>2669</v>
       </c>
       <c r="B128" t="s">
-        <v>2741</v>
+        <v>2745</v>
       </c>
       <c r="C128" t="s">
-        <v>2742</v>
+        <v>2746</v>
       </c>
       <c r="D128" t="s">
         <v>22</v>
@@ -35790,10 +35839,10 @@
     <row r="129">
       <c r="A129"/>
       <c r="B129" t="s">
-        <v>2743</v>
+        <v>2747</v>
       </c>
       <c r="C129" t="s">
-        <v>2744</v>
+        <v>2748</v>
       </c>
       <c r="D129" t="s">
         <v>22</v>
@@ -35805,10 +35854,10 @@
     <row r="130">
       <c r="A130"/>
       <c r="B130" t="s">
-        <v>2745</v>
+        <v>2749</v>
       </c>
       <c r="C130" t="s">
-        <v>2746</v>
+        <v>2750</v>
       </c>
       <c r="D130" t="s">
         <v>22</v>
@@ -35820,10 +35869,10 @@
     <row r="131">
       <c r="A131"/>
       <c r="B131" t="s">
-        <v>2747</v>
+        <v>2751</v>
       </c>
       <c r="C131" t="s">
-        <v>2748</v>
+        <v>2752</v>
       </c>
       <c r="D131" t="s">
         <v>22</v>
@@ -35835,10 +35884,10 @@
     <row r="132">
       <c r="A132"/>
       <c r="B132" t="s">
-        <v>2749</v>
+        <v>2753</v>
       </c>
       <c r="C132" t="s">
-        <v>2750</v>
+        <v>2754</v>
       </c>
       <c r="D132" t="s">
         <v>22</v>
@@ -36740,13 +36789,13 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>2695</v>
+        <v>2699</v>
       </c>
       <c r="B194" t="s">
-        <v>2751</v>
+        <v>2755</v>
       </c>
       <c r="C194" t="s">
-        <v>2752</v>
+        <v>2756</v>
       </c>
       <c r="D194" t="s">
         <v>22</v>
@@ -36761,7 +36810,7 @@
         <v>2354</v>
       </c>
       <c r="C195" t="s">
-        <v>2753</v>
+        <v>2757</v>
       </c>
       <c r="D195" t="s">
         <v>22</v>
@@ -36776,7 +36825,7 @@
         <v>2356</v>
       </c>
       <c r="C196" t="s">
-        <v>2754</v>
+        <v>2758</v>
       </c>
       <c r="D196" t="s">
         <v>22</v>
@@ -36788,10 +36837,10 @@
     <row r="197">
       <c r="A197"/>
       <c r="B197" t="s">
-        <v>2755</v>
+        <v>2759</v>
       </c>
       <c r="C197" t="s">
-        <v>2756</v>
+        <v>2760</v>
       </c>
       <c r="D197" t="s">
         <v>22</v>
@@ -36803,10 +36852,10 @@
     <row r="198">
       <c r="A198"/>
       <c r="B198" t="s">
-        <v>2757</v>
+        <v>2761</v>
       </c>
       <c r="C198" t="s">
-        <v>2758</v>
+        <v>2762</v>
       </c>
       <c r="D198" t="s">
         <v>22</v>
@@ -36849,7 +36898,7 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>2698</v>
+        <v>2702</v>
       </c>
       <c r="B202" t="s">
         <v>941</v>
@@ -36928,13 +36977,13 @@
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>2702</v>
+        <v>2706</v>
       </c>
       <c r="B208" t="s">
-        <v>2759</v>
+        <v>2763</v>
       </c>
       <c r="C208" t="s">
-        <v>2760</v>
+        <v>2764</v>
       </c>
       <c r="D208" t="s">
         <v>22</v>
@@ -36946,10 +36995,10 @@
     <row r="209">
       <c r="A209"/>
       <c r="B209" t="s">
-        <v>2761</v>
+        <v>2765</v>
       </c>
       <c r="C209" t="s">
-        <v>2762</v>
+        <v>2766</v>
       </c>
       <c r="D209" t="s">
         <v>22</v>
@@ -36961,10 +37010,10 @@
     <row r="210">
       <c r="A210"/>
       <c r="B210" t="s">
-        <v>2763</v>
+        <v>2767</v>
       </c>
       <c r="C210" t="s">
-        <v>2764</v>
+        <v>2768</v>
       </c>
       <c r="D210" t="s">
         <v>22</v>
@@ -36976,10 +37025,10 @@
     <row r="211">
       <c r="A211"/>
       <c r="B211" t="s">
-        <v>2765</v>
+        <v>2769</v>
       </c>
       <c r="C211" t="s">
-        <v>2766</v>
+        <v>2770</v>
       </c>
       <c r="D211" t="s">
         <v>22</v>
@@ -36991,10 +37040,10 @@
     <row r="212">
       <c r="A212"/>
       <c r="B212" t="s">
-        <v>2767</v>
+        <v>2771</v>
       </c>
       <c r="C212" t="s">
-        <v>2768</v>
+        <v>2772</v>
       </c>
       <c r="D212" t="s">
         <v>22</v>
@@ -37006,10 +37055,10 @@
     <row r="213">
       <c r="A213"/>
       <c r="B213" t="s">
-        <v>2769</v>
+        <v>2773</v>
       </c>
       <c r="C213" t="s">
-        <v>2770</v>
+        <v>2774</v>
       </c>
       <c r="D213" t="s">
         <v>22</v>
@@ -37052,13 +37101,13 @@
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>2705</v>
+        <v>2709</v>
       </c>
       <c r="B217" t="s">
-        <v>2771</v>
+        <v>2775</v>
       </c>
       <c r="C217" t="s">
-        <v>2772</v>
+        <v>2776</v>
       </c>
       <c r="D217" t="s">
         <v>22</v>
@@ -37070,10 +37119,10 @@
     <row r="218">
       <c r="A218"/>
       <c r="B218" t="s">
-        <v>2773</v>
+        <v>2777</v>
       </c>
       <c r="C218" t="s">
-        <v>2774</v>
+        <v>2778</v>
       </c>
       <c r="D218" t="s">
         <v>22</v>
@@ -37085,10 +37134,10 @@
     <row r="219">
       <c r="A219"/>
       <c r="B219" t="s">
-        <v>2775</v>
+        <v>2779</v>
       </c>
       <c r="C219" t="s">
-        <v>2776</v>
+        <v>2780</v>
       </c>
       <c r="D219" t="s">
         <v>22</v>
@@ -37100,10 +37149,10 @@
     <row r="220">
       <c r="A220"/>
       <c r="B220" t="s">
-        <v>2777</v>
+        <v>2781</v>
       </c>
       <c r="C220" t="s">
-        <v>2778</v>
+        <v>2782</v>
       </c>
       <c r="D220" t="s">
         <v>22</v>
@@ -37115,10 +37164,10 @@
     <row r="221">
       <c r="A221"/>
       <c r="B221" t="s">
-        <v>2779</v>
+        <v>2783</v>
       </c>
       <c r="C221" t="s">
-        <v>2780</v>
+        <v>2784</v>
       </c>
       <c r="D221" t="s">
         <v>22</v>
@@ -37161,13 +37210,13 @@
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>2708</v>
+        <v>2712</v>
       </c>
       <c r="B225" t="s">
-        <v>2781</v>
+        <v>2785</v>
       </c>
       <c r="C225" t="s">
-        <v>2782</v>
+        <v>2786</v>
       </c>
       <c r="D225" t="s">
         <v>22</v>
@@ -37179,10 +37228,10 @@
     <row r="226">
       <c r="A226"/>
       <c r="B226" t="s">
-        <v>2783</v>
+        <v>2787</v>
       </c>
       <c r="C226" t="s">
-        <v>2784</v>
+        <v>2788</v>
       </c>
       <c r="D226" t="s">
         <v>22</v>
@@ -37194,10 +37243,10 @@
     <row r="227">
       <c r="A227"/>
       <c r="B227" t="s">
-        <v>2785</v>
+        <v>2789</v>
       </c>
       <c r="C227" t="s">
-        <v>2786</v>
+        <v>2790</v>
       </c>
       <c r="D227" t="s">
         <v>22</v>
@@ -37209,10 +37258,10 @@
     <row r="228">
       <c r="A228"/>
       <c r="B228" t="s">
-        <v>2787</v>
+        <v>2791</v>
       </c>
       <c r="C228" t="s">
-        <v>2788</v>
+        <v>2792</v>
       </c>
       <c r="D228" t="s">
         <v>22</v>
@@ -37224,10 +37273,10 @@
     <row r="229">
       <c r="A229"/>
       <c r="B229" t="s">
-        <v>2789</v>
+        <v>2793</v>
       </c>
       <c r="C229" t="s">
-        <v>2790</v>
+        <v>2794</v>
       </c>
       <c r="D229" t="s">
         <v>22</v>
@@ -37255,7 +37304,7 @@
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>2717</v>
+        <v>2721</v>
       </c>
       <c r="B232" t="s">
         <v>183</v>
@@ -37273,10 +37322,10 @@
     <row r="233">
       <c r="A233"/>
       <c r="B233" t="s">
-        <v>2791</v>
+        <v>2795</v>
       </c>
       <c r="C233" t="s">
-        <v>2792</v>
+        <v>2796</v>
       </c>
       <c r="D233" t="s">
         <v>22</v>
@@ -37288,10 +37337,10 @@
     <row r="234">
       <c r="A234"/>
       <c r="B234" t="s">
-        <v>2793</v>
+        <v>2797</v>
       </c>
       <c r="C234" t="s">
-        <v>2794</v>
+        <v>2798</v>
       </c>
       <c r="D234" t="s">
         <v>22</v>
@@ -37412,7 +37461,7 @@
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2557</v>
+        <v>2560</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>22</v>
@@ -37453,7 +37502,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2795</v>
+        <v>2799</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>12</v>
@@ -37462,7 +37511,7 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>2796</v>
+        <v>2800</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>22</v>
@@ -37673,14 +37722,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2797</v>
+        <v>2801</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>2798</v>
+        <v>2802</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2799</v>
+        <v>2803</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>22</v>
@@ -37719,14 +37768,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2800</v>
+        <v>2804</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>2801</v>
+        <v>2805</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2802</v>
+        <v>2806</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>22</v>
@@ -37741,14 +37790,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2527</v>
+        <v>2530</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>2803</v>
+        <v>2807</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2529</v>
+        <v>2532</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>22</v>
@@ -37763,7 +37812,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2804</v>
+        <v>2808</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>55</v>
@@ -37787,14 +37836,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2805</v>
+        <v>2809</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>2806</v>
+        <v>2810</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2807</v>
+        <v>2811</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>22</v>
@@ -37809,7 +37858,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2537</v>
+        <v>2540</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>55</v>
@@ -37831,14 +37880,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2541</v>
+        <v>2544</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>666</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2542</v>
+        <v>2545</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>22</v>
@@ -37853,14 +37902,14 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2808</v>
+        <v>2812</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>2644</v>
+        <v>2648</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>22</v>
@@ -37897,14 +37946,14 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2809</v>
+        <v>2813</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>2548</v>
+        <v>2551</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>22</v>
@@ -37919,14 +37968,14 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2810</v>
+        <v>2814</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>666</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>2811</v>
+        <v>2815</v>
       </c>
       <c r="E13" s="24" t="s">
         <v>22</v>
@@ -37958,13 +38007,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2798</v>
+        <v>2802</v>
       </c>
       <c r="B16" t="s">
-        <v>2556</v>
+        <v>2559</v>
       </c>
       <c r="C16" t="s">
-        <v>2557</v>
+        <v>2560</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -37992,13 +38041,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2801</v>
+        <v>2805</v>
       </c>
       <c r="B19" t="s">
-        <v>2812</v>
+        <v>2816</v>
       </c>
       <c r="C19" t="s">
-        <v>2813</v>
+        <v>2817</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -38010,10 +38059,10 @@
     <row r="20">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>2575</v>
+        <v>2579</v>
       </c>
       <c r="C20" t="s">
-        <v>2814</v>
+        <v>2818</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -38025,10 +38074,10 @@
     <row r="21">
       <c r="A21"/>
       <c r="B21" t="s">
-        <v>2815</v>
+        <v>2819</v>
       </c>
       <c r="C21" t="s">
-        <v>2816</v>
+        <v>2820</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -38040,10 +38089,10 @@
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>2579</v>
+        <v>2583</v>
       </c>
       <c r="C22" t="s">
-        <v>2817</v>
+        <v>2821</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -38055,10 +38104,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>2818</v>
+        <v>2822</v>
       </c>
       <c r="C23" t="s">
-        <v>2819</v>
+        <v>2823</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -38070,10 +38119,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>2820</v>
+        <v>2824</v>
       </c>
       <c r="C24" t="s">
-        <v>2821</v>
+        <v>2825</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -38085,10 +38134,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>2822</v>
+        <v>2826</v>
       </c>
       <c r="C25" t="s">
-        <v>2823</v>
+        <v>2827</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -38100,10 +38149,10 @@
     <row r="26">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>2824</v>
+        <v>2828</v>
       </c>
       <c r="C26" t="s">
-        <v>2825</v>
+        <v>2829</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
@@ -38115,10 +38164,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>2826</v>
+        <v>2830</v>
       </c>
       <c r="C27" t="s">
-        <v>2827</v>
+        <v>2831</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
@@ -38161,13 +38210,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>2803</v>
+        <v>2807</v>
       </c>
       <c r="B31" t="s">
-        <v>2612</v>
+        <v>2616</v>
       </c>
       <c r="C31" t="s">
-        <v>2613</v>
+        <v>2617</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
@@ -38179,10 +38228,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>2614</v>
+        <v>2618</v>
       </c>
       <c r="C32" t="s">
-        <v>2615</v>
+        <v>2619</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
@@ -38194,10 +38243,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>2616</v>
+        <v>2620</v>
       </c>
       <c r="C33" t="s">
-        <v>2617</v>
+        <v>2621</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -38225,7 +38274,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>2806</v>
+        <v>2810</v>
       </c>
       <c r="B36" t="s">
         <v>988</v>
@@ -38243,10 +38292,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>2828</v>
+        <v>2832</v>
       </c>
       <c r="C37" t="s">
-        <v>2829</v>
+        <v>2833</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -38347,7 +38396,7 @@
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2830</v>
+        <v>2834</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>22</v>
@@ -38408,7 +38457,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>134</v>
@@ -38430,7 +38479,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2832</v>
+        <v>2836</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>134</v>
@@ -38584,7 +38633,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2833</v>
+        <v>2837</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>58</v>
@@ -38606,7 +38655,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2834</v>
+        <v>2838</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>62</v>
@@ -38659,7 +38708,7 @@
         <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>2835</v>
+        <v>2839</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>22</v>
@@ -38718,7 +38767,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2836</v>
+        <v>2840</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>134</v>
@@ -38740,7 +38789,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2837</v>
+        <v>2841</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>134</v>
@@ -38762,14 +38811,14 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>2838</v>
+        <v>2842</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>134</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>2839</v>
+        <v>2843</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>22</v>
@@ -38784,10 +38833,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>2840</v>
+        <v>2844</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>2841</v>
+        <v>2845</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
@@ -40317,14 +40366,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2842</v>
+        <v>2846</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2843</v>
+        <v>2847</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>22</v>
@@ -40361,14 +40410,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>134</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>22</v>
@@ -40447,14 +40496,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2842</v>
+        <v>2846</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2843</v>
+        <v>2847</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>22</v>
@@ -40491,14 +40540,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>134</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>22</v>
@@ -40520,7 +40569,7 @@
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2845</v>
+        <v>2849</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>22</v>
@@ -40599,14 +40648,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2842</v>
+        <v>2846</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2843</v>
+        <v>2847</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>22</v>
@@ -40643,14 +40692,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2846</v>
+        <v>2850</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2847</v>
+        <v>2851</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>22</v>
@@ -40665,14 +40714,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2848</v>
+        <v>2852</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2849</v>
+        <v>2853</v>
       </c>
       <c r="E5" s="28" t="s">
         <v>22</v>
@@ -40687,14 +40736,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>134</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>22</v>
@@ -40795,14 +40844,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2850</v>
+        <v>2854</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2851</v>
+        <v>2855</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>22</v>
@@ -40817,14 +40866,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2852</v>
+        <v>2856</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2853</v>
+        <v>2857</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>22</v>
@@ -40839,14 +40888,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2854</v>
+        <v>2858</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>42</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2855</v>
+        <v>2859</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>22</v>
@@ -40861,14 +40910,14 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>134</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>22</v>
@@ -40905,14 +40954,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2856</v>
+        <v>2860</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>2857</v>
+        <v>2861</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2858</v>
+        <v>2862</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>22</v>
@@ -42816,14 +42865,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2850</v>
+        <v>2854</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2851</v>
+        <v>2855</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>22</v>
@@ -42838,14 +42887,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2852</v>
+        <v>2856</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2853</v>
+        <v>2857</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>22</v>
@@ -42860,14 +42909,14 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2854</v>
+        <v>2858</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>2855</v>
+        <v>2859</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>22</v>
@@ -42904,14 +42953,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>134</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>22</v>
@@ -43012,14 +43061,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2850</v>
+        <v>2854</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2851</v>
+        <v>2855</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>22</v>
@@ -43034,7 +43083,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2854</v>
+        <v>2858</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>42</v>
@@ -43100,14 +43149,14 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>134</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>22</v>
@@ -43208,14 +43257,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2850</v>
+        <v>2854</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>12</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2851</v>
+        <v>2855</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>22</v>
@@ -43523,7 +43572,7 @@
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2859</v>
+        <v>2863</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>22</v>
@@ -43545,7 +43594,7 @@
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>2860</v>
+        <v>2864</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>22</v>
@@ -43560,7 +43609,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2861</v>
+        <v>2865</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>69</v>
@@ -43582,14 +43631,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2862</v>
+        <v>2866</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>134</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2863</v>
+        <v>2867</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>22</v>
@@ -43604,14 +43653,14 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>134</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>22</v>
@@ -44697,14 +44746,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2864</v>
+        <v>2868</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>2865</v>
+        <v>2869</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2866</v>
+        <v>2870</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>22</v>
@@ -44719,14 +44768,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2850</v>
+        <v>2854</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2851</v>
+        <v>2855</v>
       </c>
       <c r="E3" s="33" t="s">
         <v>22</v>
@@ -44792,7 +44841,7 @@
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>2859</v>
+        <v>2863</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>22</v>
@@ -44814,7 +44863,7 @@
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2860</v>
+        <v>2864</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>22</v>
@@ -44829,14 +44878,14 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2867</v>
+        <v>2871</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>134</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2868</v>
+        <v>2872</v>
       </c>
       <c r="E8" s="33" t="s">
         <v>22</v>
@@ -44851,14 +44900,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2831</v>
+        <v>2835</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>134</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>22</v>
@@ -44912,13 +44961,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2865</v>
+        <v>2869</v>
       </c>
       <c r="B13" t="s">
-        <v>2869</v>
+        <v>2873</v>
       </c>
       <c r="C13" t="s">
-        <v>2870</v>
+        <v>2874</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -44930,10 +44979,10 @@
     <row r="14">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>2871</v>
+        <v>2875</v>
       </c>
       <c r="C14" t="s">
-        <v>2872</v>
+        <v>2876</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -44945,10 +44994,10 @@
     <row r="15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>2873</v>
+        <v>2877</v>
       </c>
       <c r="C15" t="s">
-        <v>2874</v>
+        <v>2878</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -45039,14 +45088,14 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2867</v>
+        <v>2871</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>134</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>2868</v>
+        <v>2872</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>22</v>
@@ -45061,14 +45110,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2875</v>
+        <v>2879</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>2876</v>
+        <v>2880</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>22</v>
@@ -45127,7 +45176,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2877</v>
+        <v>2881</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>12</v>
@@ -45149,14 +45198,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2878</v>
+        <v>2882</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>2879</v>
+        <v>2883</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>22</v>
@@ -45178,7 +45227,7 @@
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>2880</v>
+        <v>2884</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>22</v>
@@ -45193,14 +45242,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2881</v>
+        <v>2885</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>2882</v>
+        <v>2886</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>2883</v>
+        <v>2887</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>22</v>
@@ -45303,7 +45352,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2884</v>
+        <v>2888</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>72</v>
@@ -45332,7 +45381,7 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>2885</v>
+        <v>2889</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>22</v>
@@ -45347,14 +45396,14 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2886</v>
+        <v>2890</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>666</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>2887</v>
+        <v>2891</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>22</v>
@@ -45369,17 +45418,17 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>2888</v>
+        <v>2892</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>91</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>2889</v>
+        <v>2893</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>2890</v>
+        <v>2894</v>
       </c>
       <c r="F17"/>
       <c r="H17" s="34" t="s">
@@ -45391,10 +45440,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2891</v>
+        <v>2895</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>2892</v>
+        <v>2896</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
@@ -45413,14 +45462,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2893</v>
+        <v>2897</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>134</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>2894</v>
+        <v>2898</v>
       </c>
       <c r="E19" s="34" t="s">
         <v>22</v>
@@ -46363,13 +46412,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>2892</v>
+        <v>2896</v>
       </c>
       <c r="B85" t="s">
-        <v>2895</v>
+        <v>2899</v>
       </c>
       <c r="C85" t="s">
-        <v>2896</v>
+        <v>2900</v>
       </c>
       <c r="D85" t="s">
         <v>22</v>
@@ -46381,10 +46430,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>2897</v>
+        <v>2901</v>
       </c>
       <c r="C86" t="s">
-        <v>2898</v>
+        <v>2902</v>
       </c>
       <c r="D86" t="s">
         <v>22</v>
@@ -46396,10 +46445,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>2899</v>
+        <v>2903</v>
       </c>
       <c r="C87" t="s">
-        <v>2900</v>
+        <v>2904</v>
       </c>
       <c r="D87" t="s">
         <v>22</v>
@@ -46411,10 +46460,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>2901</v>
+        <v>2905</v>
       </c>
       <c r="C88" t="s">
-        <v>2902</v>
+        <v>2906</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -46426,10 +46475,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>2903</v>
+        <v>2907</v>
       </c>
       <c r="C89" t="s">
-        <v>2904</v>
+        <v>2908</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -46441,10 +46490,10 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>2905</v>
+        <v>2909</v>
       </c>
       <c r="C90" t="s">
-        <v>2906</v>
+        <v>2910</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -46456,10 +46505,10 @@
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>2907</v>
+        <v>2911</v>
       </c>
       <c r="C91" t="s">
-        <v>2908</v>
+        <v>2912</v>
       </c>
       <c r="D91" t="s">
         <v>22</v>
@@ -46471,10 +46520,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>2909</v>
+        <v>2913</v>
       </c>
       <c r="C92" t="s">
-        <v>2910</v>
+        <v>2914</v>
       </c>
       <c r="D92" t="s">
         <v>22</v>
@@ -46486,10 +46535,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>2911</v>
+        <v>2915</v>
       </c>
       <c r="C93" t="s">
-        <v>2912</v>
+        <v>2916</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -46501,10 +46550,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>2913</v>
+        <v>2917</v>
       </c>
       <c r="C94" t="s">
-        <v>2914</v>
+        <v>2918</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -46516,10 +46565,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>2915</v>
+        <v>2919</v>
       </c>
       <c r="C95" t="s">
-        <v>2916</v>
+        <v>2920</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -46531,10 +46580,10 @@
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
-        <v>2917</v>
+        <v>2921</v>
       </c>
       <c r="C96" t="s">
-        <v>2918</v>
+        <v>2922</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -46546,10 +46595,10 @@
     <row r="97">
       <c r="A97"/>
       <c r="B97" t="s">
-        <v>2919</v>
+        <v>2923</v>
       </c>
       <c r="C97" t="s">
-        <v>2920</v>
+        <v>2924</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
@@ -46561,10 +46610,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>2921</v>
+        <v>2925</v>
       </c>
       <c r="C98" t="s">
-        <v>2922</v>
+        <v>2926</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -46576,10 +46625,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>2923</v>
+        <v>2927</v>
       </c>
       <c r="C99" t="s">
-        <v>2924</v>
+        <v>2928</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -46591,10 +46640,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>2925</v>
+        <v>2929</v>
       </c>
       <c r="C100" t="s">
-        <v>2926</v>
+        <v>2930</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
@@ -46624,12 +46673,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2927</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2928</v>
+        <v>2932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#7680 Updated how field id is generated
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -4408,7 +4408,7 @@
     <t>Stay in a Medical Institution</t>
   </si>
   <si>
-    <t>CaseHospitalization.admittedToHealthFacility</t>
+    <t>Hospitalization.admittedToHealthFacility</t>
   </si>
   <si>
     <t>admittedToHealthFacility</t>
@@ -4417,7 +4417,7 @@
     <t>Was patient admitted at the facility as an inpatient?</t>
   </si>
   <si>
-    <t>CaseHospitalization.admissionDate</t>
+    <t>Hospitalization.admissionDate</t>
   </si>
   <si>
     <t>admissionDate</t>
@@ -4429,7 +4429,7 @@
     <t>Please provide the date of admission to the hospital</t>
   </si>
   <si>
-    <t>CaseHospitalization.dischargeDate</t>
+    <t>Hospitalization.dischargeDate</t>
   </si>
   <si>
     <t>dischargeDate</t>
@@ -4438,7 +4438,7 @@
     <t>Date of discharge or transfer</t>
   </si>
   <si>
-    <t>CaseHospitalization.isolated</t>
+    <t>Hospitalization.isolated</t>
   </si>
   <si>
     <t>isolated</t>
@@ -4450,7 +4450,7 @@
     <t>Is the person in isolation or currently being placed there?</t>
   </si>
   <si>
-    <t>CaseHospitalization.isolationDate</t>
+    <t>Hospitalization.isolationDate</t>
   </si>
   <si>
     <t>isolationDate</t>
@@ -4459,7 +4459,7 @@
     <t>Date of isolation</t>
   </si>
   <si>
-    <t>CaseHospitalization.leftAgainstAdvice</t>
+    <t>Hospitalization.leftAgainstAdvice</t>
   </si>
   <si>
     <t>leftAgainstAdvice</t>
@@ -4468,7 +4468,7 @@
     <t>Left against medical advice</t>
   </si>
   <si>
-    <t>CaseHospitalization.hospitalizedPreviously</t>
+    <t>Hospitalization.hospitalizedPreviously</t>
   </si>
   <si>
     <t>hospitalizedPreviously</t>
@@ -4477,7 +4477,7 @@
     <t>Was the patient hospitalized or did he/she visit a health clinic previously for this illness?</t>
   </si>
   <si>
-    <t>CaseHospitalization.previousHospitalizations</t>
+    <t>Hospitalization.previousHospitalizations</t>
   </si>
   <si>
     <t>previousHospitalizations</t>
@@ -4489,7 +4489,7 @@
     <t>Previous hospitalizations</t>
   </si>
   <si>
-    <t>CaseHospitalization.intensiveCareUnit</t>
+    <t>Hospitalization.intensiveCareUnit</t>
   </si>
   <si>
     <t>intensiveCareUnit</t>
@@ -4498,7 +4498,7 @@
     <t>Stay in the intensive care unit</t>
   </si>
   <si>
-    <t>CaseHospitalization.intensiveCareUnitStart</t>
+    <t>Hospitalization.intensiveCareUnitStart</t>
   </si>
   <si>
     <t>intensiveCareUnitStart</t>
@@ -4507,7 +4507,7 @@
     <t>Start of the stay</t>
   </si>
   <si>
-    <t>CaseHospitalization.intensiveCareUnitEnd</t>
+    <t>Hospitalization.intensiveCareUnitEnd</t>
   </si>
   <si>
     <t>intensiveCareUnitEnd</t>
@@ -4516,7 +4516,7 @@
     <t>End of the stay</t>
   </si>
   <si>
-    <t>CaseHospitalization.hospitalizationReason</t>
+    <t>Hospitalization.hospitalizationReason</t>
   </si>
   <si>
     <t>hospitalizationReason</t>
@@ -4528,7 +4528,7 @@
     <t>Reason for hospitalization</t>
   </si>
   <si>
-    <t>CaseHospitalization.otherHospitalizationReason</t>
+    <t>Hospitalization.otherHospitalizationReason</t>
   </si>
   <si>
     <t>otherHospitalizationReason</t>
@@ -4537,7 +4537,7 @@
     <t>Specify reason</t>
   </si>
   <si>
-    <t>CaseHospitalization.description</t>
+    <t>Hospitalization.description</t>
   </si>
   <si>
     <t>REPORTED_DISEASE</t>
@@ -4546,61 +4546,61 @@
     <t>Reported disease</t>
   </si>
   <si>
-    <t>CasePreviousHospitalization.admittedToHealthFacility</t>
+    <t>PreviousHospitalization.admittedToHealthFacility</t>
   </si>
   <si>
     <t xml:space="preserve">Was patient admitted at the facility as an inpatient? </t>
   </si>
   <si>
-    <t>CasePreviousHospitalization.admissionDate</t>
+    <t>PreviousHospitalization.admissionDate</t>
   </si>
   <si>
     <t>Date of admission</t>
   </si>
   <si>
-    <t>CasePreviousHospitalization.dischargeDate</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.region</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.district</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.community</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.healthFacility</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.healthFacilityDetails</t>
+    <t>PreviousHospitalization.dischargeDate</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.region</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.district</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.community</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.healthFacility</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.healthFacilityDetails</t>
   </si>
   <si>
     <t>Hospital name &amp; description</t>
   </si>
   <si>
-    <t>CasePreviousHospitalization.isolated</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.isolationDate</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.description</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.hospitalizationReason</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.otherHospitalizationReason</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.intensiveCareUnit</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.intensiveCareUnitStart</t>
-  </si>
-  <si>
-    <t>CasePreviousHospitalization.intensiveCareUnitEnd</t>
+    <t>PreviousHospitalization.isolated</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.isolationDate</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.description</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.hospitalizationReason</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.otherHospitalizationReason</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.intensiveCareUnit</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.intensiveCareUnitStart</t>
+  </si>
+  <si>
+    <t>PreviousHospitalization.intensiveCareUnitEnd</t>
   </si>
   <si>
     <t>SurveillanceReport.reportingType</t>
@@ -12244,7 +12244,7 @@
     <t>Unclear</t>
   </si>
   <si>
-    <t>TestResult.labMessage</t>
+    <t>TestReport.labMessage</t>
   </si>
   <si>
     <t>labMessage</t>
@@ -12253,55 +12253,55 @@
     <t>LabMessageReference</t>
   </si>
   <si>
-    <t>TestResult.testLabName</t>
+    <t>TestReport.testLabName</t>
   </si>
   <si>
     <t>testLabName</t>
   </si>
   <si>
-    <t>TestResult.testLabExternalId</t>
+    <t>TestReport.testLabExternalId</t>
   </si>
   <si>
     <t>testLabExternalId</t>
   </si>
   <si>
-    <t>TestResult.testLabPostalCode</t>
+    <t>TestReport.testLabPostalCode</t>
   </si>
   <si>
     <t>testLabPostalCode</t>
   </si>
   <si>
-    <t>TestResult.testLabCity</t>
+    <t>TestReport.testLabCity</t>
   </si>
   <si>
     <t>testLabCity</t>
   </si>
   <si>
-    <t>TestResult.testType</t>
-  </si>
-  <si>
-    <t>TestResult.testDateTime</t>
-  </si>
-  <si>
-    <t>TestResult.testResult</t>
-  </si>
-  <si>
-    <t>TestResult.testResultVerified</t>
-  </si>
-  <si>
-    <t>TestResult.testResultText</t>
-  </si>
-  <si>
-    <t>TestResult.typingId</t>
-  </si>
-  <si>
-    <t>TestResult.externalId</t>
-  </si>
-  <si>
-    <t>TestResult.externalOrderId</t>
-  </si>
-  <si>
-    <t>TestResult.preliminary</t>
+    <t>TestReport.testType</t>
+  </si>
+  <si>
+    <t>TestReport.testDateTime</t>
+  </si>
+  <si>
+    <t>TestReport.testResult</t>
+  </si>
+  <si>
+    <t>TestReport.testResultVerified</t>
+  </si>
+  <si>
+    <t>TestReport.testResultText</t>
+  </si>
+  <si>
+    <t>TestReport.typingId</t>
+  </si>
+  <si>
+    <t>TestReport.externalId</t>
+  </si>
+  <si>
+    <t>TestReport.externalOrderId</t>
+  </si>
+  <si>
+    <t>TestReport.preliminary</t>
   </si>
   <si>
     <t>SORMAS Version</t>

</xml_diff>

<commit_message>
[#7813] do not inject
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15777" uniqueCount="4093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15783" uniqueCount="4095">
   <si>
     <t>Field ID</t>
   </si>
@@ -12323,6 +12323,12 @@
   </si>
   <si>
     <t>TestReport.preliminary</t>
+  </si>
+  <si>
+    <t>TestReport.testPcrTestSpecification</t>
+  </si>
+  <si>
+    <t>testPcrTestSpecification</t>
   </si>
   <si>
     <t>SORMAS Version</t>
@@ -14293,7 +14299,7 @@
 </file>
 
 <file path=xl/tables/table204.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="204" name="TestReport" displayName="TestReport" ref="A1:L18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="204" name="TestReport" displayName="TestReport" ref="A1:L19">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14314,7 +14320,7 @@
 </file>
 
 <file path=xl/tables/table205.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="205" name="TestReportPathogenTestType" displayName="TestReportPathogenTestType" ref="A20:E41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="205" name="TestReportPathogenTestType" displayName="TestReportPathogenTestType" ref="A21:E42">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14328,7 +14334,7 @@
 </file>
 
 <file path=xl/tables/table206.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="206" name="TestReportPCRTestSpecification" displayName="TestReportPCRTestSpecification" ref="A43:E45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="206" name="TestReportPCRTestSpecification" displayName="TestReportPCRTestSpecification" ref="A44:E46">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14342,7 +14348,7 @@
 </file>
 
 <file path=xl/tables/table207.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="207" name="TestReportPathogenTestResultType" displayName="TestReportPathogenTestResultType" ref="A47:E52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="207" name="TestReportPathogenTestResultType" displayName="TestReportPathogenTestResultType" ref="A48:E53">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -59786,7 +59792,7 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -60288,47 +60294,58 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>213</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>223</v>
-      </c>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>4091</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4092</v>
+      </c>
+      <c r="C19" t="s" s="38">
+        <v>3048</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s" s="38">
+        <v>27</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19" t="s" s="38">
+        <v>19</v>
+      </c>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
         <v>3043</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>3098</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>3099</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22"/>
-      <c r="B22" t="s">
-        <v>3100</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3101</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -60340,10 +60357,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>3102</v>
+        <v>3100</v>
       </c>
       <c r="C23" t="s">
-        <v>3103</v>
+        <v>3101</v>
       </c>
       <c r="D23" t="s">
         <v>27</v>
@@ -60355,10 +60372,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>3104</v>
+        <v>3102</v>
       </c>
       <c r="C24" t="s">
-        <v>3105</v>
+        <v>3103</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
@@ -60370,10 +60387,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="C25" t="s">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -60385,10 +60402,10 @@
     <row r="26">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>1501</v>
+        <v>3106</v>
       </c>
       <c r="C26" t="s">
-        <v>1467</v>
+        <v>3107</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>
@@ -60400,10 +60417,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>3108</v>
+        <v>1501</v>
       </c>
       <c r="C27" t="s">
-        <v>3109</v>
+        <v>1467</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
@@ -60415,10 +60432,10 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>3110</v>
+        <v>3108</v>
       </c>
       <c r="C28" t="s">
-        <v>3111</v>
+        <v>3109</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -60430,10 +60447,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="C29" t="s">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
@@ -60445,10 +60462,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>3114</v>
+        <v>3112</v>
       </c>
       <c r="C30" t="s">
-        <v>3115</v>
+        <v>3113</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
@@ -60460,10 +60477,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>3116</v>
+        <v>3114</v>
       </c>
       <c r="C31" t="s">
-        <v>3117</v>
+        <v>3115</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
@@ -60475,10 +60492,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
       <c r="C32" t="s">
-        <v>3119</v>
+        <v>3117</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -60490,10 +60507,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>3120</v>
+        <v>3118</v>
       </c>
       <c r="C33" t="s">
-        <v>3121</v>
+        <v>3119</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -60505,10 +60522,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>3122</v>
+        <v>3120</v>
       </c>
       <c r="C34" t="s">
-        <v>3123</v>
+        <v>3121</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -60520,10 +60537,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>3124</v>
+        <v>3122</v>
       </c>
       <c r="C35" t="s">
-        <v>3125</v>
+        <v>3123</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
@@ -60535,10 +60552,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>3126</v>
+        <v>3124</v>
       </c>
       <c r="C36" t="s">
-        <v>3127</v>
+        <v>3125</v>
       </c>
       <c r="D36" t="s">
         <v>27</v>
@@ -60550,10 +60567,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>3128</v>
+        <v>3126</v>
       </c>
       <c r="C37" t="s">
-        <v>3129</v>
+        <v>3127</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -60565,10 +60582,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>3130</v>
+        <v>3128</v>
       </c>
       <c r="C38" t="s">
-        <v>3131</v>
+        <v>3129</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
@@ -60580,10 +60597,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>3132</v>
+        <v>3130</v>
       </c>
       <c r="C39" t="s">
-        <v>3133</v>
+        <v>3131</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -60595,10 +60612,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>3134</v>
+        <v>3132</v>
       </c>
       <c r="C40" t="s">
-        <v>3135</v>
+        <v>3133</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
@@ -60610,108 +60627,108 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3135</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42"/>
+      <c r="B42" t="s">
         <v>234</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>235</v>
       </c>
-      <c r="D41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" t="s">
-        <v>213</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" t="s">
-        <v>223</v>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>213</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
         <v>3048</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>3136</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>3137</v>
       </c>
-      <c r="D44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45"/>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46" t="s">
         <v>3138</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>3139</v>
       </c>
-      <c r="D45" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
-        <v>213</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" t="s">
-        <v>223</v>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
         <v>2906</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>2995</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>2996</v>
-      </c>
-      <c r="D48" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49"/>
-      <c r="B49" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1182</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -60723,10 +60740,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>2997</v>
+        <v>1180</v>
       </c>
       <c r="C50" t="s">
-        <v>2998</v>
+        <v>1182</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
@@ -60738,10 +60755,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>2999</v>
+        <v>2997</v>
       </c>
       <c r="C51" t="s">
-        <v>3000</v>
+        <v>2998</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
@@ -60753,15 +60770,30 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
+        <v>2999</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3000</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+      <c r="B53" t="s">
         <v>3001</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>3002</v>
       </c>
-      <c r="D52" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" t="s">
         <v>27</v>
       </c>
     </row>
@@ -60786,12 +60818,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4091</v>
+        <v>4093</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4092</v>
+        <v>4094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#7813] cache current user (#7821)
* [#7813] remove config face from cache

* [#7813] do not inject
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15777" uniqueCount="4093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15783" uniqueCount="4095">
   <si>
     <t>Field ID</t>
   </si>
@@ -12323,6 +12323,12 @@
   </si>
   <si>
     <t>TestReport.preliminary</t>
+  </si>
+  <si>
+    <t>TestReport.testPcrTestSpecification</t>
+  </si>
+  <si>
+    <t>testPcrTestSpecification</t>
   </si>
   <si>
     <t>SORMAS Version</t>
@@ -14293,7 +14299,7 @@
 </file>
 
 <file path=xl/tables/table204.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="204" name="TestReport" displayName="TestReport" ref="A1:L18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="204" name="TestReport" displayName="TestReport" ref="A1:L19">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14314,7 +14320,7 @@
 </file>
 
 <file path=xl/tables/table205.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="205" name="TestReportPathogenTestType" displayName="TestReportPathogenTestType" ref="A20:E41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="205" name="TestReportPathogenTestType" displayName="TestReportPathogenTestType" ref="A21:E42">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14328,7 +14334,7 @@
 </file>
 
 <file path=xl/tables/table206.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="206" name="TestReportPCRTestSpecification" displayName="TestReportPCRTestSpecification" ref="A43:E45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="206" name="TestReportPCRTestSpecification" displayName="TestReportPCRTestSpecification" ref="A44:E46">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14342,7 +14348,7 @@
 </file>
 
 <file path=xl/tables/table207.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="207" name="TestReportPathogenTestResultType" displayName="TestReportPathogenTestResultType" ref="A47:E52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="207" name="TestReportPathogenTestResultType" displayName="TestReportPathogenTestResultType" ref="A48:E53">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -59786,7 +59792,7 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -60288,47 +60294,58 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>213</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>223</v>
-      </c>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>4091</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4092</v>
+      </c>
+      <c r="C19" t="s" s="38">
+        <v>3048</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s" s="38">
+        <v>27</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19" t="s" s="38">
+        <v>19</v>
+      </c>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
         <v>3043</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>3098</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>3099</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22"/>
-      <c r="B22" t="s">
-        <v>3100</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3101</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -60340,10 +60357,10 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>3102</v>
+        <v>3100</v>
       </c>
       <c r="C23" t="s">
-        <v>3103</v>
+        <v>3101</v>
       </c>
       <c r="D23" t="s">
         <v>27</v>
@@ -60355,10 +60372,10 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>3104</v>
+        <v>3102</v>
       </c>
       <c r="C24" t="s">
-        <v>3105</v>
+        <v>3103</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
@@ -60370,10 +60387,10 @@
     <row r="25">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="C25" t="s">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -60385,10 +60402,10 @@
     <row r="26">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>1501</v>
+        <v>3106</v>
       </c>
       <c r="C26" t="s">
-        <v>1467</v>
+        <v>3107</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>
@@ -60400,10 +60417,10 @@
     <row r="27">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>3108</v>
+        <v>1501</v>
       </c>
       <c r="C27" t="s">
-        <v>3109</v>
+        <v>1467</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
@@ -60415,10 +60432,10 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>3110</v>
+        <v>3108</v>
       </c>
       <c r="C28" t="s">
-        <v>3111</v>
+        <v>3109</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -60430,10 +60447,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="C29" t="s">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
@@ -60445,10 +60462,10 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>3114</v>
+        <v>3112</v>
       </c>
       <c r="C30" t="s">
-        <v>3115</v>
+        <v>3113</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
@@ -60460,10 +60477,10 @@
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>3116</v>
+        <v>3114</v>
       </c>
       <c r="C31" t="s">
-        <v>3117</v>
+        <v>3115</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
@@ -60475,10 +60492,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
       <c r="C32" t="s">
-        <v>3119</v>
+        <v>3117</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -60490,10 +60507,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>3120</v>
+        <v>3118</v>
       </c>
       <c r="C33" t="s">
-        <v>3121</v>
+        <v>3119</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -60505,10 +60522,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>3122</v>
+        <v>3120</v>
       </c>
       <c r="C34" t="s">
-        <v>3123</v>
+        <v>3121</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -60520,10 +60537,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>3124</v>
+        <v>3122</v>
       </c>
       <c r="C35" t="s">
-        <v>3125</v>
+        <v>3123</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
@@ -60535,10 +60552,10 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>3126</v>
+        <v>3124</v>
       </c>
       <c r="C36" t="s">
-        <v>3127</v>
+        <v>3125</v>
       </c>
       <c r="D36" t="s">
         <v>27</v>
@@ -60550,10 +60567,10 @@
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>3128</v>
+        <v>3126</v>
       </c>
       <c r="C37" t="s">
-        <v>3129</v>
+        <v>3127</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -60565,10 +60582,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>3130</v>
+        <v>3128</v>
       </c>
       <c r="C38" t="s">
-        <v>3131</v>
+        <v>3129</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
@@ -60580,10 +60597,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>3132</v>
+        <v>3130</v>
       </c>
       <c r="C39" t="s">
-        <v>3133</v>
+        <v>3131</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -60595,10 +60612,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>3134</v>
+        <v>3132</v>
       </c>
       <c r="C40" t="s">
-        <v>3135</v>
+        <v>3133</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
@@ -60610,108 +60627,108 @@
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3135</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42"/>
+      <c r="B42" t="s">
         <v>234</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>235</v>
       </c>
-      <c r="D41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" t="s">
-        <v>213</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" t="s">
-        <v>223</v>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>213</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
         <v>3048</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>3136</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>3137</v>
       </c>
-      <c r="D44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45"/>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46" t="s">
         <v>3138</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>3139</v>
       </c>
-      <c r="D45" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
-        <v>213</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" t="s">
-        <v>223</v>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
         <v>2906</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>2995</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>2996</v>
-      </c>
-      <c r="D48" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49"/>
-      <c r="B49" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1182</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -60723,10 +60740,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>2997</v>
+        <v>1180</v>
       </c>
       <c r="C50" t="s">
-        <v>2998</v>
+        <v>1182</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
@@ -60738,10 +60755,10 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>2999</v>
+        <v>2997</v>
       </c>
       <c r="C51" t="s">
-        <v>3000</v>
+        <v>2998</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
@@ -60753,15 +60770,30 @@
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
+        <v>2999</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3000</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+      <c r="B53" t="s">
         <v>3001</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>3002</v>
       </c>
-      <c r="D52" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" t="s">
         <v>27</v>
       </c>
     </row>
@@ -60786,12 +60818,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4091</v>
+        <v>4093</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4092</v>
+        <v>4094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#4461: fixed review findings
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16601" uniqueCount="4310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16535" uniqueCount="4240">
   <si>
     <t>Field ID</t>
   </si>
@@ -12259,7 +12259,7 @@
     <t>userRoles</t>
   </si>
   <si>
-    <t>List of UserRole</t>
+    <t>List of UserRoleReference</t>
   </si>
   <si>
     <t>User roles</t>
@@ -12325,241 +12325,13 @@
     <t>hasConsentedToGdpr</t>
   </si>
   <si>
-    <t>UserRole</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>NATIONAL_USER</t>
-  </si>
-  <si>
-    <t>National User</t>
-  </si>
-  <si>
-    <t>NatUser</t>
-  </si>
-  <si>
-    <t>SURVEILLANCE_SUPERVISOR</t>
-  </si>
-  <si>
-    <t>Surveillance Supervisor</t>
-  </si>
-  <si>
-    <t>SurvSup</t>
-  </si>
-  <si>
-    <t>ADMIN_SUPERVISOR</t>
-  </si>
-  <si>
-    <t>Admin Surveillance Supervisor</t>
-  </si>
-  <si>
-    <t>AdminSup</t>
-  </si>
-  <si>
-    <t>SURVEILLANCE_OFFICER</t>
-  </si>
-  <si>
-    <t>Surveillance Officer</t>
-  </si>
-  <si>
-    <t>SurvOff</t>
-  </si>
-  <si>
-    <t>HOSPITAL_INFORMANT</t>
-  </si>
-  <si>
-    <t>Hospital Informant</t>
-  </si>
-  <si>
-    <t>HospInf</t>
-  </si>
-  <si>
-    <t>COMMUNITY_OFFICER</t>
-  </si>
-  <si>
-    <t>Community Officer</t>
-  </si>
-  <si>
-    <t>COMMUNITY_INFORMANT</t>
-  </si>
-  <si>
-    <t>Community Informant</t>
-  </si>
-  <si>
-    <t>CommInf</t>
-  </si>
-  <si>
-    <t>CASE_SUPERVISOR</t>
-  </si>
-  <si>
-    <t>Clinician</t>
-  </si>
-  <si>
-    <t>CASE_OFFICER</t>
-  </si>
-  <si>
-    <t>Case Officer</t>
-  </si>
-  <si>
-    <t>CaseOff</t>
-  </si>
-  <si>
-    <t>CONTACT_SUPERVISOR</t>
-  </si>
-  <si>
-    <t>Contact Supervisor</t>
-  </si>
-  <si>
-    <t>ContSup</t>
-  </si>
-  <si>
-    <t>CONTACT_OFFICER</t>
-  </si>
-  <si>
-    <t>Contact Officer</t>
-  </si>
-  <si>
-    <t>ContOff</t>
-  </si>
-  <si>
-    <t>EVENT_OFFICER</t>
-  </si>
-  <si>
-    <t>Event Officer</t>
-  </si>
-  <si>
-    <t>EventOff</t>
-  </si>
-  <si>
-    <t>LAB_USER</t>
-  </si>
-  <si>
-    <t>Lab Officer</t>
-  </si>
-  <si>
-    <t>LabOff</t>
-  </si>
-  <si>
-    <t>EXTERNAL_LAB_USER</t>
-  </si>
-  <si>
-    <t>External Lab Officer</t>
-  </si>
-  <si>
-    <t>ExtLabOff</t>
-  </si>
-  <si>
-    <t>NATIONAL_OBSERVER</t>
-  </si>
-  <si>
-    <t>National Observer</t>
-  </si>
-  <si>
-    <t>NatObs</t>
-  </si>
-  <si>
-    <t>STATE_OBSERVER</t>
-  </si>
-  <si>
-    <t>Region Observer</t>
-  </si>
-  <si>
-    <t>RegObs</t>
-  </si>
-  <si>
-    <t>DISTRICT_OBSERVER</t>
-  </si>
-  <si>
-    <t>District Observer</t>
-  </si>
-  <si>
-    <t>DistObs</t>
-  </si>
-  <si>
-    <t>NATIONAL_CLINICIAN</t>
-  </si>
-  <si>
-    <t>National Clinician</t>
-  </si>
-  <si>
-    <t>NatClin</t>
-  </si>
-  <si>
-    <t>POE_INFORMANT</t>
-  </si>
-  <si>
-    <t>POE Informant</t>
-  </si>
-  <si>
-    <t>POEInf</t>
-  </si>
-  <si>
-    <t>POE_SUPERVISOR</t>
-  </si>
-  <si>
-    <t>POE Supervisor</t>
-  </si>
-  <si>
-    <t>POESup</t>
-  </si>
-  <si>
-    <t>POE_NATIONAL_USER</t>
-  </si>
-  <si>
-    <t>POE National User</t>
-  </si>
-  <si>
-    <t>POENat</t>
-  </si>
-  <si>
-    <t>IMPORT_USER</t>
-  </si>
-  <si>
-    <t>Import User</t>
-  </si>
-  <si>
-    <t>ImpUser</t>
-  </si>
-  <si>
-    <t>REST_EXTERNAL_VISITS_USER</t>
-  </si>
-  <si>
-    <t>External Visits User</t>
-  </si>
-  <si>
-    <t>ExtVis</t>
-  </si>
-  <si>
-    <t>REST_USER</t>
-  </si>
-  <si>
-    <t>ReST User</t>
-  </si>
-  <si>
-    <t>ReST</t>
-  </si>
-  <si>
-    <t>SORMAS_TO_SORMAS_CLIENT</t>
-  </si>
-  <si>
-    <t>Sormas to Sormas Client</t>
-  </si>
-  <si>
-    <t>SormasToSormas</t>
-  </si>
-  <si>
-    <t>BAG_USER</t>
-  </si>
-  <si>
-    <t>BAG User</t>
-  </si>
-  <si>
-    <t>BAG</t>
+    <t>User.jurisdictionLevel</t>
+  </si>
+  <si>
+    <t>jurisdictionLevel</t>
+  </si>
+  <si>
+    <t>JurisdictionLevel</t>
   </si>
   <si>
     <t>EN</t>
@@ -12658,6 +12430,24 @@
     <t>Čeština</t>
   </si>
   <si>
+    <t>NATION</t>
+  </si>
+  <si>
+    <t>Nation</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>DISTRICT</t>
+  </si>
+  <si>
+    <t>HEALTH_FACILITY</t>
+  </si>
+  <si>
+    <t>EXTERNAL_LABORATORY</t>
+  </si>
+  <si>
     <t>LabMessage.type</t>
   </si>
   <si>
@@ -12979,7 +12769,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.72.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -14855,7 +14645,7 @@
 </file>
 
 <file path=xl/tables/table206.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="206" ref="A1:L19" displayName="User" name="User">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="206" ref="A1:L20" displayName="User" name="User">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14876,7 +14666,7 @@
 </file>
 
 <file path=xl/tables/table207.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="207" ref="A21:D24" displayName="UserFacilityReference" name="UserFacilityReference">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="207" ref="A22:D25" displayName="UserFacilityReference" name="UserFacilityReference">
   <autoFilter/>
   <tableColumns count="4">
     <tableColumn id="1" name="Type"/>
@@ -14889,7 +14679,7 @@
 </file>
 
 <file path=xl/tables/table208.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="208" ref="A26:E53" displayName="UserUserRole" name="UserUserRole">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="208" ref="A27:E83" displayName="UserDisease" name="UserDisease">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14903,7 +14693,7 @@
 </file>
 
 <file path=xl/tables/table209.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="209" ref="A55:E111" displayName="UserDisease" name="UserDisease">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="209" ref="A85:E101" displayName="UserLanguage" name="UserLanguage">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14931,7 +14721,7 @@
 </file>
 
 <file path=xl/tables/table210.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A113:E129" displayName="UserLanguage" name="UserLanguage">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A103:E112" displayName="UserJurisdictionLevel" name="UserJurisdictionLevel">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -58630,7 +58420,7 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -59156,204 +58946,215 @@
       <c r="K19"/>
       <c r="L19"/>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>4091</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4092</v>
+      </c>
+      <c r="C20" t="s" s="1">
+        <v>4093</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>97</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>214</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>215</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23"/>
-      <c r="B23" t="s">
-        <v>217</v>
-      </c>
-      <c r="C23" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25"/>
+      <c r="B25" t="s">
         <v>220</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>213</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>4091</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>4092</v>
+        <v>213</v>
       </c>
       <c r="C27" t="s">
-        <v>4093</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28"/>
+      <c r="A28" t="s">
+        <v>123</v>
+      </c>
       <c r="B28" t="s">
-        <v>4094</v>
+        <v>378</v>
       </c>
       <c r="C28" t="s">
-        <v>4095</v>
+        <v>379</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>4096</v>
+        <v>378</v>
       </c>
     </row>
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>4097</v>
+        <v>380</v>
       </c>
       <c r="C29" t="s">
-        <v>4098</v>
+        <v>381</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>4099</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>4100</v>
+        <v>382</v>
       </c>
       <c r="C30" t="s">
-        <v>4101</v>
+        <v>383</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
       </c>
       <c r="E30" t="s">
-        <v>4102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31">
       <c r="A31"/>
       <c r="B31" t="s">
-        <v>4103</v>
+        <v>384</v>
       </c>
       <c r="C31" t="s">
-        <v>4104</v>
+        <v>385</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>4105</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>4106</v>
+        <v>387</v>
       </c>
       <c r="C32" t="s">
-        <v>4107</v>
+        <v>388</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
       </c>
       <c r="E32" t="s">
-        <v>4108</v>
+        <v>389</v>
       </c>
     </row>
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>4109</v>
+        <v>390</v>
       </c>
       <c r="C33" t="s">
-        <v>4110</v>
+        <v>391</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>390</v>
       </c>
     </row>
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>4111</v>
+        <v>392</v>
       </c>
       <c r="C34" t="s">
-        <v>4112</v>
+        <v>393</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>4113</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>4114</v>
+        <v>394</v>
       </c>
       <c r="C35" t="s">
-        <v>4115</v>
+        <v>395</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
@@ -59365,314 +59166,325 @@
     <row r="36">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>4116</v>
+        <v>396</v>
       </c>
       <c r="C36" t="s">
-        <v>4117</v>
+        <v>397</v>
       </c>
       <c r="D36" t="s">
         <v>27</v>
       </c>
       <c r="E36" t="s">
-        <v>4118</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>4119</v>
+        <v>398</v>
       </c>
       <c r="C37" t="s">
-        <v>4120</v>
+        <v>399</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
       </c>
       <c r="E37" t="s">
-        <v>4121</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>4122</v>
+        <v>400</v>
       </c>
       <c r="C38" t="s">
-        <v>4123</v>
+        <v>401</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
       </c>
       <c r="E38" t="s">
-        <v>4124</v>
+        <v>402</v>
       </c>
     </row>
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>4125</v>
+        <v>403</v>
       </c>
       <c r="C39" t="s">
-        <v>4126</v>
+        <v>404</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
       </c>
       <c r="E39" t="s">
-        <v>4127</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>4128</v>
+        <v>405</v>
       </c>
       <c r="C40" t="s">
-        <v>4129</v>
+        <v>406</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
       </c>
       <c r="E40" t="s">
-        <v>4130</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>4131</v>
+        <v>408</v>
       </c>
       <c r="C41" t="s">
-        <v>4132</v>
+        <v>409</v>
       </c>
       <c r="D41" t="s">
         <v>27</v>
       </c>
       <c r="E41" t="s">
-        <v>4133</v>
+        <v>410</v>
       </c>
     </row>
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>4134</v>
+        <v>411</v>
       </c>
       <c r="C42" t="s">
-        <v>4135</v>
+        <v>412</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
       </c>
       <c r="E42" t="s">
-        <v>4136</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>4137</v>
+        <v>413</v>
       </c>
       <c r="C43" t="s">
-        <v>4138</v>
+        <v>414</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>4139</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>4140</v>
+        <v>415</v>
       </c>
       <c r="C44" t="s">
-        <v>4141</v>
+        <v>416</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
       </c>
       <c r="E44" t="s">
-        <v>4142</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>4143</v>
+        <v>418</v>
       </c>
       <c r="C45" t="s">
-        <v>4144</v>
+        <v>419</v>
       </c>
       <c r="D45" t="s">
         <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>4145</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>4146</v>
+        <v>420</v>
       </c>
       <c r="C46" t="s">
-        <v>4147</v>
+        <v>185</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>4148</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>4149</v>
+        <v>421</v>
       </c>
       <c r="C47" t="s">
-        <v>4150</v>
+        <v>422</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>4151</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>4152</v>
+        <v>423</v>
       </c>
       <c r="C48" t="s">
-        <v>4153</v>
+        <v>424</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>4154</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>4155</v>
+        <v>425</v>
       </c>
       <c r="C49" t="s">
-        <v>4156</v>
+        <v>426</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>4157</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>4158</v>
+        <v>427</v>
       </c>
       <c r="C50" t="s">
-        <v>4159</v>
+        <v>428</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
       </c>
       <c r="E50" t="s">
-        <v>4160</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>4161</v>
+        <v>429</v>
       </c>
       <c r="C51" t="s">
-        <v>4162</v>
+        <v>430</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
       </c>
       <c r="E51" t="s">
-        <v>4163</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>4164</v>
+        <v>431</v>
       </c>
       <c r="C52" t="s">
-        <v>4165</v>
+        <v>431</v>
       </c>
       <c r="D52" t="s">
         <v>27</v>
       </c>
       <c r="E52" t="s">
-        <v>4166</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>4167</v>
+        <v>432</v>
       </c>
       <c r="C53" t="s">
-        <v>4168</v>
+        <v>433</v>
       </c>
       <c r="D53" t="s">
         <v>27</v>
       </c>
       <c r="E53" t="s">
-        <v>4169</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54"/>
+      <c r="B54" t="s">
+        <v>434</v>
+      </c>
+      <c r="C54" t="s">
+        <v>435</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s">
-        <v>2</v>
-      </c>
+      <c r="A55"/>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>436</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>437</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>223</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s">
-        <v>123</v>
-      </c>
+      <c r="A56"/>
       <c r="B56" t="s">
-        <v>378</v>
+        <v>438</v>
       </c>
       <c r="C56" t="s">
-        <v>379</v>
+        <v>439</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
       </c>
       <c r="E56" t="s">
-        <v>378</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>380</v>
+        <v>440</v>
       </c>
       <c r="C57" t="s">
-        <v>381</v>
+        <v>441</v>
       </c>
       <c r="D57" t="s">
         <v>27</v>
@@ -59684,70 +59496,70 @@
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>382</v>
+        <v>442</v>
       </c>
       <c r="C58" t="s">
-        <v>383</v>
+        <v>443</v>
       </c>
       <c r="D58" t="s">
         <v>27</v>
       </c>
       <c r="E58" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>384</v>
+        <v>444</v>
       </c>
       <c r="C59" t="s">
-        <v>385</v>
+        <v>445</v>
       </c>
       <c r="D59" t="s">
         <v>27</v>
       </c>
       <c r="E59" t="s">
-        <v>386</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>387</v>
+        <v>446</v>
       </c>
       <c r="C60" t="s">
-        <v>388</v>
+        <v>447</v>
       </c>
       <c r="D60" t="s">
         <v>27</v>
       </c>
       <c r="E60" t="s">
-        <v>389</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>390</v>
+        <v>448</v>
       </c>
       <c r="C61" t="s">
-        <v>391</v>
+        <v>449</v>
       </c>
       <c r="D61" t="s">
         <v>27</v>
       </c>
       <c r="E61" t="s">
-        <v>390</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>392</v>
+        <v>450</v>
       </c>
       <c r="C62" t="s">
-        <v>393</v>
+        <v>451</v>
       </c>
       <c r="D62" t="s">
         <v>27</v>
@@ -59759,10 +59571,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>394</v>
+        <v>452</v>
       </c>
       <c r="C63" t="s">
-        <v>395</v>
+        <v>453</v>
       </c>
       <c r="D63" t="s">
         <v>27</v>
@@ -59774,10 +59586,10 @@
     <row r="64">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>396</v>
+        <v>454</v>
       </c>
       <c r="C64" t="s">
-        <v>397</v>
+        <v>455</v>
       </c>
       <c r="D64" t="s">
         <v>27</v>
@@ -59789,10 +59601,10 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>398</v>
+        <v>456</v>
       </c>
       <c r="C65" t="s">
-        <v>399</v>
+        <v>457</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
@@ -59804,25 +59616,25 @@
     <row r="66">
       <c r="A66"/>
       <c r="B66" t="s">
-        <v>400</v>
+        <v>458</v>
       </c>
       <c r="C66" t="s">
-        <v>401</v>
+        <v>459</v>
       </c>
       <c r="D66" t="s">
         <v>27</v>
       </c>
       <c r="E66" t="s">
-        <v>402</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67">
       <c r="A67"/>
       <c r="B67" t="s">
-        <v>403</v>
+        <v>460</v>
       </c>
       <c r="C67" t="s">
-        <v>404</v>
+        <v>461</v>
       </c>
       <c r="D67" t="s">
         <v>27</v>
@@ -59834,40 +59646,40 @@
     <row r="68">
       <c r="A68"/>
       <c r="B68" t="s">
-        <v>405</v>
+        <v>462</v>
       </c>
       <c r="C68" t="s">
-        <v>406</v>
+        <v>463</v>
       </c>
       <c r="D68" t="s">
         <v>27</v>
       </c>
       <c r="E68" t="s">
-        <v>407</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>408</v>
+        <v>464</v>
       </c>
       <c r="C69" t="s">
-        <v>409</v>
+        <v>465</v>
       </c>
       <c r="D69" t="s">
         <v>27</v>
       </c>
       <c r="E69" t="s">
-        <v>410</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70">
       <c r="A70"/>
       <c r="B70" t="s">
-        <v>411</v>
+        <v>466</v>
       </c>
       <c r="C70" t="s">
-        <v>412</v>
+        <v>467</v>
       </c>
       <c r="D70" t="s">
         <v>27</v>
@@ -59879,10 +59691,10 @@
     <row r="71">
       <c r="A71"/>
       <c r="B71" t="s">
-        <v>413</v>
+        <v>468</v>
       </c>
       <c r="C71" t="s">
-        <v>414</v>
+        <v>469</v>
       </c>
       <c r="D71" t="s">
         <v>27</v>
@@ -59894,25 +59706,25 @@
     <row r="72">
       <c r="A72"/>
       <c r="B72" t="s">
-        <v>415</v>
+        <v>470</v>
       </c>
       <c r="C72" t="s">
-        <v>416</v>
+        <v>471</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
       </c>
       <c r="E72" t="s">
-        <v>417</v>
+        <v>27</v>
       </c>
     </row>
     <row r="73">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>418</v>
+        <v>472</v>
       </c>
       <c r="C73" t="s">
-        <v>419</v>
+        <v>473</v>
       </c>
       <c r="D73" t="s">
         <v>27</v>
@@ -59924,10 +59736,10 @@
     <row r="74">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>420</v>
+        <v>474</v>
       </c>
       <c r="C74" t="s">
-        <v>185</v>
+        <v>475</v>
       </c>
       <c r="D74" t="s">
         <v>27</v>
@@ -59939,40 +59751,40 @@
     <row r="75">
       <c r="A75"/>
       <c r="B75" t="s">
-        <v>421</v>
+        <v>476</v>
       </c>
       <c r="C75" t="s">
-        <v>422</v>
+        <v>477</v>
       </c>
       <c r="D75" t="s">
         <v>27</v>
       </c>
       <c r="E75" t="s">
-        <v>27</v>
+        <v>478</v>
       </c>
     </row>
     <row r="76">
       <c r="A76"/>
       <c r="B76" t="s">
-        <v>423</v>
+        <v>479</v>
       </c>
       <c r="C76" t="s">
-        <v>424</v>
+        <v>480</v>
       </c>
       <c r="D76" t="s">
         <v>27</v>
       </c>
       <c r="E76" t="s">
-        <v>27</v>
+        <v>481</v>
       </c>
     </row>
     <row r="77">
       <c r="A77"/>
       <c r="B77" t="s">
-        <v>425</v>
+        <v>482</v>
       </c>
       <c r="C77" t="s">
-        <v>426</v>
+        <v>483</v>
       </c>
       <c r="D77" t="s">
         <v>27</v>
@@ -59984,10 +59796,10 @@
     <row r="78">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>427</v>
+        <v>484</v>
       </c>
       <c r="C78" t="s">
-        <v>428</v>
+        <v>485</v>
       </c>
       <c r="D78" t="s">
         <v>27</v>
@@ -59999,10 +59811,10 @@
     <row r="79">
       <c r="A79"/>
       <c r="B79" t="s">
-        <v>429</v>
+        <v>486</v>
       </c>
       <c r="C79" t="s">
-        <v>430</v>
+        <v>487</v>
       </c>
       <c r="D79" t="s">
         <v>27</v>
@@ -60014,10 +59826,10 @@
     <row r="80">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>431</v>
+        <v>488</v>
       </c>
       <c r="C80" t="s">
-        <v>431</v>
+        <v>489</v>
       </c>
       <c r="D80" t="s">
         <v>27</v>
@@ -60029,10 +59841,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>432</v>
+        <v>490</v>
       </c>
       <c r="C81" t="s">
-        <v>433</v>
+        <v>491</v>
       </c>
       <c r="D81" t="s">
         <v>27</v>
@@ -60044,70 +59856,59 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>434</v>
+        <v>234</v>
       </c>
       <c r="C82" t="s">
-        <v>435</v>
+        <v>492</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
       </c>
       <c r="E82" t="s">
-        <v>27</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>436</v>
+        <v>493</v>
       </c>
       <c r="C83" t="s">
-        <v>437</v>
+        <v>494</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
       </c>
       <c r="E83" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84"/>
-      <c r="B84" t="s">
-        <v>438</v>
-      </c>
-      <c r="C84" t="s">
-        <v>439</v>
-      </c>
-      <c r="D84" t="s">
-        <v>27</v>
-      </c>
-      <c r="E84" t="s">
-        <v>27</v>
+        <v>495</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85"/>
+      <c r="A85" t="s">
+        <v>2</v>
+      </c>
       <c r="B85" t="s">
-        <v>440</v>
+        <v>213</v>
       </c>
       <c r="C85" t="s">
-        <v>441</v>
+        <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>27</v>
+        <v>223</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86"/>
+      <c r="A86" t="s">
+        <v>4088</v>
+      </c>
       <c r="B86" t="s">
-        <v>442</v>
+        <v>4094</v>
       </c>
       <c r="C86" t="s">
-        <v>443</v>
+        <v>4095</v>
       </c>
       <c r="D86" t="s">
         <v>27</v>
@@ -60119,10 +59920,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>444</v>
+        <v>4096</v>
       </c>
       <c r="C87" t="s">
-        <v>445</v>
+        <v>4097</v>
       </c>
       <c r="D87" t="s">
         <v>27</v>
@@ -60134,10 +59935,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>446</v>
+        <v>4098</v>
       </c>
       <c r="C88" t="s">
-        <v>447</v>
+        <v>4099</v>
       </c>
       <c r="D88" t="s">
         <v>27</v>
@@ -60149,10 +59950,10 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>448</v>
+        <v>4100</v>
       </c>
       <c r="C89" t="s">
-        <v>449</v>
+        <v>4101</v>
       </c>
       <c r="D89" t="s">
         <v>27</v>
@@ -60164,10 +59965,10 @@
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>450</v>
+        <v>4102</v>
       </c>
       <c r="C90" t="s">
-        <v>451</v>
+        <v>4103</v>
       </c>
       <c r="D90" t="s">
         <v>27</v>
@@ -60179,10 +59980,10 @@
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>452</v>
+        <v>4104</v>
       </c>
       <c r="C91" t="s">
-        <v>453</v>
+        <v>4105</v>
       </c>
       <c r="D91" t="s">
         <v>27</v>
@@ -60194,10 +59995,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>454</v>
+        <v>4106</v>
       </c>
       <c r="C92" t="s">
-        <v>455</v>
+        <v>4107</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -60209,10 +60010,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>456</v>
+        <v>4108</v>
       </c>
       <c r="C93" t="s">
-        <v>457</v>
+        <v>4109</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
@@ -60224,10 +60025,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>458</v>
+        <v>4110</v>
       </c>
       <c r="C94" t="s">
-        <v>459</v>
+        <v>4111</v>
       </c>
       <c r="D94" t="s">
         <v>27</v>
@@ -60239,10 +60040,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>460</v>
+        <v>4112</v>
       </c>
       <c r="C95" t="s">
-        <v>461</v>
+        <v>4113</v>
       </c>
       <c r="D95" t="s">
         <v>27</v>
@@ -60254,10 +60055,10 @@
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
-        <v>462</v>
+        <v>4114</v>
       </c>
       <c r="C96" t="s">
-        <v>463</v>
+        <v>4115</v>
       </c>
       <c r="D96" t="s">
         <v>27</v>
@@ -60269,10 +60070,10 @@
     <row r="97">
       <c r="A97"/>
       <c r="B97" t="s">
-        <v>464</v>
+        <v>4116</v>
       </c>
       <c r="C97" t="s">
-        <v>465</v>
+        <v>4117</v>
       </c>
       <c r="D97" t="s">
         <v>27</v>
@@ -60284,10 +60085,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>466</v>
+        <v>4118</v>
       </c>
       <c r="C98" t="s">
-        <v>467</v>
+        <v>4119</v>
       </c>
       <c r="D98" t="s">
         <v>27</v>
@@ -60299,10 +60100,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>468</v>
+        <v>4120</v>
       </c>
       <c r="C99" t="s">
-        <v>469</v>
+        <v>4121</v>
       </c>
       <c r="D99" t="s">
         <v>27</v>
@@ -60314,10 +60115,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>470</v>
+        <v>4122</v>
       </c>
       <c r="C100" t="s">
-        <v>471</v>
+        <v>4123</v>
       </c>
       <c r="D100" t="s">
         <v>27</v>
@@ -60329,10 +60130,10 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
-        <v>472</v>
+        <v>4124</v>
       </c>
       <c r="C101" t="s">
-        <v>473</v>
+        <v>4125</v>
       </c>
       <c r="D101" t="s">
         <v>27</v>
@@ -60341,58 +60142,47 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102"/>
-      <c r="B102" t="s">
-        <v>474</v>
-      </c>
-      <c r="C102" t="s">
-        <v>475</v>
-      </c>
-      <c r="D102" t="s">
-        <v>27</v>
-      </c>
-      <c r="E102" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="103">
-      <c r="A103"/>
+      <c r="A103" t="s">
+        <v>2</v>
+      </c>
       <c r="B103" t="s">
-        <v>476</v>
+        <v>213</v>
       </c>
       <c r="C103" t="s">
-        <v>477</v>
+        <v>4</v>
       </c>
       <c r="D103" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E103" t="s">
-        <v>478</v>
+        <v>223</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104"/>
+      <c r="A104" t="s">
+        <v>4093</v>
+      </c>
       <c r="B104" t="s">
-        <v>479</v>
+        <v>502</v>
       </c>
       <c r="C104" t="s">
-        <v>480</v>
+        <v>1267</v>
       </c>
       <c r="D104" t="s">
         <v>27</v>
       </c>
       <c r="E104" t="s">
-        <v>481</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105">
       <c r="A105"/>
       <c r="B105" t="s">
-        <v>482</v>
+        <v>4126</v>
       </c>
       <c r="C105" t="s">
-        <v>483</v>
+        <v>4127</v>
       </c>
       <c r="D105" t="s">
         <v>27</v>
@@ -60404,10 +60194,10 @@
     <row r="106">
       <c r="A106"/>
       <c r="B106" t="s">
-        <v>484</v>
+        <v>4128</v>
       </c>
       <c r="C106" t="s">
-        <v>485</v>
+        <v>654</v>
       </c>
       <c r="D106" t="s">
         <v>27</v>
@@ -60419,10 +60209,10 @@
     <row r="107">
       <c r="A107"/>
       <c r="B107" t="s">
-        <v>486</v>
+        <v>4129</v>
       </c>
       <c r="C107" t="s">
-        <v>487</v>
+        <v>657</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -60434,10 +60224,10 @@
     <row r="108">
       <c r="A108"/>
       <c r="B108" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="C108" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="D108" t="s">
         <v>27</v>
@@ -60449,10 +60239,10 @@
     <row r="109">
       <c r="A109"/>
       <c r="B109" t="s">
-        <v>490</v>
+        <v>4130</v>
       </c>
       <c r="C109" t="s">
-        <v>491</v>
+        <v>703</v>
       </c>
       <c r="D109" t="s">
         <v>27</v>
@@ -60464,289 +60254,45 @@
     <row r="110">
       <c r="A110"/>
       <c r="B110" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="C110" t="s">
-        <v>492</v>
+        <v>285</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
       </c>
       <c r="E110" t="s">
-        <v>235</v>
+        <v>27</v>
       </c>
     </row>
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>493</v>
+        <v>4131</v>
       </c>
       <c r="C111" t="s">
-        <v>494</v>
+        <v>4131</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
       </c>
       <c r="E111" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" t="s">
-        <v>213</v>
-      </c>
-      <c r="C113" t="s">
-        <v>4</v>
-      </c>
-      <c r="D113" t="s">
-        <v>5</v>
-      </c>
-      <c r="E113" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="s">
-        <v>4088</v>
-      </c>
-      <c r="B114" t="s">
-        <v>4170</v>
-      </c>
-      <c r="C114" t="s">
-        <v>4171</v>
-      </c>
-      <c r="D114" t="s">
-        <v>27</v>
-      </c>
-      <c r="E114" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115"/>
-      <c r="B115" t="s">
-        <v>4172</v>
-      </c>
-      <c r="C115" t="s">
-        <v>4173</v>
-      </c>
-      <c r="D115" t="s">
-        <v>27</v>
-      </c>
-      <c r="E115" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116"/>
-      <c r="B116" t="s">
-        <v>4174</v>
-      </c>
-      <c r="C116" t="s">
-        <v>4175</v>
-      </c>
-      <c r="D116" t="s">
-        <v>27</v>
-      </c>
-      <c r="E116" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117"/>
-      <c r="B117" t="s">
-        <v>4176</v>
-      </c>
-      <c r="C117" t="s">
-        <v>4177</v>
-      </c>
-      <c r="D117" t="s">
-        <v>27</v>
-      </c>
-      <c r="E117" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118"/>
-      <c r="B118" t="s">
-        <v>4178</v>
-      </c>
-      <c r="C118" t="s">
-        <v>4179</v>
-      </c>
-      <c r="D118" t="s">
-        <v>27</v>
-      </c>
-      <c r="E118" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119"/>
-      <c r="B119" t="s">
-        <v>4180</v>
-      </c>
-      <c r="C119" t="s">
-        <v>4181</v>
-      </c>
-      <c r="D119" t="s">
-        <v>27</v>
-      </c>
-      <c r="E119" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120"/>
-      <c r="B120" t="s">
-        <v>4182</v>
-      </c>
-      <c r="C120" t="s">
-        <v>4183</v>
-      </c>
-      <c r="D120" t="s">
-        <v>27</v>
-      </c>
-      <c r="E120" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121"/>
-      <c r="B121" t="s">
-        <v>4184</v>
-      </c>
-      <c r="C121" t="s">
-        <v>4185</v>
-      </c>
-      <c r="D121" t="s">
-        <v>27</v>
-      </c>
-      <c r="E121" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122"/>
-      <c r="B122" t="s">
-        <v>4186</v>
-      </c>
-      <c r="C122" t="s">
-        <v>4187</v>
-      </c>
-      <c r="D122" t="s">
-        <v>27</v>
-      </c>
-      <c r="E122" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123"/>
-      <c r="B123" t="s">
-        <v>4188</v>
-      </c>
-      <c r="C123" t="s">
-        <v>4189</v>
-      </c>
-      <c r="D123" t="s">
-        <v>27</v>
-      </c>
-      <c r="E123" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124"/>
-      <c r="B124" t="s">
-        <v>4190</v>
-      </c>
-      <c r="C124" t="s">
-        <v>4191</v>
-      </c>
-      <c r="D124" t="s">
-        <v>27</v>
-      </c>
-      <c r="E124" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125"/>
-      <c r="B125" t="s">
-        <v>4192</v>
-      </c>
-      <c r="C125" t="s">
-        <v>4193</v>
-      </c>
-      <c r="D125" t="s">
-        <v>27</v>
-      </c>
-      <c r="E125" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126"/>
-      <c r="B126" t="s">
-        <v>4194</v>
-      </c>
-      <c r="C126" t="s">
-        <v>4195</v>
-      </c>
-      <c r="D126" t="s">
-        <v>27</v>
-      </c>
-      <c r="E126" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127"/>
-      <c r="B127" t="s">
-        <v>4196</v>
-      </c>
-      <c r="C127" t="s">
-        <v>4197</v>
-      </c>
-      <c r="D127" t="s">
-        <v>27</v>
-      </c>
-      <c r="E127" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128"/>
-      <c r="B128" t="s">
-        <v>4198</v>
-      </c>
-      <c r="C128" t="s">
-        <v>4199</v>
-      </c>
-      <c r="D128" t="s">
-        <v>27</v>
-      </c>
-      <c r="E128" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129"/>
-      <c r="B129" t="s">
-        <v>4200</v>
-      </c>
-      <c r="C129" t="s">
-        <v>4201</v>
-      </c>
-      <c r="D129" t="s">
-        <v>27</v>
-      </c>
-      <c r="E129" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112"/>
+      <c r="B112" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C112" t="s">
+        <v>944</v>
+      </c>
+      <c r="D112" t="s">
+        <v>27</v>
+      </c>
+      <c r="E112" t="s">
         <v>27</v>
       </c>
     </row>
@@ -60824,13 +60370,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4202</v>
+        <v>4132</v>
       </c>
       <c r="B2" t="s">
         <v>4028</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4203</v>
+        <v>4133</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -60850,7 +60396,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4204</v>
+        <v>4134</v>
       </c>
       <c r="B3" t="s">
         <v>3142</v>
@@ -60876,17 +60422,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4205</v>
+        <v>4135</v>
       </c>
       <c r="B4" t="s">
-        <v>4206</v>
+        <v>4136</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>4207</v>
+        <v>4137</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -60902,7 +60448,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4208</v>
+        <v>4138</v>
       </c>
       <c r="B5" t="s">
         <v>2892</v>
@@ -60928,17 +60474,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4209</v>
+        <v>4139</v>
       </c>
       <c r="B6" t="s">
-        <v>4210</v>
+        <v>4140</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4211</v>
+        <v>4141</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -60954,10 +60500,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4212</v>
+        <v>4142</v>
       </c>
       <c r="B7" t="s">
-        <v>4213</v>
+        <v>4143</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>14</v>
@@ -60980,7 +60526,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4214</v>
+        <v>4144</v>
       </c>
       <c r="B8" t="s">
         <v>2901</v>
@@ -61006,7 +60552,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4215</v>
+        <v>4145</v>
       </c>
       <c r="B9" t="s">
         <v>2905</v>
@@ -61032,7 +60578,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4216</v>
+        <v>4146</v>
       </c>
       <c r="B10" t="s">
         <v>2926</v>
@@ -61058,17 +60604,17 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4217</v>
+        <v>4147</v>
       </c>
       <c r="B11" t="s">
-        <v>4218</v>
+        <v>4148</v>
       </c>
       <c r="C11" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>4219</v>
+        <v>4149</v>
       </c>
       <c r="F11" t="s" s="1">
         <v>27</v>
@@ -61084,17 +60630,17 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4220</v>
+        <v>4150</v>
       </c>
       <c r="B12" t="s">
-        <v>4221</v>
+        <v>4151</v>
       </c>
       <c r="C12" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>4222</v>
+        <v>4152</v>
       </c>
       <c r="F12" t="s" s="1">
         <v>27</v>
@@ -61110,17 +60656,17 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4223</v>
+        <v>4153</v>
       </c>
       <c r="B13" t="s">
-        <v>4224</v>
+        <v>4154</v>
       </c>
       <c r="C13" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>4225</v>
+        <v>4155</v>
       </c>
       <c r="F13" t="s" s="1">
         <v>27</v>
@@ -61136,17 +60682,17 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4226</v>
+        <v>4156</v>
       </c>
       <c r="B14" t="s">
-        <v>4227</v>
+        <v>4157</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>4228</v>
+        <v>4158</v>
       </c>
       <c r="F14" t="s" s="1">
         <v>27</v>
@@ -61162,10 +60708,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4229</v>
+        <v>4159</v>
       </c>
       <c r="B15" t="s">
-        <v>4230</v>
+        <v>4160</v>
       </c>
       <c r="C15" t="s" s="1">
         <v>14</v>
@@ -61188,10 +60734,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4231</v>
+        <v>4161</v>
       </c>
       <c r="B16" t="s">
-        <v>4232</v>
+        <v>4162</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>14</v>
@@ -61214,10 +60760,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4233</v>
+        <v>4163</v>
       </c>
       <c r="B17" t="s">
-        <v>4234</v>
+        <v>4164</v>
       </c>
       <c r="C17" t="s" s="1">
         <v>53</v>
@@ -61240,10 +60786,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4235</v>
+        <v>4165</v>
       </c>
       <c r="B18" t="s">
-        <v>4236</v>
+        <v>4166</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>57</v>
@@ -61266,10 +60812,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4237</v>
+        <v>4167</v>
       </c>
       <c r="B19" t="s">
-        <v>4238</v>
+        <v>4168</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>57</v>
@@ -61292,10 +60838,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4239</v>
+        <v>4169</v>
       </c>
       <c r="B20" t="s">
-        <v>4240</v>
+        <v>4170</v>
       </c>
       <c r="C20" t="s" s="1">
         <v>57</v>
@@ -61318,10 +60864,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4241</v>
+        <v>4171</v>
       </c>
       <c r="B21" t="s">
-        <v>4242</v>
+        <v>4172</v>
       </c>
       <c r="C21" t="s" s="1">
         <v>14</v>
@@ -61344,10 +60890,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>4243</v>
+        <v>4173</v>
       </c>
       <c r="B22" t="s">
-        <v>4244</v>
+        <v>4174</v>
       </c>
       <c r="C22" t="s" s="1">
         <v>14</v>
@@ -61370,10 +60916,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>4245</v>
+        <v>4175</v>
       </c>
       <c r="B23" t="s">
-        <v>4246</v>
+        <v>4176</v>
       </c>
       <c r="C23" t="s" s="1">
         <v>14</v>
@@ -61396,10 +60942,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>4247</v>
+        <v>4177</v>
       </c>
       <c r="B24" t="s">
-        <v>4248</v>
+        <v>4178</v>
       </c>
       <c r="C24" t="s" s="1">
         <v>14</v>
@@ -61422,10 +60968,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>4249</v>
+        <v>4179</v>
       </c>
       <c r="B25" t="s">
-        <v>4250</v>
+        <v>4180</v>
       </c>
       <c r="C25" t="s" s="1">
         <v>14</v>
@@ -61448,10 +60994,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>4251</v>
+        <v>4181</v>
       </c>
       <c r="B26" t="s">
-        <v>4252</v>
+        <v>4182</v>
       </c>
       <c r="C26" t="s" s="1">
         <v>14</v>
@@ -61474,7 +61020,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>4253</v>
+        <v>4183</v>
       </c>
       <c r="B27" t="s">
         <v>3140</v>
@@ -61500,13 +61046,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4254</v>
+        <v>4184</v>
       </c>
       <c r="B28" t="s">
-        <v>4255</v>
+        <v>4185</v>
       </c>
       <c r="C28" t="s" s="1">
-        <v>4256</v>
+        <v>4186</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
@@ -61526,17 +61072,17 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>4257</v>
+        <v>4187</v>
       </c>
       <c r="B29" t="s">
-        <v>4258</v>
+        <v>4188</v>
       </c>
       <c r="C29" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>4259</v>
+        <v>4189</v>
       </c>
       <c r="F29" t="s" s="1">
         <v>27</v>
@@ -61552,17 +61098,17 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>4260</v>
+        <v>4190</v>
       </c>
       <c r="B30" t="s">
-        <v>4261</v>
+        <v>4191</v>
       </c>
       <c r="C30" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="s">
-        <v>4262</v>
+        <v>4192</v>
       </c>
       <c r="F30" t="s" s="1">
         <v>27</v>
@@ -61578,17 +61124,17 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4263</v>
+        <v>4193</v>
       </c>
       <c r="B31" t="s">
-        <v>4264</v>
+        <v>4194</v>
       </c>
       <c r="C31" t="s" s="1">
         <v>2949</v>
       </c>
       <c r="D31"/>
       <c r="E31" t="s">
-        <v>4265</v>
+        <v>4195</v>
       </c>
       <c r="F31" t="s" s="1">
         <v>27</v>
@@ -61604,17 +61150,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>4266</v>
+        <v>4196</v>
       </c>
       <c r="B32" t="s">
-        <v>4267</v>
+        <v>4197</v>
       </c>
       <c r="C32" t="s" s="1">
-        <v>4268</v>
+        <v>4198</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>4269</v>
+        <v>4199</v>
       </c>
       <c r="F32" t="s" s="1">
         <v>27</v>
@@ -61630,17 +61176,17 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>4270</v>
+        <v>4200</v>
       </c>
       <c r="B33" t="s">
-        <v>4271</v>
+        <v>4201</v>
       </c>
       <c r="C33" t="s" s="1">
         <v>772</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>4272</v>
+        <v>4202</v>
       </c>
       <c r="F33" t="s" s="1">
         <v>27</v>
@@ -61656,7 +61202,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>4273</v>
+        <v>4203</v>
       </c>
       <c r="B34" t="s">
         <v>771</v>
@@ -61699,13 +61245,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>4203</v>
+        <v>4133</v>
       </c>
       <c r="B37" t="s">
-        <v>4274</v>
+        <v>4204</v>
       </c>
       <c r="C37" t="s">
-        <v>4275</v>
+        <v>4205</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -61717,10 +61263,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>4276</v>
+        <v>4206</v>
       </c>
       <c r="C38" t="s">
-        <v>4277</v>
+        <v>4207</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
@@ -63208,13 +62754,13 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>4268</v>
+        <v>4198</v>
       </c>
       <c r="B142" t="s">
-        <v>4278</v>
+        <v>4208</v>
       </c>
       <c r="C142" t="s">
-        <v>4279</v>
+        <v>4209</v>
       </c>
       <c r="D142" t="s">
         <v>27</v>
@@ -63241,10 +62787,10 @@
     <row r="144">
       <c r="A144"/>
       <c r="B144" t="s">
-        <v>4280</v>
+        <v>4210</v>
       </c>
       <c r="C144" t="s">
-        <v>4281</v>
+        <v>4211</v>
       </c>
       <c r="D144" t="s">
         <v>27</v>
@@ -63256,10 +62802,10 @@
     <row r="145">
       <c r="A145"/>
       <c r="B145" t="s">
-        <v>4282</v>
+        <v>4212</v>
       </c>
       <c r="C145" t="s">
-        <v>4283</v>
+        <v>4213</v>
       </c>
       <c r="D145" t="s">
         <v>27</v>
@@ -63345,13 +62891,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4284</v>
+        <v>4214</v>
       </c>
       <c r="B2" t="s">
-        <v>4285</v>
+        <v>4215</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4286</v>
+        <v>4216</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -63373,17 +62919,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4287</v>
+        <v>4217</v>
       </c>
       <c r="B3" t="s">
-        <v>4288</v>
+        <v>4218</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4219</v>
+        <v>4149</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -63399,17 +62945,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4289</v>
+        <v>4219</v>
       </c>
       <c r="B4" t="s">
-        <v>4290</v>
+        <v>4220</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>4222</v>
+        <v>4152</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -63425,17 +62971,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4291</v>
+        <v>4221</v>
       </c>
       <c r="B5" t="s">
-        <v>4292</v>
+        <v>4222</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4225</v>
+        <v>4155</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -63451,17 +62997,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4293</v>
+        <v>4223</v>
       </c>
       <c r="B6" t="s">
-        <v>4294</v>
+        <v>4224</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4228</v>
+        <v>4158</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -63477,7 +63023,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4295</v>
+        <v>4225</v>
       </c>
       <c r="B7" t="s">
         <v>3158</v>
@@ -63503,7 +63049,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4296</v>
+        <v>4226</v>
       </c>
       <c r="B8" t="s">
         <v>3170</v>
@@ -63529,7 +63075,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4297</v>
+        <v>4227</v>
       </c>
       <c r="B9" t="s">
         <v>3180</v>
@@ -63555,7 +63101,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4298</v>
+        <v>4228</v>
       </c>
       <c r="B10" t="s">
         <v>3188</v>
@@ -63581,7 +63127,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4299</v>
+        <v>4229</v>
       </c>
       <c r="B11" t="s">
         <v>3184</v>
@@ -63607,7 +63153,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4300</v>
+        <v>4230</v>
       </c>
       <c r="B12" t="s">
         <v>3155</v>
@@ -63633,7 +63179,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4301</v>
+        <v>4231</v>
       </c>
       <c r="B13" t="s">
         <v>195</v>
@@ -63659,7 +63205,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4302</v>
+        <v>4232</v>
       </c>
       <c r="B14" t="s">
         <v>3208</v>
@@ -63685,7 +63231,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4303</v>
+        <v>4233</v>
       </c>
       <c r="B15" t="s">
         <v>3146</v>
@@ -63711,7 +63257,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4304</v>
+        <v>4234</v>
       </c>
       <c r="B16" t="s">
         <v>3153</v>
@@ -63737,7 +63283,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4305</v>
+        <v>4235</v>
       </c>
       <c r="B17" t="s">
         <v>3211</v>
@@ -63763,10 +63309,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4306</v>
+        <v>4236</v>
       </c>
       <c r="B18" t="s">
-        <v>4307</v>
+        <v>4237</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3163</v>
@@ -64285,12 +63831,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4308</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4309</v>
+        <v>4239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#8895: Create a dedicated menu for messages (#9316)
* #8895: Create a dedicated menu for messages

* #4461: fixed review findings

* #4461: fixed review findings

* #8895: fixed review finding

* #8895: fixed review findings

* #8895 allow UI users to fetch

* #8895: Canged jndiName example

Co-authored-by: FredrikSchäferVitagroup <fredrik.schaefer@vitagroup.ag>
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -42,7 +42,7 @@
     <sheet name="Facility" r:id="rId36" sheetId="34"/>
     <sheet name="Point of entry" r:id="rId37" sheetId="35"/>
     <sheet name="User" r:id="rId38" sheetId="36"/>
-    <sheet name="Lab Message" r:id="rId39" sheetId="37"/>
+    <sheet name="Message" r:id="rId39" sheetId="37"/>
     <sheet name="Test report" r:id="rId40" sheetId="38"/>
     <sheet name="About" r:id="rId41" sheetId="39"/>
   </sheets>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16535" uniqueCount="4240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16535" uniqueCount="4242">
   <si>
     <t>Field ID</t>
   </si>
@@ -12448,16 +12448,16 @@
     <t>EXTERNAL_LABORATORY</t>
   </si>
   <si>
-    <t>LabMessage.type</t>
+    <t>ExternalMessage.type</t>
   </si>
   <si>
     <t>ExternalMessageType</t>
   </si>
   <si>
-    <t>LabMessage.testedDisease</t>
-  </si>
-  <si>
-    <t>LabMessage.messageDateTime</t>
+    <t>ExternalMessage.testedDisease</t>
+  </si>
+  <si>
+    <t>ExternalMessage.messageDateTime</t>
   </si>
   <si>
     <t>messageDateTime</t>
@@ -12466,10 +12466,10 @@
     <t>Message date</t>
   </si>
   <si>
-    <t>LabMessage.sampleDateTime</t>
-  </si>
-  <si>
-    <t>LabMessage.sampleReceivedDate</t>
+    <t>ExternalMessage.sampleDateTime</t>
+  </si>
+  <si>
+    <t>ExternalMessage.sampleReceivedDate</t>
   </si>
   <si>
     <t>sampleReceivedDate</t>
@@ -12478,253 +12478,259 @@
     <t>Sample received</t>
   </si>
   <si>
-    <t>LabMessage.labSampleId</t>
+    <t>ExternalMessage.labSampleId</t>
   </si>
   <si>
     <t>labSampleId</t>
   </si>
   <si>
-    <t>LabMessage.sampleMaterial</t>
-  </si>
-  <si>
-    <t>LabMessage.sampleMaterialText</t>
-  </si>
-  <si>
-    <t>LabMessage.specimenCondition</t>
-  </si>
-  <si>
-    <t>LabMessage.labName</t>
-  </si>
-  <si>
-    <t>labName</t>
+    <t>ExternalMessage.sampleMaterial</t>
+  </si>
+  <si>
+    <t>ExternalMessage.sampleMaterialText</t>
+  </si>
+  <si>
+    <t>ExternalMessage.specimenCondition</t>
+  </si>
+  <si>
+    <t>ExternalMessage.reporterName</t>
+  </si>
+  <si>
+    <t>reporterName</t>
+  </si>
+  <si>
+    <t>Reporter name</t>
+  </si>
+  <si>
+    <t>ExternalMessage.labExternalId</t>
+  </si>
+  <si>
+    <t>labExternalId</t>
+  </si>
+  <si>
+    <t>Lab external ID</t>
+  </si>
+  <si>
+    <t>ExternalMessage.reporterPostalCode</t>
+  </si>
+  <si>
+    <t>reporterPostalCode</t>
+  </si>
+  <si>
+    <t>Reporter postal code</t>
+  </si>
+  <si>
+    <t>ExternalMessage.reporterCity</t>
+  </si>
+  <si>
+    <t>reporterCity</t>
+  </si>
+  <si>
+    <t>Reporter city</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personFirstName</t>
+  </si>
+  <si>
+    <t>personFirstName</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personLastName</t>
+  </si>
+  <si>
+    <t>personLastName</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personSex</t>
+  </si>
+  <si>
+    <t>personSex</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personBirthDateDD</t>
+  </si>
+  <si>
+    <t>personBirthDateDD</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personBirthDateMM</t>
+  </si>
+  <si>
+    <t>personBirthDateMM</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personBirthDateYYYY</t>
+  </si>
+  <si>
+    <t>personBirthDateYYYY</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personPostalCode</t>
+  </si>
+  <si>
+    <t>personPostalCode</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personCity</t>
+  </si>
+  <si>
+    <t>personCity</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personStreet</t>
+  </si>
+  <si>
+    <t>personStreet</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personHouseNumber</t>
+  </si>
+  <si>
+    <t>personHouseNumber</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personPhone</t>
+  </si>
+  <si>
+    <t>personPhone</t>
+  </si>
+  <si>
+    <t>ExternalMessage.personEmail</t>
+  </si>
+  <si>
+    <t>personEmail</t>
+  </si>
+  <si>
+    <t>ExternalMessage.sample</t>
+  </si>
+  <si>
+    <t>ExternalMessage.testReports</t>
+  </si>
+  <si>
+    <t>testReports</t>
+  </si>
+  <si>
+    <t>List of TestReport</t>
+  </si>
+  <si>
+    <t>ExternalMessage.externalMessageDetails</t>
+  </si>
+  <si>
+    <t>externalMessageDetails</t>
+  </si>
+  <si>
+    <t>ExternalMessage.reportId</t>
+  </si>
+  <si>
+    <t>reportId</t>
+  </si>
+  <si>
+    <t>Report ID</t>
+  </si>
+  <si>
+    <t>ExternalMessage.sampleOverallTestResult</t>
+  </si>
+  <si>
+    <t>sampleOverallTestResult</t>
+  </si>
+  <si>
+    <t>Overall test result</t>
+  </si>
+  <si>
+    <t>ExternalMessage.status</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>ExternalMessageStatus</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ExternalMessage.assignee</t>
+  </si>
+  <si>
+    <t>assignee</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>ExternalMessage.reportingUser</t>
+  </si>
+  <si>
+    <t>LAB_MESSAGE</t>
+  </si>
+  <si>
+    <t>Lab message</t>
+  </si>
+  <si>
+    <t>PHYSICIANS_REPORT</t>
+  </si>
+  <si>
+    <t>Physician's report</t>
+  </si>
+  <si>
+    <t>UNPROCESSED</t>
+  </si>
+  <si>
+    <t>Unprocessed</t>
+  </si>
+  <si>
+    <t>FORWARDED</t>
+  </si>
+  <si>
+    <t>Forwarded</t>
+  </si>
+  <si>
+    <t>UNCLEAR</t>
+  </si>
+  <si>
+    <t>Unclear</t>
+  </si>
+  <si>
+    <t>TestReport.labMessage</t>
+  </si>
+  <si>
+    <t>labMessage</t>
+  </si>
+  <si>
+    <t>ExternalMessageReference</t>
+  </si>
+  <si>
+    <t>TestReport.testLabName</t>
+  </si>
+  <si>
+    <t>testLabName</t>
   </si>
   <si>
     <t>Lab name</t>
   </si>
   <si>
-    <t>LabMessage.labExternalId</t>
-  </si>
-  <si>
-    <t>labExternalId</t>
-  </si>
-  <si>
-    <t>Lab external ID</t>
-  </si>
-  <si>
-    <t>LabMessage.labPostalCode</t>
-  </si>
-  <si>
-    <t>labPostalCode</t>
+    <t>TestReport.testLabExternalId</t>
+  </si>
+  <si>
+    <t>testLabExternalId</t>
+  </si>
+  <si>
+    <t>TestReport.testLabPostalCode</t>
+  </si>
+  <si>
+    <t>testLabPostalCode</t>
   </si>
   <si>
     <t>Lab postal code</t>
   </si>
   <si>
-    <t>LabMessage.labCity</t>
-  </si>
-  <si>
-    <t>labCity</t>
+    <t>TestReport.testLabCity</t>
+  </si>
+  <si>
+    <t>testLabCity</t>
   </si>
   <si>
     <t>Lab city</t>
-  </si>
-  <si>
-    <t>LabMessage.personFirstName</t>
-  </si>
-  <si>
-    <t>personFirstName</t>
-  </si>
-  <si>
-    <t>LabMessage.personLastName</t>
-  </si>
-  <si>
-    <t>personLastName</t>
-  </si>
-  <si>
-    <t>LabMessage.personSex</t>
-  </si>
-  <si>
-    <t>personSex</t>
-  </si>
-  <si>
-    <t>LabMessage.personBirthDateDD</t>
-  </si>
-  <si>
-    <t>personBirthDateDD</t>
-  </si>
-  <si>
-    <t>LabMessage.personBirthDateMM</t>
-  </si>
-  <si>
-    <t>personBirthDateMM</t>
-  </si>
-  <si>
-    <t>LabMessage.personBirthDateYYYY</t>
-  </si>
-  <si>
-    <t>personBirthDateYYYY</t>
-  </si>
-  <si>
-    <t>LabMessage.personPostalCode</t>
-  </si>
-  <si>
-    <t>personPostalCode</t>
-  </si>
-  <si>
-    <t>LabMessage.personCity</t>
-  </si>
-  <si>
-    <t>personCity</t>
-  </si>
-  <si>
-    <t>LabMessage.personStreet</t>
-  </si>
-  <si>
-    <t>personStreet</t>
-  </si>
-  <si>
-    <t>LabMessage.personHouseNumber</t>
-  </si>
-  <si>
-    <t>personHouseNumber</t>
-  </si>
-  <si>
-    <t>LabMessage.personPhone</t>
-  </si>
-  <si>
-    <t>personPhone</t>
-  </si>
-  <si>
-    <t>LabMessage.personEmail</t>
-  </si>
-  <si>
-    <t>personEmail</t>
-  </si>
-  <si>
-    <t>LabMessage.sample</t>
-  </si>
-  <si>
-    <t>LabMessage.testReports</t>
-  </si>
-  <si>
-    <t>testReports</t>
-  </si>
-  <si>
-    <t>List of TestReport</t>
-  </si>
-  <si>
-    <t>LabMessage.labMessageDetails</t>
-  </si>
-  <si>
-    <t>labMessageDetails</t>
-  </si>
-  <si>
-    <t>Lab message details</t>
-  </si>
-  <si>
-    <t>LabMessage.reportId</t>
-  </si>
-  <si>
-    <t>reportId</t>
-  </si>
-  <si>
-    <t>Report ID</t>
-  </si>
-  <si>
-    <t>LabMessage.sampleOverallTestResult</t>
-  </si>
-  <si>
-    <t>sampleOverallTestResult</t>
-  </si>
-  <si>
-    <t>Overall test result</t>
-  </si>
-  <si>
-    <t>LabMessage.status</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>LabMessageStatus</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>LabMessage.assignee</t>
-  </si>
-  <si>
-    <t>assignee</t>
-  </si>
-  <si>
-    <t>Assignee</t>
-  </si>
-  <si>
-    <t>LabMessage.reportingUser</t>
-  </si>
-  <si>
-    <t>LAB_MESSAGE</t>
-  </si>
-  <si>
-    <t>Lab message</t>
-  </si>
-  <si>
-    <t>PHYSICIANS_REPORT</t>
-  </si>
-  <si>
-    <t>Physician's report</t>
-  </si>
-  <si>
-    <t>UNPROCESSED</t>
-  </si>
-  <si>
-    <t>Unprocessed</t>
-  </si>
-  <si>
-    <t>FORWARDED</t>
-  </si>
-  <si>
-    <t>Forwarded</t>
-  </si>
-  <si>
-    <t>UNCLEAR</t>
-  </si>
-  <si>
-    <t>Unclear</t>
-  </si>
-  <si>
-    <t>TestReport.labMessage</t>
-  </si>
-  <si>
-    <t>labMessage</t>
-  </si>
-  <si>
-    <t>LabMessageReference</t>
-  </si>
-  <si>
-    <t>TestReport.testLabName</t>
-  </si>
-  <si>
-    <t>testLabName</t>
-  </si>
-  <si>
-    <t>TestReport.testLabExternalId</t>
-  </si>
-  <si>
-    <t>testLabExternalId</t>
-  </si>
-  <si>
-    <t>TestReport.testLabPostalCode</t>
-  </si>
-  <si>
-    <t>testLabPostalCode</t>
-  </si>
-  <si>
-    <t>TestReport.testLabCity</t>
-  </si>
-  <si>
-    <t>testLabCity</t>
   </si>
   <si>
     <t>TestReport.testType</t>
@@ -14735,7 +14741,7 @@
 </file>
 
 <file path=xl/tables/table211.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A1:L34" displayName="Lab_Message" name="Lab_Message">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A1:L34" displayName="Message" name="Message">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14756,7 +14762,7 @@
 </file>
 
 <file path=xl/tables/table212.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A36:E38" displayName="Lab_MessageExternalMessageType" name="Lab_MessageExternalMessageType">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A36:E38" displayName="MessageExternalMessageType" name="MessageExternalMessageType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14770,7 +14776,7 @@
 </file>
 
 <file path=xl/tables/table213.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A40:E96" displayName="Lab_MessageDisease" name="Lab_MessageDisease">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A40:E96" displayName="MessageDisease" name="MessageDisease">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14784,7 +14790,7 @@
 </file>
 
 <file path=xl/tables/table214.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A98:E122" displayName="Lab_MessageSampleMaterial" name="Lab_MessageSampleMaterial">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A98:E122" displayName="MessageSampleMaterial" name="MessageSampleMaterial">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14798,7 +14804,7 @@
 </file>
 
 <file path=xl/tables/table215.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A124:E126" displayName="Lab_MessageSpecimenCondition" name="Lab_MessageSpecimenCondition">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A124:E126" displayName="MessageSpecimenCondition" name="MessageSpecimenCondition">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14812,7 +14818,7 @@
 </file>
 
 <file path=xl/tables/table216.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="216" ref="A128:E132" displayName="Lab_MessageSex" name="Lab_MessageSex">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="216" ref="A128:E132" displayName="MessageSex" name="MessageSex">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14826,7 +14832,7 @@
 </file>
 
 <file path=xl/tables/table217.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="217" ref="A134:E139" displayName="Lab_MessagePathogenTestResultType" name="Lab_MessagePathogenTestResultType">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="217" ref="A134:E139" displayName="MessagePathogenTestResultType" name="MessagePathogenTestResultType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14840,7 +14846,7 @@
 </file>
 
 <file path=xl/tables/table218.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="218" ref="A141:E145" displayName="Lab_MessageLabMessageStatus" name="Lab_MessageLabMessageStatus">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="218" ref="A141:E145" displayName="MessageExternalMessageStatus" name="MessageExternalMessageStatus">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -61082,7 +61088,7 @@
       </c>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>4189</v>
+        <v>27</v>
       </c>
       <c r="F29" t="s" s="1">
         <v>27</v>
@@ -61098,17 +61104,17 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>4189</v>
+      </c>
+      <c r="B30" t="s">
         <v>4190</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4191</v>
       </c>
       <c r="C30" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="s">
-        <v>4192</v>
+        <v>4191</v>
       </c>
       <c r="F30" t="s" s="1">
         <v>27</v>
@@ -61124,17 +61130,17 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>4192</v>
+      </c>
+      <c r="B31" t="s">
         <v>4193</v>
-      </c>
-      <c r="B31" t="s">
-        <v>4194</v>
       </c>
       <c r="C31" t="s" s="1">
         <v>2949</v>
       </c>
       <c r="D31"/>
       <c r="E31" t="s">
-        <v>4195</v>
+        <v>4194</v>
       </c>
       <c r="F31" t="s" s="1">
         <v>27</v>
@@ -61150,17 +61156,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>4195</v>
+      </c>
+      <c r="B32" t="s">
         <v>4196</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s" s="1">
         <v>4197</v>
-      </c>
-      <c r="C32" t="s" s="1">
-        <v>4198</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>4199</v>
+        <v>4198</v>
       </c>
       <c r="F32" t="s" s="1">
         <v>27</v>
@@ -61176,17 +61182,17 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>4199</v>
+      </c>
+      <c r="B33" t="s">
         <v>4200</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4201</v>
       </c>
       <c r="C33" t="s" s="1">
         <v>772</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>4202</v>
+        <v>4201</v>
       </c>
       <c r="F33" t="s" s="1">
         <v>27</v>
@@ -61202,7 +61208,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>4203</v>
+        <v>4202</v>
       </c>
       <c r="B34" t="s">
         <v>771</v>
@@ -61248,10 +61254,10 @@
         <v>4133</v>
       </c>
       <c r="B37" t="s">
+        <v>4203</v>
+      </c>
+      <c r="C37" t="s">
         <v>4204</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4205</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -61263,10 +61269,10 @@
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
+        <v>4205</v>
+      </c>
+      <c r="C38" t="s">
         <v>4206</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4207</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
@@ -62754,13 +62760,13 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>4198</v>
+        <v>4197</v>
       </c>
       <c r="B142" t="s">
+        <v>4207</v>
+      </c>
+      <c r="C142" t="s">
         <v>4208</v>
-      </c>
-      <c r="C142" t="s">
-        <v>4209</v>
       </c>
       <c r="D142" t="s">
         <v>27</v>
@@ -62787,10 +62793,10 @@
     <row r="144">
       <c r="A144"/>
       <c r="B144" t="s">
+        <v>4209</v>
+      </c>
+      <c r="C144" t="s">
         <v>4210</v>
-      </c>
-      <c r="C144" t="s">
-        <v>4211</v>
       </c>
       <c r="D144" t="s">
         <v>27</v>
@@ -62802,10 +62808,10 @@
     <row r="145">
       <c r="A145"/>
       <c r="B145" t="s">
+        <v>4211</v>
+      </c>
+      <c r="C145" t="s">
         <v>4212</v>
-      </c>
-      <c r="C145" t="s">
-        <v>4213</v>
       </c>
       <c r="D145" t="s">
         <v>27</v>
@@ -62891,13 +62897,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>4213</v>
+      </c>
+      <c r="B2" t="s">
         <v>4214</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s" s="1">
         <v>4215</v>
-      </c>
-      <c r="C2" t="s" s="1">
-        <v>4216</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -62919,17 +62925,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>4216</v>
+      </c>
+      <c r="B3" t="s">
         <v>4217</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4218</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4149</v>
+        <v>4218</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -62981,7 +62987,7 @@
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4155</v>
+        <v>4223</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -62997,17 +63003,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4223</v>
+        <v>4224</v>
       </c>
       <c r="B6" t="s">
-        <v>4224</v>
+        <v>4225</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4158</v>
+        <v>4226</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -63023,7 +63029,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4225</v>
+        <v>4227</v>
       </c>
       <c r="B7" t="s">
         <v>3158</v>
@@ -63049,7 +63055,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4226</v>
+        <v>4228</v>
       </c>
       <c r="B8" t="s">
         <v>3170</v>
@@ -63075,7 +63081,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4227</v>
+        <v>4229</v>
       </c>
       <c r="B9" t="s">
         <v>3180</v>
@@ -63101,7 +63107,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4228</v>
+        <v>4230</v>
       </c>
       <c r="B10" t="s">
         <v>3188</v>
@@ -63127,7 +63133,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4229</v>
+        <v>4231</v>
       </c>
       <c r="B11" t="s">
         <v>3184</v>
@@ -63153,7 +63159,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4230</v>
+        <v>4232</v>
       </c>
       <c r="B12" t="s">
         <v>3155</v>
@@ -63179,7 +63185,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4231</v>
+        <v>4233</v>
       </c>
       <c r="B13" t="s">
         <v>195</v>
@@ -63205,7 +63211,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4232</v>
+        <v>4234</v>
       </c>
       <c r="B14" t="s">
         <v>3208</v>
@@ -63231,7 +63237,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4233</v>
+        <v>4235</v>
       </c>
       <c r="B15" t="s">
         <v>3146</v>
@@ -63257,7 +63263,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4234</v>
+        <v>4236</v>
       </c>
       <c r="B16" t="s">
         <v>3153</v>
@@ -63283,7 +63289,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4235</v>
+        <v>4237</v>
       </c>
       <c r="B17" t="s">
         <v>3211</v>
@@ -63309,10 +63315,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4236</v>
+        <v>4238</v>
       </c>
       <c r="B18" t="s">
-        <v>4237</v>
+        <v>4239</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3163</v>
@@ -63831,12 +63837,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4238</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4239</v>
+        <v>4241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Data Dictionary and User Rights file
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16535" uniqueCount="4242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16568" uniqueCount="4245">
   <si>
     <t>Field ID</t>
   </si>
@@ -12502,13 +12502,13 @@
     <t>Reporter name</t>
   </si>
   <si>
-    <t>ExternalMessage.labExternalId</t>
-  </si>
-  <si>
-    <t>labExternalId</t>
-  </si>
-  <si>
-    <t>Lab external ID</t>
+    <t>ExternalMessage.reporterExternalIds</t>
+  </si>
+  <si>
+    <t>reporterExternalIds</t>
+  </si>
+  <si>
+    <t>List of String</t>
   </si>
   <si>
     <t>ExternalMessage.reporterPostalCode</t>
@@ -12547,6 +12547,12 @@
     <t>personSex</t>
   </si>
   <si>
+    <t>ExternalMessage.personPresentCondition</t>
+  </si>
+  <si>
+    <t>personPresentCondition</t>
+  </si>
+  <si>
     <t>ExternalMessage.personBirthDateDD</t>
   </si>
   <si>
@@ -12604,6 +12610,9 @@
     <t>ExternalMessage.sample</t>
   </si>
   <si>
+    <t>ExternalMessage.caze</t>
+  </si>
+  <si>
     <t>ExternalMessage.testReports</t>
   </si>
   <si>
@@ -12709,10 +12718,10 @@
     <t>Lab name</t>
   </si>
   <si>
-    <t>TestReport.testLabExternalId</t>
-  </si>
-  <si>
-    <t>testLabExternalId</t>
+    <t>TestReport.testLabExternalIds</t>
+  </si>
+  <si>
+    <t>testLabExternalIds</t>
   </si>
   <si>
     <t>TestReport.testLabPostalCode</t>
@@ -14741,7 +14750,7 @@
 </file>
 
 <file path=xl/tables/table211.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A1:L34" displayName="Message" name="Message">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A1:L36" displayName="Message" name="Message">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14762,7 +14771,7 @@
 </file>
 
 <file path=xl/tables/table212.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A36:E38" displayName="MessageExternalMessageType" name="MessageExternalMessageType">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A38:E40" displayName="MessageExternalMessageType" name="MessageExternalMessageType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14776,7 +14785,7 @@
 </file>
 
 <file path=xl/tables/table213.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A40:E96" displayName="MessageDisease" name="MessageDisease">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A42:E98" displayName="MessageDisease" name="MessageDisease">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14790,7 +14799,7 @@
 </file>
 
 <file path=xl/tables/table214.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A98:E122" displayName="MessageSampleMaterial" name="MessageSampleMaterial">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A100:E124" displayName="MessageSampleMaterial" name="MessageSampleMaterial">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14804,7 +14813,7 @@
 </file>
 
 <file path=xl/tables/table215.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A124:E126" displayName="MessageSpecimenCondition" name="MessageSpecimenCondition">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A126:E128" displayName="MessageSpecimenCondition" name="MessageSpecimenCondition">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14818,7 +14827,7 @@
 </file>
 
 <file path=xl/tables/table216.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="216" ref="A128:E132" displayName="MessageSex" name="MessageSex">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="216" ref="A130:E134" displayName="MessageSex" name="MessageSex">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14832,7 +14841,7 @@
 </file>
 
 <file path=xl/tables/table217.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="217" ref="A134:E139" displayName="MessagePathogenTestResultType" name="MessagePathogenTestResultType">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="217" ref="A136:E140" displayName="MessagePresentCondition" name="MessagePresentCondition">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14846,7 +14855,7 @@
 </file>
 
 <file path=xl/tables/table218.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="218" ref="A141:E145" displayName="MessageExternalMessageStatus" name="MessageExternalMessageStatus">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="218" ref="A142:E147" displayName="MessagePathogenTestResultType" name="MessagePathogenTestResultType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14860,7 +14869,35 @@
 </file>
 
 <file path=xl/tables/table219.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="219" ref="A1:L18" displayName="Test_report" name="Test_report">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="219" ref="A149:E153" displayName="MessageExternalMessageStatus" name="MessageExternalMessageStatus">
+  <autoFilter/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Type"/>
+    <tableColumn id="2" name="Value"/>
+    <tableColumn id="3" name="Caption"/>
+    <tableColumn id="4" name="Description"/>
+    <tableColumn id="5" name="Short"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" ref="A38:E45" displayName="LocationPersonAddressType" name="LocationPersonAddressType">
+  <autoFilter/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Type"/>
+    <tableColumn id="2" name="Value"/>
+    <tableColumn id="3" name="Caption"/>
+    <tableColumn id="4" name="Description"/>
+    <tableColumn id="5" name="Short"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
+</table>
+</file>
+
+<file path=xl/tables/table220.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="220" ref="A1:L18" displayName="Test_report" name="Test_report">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14880,36 +14917,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" ref="A38:E45" displayName="LocationPersonAddressType" name="LocationPersonAddressType">
-  <autoFilter/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Type"/>
-    <tableColumn id="2" name="Value"/>
-    <tableColumn id="3" name="Caption"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Short"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
-</table>
-</file>
-
-<file path=xl/tables/table220.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="220" ref="A20:E41" displayName="Test_reportPathogenTestType" name="Test_reportPathogenTestType">
-  <autoFilter/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Type"/>
-    <tableColumn id="2" name="Value"/>
-    <tableColumn id="3" name="Caption"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Short"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
-</table>
-</file>
-
 <file path=xl/tables/table221.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="221" ref="A43:E48" displayName="Test_reportPathogenTestResultType" name="Test_reportPathogenTestResultType">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="221" ref="A20:E41" displayName="Test_reportPathogenTestType" name="Test_reportPathogenTestType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14923,7 +14932,21 @@
 </file>
 
 <file path=xl/tables/table222.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="222" ref="A50:E52" displayName="Test_reportPCRTestSpecification" name="Test_reportPCRTestSpecification">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="222" ref="A43:E48" displayName="Test_reportPathogenTestResultType" name="Test_reportPathogenTestResultType">
+  <autoFilter/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Type"/>
+    <tableColumn id="2" name="Value"/>
+    <tableColumn id="3" name="Caption"/>
+    <tableColumn id="4" name="Description"/>
+    <tableColumn id="5" name="Short"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
+</table>
+</file>
+
+<file path=xl/tables/table223.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="223" ref="A50:E52" displayName="Test_reportPCRTestSpecification" name="Test_reportPCRTestSpecification">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -60245,10 +60268,10 @@
     <row r="109">
       <c r="A109"/>
       <c r="B109" t="s">
-        <v>4130</v>
+        <v>1226</v>
       </c>
       <c r="C109" t="s">
-        <v>703</v>
+        <v>944</v>
       </c>
       <c r="D109" t="s">
         <v>27</v>
@@ -60260,10 +60283,10 @@
     <row r="110">
       <c r="A110"/>
       <c r="B110" t="s">
-        <v>284</v>
+        <v>4130</v>
       </c>
       <c r="C110" t="s">
-        <v>285</v>
+        <v>703</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -60275,10 +60298,10 @@
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>4131</v>
+        <v>284</v>
       </c>
       <c r="C111" t="s">
-        <v>4131</v>
+        <v>285</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -60290,10 +60313,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>1226</v>
+        <v>4131</v>
       </c>
       <c r="C112" t="s">
-        <v>944</v>
+        <v>4131</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
@@ -60316,7 +60339,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L153"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -60642,11 +60665,11 @@
         <v>4151</v>
       </c>
       <c r="C12" t="s" s="1">
-        <v>14</v>
+        <v>4152</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>4152</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s" s="1">
         <v>27</v>
@@ -60798,11 +60821,11 @@
         <v>4166</v>
       </c>
       <c r="C18" t="s" s="1">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s" s="1">
         <v>27</v>
@@ -60828,7 +60851,7 @@
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s" s="1">
         <v>27</v>
@@ -60854,7 +60877,7 @@
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s" s="1">
         <v>27</v>
@@ -60876,11 +60899,11 @@
         <v>4172</v>
       </c>
       <c r="C21" t="s" s="1">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>684</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s" s="1">
         <v>27</v>
@@ -60906,7 +60929,7 @@
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>664</v>
+        <v>684</v>
       </c>
       <c r="F22" t="s" s="1">
         <v>27</v>
@@ -60932,7 +60955,7 @@
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>687</v>
+        <v>664</v>
       </c>
       <c r="F23" t="s" s="1">
         <v>27</v>
@@ -60958,7 +60981,7 @@
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="F24" t="s" s="1">
         <v>27</v>
@@ -60984,7 +61007,7 @@
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>690</v>
       </c>
       <c r="F25" t="s" s="1">
         <v>27</v>
@@ -61029,10 +61052,10 @@
         <v>4183</v>
       </c>
       <c r="B27" t="s">
-        <v>3140</v>
+        <v>4184</v>
       </c>
       <c r="C27" t="s" s="1">
-        <v>2940</v>
+        <v>14</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
@@ -61052,13 +61075,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4184</v>
+        <v>4185</v>
       </c>
       <c r="B28" t="s">
-        <v>4185</v>
+        <v>3140</v>
       </c>
       <c r="C28" t="s" s="1">
-        <v>4186</v>
+        <v>2940</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
@@ -61078,13 +61101,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>4187</v>
+        <v>4186</v>
       </c>
       <c r="B29" t="s">
-        <v>4188</v>
+        <v>1588</v>
       </c>
       <c r="C29" t="s" s="1">
-        <v>14</v>
+        <v>1589</v>
       </c>
       <c r="D29"/>
       <c r="E29" t="s">
@@ -61104,17 +61127,17 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>4187</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4188</v>
+      </c>
+      <c r="C30" t="s" s="1">
         <v>4189</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4190</v>
-      </c>
-      <c r="C30" t="s" s="1">
-        <v>14</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="s">
-        <v>4191</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s" s="1">
         <v>27</v>
@@ -61130,17 +61153,17 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4192</v>
+        <v>4190</v>
       </c>
       <c r="B31" t="s">
-        <v>4193</v>
+        <v>4191</v>
       </c>
       <c r="C31" t="s" s="1">
-        <v>2949</v>
+        <v>14</v>
       </c>
       <c r="D31"/>
       <c r="E31" t="s">
-        <v>4194</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s" s="1">
         <v>27</v>
@@ -61156,17 +61179,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>4195</v>
+        <v>4192</v>
       </c>
       <c r="B32" t="s">
-        <v>4196</v>
+        <v>4193</v>
       </c>
       <c r="C32" t="s" s="1">
-        <v>4197</v>
+        <v>14</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>4198</v>
+        <v>4194</v>
       </c>
       <c r="F32" t="s" s="1">
         <v>27</v>
@@ -61182,17 +61205,17 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>4199</v>
+        <v>4195</v>
       </c>
       <c r="B33" t="s">
-        <v>4200</v>
+        <v>4196</v>
       </c>
       <c r="C33" t="s" s="1">
-        <v>772</v>
+        <v>2949</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>4201</v>
+        <v>4197</v>
       </c>
       <c r="F33" t="s" s="1">
         <v>27</v>
@@ -61208,17 +61231,17 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>4202</v>
+        <v>4198</v>
       </c>
       <c r="B34" t="s">
-        <v>771</v>
+        <v>4199</v>
       </c>
       <c r="C34" t="s" s="1">
-        <v>772</v>
+        <v>4200</v>
       </c>
       <c r="D34"/>
       <c r="E34" t="s">
-        <v>773</v>
+        <v>4201</v>
       </c>
       <c r="F34" t="s" s="1">
         <v>27</v>
@@ -61232,201 +61255,223 @@
       <c r="K34"/>
       <c r="L34"/>
     </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>4202</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4203</v>
+      </c>
+      <c r="C35" t="s" s="1">
+        <v>772</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35" t="s">
+        <v>4204</v>
+      </c>
+      <c r="F35" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+    </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>4205</v>
+      </c>
+      <c r="B36" t="s">
+        <v>771</v>
+      </c>
+      <c r="C36" t="s" s="1">
+        <v>772</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36" t="s">
+        <v>773</v>
+      </c>
+      <c r="F36" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
         <v>2</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>213</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>4</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" t="s">
         <v>5</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E38" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="s">
+    <row r="39">
+      <c r="A39" t="s">
         <v>4133</v>
       </c>
-      <c r="B37" t="s">
-        <v>4203</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4204</v>
-      </c>
-      <c r="D37" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38"/>
-      <c r="B38" t="s">
-        <v>4205</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B39" t="s">
         <v>4206</v>
       </c>
-      <c r="D38" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="C39" t="s">
+        <v>4207</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
+      <c r="A40"/>
+      <c r="B40" t="s">
+        <v>4208</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4209</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
         <v>2</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>213</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>4</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D42" t="s">
         <v>5</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E42" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s">
+    <row r="43">
+      <c r="A43" t="s">
         <v>123</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>378</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>379</v>
       </c>
-      <c r="D41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" t="s">
         <v>378</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42"/>
-      <c r="B42" t="s">
-        <v>380</v>
-      </c>
-      <c r="C42" t="s">
-        <v>381</v>
-      </c>
-      <c r="D42" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43"/>
-      <c r="B43" t="s">
-        <v>382</v>
-      </c>
-      <c r="C43" t="s">
-        <v>383</v>
-      </c>
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C44" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
       </c>
       <c r="E44" t="s">
-        <v>386</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C45" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D45" t="s">
         <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>389</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C46" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C47" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>27</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C48" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>27</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C49" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -61438,10 +61483,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C50" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
@@ -61453,25 +61498,25 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C51" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
       </c>
       <c r="E51" t="s">
-        <v>402</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C52" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D52" t="s">
         <v>27</v>
@@ -61483,85 +61528,85 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C53" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D53" t="s">
         <v>27</v>
       </c>
       <c r="E53" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C54" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D54" t="s">
         <v>27</v>
       </c>
       <c r="E54" t="s">
-        <v>410</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55">
       <c r="A55"/>
       <c r="B55" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C55" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D55" t="s">
         <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>27</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C56" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
       </c>
       <c r="E56" t="s">
-        <v>27</v>
+        <v>410</v>
       </c>
     </row>
     <row r="57">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C57" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D57" t="s">
         <v>27</v>
       </c>
       <c r="E57" t="s">
-        <v>417</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C58" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D58" t="s">
         <v>27</v>
@@ -61573,25 +61618,25 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C59" t="s">
-        <v>185</v>
+        <v>416</v>
       </c>
       <c r="D59" t="s">
         <v>27</v>
       </c>
       <c r="E59" t="s">
-        <v>27</v>
+        <v>417</v>
       </c>
     </row>
     <row r="60">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C60" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D60" t="s">
         <v>27</v>
@@ -61603,10 +61648,10 @@
     <row r="61">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C61" t="s">
-        <v>424</v>
+        <v>185</v>
       </c>
       <c r="D61" t="s">
         <v>27</v>
@@ -61618,10 +61663,10 @@
     <row r="62">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C62" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="D62" t="s">
         <v>27</v>
@@ -61633,10 +61678,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C63" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D63" t="s">
         <v>27</v>
@@ -61648,10 +61693,10 @@
     <row r="64">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C64" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D64" t="s">
         <v>27</v>
@@ -61663,10 +61708,10 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C65" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
@@ -61678,10 +61723,10 @@
     <row r="66">
       <c r="A66"/>
       <c r="B66" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C66" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D66" t="s">
         <v>27</v>
@@ -61693,10 +61738,10 @@
     <row r="67">
       <c r="A67"/>
       <c r="B67" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C67" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D67" t="s">
         <v>27</v>
@@ -61708,10 +61753,10 @@
     <row r="68">
       <c r="A68"/>
       <c r="B68" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C68" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D68" t="s">
         <v>27</v>
@@ -61723,10 +61768,10 @@
     <row r="69">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C69" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D69" t="s">
         <v>27</v>
@@ -61738,10 +61783,10 @@
     <row r="70">
       <c r="A70"/>
       <c r="B70" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C70" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D70" t="s">
         <v>27</v>
@@ -61753,10 +61798,10 @@
     <row r="71">
       <c r="A71"/>
       <c r="B71" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C71" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D71" t="s">
         <v>27</v>
@@ -61768,10 +61813,10 @@
     <row r="72">
       <c r="A72"/>
       <c r="B72" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C72" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
@@ -61783,10 +61828,10 @@
     <row r="73">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C73" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D73" t="s">
         <v>27</v>
@@ -61798,10 +61843,10 @@
     <row r="74">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C74" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D74" t="s">
         <v>27</v>
@@ -61813,10 +61858,10 @@
     <row r="75">
       <c r="A75"/>
       <c r="B75" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C75" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D75" t="s">
         <v>27</v>
@@ -61828,10 +61873,10 @@
     <row r="76">
       <c r="A76"/>
       <c r="B76" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C76" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D76" t="s">
         <v>27</v>
@@ -61843,10 +61888,10 @@
     <row r="77">
       <c r="A77"/>
       <c r="B77" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C77" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D77" t="s">
         <v>27</v>
@@ -61858,10 +61903,10 @@
     <row r="78">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C78" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D78" t="s">
         <v>27</v>
@@ -61873,10 +61918,10 @@
     <row r="79">
       <c r="A79"/>
       <c r="B79" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C79" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D79" t="s">
         <v>27</v>
@@ -61888,10 +61933,10 @@
     <row r="80">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C80" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D80" t="s">
         <v>27</v>
@@ -61903,10 +61948,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C81" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D81" t="s">
         <v>27</v>
@@ -61918,10 +61963,10 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C82" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
@@ -61933,10 +61978,10 @@
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C83" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
@@ -61948,10 +61993,10 @@
     <row r="84">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C84" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D84" t="s">
         <v>27</v>
@@ -61963,10 +62008,10 @@
     <row r="85">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C85" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D85" t="s">
         <v>27</v>
@@ -61978,10 +62023,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C86" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D86" t="s">
         <v>27</v>
@@ -61993,10 +62038,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C87" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D87" t="s">
         <v>27</v>
@@ -62008,70 +62053,70 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C88" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D88" t="s">
         <v>27</v>
       </c>
       <c r="E88" t="s">
-        <v>478</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C89" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D89" t="s">
         <v>27</v>
       </c>
       <c r="E89" t="s">
-        <v>481</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C90" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="D90" t="s">
         <v>27</v>
       </c>
       <c r="E90" t="s">
-        <v>27</v>
+        <v>478</v>
       </c>
     </row>
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C91" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D91" t="s">
         <v>27</v>
       </c>
       <c r="E91" t="s">
-        <v>27</v>
+        <v>481</v>
       </c>
     </row>
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C92" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -62083,10 +62128,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C93" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
@@ -62098,10 +62143,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C94" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D94" t="s">
         <v>27</v>
@@ -62113,89 +62158,89 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>234</v>
+        <v>488</v>
       </c>
       <c r="C95" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D95" t="s">
         <v>27</v>
       </c>
       <c r="E95" t="s">
-        <v>235</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
+        <v>490</v>
+      </c>
+      <c r="C96" t="s">
+        <v>491</v>
+      </c>
+      <c r="D96" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97"/>
+      <c r="B97" t="s">
+        <v>234</v>
+      </c>
+      <c r="C97" t="s">
+        <v>492</v>
+      </c>
+      <c r="D97" t="s">
+        <v>27</v>
+      </c>
+      <c r="E97" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98"/>
+      <c r="B98" t="s">
         <v>493</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>494</v>
       </c>
-      <c r="D96" t="s">
-        <v>27</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="D98" t="s">
+        <v>27</v>
+      </c>
+      <c r="E98" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="s">
+    <row r="100">
+      <c r="A100" t="s">
         <v>2</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>213</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C100" t="s">
         <v>4</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D100" t="s">
         <v>5</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E100" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="s">
+    <row r="101">
+      <c r="A101" t="s">
         <v>2902</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B101" t="s">
         <v>2981</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C101" t="s">
         <v>2982</v>
-      </c>
-      <c r="D99" t="s">
-        <v>27</v>
-      </c>
-      <c r="E99" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100"/>
-      <c r="B100" t="s">
-        <v>2983</v>
-      </c>
-      <c r="C100" t="s">
-        <v>2984</v>
-      </c>
-      <c r="D100" t="s">
-        <v>27</v>
-      </c>
-      <c r="E100" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101"/>
-      <c r="B101" t="s">
-        <v>2985</v>
-      </c>
-      <c r="C101" t="s">
-        <v>2986</v>
       </c>
       <c r="D101" t="s">
         <v>27</v>
@@ -62207,10 +62252,10 @@
     <row r="102">
       <c r="A102"/>
       <c r="B102" t="s">
-        <v>2987</v>
+        <v>2983</v>
       </c>
       <c r="C102" t="s">
-        <v>2988</v>
+        <v>2984</v>
       </c>
       <c r="D102" t="s">
         <v>27</v>
@@ -62222,10 +62267,10 @@
     <row r="103">
       <c r="A103"/>
       <c r="B103" t="s">
-        <v>2989</v>
+        <v>2985</v>
       </c>
       <c r="C103" t="s">
-        <v>2990</v>
+        <v>2986</v>
       </c>
       <c r="D103" t="s">
         <v>27</v>
@@ -62237,10 +62282,10 @@
     <row r="104">
       <c r="A104"/>
       <c r="B104" t="s">
-        <v>2991</v>
+        <v>2987</v>
       </c>
       <c r="C104" t="s">
-        <v>2992</v>
+        <v>2988</v>
       </c>
       <c r="D104" t="s">
         <v>27</v>
@@ -62252,10 +62297,10 @@
     <row r="105">
       <c r="A105"/>
       <c r="B105" t="s">
-        <v>2993</v>
+        <v>2989</v>
       </c>
       <c r="C105" t="s">
-        <v>2994</v>
+        <v>2990</v>
       </c>
       <c r="D105" t="s">
         <v>27</v>
@@ -62267,10 +62312,10 @@
     <row r="106">
       <c r="A106"/>
       <c r="B106" t="s">
-        <v>2995</v>
+        <v>2991</v>
       </c>
       <c r="C106" t="s">
-        <v>2996</v>
+        <v>2992</v>
       </c>
       <c r="D106" t="s">
         <v>27</v>
@@ -62282,10 +62327,10 @@
     <row r="107">
       <c r="A107"/>
       <c r="B107" t="s">
-        <v>2997</v>
+        <v>2993</v>
       </c>
       <c r="C107" t="s">
-        <v>2998</v>
+        <v>2994</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -62297,10 +62342,10 @@
     <row r="108">
       <c r="A108"/>
       <c r="B108" t="s">
-        <v>2999</v>
+        <v>2995</v>
       </c>
       <c r="C108" t="s">
-        <v>3000</v>
+        <v>2996</v>
       </c>
       <c r="D108" t="s">
         <v>27</v>
@@ -62312,10 +62357,10 @@
     <row r="109">
       <c r="A109"/>
       <c r="B109" t="s">
-        <v>3001</v>
+        <v>2997</v>
       </c>
       <c r="C109" t="s">
-        <v>3002</v>
+        <v>2998</v>
       </c>
       <c r="D109" t="s">
         <v>27</v>
@@ -62327,10 +62372,10 @@
     <row r="110">
       <c r="A110"/>
       <c r="B110" t="s">
-        <v>3003</v>
+        <v>2999</v>
       </c>
       <c r="C110" t="s">
-        <v>3004</v>
+        <v>3000</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -62342,10 +62387,10 @@
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>3005</v>
+        <v>3001</v>
       </c>
       <c r="C111" t="s">
-        <v>3006</v>
+        <v>3002</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -62357,10 +62402,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>3007</v>
+        <v>3003</v>
       </c>
       <c r="C112" t="s">
-        <v>3008</v>
+        <v>3004</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
@@ -62372,10 +62417,10 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>3009</v>
+        <v>3005</v>
       </c>
       <c r="C113" t="s">
-        <v>3010</v>
+        <v>3006</v>
       </c>
       <c r="D113" t="s">
         <v>27</v>
@@ -62387,10 +62432,10 @@
     <row r="114">
       <c r="A114"/>
       <c r="B114" t="s">
-        <v>3011</v>
+        <v>3007</v>
       </c>
       <c r="C114" t="s">
-        <v>3012</v>
+        <v>3008</v>
       </c>
       <c r="D114" t="s">
         <v>27</v>
@@ -62402,10 +62447,10 @@
     <row r="115">
       <c r="A115"/>
       <c r="B115" t="s">
-        <v>3013</v>
+        <v>3009</v>
       </c>
       <c r="C115" t="s">
-        <v>3014</v>
+        <v>3010</v>
       </c>
       <c r="D115" t="s">
         <v>27</v>
@@ -62417,10 +62462,10 @@
     <row r="116">
       <c r="A116"/>
       <c r="B116" t="s">
-        <v>3015</v>
+        <v>3011</v>
       </c>
       <c r="C116" t="s">
-        <v>3016</v>
+        <v>3012</v>
       </c>
       <c r="D116" t="s">
         <v>27</v>
@@ -62432,10 +62477,10 @@
     <row r="117">
       <c r="A117"/>
       <c r="B117" t="s">
-        <v>3017</v>
+        <v>3013</v>
       </c>
       <c r="C117" t="s">
-        <v>3018</v>
+        <v>3014</v>
       </c>
       <c r="D117" t="s">
         <v>27</v>
@@ -62447,10 +62492,10 @@
     <row r="118">
       <c r="A118"/>
       <c r="B118" t="s">
-        <v>3019</v>
+        <v>3015</v>
       </c>
       <c r="C118" t="s">
-        <v>3020</v>
+        <v>3016</v>
       </c>
       <c r="D118" t="s">
         <v>27</v>
@@ -62462,10 +62507,10 @@
     <row r="119">
       <c r="A119"/>
       <c r="B119" t="s">
-        <v>3021</v>
+        <v>3017</v>
       </c>
       <c r="C119" t="s">
-        <v>3022</v>
+        <v>3018</v>
       </c>
       <c r="D119" t="s">
         <v>27</v>
@@ -62477,10 +62522,10 @@
     <row r="120">
       <c r="A120"/>
       <c r="B120" t="s">
-        <v>3023</v>
+        <v>3019</v>
       </c>
       <c r="C120" t="s">
-        <v>3024</v>
+        <v>3020</v>
       </c>
       <c r="D120" t="s">
         <v>27</v>
@@ -62492,10 +62537,10 @@
     <row r="121">
       <c r="A121"/>
       <c r="B121" t="s">
-        <v>3025</v>
+        <v>3021</v>
       </c>
       <c r="C121" t="s">
-        <v>3026</v>
+        <v>3022</v>
       </c>
       <c r="D121" t="s">
         <v>27</v>
@@ -62507,123 +62552,123 @@
     <row r="122">
       <c r="A122"/>
       <c r="B122" t="s">
+        <v>3023</v>
+      </c>
+      <c r="C122" t="s">
+        <v>3024</v>
+      </c>
+      <c r="D122" t="s">
+        <v>27</v>
+      </c>
+      <c r="E122" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123"/>
+      <c r="B123" t="s">
+        <v>3025</v>
+      </c>
+      <c r="C123" t="s">
+        <v>3026</v>
+      </c>
+      <c r="D123" t="s">
+        <v>27</v>
+      </c>
+      <c r="E123" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124"/>
+      <c r="B124" t="s">
         <v>234</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C124" t="s">
         <v>235</v>
       </c>
-      <c r="D122" t="s">
-        <v>27</v>
-      </c>
-      <c r="E122" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="s">
+      <c r="D124" t="s">
+        <v>27</v>
+      </c>
+      <c r="E124" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
         <v>2</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B126" t="s">
         <v>213</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C126" t="s">
         <v>4</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D126" t="s">
         <v>5</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E126" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" t="s">
+    <row r="127">
+      <c r="A127" t="s">
         <v>2927</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B127" t="s">
         <v>3031</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C127" t="s">
         <v>3032</v>
       </c>
-      <c r="D125" t="s">
-        <v>27</v>
-      </c>
-      <c r="E125" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126"/>
-      <c r="B126" t="s">
+      <c r="D127" t="s">
+        <v>27</v>
+      </c>
+      <c r="E127" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128"/>
+      <c r="B128" t="s">
         <v>3033</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C128" t="s">
         <v>3034</v>
       </c>
-      <c r="D126" t="s">
-        <v>27</v>
-      </c>
-      <c r="E126" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s">
+      <c r="D128" t="s">
+        <v>27</v>
+      </c>
+      <c r="E128" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
         <v>2</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B130" t="s">
         <v>213</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C130" t="s">
         <v>4</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D130" t="s">
         <v>5</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E130" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" t="s">
+    <row r="131">
+      <c r="A131" t="s">
         <v>53</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B131" t="s">
         <v>236</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C131" t="s">
         <v>237</v>
-      </c>
-      <c r="D129" t="s">
-        <v>27</v>
-      </c>
-      <c r="E129" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130"/>
-      <c r="B130" t="s">
-        <v>238</v>
-      </c>
-      <c r="C130" t="s">
-        <v>239</v>
-      </c>
-      <c r="D130" t="s">
-        <v>27</v>
-      </c>
-      <c r="E130" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131"/>
-      <c r="B131" t="s">
-        <v>234</v>
-      </c>
-      <c r="C131" t="s">
-        <v>235</v>
       </c>
       <c r="D131" t="s">
         <v>27</v>
@@ -62635,74 +62680,74 @@
     <row r="132">
       <c r="A132"/>
       <c r="B132" t="s">
+        <v>238</v>
+      </c>
+      <c r="C132" t="s">
+        <v>239</v>
+      </c>
+      <c r="D132" t="s">
+        <v>27</v>
+      </c>
+      <c r="E132" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133"/>
+      <c r="B133" t="s">
+        <v>234</v>
+      </c>
+      <c r="C133" t="s">
+        <v>235</v>
+      </c>
+      <c r="D133" t="s">
+        <v>27</v>
+      </c>
+      <c r="E133" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134"/>
+      <c r="B134" t="s">
         <v>240</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C134" t="s">
         <v>241</v>
       </c>
-      <c r="D132" t="s">
-        <v>27</v>
-      </c>
-      <c r="E132" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="s">
+      <c r="D134" t="s">
+        <v>27</v>
+      </c>
+      <c r="E134" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
         <v>2</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B136" t="s">
         <v>213</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C136" t="s">
         <v>4</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D136" t="s">
         <v>5</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E136" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" t="s">
-        <v>2949</v>
-      </c>
-      <c r="B135" t="s">
-        <v>3041</v>
-      </c>
-      <c r="C135" t="s">
-        <v>3042</v>
-      </c>
-      <c r="D135" t="s">
-        <v>27</v>
-      </c>
-      <c r="E135" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136"/>
-      <c r="B136" t="s">
-        <v>1195</v>
-      </c>
-      <c r="C136" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E136" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="137">
-      <c r="A137"/>
+      <c r="A137" t="s">
+        <v>110</v>
+      </c>
       <c r="B137" t="s">
-        <v>3043</v>
+        <v>368</v>
       </c>
       <c r="C137" t="s">
-        <v>3044</v>
+        <v>369</v>
       </c>
       <c r="D137" t="s">
         <v>27</v>
@@ -62714,10 +62759,10 @@
     <row r="138">
       <c r="A138"/>
       <c r="B138" t="s">
-        <v>3045</v>
+        <v>370</v>
       </c>
       <c r="C138" t="s">
-        <v>3046</v>
+        <v>371</v>
       </c>
       <c r="D138" t="s">
         <v>27</v>
@@ -62729,10 +62774,10 @@
     <row r="139">
       <c r="A139"/>
       <c r="B139" t="s">
-        <v>3047</v>
+        <v>372</v>
       </c>
       <c r="C139" t="s">
-        <v>3048</v>
+        <v>373</v>
       </c>
       <c r="D139" t="s">
         <v>27</v>
@@ -62741,47 +62786,47 @@
         <v>27</v>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" t="s">
-        <v>2</v>
-      </c>
-      <c r="B141" t="s">
-        <v>213</v>
-      </c>
-      <c r="C141" t="s">
-        <v>4</v>
-      </c>
-      <c r="D141" t="s">
-        <v>5</v>
-      </c>
-      <c r="E141" t="s">
-        <v>223</v>
+    <row r="140">
+      <c r="A140"/>
+      <c r="B140" t="s">
+        <v>240</v>
+      </c>
+      <c r="C140" t="s">
+        <v>241</v>
+      </c>
+      <c r="D140" t="s">
+        <v>27</v>
+      </c>
+      <c r="E140" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>4197</v>
+        <v>2</v>
       </c>
       <c r="B142" t="s">
-        <v>4207</v>
+        <v>213</v>
       </c>
       <c r="C142" t="s">
-        <v>4208</v>
+        <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E142" t="s">
-        <v>27</v>
+        <v>223</v>
       </c>
     </row>
     <row r="143">
-      <c r="A143"/>
+      <c r="A143" t="s">
+        <v>2949</v>
+      </c>
       <c r="B143" t="s">
-        <v>2405</v>
+        <v>3041</v>
       </c>
       <c r="C143" t="s">
-        <v>2406</v>
+        <v>3042</v>
       </c>
       <c r="D143" t="s">
         <v>27</v>
@@ -62793,10 +62838,10 @@
     <row r="144">
       <c r="A144"/>
       <c r="B144" t="s">
-        <v>4209</v>
+        <v>1195</v>
       </c>
       <c r="C144" t="s">
-        <v>4210</v>
+        <v>1197</v>
       </c>
       <c r="D144" t="s">
         <v>27</v>
@@ -62808,15 +62853,124 @@
     <row r="145">
       <c r="A145"/>
       <c r="B145" t="s">
+        <v>3043</v>
+      </c>
+      <c r="C145" t="s">
+        <v>3044</v>
+      </c>
+      <c r="D145" t="s">
+        <v>27</v>
+      </c>
+      <c r="E145" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146"/>
+      <c r="B146" t="s">
+        <v>3045</v>
+      </c>
+      <c r="C146" t="s">
+        <v>3046</v>
+      </c>
+      <c r="D146" t="s">
+        <v>27</v>
+      </c>
+      <c r="E146" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147"/>
+      <c r="B147" t="s">
+        <v>3047</v>
+      </c>
+      <c r="C147" t="s">
+        <v>3048</v>
+      </c>
+      <c r="D147" t="s">
+        <v>27</v>
+      </c>
+      <c r="E147" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>2</v>
+      </c>
+      <c r="B149" t="s">
+        <v>213</v>
+      </c>
+      <c r="C149" t="s">
+        <v>4</v>
+      </c>
+      <c r="D149" t="s">
+        <v>5</v>
+      </c>
+      <c r="E149" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>4200</v>
+      </c>
+      <c r="B150" t="s">
+        <v>4210</v>
+      </c>
+      <c r="C150" t="s">
         <v>4211</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D150" t="s">
+        <v>27</v>
+      </c>
+      <c r="E150" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151"/>
+      <c r="B151" t="s">
+        <v>2405</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2406</v>
+      </c>
+      <c r="D151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E151" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152"/>
+      <c r="B152" t="s">
         <v>4212</v>
       </c>
-      <c r="D145" t="s">
-        <v>27</v>
-      </c>
-      <c r="E145" t="s">
+      <c r="C152" t="s">
+        <v>4213</v>
+      </c>
+      <c r="D152" t="s">
+        <v>27</v>
+      </c>
+      <c r="E152" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153"/>
+      <c r="B153" t="s">
+        <v>4214</v>
+      </c>
+      <c r="C153" t="s">
+        <v>4215</v>
+      </c>
+      <c r="D153" t="s">
+        <v>27</v>
+      </c>
+      <c r="E153" t="s">
         <v>27</v>
       </c>
     </row>
@@ -62831,6 +62985,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -62897,13 +63052,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4213</v>
+        <v>4216</v>
       </c>
       <c r="B2" t="s">
-        <v>4214</v>
+        <v>4217</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4215</v>
+        <v>4218</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -62925,17 +63080,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
       <c r="B3" t="s">
-        <v>4217</v>
+        <v>4220</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4218</v>
+        <v>4221</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -62951,17 +63106,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4219</v>
+        <v>4222</v>
       </c>
       <c r="B4" t="s">
-        <v>4220</v>
+        <v>4223</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>14</v>
+        <v>4152</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>4152</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -62977,17 +63132,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4221</v>
+        <v>4224</v>
       </c>
       <c r="B5" t="s">
-        <v>4222</v>
+        <v>4225</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4223</v>
+        <v>4226</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -63003,17 +63158,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4224</v>
+        <v>4227</v>
       </c>
       <c r="B6" t="s">
-        <v>4225</v>
+        <v>4228</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4226</v>
+        <v>4229</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -63029,7 +63184,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4227</v>
+        <v>4230</v>
       </c>
       <c r="B7" t="s">
         <v>3158</v>
@@ -63055,7 +63210,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4228</v>
+        <v>4231</v>
       </c>
       <c r="B8" t="s">
         <v>3170</v>
@@ -63081,7 +63236,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4229</v>
+        <v>4232</v>
       </c>
       <c r="B9" t="s">
         <v>3180</v>
@@ -63107,7 +63262,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4230</v>
+        <v>4233</v>
       </c>
       <c r="B10" t="s">
         <v>3188</v>
@@ -63133,7 +63288,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4231</v>
+        <v>4234</v>
       </c>
       <c r="B11" t="s">
         <v>3184</v>
@@ -63159,7 +63314,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4232</v>
+        <v>4235</v>
       </c>
       <c r="B12" t="s">
         <v>3155</v>
@@ -63185,7 +63340,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4233</v>
+        <v>4236</v>
       </c>
       <c r="B13" t="s">
         <v>195</v>
@@ -63211,7 +63366,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4234</v>
+        <v>4237</v>
       </c>
       <c r="B14" t="s">
         <v>3208</v>
@@ -63237,7 +63392,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4235</v>
+        <v>4238</v>
       </c>
       <c r="B15" t="s">
         <v>3146</v>
@@ -63263,7 +63418,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4236</v>
+        <v>4239</v>
       </c>
       <c r="B16" t="s">
         <v>3153</v>
@@ -63289,7 +63444,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4237</v>
+        <v>4240</v>
       </c>
       <c r="B17" t="s">
         <v>3211</v>
@@ -63315,10 +63470,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4238</v>
+        <v>4241</v>
       </c>
       <c r="B18" t="s">
-        <v>4239</v>
+        <v>4242</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3163</v>
@@ -63837,12 +63992,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4240</v>
+        <v>4243</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4241</v>
+        <v>4244</v>
       </c>
     </row>
   </sheetData>
@@ -65011,9 +65166,7 @@
       <c r="F40" t="s" s="1">
         <v>27</v>
       </c>
-      <c r="G40" t="s">
-        <v>18</v>
-      </c>
+      <c r="G40"/>
       <c r="H40"/>
       <c r="I40" t="s" s="1">
         <v>19</v>

</xml_diff>

<commit_message>
#8920: Added distinction between create and edit user rights
#8920: Fixed review finding

#8920: Fixed failing tests

#8920: revert changes in DefaultUserRole

#4463 Edit and create user roles - fix tests
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16568" uniqueCount="4245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16576" uniqueCount="4247">
   <si>
     <t>Field ID</t>
   </si>
@@ -8428,7 +8428,7 @@
     <t>MEDICAL_SAFE</t>
   </si>
   <si>
-    <t>Medical personnel at save proximity (&gt; 2 meter) or with protective equipment</t>
+    <t>Medical personnel at safe proximity (&gt; 2 meter) or with protective equipment</t>
   </si>
   <si>
     <t>MEDICAL_SAME_ROOM</t>
@@ -8446,7 +8446,7 @@
     <t>MEDICAL_DISTANT</t>
   </si>
   <si>
-    <t>Medical personnel at save proximity (&gt; 2 meter), without direct contact with secretions or excretions of the patient and without aerosol exposure</t>
+    <t>Medical personnel at safe proximity (&gt; 2 meter), without direct contact with secretions or excretions of the patient and without aerosol exposure</t>
   </si>
   <si>
     <t>MEDICAL_LIMITED</t>
@@ -12307,7 +12307,7 @@
     <t>Limited disease</t>
   </si>
   <si>
-    <t>Select a disease here if the user should be restricted to only see data for one disease</t>
+    <t>Select a disease here if the user should be restricted to only see data for one case-based disease</t>
   </si>
   <si>
     <t>User.language</t>
@@ -12430,6 +12430,12 @@
     <t>Čeština</t>
   </si>
   <si>
+    <t>UR_PK</t>
+  </si>
+  <si>
+    <t>Urdu</t>
+  </si>
+  <si>
     <t>NATION</t>
   </si>
   <si>
@@ -12784,7 +12790,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.73.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -14708,7 +14714,7 @@
 </file>
 
 <file path=xl/tables/table209.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="209" ref="A85:E101" displayName="UserLanguage" name="UserLanguage">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="209" ref="A85:E102" displayName="UserLanguage" name="UserLanguage">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14736,7 +14742,7 @@
 </file>
 
 <file path=xl/tables/table210.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A103:E112" displayName="UserJurisdictionLevel" name="UserJurisdictionLevel">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A104:E113" displayName="UserJurisdictionLevel" name="UserJurisdictionLevel">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -54305,7 +54311,9 @@
       <c r="C23" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="D23"/>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
       <c r="E23" t="s">
         <v>708</v>
       </c>
@@ -54331,7 +54339,9 @@
       <c r="C24" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="D24"/>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
       <c r="E24" t="s">
         <v>711</v>
       </c>
@@ -54357,7 +54367,9 @@
       <c r="C25" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="D25"/>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
       <c r="E25" t="s">
         <v>714</v>
       </c>
@@ -54383,7 +54395,9 @@
       <c r="C26" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="D26"/>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
       <c r="E26" t="s">
         <v>717</v>
       </c>
@@ -58449,7 +58463,7 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L112"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -60171,47 +60185,47 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" t="s">
-        <v>213</v>
-      </c>
-      <c r="C103" t="s">
-        <v>4</v>
-      </c>
-      <c r="D103" t="s">
-        <v>5</v>
-      </c>
-      <c r="E103" t="s">
-        <v>223</v>
+    <row r="102">
+      <c r="A102"/>
+      <c r="B102" t="s">
+        <v>4126</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4127</v>
+      </c>
+      <c r="D102" t="s">
+        <v>27</v>
+      </c>
+      <c r="E102" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" t="s">
+        <v>213</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
         <v>4093</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>502</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>1267</v>
-      </c>
-      <c r="D104" t="s">
-        <v>27</v>
-      </c>
-      <c r="E104" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105"/>
-      <c r="B105" t="s">
-        <v>4126</v>
-      </c>
-      <c r="C105" t="s">
-        <v>4127</v>
       </c>
       <c r="D105" t="s">
         <v>27</v>
@@ -60226,7 +60240,7 @@
         <v>4128</v>
       </c>
       <c r="C106" t="s">
-        <v>654</v>
+        <v>4129</v>
       </c>
       <c r="D106" t="s">
         <v>27</v>
@@ -60238,10 +60252,10 @@
     <row r="107">
       <c r="A107"/>
       <c r="B107" t="s">
-        <v>4129</v>
+        <v>4130</v>
       </c>
       <c r="C107" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -60253,10 +60267,10 @@
     <row r="108">
       <c r="A108"/>
       <c r="B108" t="s">
-        <v>496</v>
+        <v>4131</v>
       </c>
       <c r="C108" t="s">
-        <v>497</v>
+        <v>657</v>
       </c>
       <c r="D108" t="s">
         <v>27</v>
@@ -60268,10 +60282,10 @@
     <row r="109">
       <c r="A109"/>
       <c r="B109" t="s">
-        <v>1226</v>
+        <v>496</v>
       </c>
       <c r="C109" t="s">
-        <v>944</v>
+        <v>497</v>
       </c>
       <c r="D109" t="s">
         <v>27</v>
@@ -60283,10 +60297,10 @@
     <row r="110">
       <c r="A110"/>
       <c r="B110" t="s">
-        <v>4130</v>
+        <v>1226</v>
       </c>
       <c r="C110" t="s">
-        <v>703</v>
+        <v>944</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -60298,10 +60312,10 @@
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>284</v>
+        <v>4132</v>
       </c>
       <c r="C111" t="s">
-        <v>285</v>
+        <v>703</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -60313,15 +60327,30 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>4131</v>
+        <v>284</v>
       </c>
       <c r="C112" t="s">
-        <v>4131</v>
+        <v>285</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
       </c>
       <c r="E112" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113"/>
+      <c r="B113" t="s">
+        <v>4133</v>
+      </c>
+      <c r="C113" t="s">
+        <v>4133</v>
+      </c>
+      <c r="D113" t="s">
+        <v>27</v>
+      </c>
+      <c r="E113" t="s">
         <v>27</v>
       </c>
     </row>
@@ -60399,13 +60428,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4132</v>
+        <v>4134</v>
       </c>
       <c r="B2" t="s">
         <v>4028</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4133</v>
+        <v>4135</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -60425,7 +60454,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4134</v>
+        <v>4136</v>
       </c>
       <c r="B3" t="s">
         <v>3142</v>
@@ -60451,17 +60480,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4135</v>
+        <v>4137</v>
       </c>
       <c r="B4" t="s">
-        <v>4136</v>
+        <v>4138</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>4137</v>
+        <v>4139</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -60477,7 +60506,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4138</v>
+        <v>4140</v>
       </c>
       <c r="B5" t="s">
         <v>2892</v>
@@ -60503,17 +60532,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4139</v>
+        <v>4141</v>
       </c>
       <c r="B6" t="s">
-        <v>4140</v>
+        <v>4142</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4141</v>
+        <v>4143</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -60529,10 +60558,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4142</v>
+        <v>4144</v>
       </c>
       <c r="B7" t="s">
-        <v>4143</v>
+        <v>4145</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>14</v>
@@ -60555,7 +60584,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4144</v>
+        <v>4146</v>
       </c>
       <c r="B8" t="s">
         <v>2901</v>
@@ -60581,7 +60610,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4145</v>
+        <v>4147</v>
       </c>
       <c r="B9" t="s">
         <v>2905</v>
@@ -60607,7 +60636,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4146</v>
+        <v>4148</v>
       </c>
       <c r="B10" t="s">
         <v>2926</v>
@@ -60633,17 +60662,17 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4147</v>
+        <v>4149</v>
       </c>
       <c r="B11" t="s">
-        <v>4148</v>
+        <v>4150</v>
       </c>
       <c r="C11" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>4149</v>
+        <v>4151</v>
       </c>
       <c r="F11" t="s" s="1">
         <v>27</v>
@@ -60659,13 +60688,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4150</v>
+        <v>4152</v>
       </c>
       <c r="B12" t="s">
-        <v>4151</v>
+        <v>4153</v>
       </c>
       <c r="C12" t="s" s="1">
-        <v>4152</v>
+        <v>4154</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
@@ -60685,17 +60714,17 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4153</v>
+        <v>4155</v>
       </c>
       <c r="B13" t="s">
-        <v>4154</v>
+        <v>4156</v>
       </c>
       <c r="C13" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>4155</v>
+        <v>4157</v>
       </c>
       <c r="F13" t="s" s="1">
         <v>27</v>
@@ -60711,17 +60740,17 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4156</v>
+        <v>4158</v>
       </c>
       <c r="B14" t="s">
-        <v>4157</v>
+        <v>4159</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>4158</v>
+        <v>4160</v>
       </c>
       <c r="F14" t="s" s="1">
         <v>27</v>
@@ -60737,10 +60766,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4159</v>
+        <v>4161</v>
       </c>
       <c r="B15" t="s">
-        <v>4160</v>
+        <v>4162</v>
       </c>
       <c r="C15" t="s" s="1">
         <v>14</v>
@@ -60763,10 +60792,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4161</v>
+        <v>4163</v>
       </c>
       <c r="B16" t="s">
-        <v>4162</v>
+        <v>4164</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>14</v>
@@ -60789,10 +60818,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4163</v>
+        <v>4165</v>
       </c>
       <c r="B17" t="s">
-        <v>4164</v>
+        <v>4166</v>
       </c>
       <c r="C17" t="s" s="1">
         <v>53</v>
@@ -60815,10 +60844,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4165</v>
+        <v>4167</v>
       </c>
       <c r="B18" t="s">
-        <v>4166</v>
+        <v>4168</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>110</v>
@@ -60841,10 +60870,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4167</v>
+        <v>4169</v>
       </c>
       <c r="B19" t="s">
-        <v>4168</v>
+        <v>4170</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>57</v>
@@ -60867,10 +60896,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4169</v>
+        <v>4171</v>
       </c>
       <c r="B20" t="s">
-        <v>4170</v>
+        <v>4172</v>
       </c>
       <c r="C20" t="s" s="1">
         <v>57</v>
@@ -60893,10 +60922,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4171</v>
+        <v>4173</v>
       </c>
       <c r="B21" t="s">
-        <v>4172</v>
+        <v>4174</v>
       </c>
       <c r="C21" t="s" s="1">
         <v>57</v>
@@ -60919,10 +60948,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>4173</v>
+        <v>4175</v>
       </c>
       <c r="B22" t="s">
-        <v>4174</v>
+        <v>4176</v>
       </c>
       <c r="C22" t="s" s="1">
         <v>14</v>
@@ -60945,10 +60974,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>4175</v>
+        <v>4177</v>
       </c>
       <c r="B23" t="s">
-        <v>4176</v>
+        <v>4178</v>
       </c>
       <c r="C23" t="s" s="1">
         <v>14</v>
@@ -60971,10 +61000,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>4177</v>
+        <v>4179</v>
       </c>
       <c r="B24" t="s">
-        <v>4178</v>
+        <v>4180</v>
       </c>
       <c r="C24" t="s" s="1">
         <v>14</v>
@@ -60997,10 +61026,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>4179</v>
+        <v>4181</v>
       </c>
       <c r="B25" t="s">
-        <v>4180</v>
+        <v>4182</v>
       </c>
       <c r="C25" t="s" s="1">
         <v>14</v>
@@ -61023,10 +61052,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>4181</v>
+        <v>4183</v>
       </c>
       <c r="B26" t="s">
-        <v>4182</v>
+        <v>4184</v>
       </c>
       <c r="C26" t="s" s="1">
         <v>14</v>
@@ -61049,10 +61078,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>4183</v>
+        <v>4185</v>
       </c>
       <c r="B27" t="s">
-        <v>4184</v>
+        <v>4186</v>
       </c>
       <c r="C27" t="s" s="1">
         <v>14</v>
@@ -61075,7 +61104,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4185</v>
+        <v>4187</v>
       </c>
       <c r="B28" t="s">
         <v>3140</v>
@@ -61101,7 +61130,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>4186</v>
+        <v>4188</v>
       </c>
       <c r="B29" t="s">
         <v>1588</v>
@@ -61127,13 +61156,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>4187</v>
+        <v>4189</v>
       </c>
       <c r="B30" t="s">
-        <v>4188</v>
+        <v>4190</v>
       </c>
       <c r="C30" t="s" s="1">
-        <v>4189</v>
+        <v>4191</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="s">
@@ -61153,10 +61182,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4190</v>
+        <v>4192</v>
       </c>
       <c r="B31" t="s">
-        <v>4191</v>
+        <v>4193</v>
       </c>
       <c r="C31" t="s" s="1">
         <v>14</v>
@@ -61179,17 +61208,17 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>4192</v>
+        <v>4194</v>
       </c>
       <c r="B32" t="s">
-        <v>4193</v>
+        <v>4195</v>
       </c>
       <c r="C32" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>4194</v>
+        <v>4196</v>
       </c>
       <c r="F32" t="s" s="1">
         <v>27</v>
@@ -61205,17 +61234,17 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>4195</v>
+        <v>4197</v>
       </c>
       <c r="B33" t="s">
-        <v>4196</v>
+        <v>4198</v>
       </c>
       <c r="C33" t="s" s="1">
         <v>2949</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>4197</v>
+        <v>4199</v>
       </c>
       <c r="F33" t="s" s="1">
         <v>27</v>
@@ -61231,17 +61260,17 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>4198</v>
+        <v>4200</v>
       </c>
       <c r="B34" t="s">
-        <v>4199</v>
+        <v>4201</v>
       </c>
       <c r="C34" t="s" s="1">
-        <v>4200</v>
+        <v>4202</v>
       </c>
       <c r="D34"/>
       <c r="E34" t="s">
-        <v>4201</v>
+        <v>4203</v>
       </c>
       <c r="F34" t="s" s="1">
         <v>27</v>
@@ -61257,17 +61286,17 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>4202</v>
+        <v>4204</v>
       </c>
       <c r="B35" t="s">
-        <v>4203</v>
+        <v>4205</v>
       </c>
       <c r="C35" t="s" s="1">
         <v>772</v>
       </c>
       <c r="D35"/>
       <c r="E35" t="s">
-        <v>4204</v>
+        <v>4206</v>
       </c>
       <c r="F35" t="s" s="1">
         <v>27</v>
@@ -61283,7 +61312,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>4205</v>
+        <v>4207</v>
       </c>
       <c r="B36" t="s">
         <v>771</v>
@@ -61326,13 +61355,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>4133</v>
+        <v>4135</v>
       </c>
       <c r="B39" t="s">
-        <v>4206</v>
+        <v>4208</v>
       </c>
       <c r="C39" t="s">
-        <v>4207</v>
+        <v>4209</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -61344,10 +61373,10 @@
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>4208</v>
+        <v>4210</v>
       </c>
       <c r="C40" t="s">
-        <v>4209</v>
+        <v>4211</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
@@ -62914,13 +62943,13 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>4200</v>
+        <v>4202</v>
       </c>
       <c r="B150" t="s">
-        <v>4210</v>
+        <v>4212</v>
       </c>
       <c r="C150" t="s">
-        <v>4211</v>
+        <v>4213</v>
       </c>
       <c r="D150" t="s">
         <v>27</v>
@@ -62947,10 +62976,10 @@
     <row r="152">
       <c r="A152"/>
       <c r="B152" t="s">
-        <v>4212</v>
+        <v>4214</v>
       </c>
       <c r="C152" t="s">
-        <v>4213</v>
+        <v>4215</v>
       </c>
       <c r="D152" t="s">
         <v>27</v>
@@ -62962,10 +62991,10 @@
     <row r="153">
       <c r="A153"/>
       <c r="B153" t="s">
-        <v>4214</v>
+        <v>4216</v>
       </c>
       <c r="C153" t="s">
-        <v>4215</v>
+        <v>4217</v>
       </c>
       <c r="D153" t="s">
         <v>27</v>
@@ -63052,13 +63081,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4216</v>
+        <v>4218</v>
       </c>
       <c r="B2" t="s">
-        <v>4217</v>
+        <v>4219</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4218</v>
+        <v>4220</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -63080,17 +63109,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4219</v>
+        <v>4221</v>
       </c>
       <c r="B3" t="s">
-        <v>4220</v>
+        <v>4222</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4221</v>
+        <v>4223</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -63106,13 +63135,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4222</v>
+        <v>4224</v>
       </c>
       <c r="B4" t="s">
-        <v>4223</v>
+        <v>4225</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>4152</v>
+        <v>4154</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
@@ -63132,17 +63161,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4224</v>
+        <v>4226</v>
       </c>
       <c r="B5" t="s">
-        <v>4225</v>
+        <v>4227</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4226</v>
+        <v>4228</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -63158,17 +63187,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4227</v>
+        <v>4229</v>
       </c>
       <c r="B6" t="s">
-        <v>4228</v>
+        <v>4230</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4229</v>
+        <v>4231</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -63184,7 +63213,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4230</v>
+        <v>4232</v>
       </c>
       <c r="B7" t="s">
         <v>3158</v>
@@ -63210,7 +63239,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4231</v>
+        <v>4233</v>
       </c>
       <c r="B8" t="s">
         <v>3170</v>
@@ -63236,7 +63265,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4232</v>
+        <v>4234</v>
       </c>
       <c r="B9" t="s">
         <v>3180</v>
@@ -63262,7 +63291,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4233</v>
+        <v>4235</v>
       </c>
       <c r="B10" t="s">
         <v>3188</v>
@@ -63288,7 +63317,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4234</v>
+        <v>4236</v>
       </c>
       <c r="B11" t="s">
         <v>3184</v>
@@ -63314,7 +63343,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4235</v>
+        <v>4237</v>
       </c>
       <c r="B12" t="s">
         <v>3155</v>
@@ -63340,7 +63369,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4236</v>
+        <v>4238</v>
       </c>
       <c r="B13" t="s">
         <v>195</v>
@@ -63366,7 +63395,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4237</v>
+        <v>4239</v>
       </c>
       <c r="B14" t="s">
         <v>3208</v>
@@ -63392,7 +63421,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4238</v>
+        <v>4240</v>
       </c>
       <c r="B15" t="s">
         <v>3146</v>
@@ -63418,7 +63447,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4239</v>
+        <v>4241</v>
       </c>
       <c r="B16" t="s">
         <v>3153</v>
@@ -63444,7 +63473,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4240</v>
+        <v>4242</v>
       </c>
       <c r="B17" t="s">
         <v>3211</v>
@@ -63470,10 +63499,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4241</v>
+        <v>4243</v>
       </c>
       <c r="B18" t="s">
-        <v>4242</v>
+        <v>4244</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3163</v>
@@ -63992,12 +64021,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4243</v>
+        <v>4245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4244</v>
+        <v>4246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#10208 fixed unit tests not working correctly with instances and uuids
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16655" uniqueCount="4190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16468" uniqueCount="4177">
   <si>
     <t>Field ID</t>
   </si>
@@ -12301,33 +12301,6 @@
     <t>Message date</t>
   </si>
   <si>
-    <t>ExternalMessage.sampleDateTime</t>
-  </si>
-  <si>
-    <t>ExternalMessage.sampleReceivedDate</t>
-  </si>
-  <si>
-    <t>sampleReceivedDate</t>
-  </si>
-  <si>
-    <t>Sample received</t>
-  </si>
-  <si>
-    <t>ExternalMessage.labSampleId</t>
-  </si>
-  <si>
-    <t>labSampleId</t>
-  </si>
-  <si>
-    <t>ExternalMessage.sampleMaterial</t>
-  </si>
-  <si>
-    <t>ExternalMessage.sampleMaterialText</t>
-  </si>
-  <si>
-    <t>ExternalMessage.specimenCondition</t>
-  </si>
-  <si>
     <t>ExternalMessage.reporterName</t>
   </si>
   <si>
@@ -12442,21 +12415,18 @@
     <t>personEmail</t>
   </si>
   <si>
-    <t>ExternalMessage.sample</t>
+    <t>ExternalMessage.sampleReports</t>
+  </si>
+  <si>
+    <t>sampleReports</t>
+  </si>
+  <si>
+    <t>List of SampleReport</t>
   </si>
   <si>
     <t>ExternalMessage.caze</t>
   </si>
   <si>
-    <t>ExternalMessage.testReports</t>
-  </si>
-  <si>
-    <t>testReports</t>
-  </si>
-  <si>
-    <t>List of TestReport</t>
-  </si>
-  <si>
     <t>ExternalMessage.externalMessageDetails</t>
   </si>
   <si>
@@ -12472,15 +12442,6 @@
     <t>Report ID</t>
   </si>
   <si>
-    <t>ExternalMessage.sampleOverallTestResult</t>
-  </si>
-  <si>
-    <t>sampleOverallTestResult</t>
-  </si>
-  <si>
-    <t>Overall test result</t>
-  </si>
-  <si>
     <t>ExternalMessage.status</t>
   </si>
   <si>
@@ -12535,13 +12496,13 @@
     <t>Unclear</t>
   </si>
   <si>
-    <t>TestReport.labMessage</t>
-  </si>
-  <si>
-    <t>labMessage</t>
-  </si>
-  <si>
-    <t>ExternalMessageReference</t>
+    <t>TestReport.sampleReport</t>
+  </si>
+  <si>
+    <t>sampleReport</t>
+  </si>
+  <si>
+    <t>SampleReportReference</t>
   </si>
   <si>
     <t>TestReport.testLabName</t>
@@ -12619,7 +12580,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.76.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -14564,7 +14525,7 @@
 </file>
 
 <file path=xl/tables/table210.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A1:L36" displayName="Message" name="Message">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A1:L28" displayName="Message" name="Message">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14585,7 +14546,7 @@
 </file>
 
 <file path=xl/tables/table211.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A38:E40" displayName="MessageExternalMessageType" name="MessageExternalMessageType">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A30:E32" displayName="MessageExternalMessageType" name="MessageExternalMessageType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14599,7 +14560,7 @@
 </file>
 
 <file path=xl/tables/table212.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A42:E103" displayName="MessageDisease" name="MessageDisease">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A34:E95" displayName="MessageDisease" name="MessageDisease">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14613,7 +14574,7 @@
 </file>
 
 <file path=xl/tables/table213.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A105:E129" displayName="MessageSampleMaterial" name="MessageSampleMaterial">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A97:E101" displayName="MessageSex" name="MessageSex">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14627,7 +14588,7 @@
 </file>
 
 <file path=xl/tables/table214.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A131:E133" displayName="MessageSpecimenCondition" name="MessageSpecimenCondition">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A103:E107" displayName="MessagePresentCondition" name="MessagePresentCondition">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14641,7 +14602,7 @@
 </file>
 
 <file path=xl/tables/table215.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A135:E139" displayName="MessageSex" name="MessageSex">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A109:E113" displayName="MessageExternalMessageStatus" name="MessageExternalMessageStatus">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14655,49 +14616,7 @@
 </file>
 
 <file path=xl/tables/table216.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="216" ref="A141:E145" displayName="MessagePresentCondition" name="MessagePresentCondition">
-  <autoFilter/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Type"/>
-    <tableColumn id="2" name="Value"/>
-    <tableColumn id="3" name="Caption"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Short"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
-</table>
-</file>
-
-<file path=xl/tables/table217.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="217" ref="A147:E152" displayName="MessagePathogenTestResultType" name="MessagePathogenTestResultType">
-  <autoFilter/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Type"/>
-    <tableColumn id="2" name="Value"/>
-    <tableColumn id="3" name="Caption"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Short"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
-</table>
-</file>
-
-<file path=xl/tables/table218.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="218" ref="A154:E158" displayName="MessageExternalMessageStatus" name="MessageExternalMessageStatus">
-  <autoFilter/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Type"/>
-    <tableColumn id="2" name="Value"/>
-    <tableColumn id="3" name="Caption"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Short"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
-</table>
-</file>
-
-<file path=xl/tables/table219.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="219" ref="A1:L18" displayName="Test_report" name="Test_report">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="216" ref="A1:L18" displayName="Test_report" name="Test_report">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14717,8 +14636,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" ref="A47:E107" displayName="LocationFacilityType" name="LocationFacilityType">
+<file path=xl/tables/table217.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="217" ref="A20:E41" displayName="Test_reportPathogenTestType" name="Test_reportPathogenTestType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14731,8 +14650,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table220.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="220" ref="A20:E41" displayName="Test_reportPathogenTestType" name="Test_reportPathogenTestType">
+<file path=xl/tables/table218.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="218" ref="A43:E48" displayName="Test_reportPathogenTestResultType" name="Test_reportPathogenTestResultType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14745,8 +14664,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table221.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="221" ref="A43:E48" displayName="Test_reportPathogenTestResultType" name="Test_reportPathogenTestResultType">
+<file path=xl/tables/table219.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="219" ref="A50:E52" displayName="Test_reportPCRTestSpecification" name="Test_reportPCRTestSpecification">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14759,8 +14678,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table222.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="222" ref="A50:E52" displayName="Test_reportPCRTestSpecification" name="Test_reportPCRTestSpecification">
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" ref="A47:E107" displayName="LocationFacilityType" name="LocationFacilityType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -60323,7 +60242,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L158"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -60464,14 +60383,14 @@
         <v>4083</v>
       </c>
       <c r="B5" t="s">
-        <v>2833</v>
+        <v>4084</v>
       </c>
       <c r="C5" t="s" s="1">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>2834</v>
+        <v>4085</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -60487,17 +60406,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4084</v>
+        <v>4086</v>
       </c>
       <c r="B6" t="s">
-        <v>4085</v>
+        <v>4087</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>75</v>
+        <v>4088</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4086</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -60513,17 +60432,17 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4087</v>
+        <v>4089</v>
       </c>
       <c r="B7" t="s">
-        <v>4088</v>
+        <v>4090</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>2828</v>
+        <v>4091</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -60539,17 +60458,17 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4089</v>
+        <v>4092</v>
       </c>
       <c r="B8" t="s">
-        <v>2842</v>
+        <v>4093</v>
       </c>
       <c r="C8" t="s" s="1">
-        <v>2843</v>
+        <v>14</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>2844</v>
+        <v>4094</v>
       </c>
       <c r="F8" t="s" s="1">
         <v>27</v>
@@ -60565,17 +60484,17 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4090</v>
+        <v>4095</v>
       </c>
       <c r="B9" t="s">
-        <v>2846</v>
+        <v>4096</v>
       </c>
       <c r="C9" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s" s="1">
         <v>27</v>
@@ -60591,17 +60510,17 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4091</v>
+        <v>4097</v>
       </c>
       <c r="B10" t="s">
-        <v>2867</v>
+        <v>4098</v>
       </c>
       <c r="C10" t="s" s="1">
-        <v>2868</v>
+        <v>14</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>2869</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s" s="1">
         <v>27</v>
@@ -60617,17 +60536,17 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4092</v>
+        <v>4099</v>
       </c>
       <c r="B11" t="s">
-        <v>4093</v>
+        <v>4100</v>
       </c>
       <c r="C11" t="s" s="1">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>4094</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s" s="1">
         <v>27</v>
@@ -60643,13 +60562,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4095</v>
+        <v>4101</v>
       </c>
       <c r="B12" t="s">
-        <v>4096</v>
+        <v>4102</v>
       </c>
       <c r="C12" t="s" s="1">
-        <v>4097</v>
+        <v>110</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
@@ -60669,17 +60588,17 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4098</v>
+        <v>4103</v>
       </c>
       <c r="B13" t="s">
-        <v>4099</v>
+        <v>4104</v>
       </c>
       <c r="C13" t="s" s="1">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>4100</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s" s="1">
         <v>27</v>
@@ -60695,17 +60614,17 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4101</v>
+        <v>4105</v>
       </c>
       <c r="B14" t="s">
-        <v>4102</v>
+        <v>4106</v>
       </c>
       <c r="C14" t="s" s="1">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>4103</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s" s="1">
         <v>27</v>
@@ -60721,17 +60640,17 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4104</v>
+        <v>4107</v>
       </c>
       <c r="B15" t="s">
-        <v>4105</v>
+        <v>4108</v>
       </c>
       <c r="C15" t="s" s="1">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s" s="1">
         <v>27</v>
@@ -60747,17 +60666,17 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4106</v>
+        <v>4109</v>
       </c>
       <c r="B16" t="s">
-        <v>4107</v>
+        <v>4110</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>625</v>
       </c>
       <c r="F16" t="s" s="1">
         <v>27</v>
@@ -60773,17 +60692,17 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4108</v>
+        <v>4111</v>
       </c>
       <c r="B17" t="s">
-        <v>4109</v>
+        <v>4112</v>
       </c>
       <c r="C17" t="s" s="1">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>605</v>
       </c>
       <c r="F17" t="s" s="1">
         <v>27</v>
@@ -60799,17 +60718,17 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4110</v>
+        <v>4113</v>
       </c>
       <c r="B18" t="s">
-        <v>4111</v>
+        <v>4114</v>
       </c>
       <c r="C18" t="s" s="1">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>628</v>
       </c>
       <c r="F18" t="s" s="1">
         <v>27</v>
@@ -60825,17 +60744,17 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4112</v>
+        <v>4115</v>
       </c>
       <c r="B19" t="s">
-        <v>4113</v>
+        <v>4116</v>
       </c>
       <c r="C19" t="s" s="1">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>631</v>
       </c>
       <c r="F19" t="s" s="1">
         <v>27</v>
@@ -60851,17 +60770,17 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4114</v>
+        <v>4117</v>
       </c>
       <c r="B20" t="s">
-        <v>4115</v>
+        <v>4118</v>
       </c>
       <c r="C20" t="s" s="1">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s" s="1">
         <v>27</v>
@@ -60877,17 +60796,17 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4116</v>
+        <v>4119</v>
       </c>
       <c r="B21" t="s">
-        <v>4117</v>
+        <v>4120</v>
       </c>
       <c r="C21" t="s" s="1">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s" s="1">
         <v>27</v>
@@ -60903,17 +60822,17 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>4118</v>
+        <v>4121</v>
       </c>
       <c r="B22" t="s">
-        <v>4119</v>
+        <v>4122</v>
       </c>
       <c r="C22" t="s" s="1">
-        <v>14</v>
+        <v>4123</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>625</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s" s="1">
         <v>27</v>
@@ -60929,17 +60848,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>4120</v>
+        <v>4124</v>
       </c>
       <c r="B23" t="s">
-        <v>4121</v>
+        <v>1529</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>14</v>
+        <v>1530</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>605</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s" s="1">
         <v>27</v>
@@ -60955,17 +60874,17 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>4122</v>
+        <v>4125</v>
       </c>
       <c r="B24" t="s">
-        <v>4123</v>
+        <v>4126</v>
       </c>
       <c r="C24" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>628</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s" s="1">
         <v>27</v>
@@ -60981,17 +60900,17 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>4124</v>
+        <v>4127</v>
       </c>
       <c r="B25" t="s">
-        <v>4125</v>
+        <v>4128</v>
       </c>
       <c r="C25" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>631</v>
+        <v>4129</v>
       </c>
       <c r="F25" t="s" s="1">
         <v>27</v>
@@ -61007,17 +60926,17 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>4126</v>
+        <v>4130</v>
       </c>
       <c r="B26" t="s">
-        <v>4127</v>
+        <v>4131</v>
       </c>
       <c r="C26" t="s" s="1">
-        <v>14</v>
+        <v>4132</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>4133</v>
       </c>
       <c r="F26" t="s" s="1">
         <v>27</v>
@@ -61033,17 +60952,17 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>4128</v>
+        <v>4134</v>
       </c>
       <c r="B27" t="s">
-        <v>4129</v>
+        <v>4135</v>
       </c>
       <c r="C27" t="s" s="1">
-        <v>14</v>
+        <v>713</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>4136</v>
       </c>
       <c r="F27" t="s" s="1">
         <v>27</v>
@@ -61059,17 +60978,17 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4130</v>
+        <v>4137</v>
       </c>
       <c r="B28" t="s">
-        <v>3081</v>
+        <v>712</v>
       </c>
       <c r="C28" t="s" s="1">
-        <v>2881</v>
+        <v>713</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>714</v>
       </c>
       <c r="F28" t="s" s="1">
         <v>27</v>
@@ -61083,304 +61002,216 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>4131</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1529</v>
-      </c>
-      <c r="C29" t="s" s="1">
-        <v>1530</v>
-      </c>
-      <c r="D29"/>
-      <c r="E29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-    </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>4132</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>4133</v>
-      </c>
-      <c r="C30" t="s" s="1">
-        <v>4134</v>
-      </c>
-      <c r="D30"/>
+        <v>214</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
       <c r="E30" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
+        <v>224</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4135</v>
+        <v>4078</v>
       </c>
       <c r="B31" t="s">
-        <v>4136</v>
-      </c>
-      <c r="C31" t="s" s="1">
-        <v>14</v>
-      </c>
-      <c r="D31"/>
+        <v>4138</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4139</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
       <c r="E31" t="s">
         <v>27</v>
       </c>
-      <c r="F31" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>4137</v>
-      </c>
+      <c r="A32"/>
       <c r="B32" t="s">
-        <v>4138</v>
-      </c>
-      <c r="C32" t="s" s="1">
-        <v>14</v>
-      </c>
-      <c r="D32"/>
+        <v>4140</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4141</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
       <c r="E32" t="s">
-        <v>4139</v>
-      </c>
-      <c r="F32" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>4140</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4141</v>
-      </c>
-      <c r="C33" t="s" s="1">
-        <v>2890</v>
-      </c>
-      <c r="D33"/>
-      <c r="E33" t="s">
-        <v>4142</v>
-      </c>
-      <c r="F33" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>4143</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>4144</v>
-      </c>
-      <c r="C34" t="s" s="1">
-        <v>4145</v>
-      </c>
-      <c r="D34"/>
+        <v>214</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
       <c r="E34" t="s">
-        <v>4146</v>
-      </c>
-      <c r="F34" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
+        <v>224</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>4147</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>4148</v>
-      </c>
-      <c r="C35" t="s" s="1">
-        <v>713</v>
-      </c>
-      <c r="D35"/>
+        <v>379</v>
+      </c>
+      <c r="C35" t="s">
+        <v>380</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
       <c r="E35" t="s">
-        <v>4149</v>
-      </c>
-      <c r="F35" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
+        <v>379</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>4150</v>
-      </c>
+      <c r="A36"/>
       <c r="B36" t="s">
-        <v>712</v>
-      </c>
-      <c r="C36" t="s" s="1">
-        <v>713</v>
-      </c>
-      <c r="D36"/>
+        <v>381</v>
+      </c>
+      <c r="C36" t="s">
+        <v>382</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
       <c r="E36" t="s">
-        <v>714</v>
-      </c>
-      <c r="F36" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36" t="s" s="1">
-        <v>19</v>
-      </c>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37"/>
+      <c r="B37" t="s">
+        <v>383</v>
+      </c>
+      <c r="C37" t="s">
+        <v>384</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>2</v>
-      </c>
+      <c r="A38"/>
       <c r="B38" t="s">
-        <v>214</v>
+        <v>385</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>386</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E38" t="s">
-        <v>224</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>4078</v>
-      </c>
+      <c r="A39"/>
       <c r="B39" t="s">
-        <v>4151</v>
+        <v>388</v>
       </c>
       <c r="C39" t="s">
-        <v>4152</v>
+        <v>389</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
       </c>
       <c r="E39" t="s">
-        <v>27</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>4153</v>
+        <v>391</v>
       </c>
       <c r="C40" t="s">
-        <v>4154</v>
+        <v>392</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
       </c>
       <c r="E40" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41"/>
+      <c r="B41" t="s">
+        <v>393</v>
+      </c>
+      <c r="C41" t="s">
+        <v>394</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>2</v>
-      </c>
+      <c r="A42"/>
       <c r="B42" t="s">
-        <v>214</v>
+        <v>395</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>396</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E42" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>123</v>
-      </c>
+      <c r="A43"/>
       <c r="B43" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
       <c r="C43" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>379</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>381</v>
+        <v>399</v>
       </c>
       <c r="C44" t="s">
-        <v>382</v>
+        <v>400</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
@@ -61392,70 +61223,70 @@
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>383</v>
+        <v>401</v>
       </c>
       <c r="C45" t="s">
-        <v>384</v>
+        <v>402</v>
       </c>
       <c r="D45" t="s">
         <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>385</v>
+        <v>404</v>
       </c>
       <c r="C46" t="s">
-        <v>386</v>
+        <v>405</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>387</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="C47" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>391</v>
+        <v>409</v>
       </c>
       <c r="C48" t="s">
-        <v>392</v>
+        <v>410</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>393</v>
+        <v>412</v>
       </c>
       <c r="C49" t="s">
-        <v>394</v>
+        <v>413</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -61467,10 +61298,10 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>395</v>
+        <v>414</v>
       </c>
       <c r="C50" t="s">
-        <v>396</v>
+        <v>415</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
@@ -61482,25 +61313,25 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>397</v>
+        <v>416</v>
       </c>
       <c r="C51" t="s">
-        <v>398</v>
+        <v>417</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
       </c>
       <c r="E51" t="s">
-        <v>27</v>
+        <v>418</v>
       </c>
     </row>
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="C52" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D52" t="s">
         <v>27</v>
@@ -61512,25 +61343,25 @@
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
       <c r="C53" t="s">
-        <v>402</v>
+        <v>186</v>
       </c>
       <c r="D53" t="s">
         <v>27</v>
       </c>
       <c r="E53" t="s">
-        <v>403</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>404</v>
+        <v>422</v>
       </c>
       <c r="C54" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="D54" t="s">
         <v>27</v>
@@ -61542,40 +61373,40 @@
     <row r="55">
       <c r="A55"/>
       <c r="B55" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="C55" t="s">
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="D55" t="s">
         <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>408</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
       <c r="C56" t="s">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
       </c>
       <c r="E56" t="s">
-        <v>411</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>412</v>
+        <v>428</v>
       </c>
       <c r="C57" t="s">
-        <v>413</v>
+        <v>429</v>
       </c>
       <c r="D57" t="s">
         <v>27</v>
@@ -61587,10 +61418,10 @@
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="C58" t="s">
-        <v>415</v>
+        <v>431</v>
       </c>
       <c r="D58" t="s">
         <v>27</v>
@@ -61602,25 +61433,25 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>416</v>
+        <v>432</v>
       </c>
       <c r="C59" t="s">
-        <v>417</v>
+        <v>432</v>
       </c>
       <c r="D59" t="s">
         <v>27</v>
       </c>
       <c r="E59" t="s">
-        <v>418</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="C60" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="D60" t="s">
         <v>27</v>
@@ -61632,10 +61463,10 @@
     <row r="61">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="C61" t="s">
-        <v>186</v>
+        <v>436</v>
       </c>
       <c r="D61" t="s">
         <v>27</v>
@@ -61647,10 +61478,10 @@
     <row r="62">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>422</v>
+        <v>437</v>
       </c>
       <c r="C62" t="s">
-        <v>423</v>
+        <v>438</v>
       </c>
       <c r="D62" t="s">
         <v>27</v>
@@ -61662,10 +61493,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>424</v>
+        <v>439</v>
       </c>
       <c r="C63" t="s">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="D63" t="s">
         <v>27</v>
@@ -61677,10 +61508,10 @@
     <row r="64">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>426</v>
+        <v>441</v>
       </c>
       <c r="C64" t="s">
-        <v>427</v>
+        <v>442</v>
       </c>
       <c r="D64" t="s">
         <v>27</v>
@@ -61692,10 +61523,10 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>428</v>
+        <v>443</v>
       </c>
       <c r="C65" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
@@ -61707,10 +61538,10 @@
     <row r="66">
       <c r="A66"/>
       <c r="B66" t="s">
-        <v>430</v>
+        <v>445</v>
       </c>
       <c r="C66" t="s">
-        <v>431</v>
+        <v>446</v>
       </c>
       <c r="D66" t="s">
         <v>27</v>
@@ -61722,10 +61553,10 @@
     <row r="67">
       <c r="A67"/>
       <c r="B67" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="C67" t="s">
-        <v>432</v>
+        <v>448</v>
       </c>
       <c r="D67" t="s">
         <v>27</v>
@@ -61737,10 +61568,10 @@
     <row r="68">
       <c r="A68"/>
       <c r="B68" t="s">
-        <v>433</v>
+        <v>449</v>
       </c>
       <c r="C68" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
       <c r="D68" t="s">
         <v>27</v>
@@ -61752,10 +61583,10 @@
     <row r="69">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>435</v>
+        <v>451</v>
       </c>
       <c r="C69" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="D69" t="s">
         <v>27</v>
@@ -61767,10 +61598,10 @@
     <row r="70">
       <c r="A70"/>
       <c r="B70" t="s">
-        <v>437</v>
+        <v>453</v>
       </c>
       <c r="C70" t="s">
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="D70" t="s">
         <v>27</v>
@@ -61782,10 +61613,10 @@
     <row r="71">
       <c r="A71"/>
       <c r="B71" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="C71" t="s">
-        <v>440</v>
+        <v>456</v>
       </c>
       <c r="D71" t="s">
         <v>27</v>
@@ -61797,10 +61628,10 @@
     <row r="72">
       <c r="A72"/>
       <c r="B72" t="s">
-        <v>441</v>
+        <v>457</v>
       </c>
       <c r="C72" t="s">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
@@ -61812,10 +61643,10 @@
     <row r="73">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>443</v>
+        <v>459</v>
       </c>
       <c r="C73" t="s">
-        <v>444</v>
+        <v>460</v>
       </c>
       <c r="D73" t="s">
         <v>27</v>
@@ -61827,10 +61658,10 @@
     <row r="74">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>445</v>
+        <v>461</v>
       </c>
       <c r="C74" t="s">
-        <v>446</v>
+        <v>462</v>
       </c>
       <c r="D74" t="s">
         <v>27</v>
@@ -61842,10 +61673,10 @@
     <row r="75">
       <c r="A75"/>
       <c r="B75" t="s">
-        <v>447</v>
+        <v>463</v>
       </c>
       <c r="C75" t="s">
-        <v>448</v>
+        <v>464</v>
       </c>
       <c r="D75" t="s">
         <v>27</v>
@@ -61857,10 +61688,10 @@
     <row r="76">
       <c r="A76"/>
       <c r="B76" t="s">
-        <v>449</v>
+        <v>465</v>
       </c>
       <c r="C76" t="s">
-        <v>450</v>
+        <v>466</v>
       </c>
       <c r="D76" t="s">
         <v>27</v>
@@ -61872,10 +61703,10 @@
     <row r="77">
       <c r="A77"/>
       <c r="B77" t="s">
-        <v>451</v>
+        <v>467</v>
       </c>
       <c r="C77" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="D77" t="s">
         <v>27</v>
@@ -61887,10 +61718,10 @@
     <row r="78">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
       <c r="C78" t="s">
-        <v>454</v>
+        <v>470</v>
       </c>
       <c r="D78" t="s">
         <v>27</v>
@@ -61902,10 +61733,10 @@
     <row r="79">
       <c r="A79"/>
       <c r="B79" t="s">
-        <v>455</v>
+        <v>471</v>
       </c>
       <c r="C79" t="s">
-        <v>456</v>
+        <v>472</v>
       </c>
       <c r="D79" t="s">
         <v>27</v>
@@ -61917,10 +61748,10 @@
     <row r="80">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>457</v>
+        <v>473</v>
       </c>
       <c r="C80" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="D80" t="s">
         <v>27</v>
@@ -61932,10 +61763,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="C81" t="s">
-        <v>460</v>
+        <v>476</v>
       </c>
       <c r="D81" t="s">
         <v>27</v>
@@ -61947,40 +61778,40 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>461</v>
+        <v>477</v>
       </c>
       <c r="C82" t="s">
-        <v>462</v>
+        <v>478</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
       </c>
       <c r="E82" t="s">
-        <v>27</v>
+        <v>479</v>
       </c>
     </row>
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>463</v>
+        <v>480</v>
       </c>
       <c r="C83" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
       </c>
       <c r="E83" t="s">
-        <v>27</v>
+        <v>482</v>
       </c>
     </row>
     <row r="84">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>465</v>
+        <v>483</v>
       </c>
       <c r="C84" t="s">
-        <v>466</v>
+        <v>484</v>
       </c>
       <c r="D84" t="s">
         <v>27</v>
@@ -61992,10 +61823,10 @@
     <row r="85">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>467</v>
+        <v>485</v>
       </c>
       <c r="C85" t="s">
-        <v>468</v>
+        <v>486</v>
       </c>
       <c r="D85" t="s">
         <v>27</v>
@@ -62007,10 +61838,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>469</v>
+        <v>487</v>
       </c>
       <c r="C86" t="s">
-        <v>470</v>
+        <v>488</v>
       </c>
       <c r="D86" t="s">
         <v>27</v>
@@ -62022,10 +61853,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>471</v>
+        <v>489</v>
       </c>
       <c r="C87" t="s">
-        <v>472</v>
+        <v>490</v>
       </c>
       <c r="D87" t="s">
         <v>27</v>
@@ -62037,10 +61868,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>473</v>
+        <v>491</v>
       </c>
       <c r="C88" t="s">
-        <v>474</v>
+        <v>492</v>
       </c>
       <c r="D88" t="s">
         <v>27</v>
@@ -62052,55 +61883,55 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>475</v>
+        <v>493</v>
       </c>
       <c r="C89" t="s">
-        <v>476</v>
+        <v>494</v>
       </c>
       <c r="D89" t="s">
         <v>27</v>
       </c>
       <c r="E89" t="s">
-        <v>27</v>
+        <v>493</v>
       </c>
     </row>
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>477</v>
+        <v>495</v>
       </c>
       <c r="C90" t="s">
-        <v>478</v>
+        <v>496</v>
       </c>
       <c r="D90" t="s">
         <v>27</v>
       </c>
       <c r="E90" t="s">
-        <v>479</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>480</v>
+        <v>497</v>
       </c>
       <c r="C91" t="s">
-        <v>481</v>
+        <v>498</v>
       </c>
       <c r="D91" t="s">
         <v>27</v>
       </c>
       <c r="E91" t="s">
-        <v>482</v>
+        <v>27</v>
       </c>
     </row>
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>483</v>
+        <v>499</v>
       </c>
       <c r="C92" t="s">
-        <v>484</v>
+        <v>500</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -62112,85 +61943,74 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>485</v>
+        <v>501</v>
       </c>
       <c r="C93" t="s">
-        <v>486</v>
+        <v>502</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
       </c>
       <c r="E93" t="s">
-        <v>27</v>
+        <v>501</v>
       </c>
     </row>
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>487</v>
+        <v>235</v>
       </c>
       <c r="C94" t="s">
-        <v>488</v>
+        <v>503</v>
       </c>
       <c r="D94" t="s">
         <v>27</v>
       </c>
       <c r="E94" t="s">
-        <v>27</v>
+        <v>236</v>
       </c>
     </row>
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>489</v>
+        <v>504</v>
       </c>
       <c r="C95" t="s">
-        <v>490</v>
+        <v>505</v>
       </c>
       <c r="D95" t="s">
         <v>27</v>
       </c>
       <c r="E95" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96"/>
-      <c r="B96" t="s">
-        <v>491</v>
-      </c>
-      <c r="C96" t="s">
-        <v>492</v>
-      </c>
-      <c r="D96" t="s">
-        <v>27</v>
-      </c>
-      <c r="E96" t="s">
-        <v>27</v>
+        <v>506</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97"/>
+      <c r="A97" t="s">
+        <v>2</v>
+      </c>
       <c r="B97" t="s">
-        <v>493</v>
+        <v>214</v>
       </c>
       <c r="C97" t="s">
-        <v>494</v>
+        <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E97" t="s">
-        <v>493</v>
+        <v>224</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98"/>
+      <c r="A98" t="s">
+        <v>53</v>
+      </c>
       <c r="B98" t="s">
-        <v>495</v>
+        <v>237</v>
       </c>
       <c r="C98" t="s">
-        <v>496</v>
+        <v>238</v>
       </c>
       <c r="D98" t="s">
         <v>27</v>
@@ -62202,10 +62022,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>497</v>
+        <v>239</v>
       </c>
       <c r="C99" t="s">
-        <v>498</v>
+        <v>240</v>
       </c>
       <c r="D99" t="s">
         <v>27</v>
@@ -62217,10 +62037,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>499</v>
+        <v>235</v>
       </c>
       <c r="C100" t="s">
-        <v>500</v>
+        <v>236</v>
       </c>
       <c r="D100" t="s">
         <v>27</v>
@@ -62232,74 +62052,74 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
-        <v>501</v>
+        <v>241</v>
       </c>
       <c r="C101" t="s">
-        <v>502</v>
+        <v>242</v>
       </c>
       <c r="D101" t="s">
         <v>27</v>
       </c>
       <c r="E101" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102"/>
-      <c r="B102" t="s">
-        <v>235</v>
-      </c>
-      <c r="C102" t="s">
-        <v>503</v>
-      </c>
-      <c r="D102" t="s">
-        <v>27</v>
-      </c>
-      <c r="E102" t="s">
-        <v>236</v>
+        <v>27</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103"/>
+      <c r="A103" t="s">
+        <v>2</v>
+      </c>
       <c r="B103" t="s">
-        <v>504</v>
+        <v>214</v>
       </c>
       <c r="C103" t="s">
-        <v>505</v>
+        <v>4</v>
       </c>
       <c r="D103" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E103" t="s">
-        <v>506</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104" t="s">
+        <v>369</v>
+      </c>
+      <c r="C104" t="s">
+        <v>370</v>
+      </c>
+      <c r="D104" t="s">
+        <v>27</v>
+      </c>
+      <c r="E104" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="s">
-        <v>2</v>
-      </c>
+      <c r="A105"/>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>371</v>
       </c>
       <c r="C105" t="s">
-        <v>4</v>
+        <v>372</v>
       </c>
       <c r="D105" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E105" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="s">
-        <v>2843</v>
-      </c>
+      <c r="A106"/>
       <c r="B106" t="s">
-        <v>2922</v>
+        <v>373</v>
       </c>
       <c r="C106" t="s">
-        <v>2923</v>
+        <v>374</v>
       </c>
       <c r="D106" t="s">
         <v>27</v>
@@ -62311,10 +62131,10 @@
     <row r="107">
       <c r="A107"/>
       <c r="B107" t="s">
-        <v>2924</v>
+        <v>241</v>
       </c>
       <c r="C107" t="s">
-        <v>2925</v>
+        <v>242</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -62323,43 +62143,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108"/>
-      <c r="B108" t="s">
-        <v>2926</v>
-      </c>
-      <c r="C108" t="s">
-        <v>2927</v>
-      </c>
-      <c r="D108" t="s">
-        <v>27</v>
-      </c>
-      <c r="E108" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="109">
-      <c r="A109"/>
+      <c r="A109" t="s">
+        <v>2</v>
+      </c>
       <c r="B109" t="s">
-        <v>2928</v>
+        <v>214</v>
       </c>
       <c r="C109" t="s">
-        <v>2929</v>
+        <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110"/>
+      <c r="A110" t="s">
+        <v>4132</v>
+      </c>
       <c r="B110" t="s">
-        <v>2930</v>
+        <v>4142</v>
       </c>
       <c r="C110" t="s">
-        <v>2931</v>
+        <v>4143</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -62371,10 +62180,10 @@
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>2932</v>
+        <v>2346</v>
       </c>
       <c r="C111" t="s">
-        <v>2933</v>
+        <v>2347</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -62386,10 +62195,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>2934</v>
+        <v>4144</v>
       </c>
       <c r="C112" t="s">
-        <v>2935</v>
+        <v>4145</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
@@ -62401,635 +62210,15 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>2936</v>
+        <v>4146</v>
       </c>
       <c r="C113" t="s">
-        <v>2937</v>
+        <v>4147</v>
       </c>
       <c r="D113" t="s">
         <v>27</v>
       </c>
       <c r="E113" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114"/>
-      <c r="B114" t="s">
-        <v>2938</v>
-      </c>
-      <c r="C114" t="s">
-        <v>2939</v>
-      </c>
-      <c r="D114" t="s">
-        <v>27</v>
-      </c>
-      <c r="E114" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115"/>
-      <c r="B115" t="s">
-        <v>2940</v>
-      </c>
-      <c r="C115" t="s">
-        <v>2941</v>
-      </c>
-      <c r="D115" t="s">
-        <v>27</v>
-      </c>
-      <c r="E115" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116"/>
-      <c r="B116" t="s">
-        <v>2942</v>
-      </c>
-      <c r="C116" t="s">
-        <v>2943</v>
-      </c>
-      <c r="D116" t="s">
-        <v>27</v>
-      </c>
-      <c r="E116" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117"/>
-      <c r="B117" t="s">
-        <v>2944</v>
-      </c>
-      <c r="C117" t="s">
-        <v>2945</v>
-      </c>
-      <c r="D117" t="s">
-        <v>27</v>
-      </c>
-      <c r="E117" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118"/>
-      <c r="B118" t="s">
-        <v>2946</v>
-      </c>
-      <c r="C118" t="s">
-        <v>2947</v>
-      </c>
-      <c r="D118" t="s">
-        <v>27</v>
-      </c>
-      <c r="E118" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119"/>
-      <c r="B119" t="s">
-        <v>2948</v>
-      </c>
-      <c r="C119" t="s">
-        <v>2949</v>
-      </c>
-      <c r="D119" t="s">
-        <v>27</v>
-      </c>
-      <c r="E119" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120"/>
-      <c r="B120" t="s">
-        <v>2950</v>
-      </c>
-      <c r="C120" t="s">
-        <v>2951</v>
-      </c>
-      <c r="D120" t="s">
-        <v>27</v>
-      </c>
-      <c r="E120" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121"/>
-      <c r="B121" t="s">
-        <v>2952</v>
-      </c>
-      <c r="C121" t="s">
-        <v>2953</v>
-      </c>
-      <c r="D121" t="s">
-        <v>27</v>
-      </c>
-      <c r="E121" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122"/>
-      <c r="B122" t="s">
-        <v>2954</v>
-      </c>
-      <c r="C122" t="s">
-        <v>2955</v>
-      </c>
-      <c r="D122" t="s">
-        <v>27</v>
-      </c>
-      <c r="E122" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123"/>
-      <c r="B123" t="s">
-        <v>2956</v>
-      </c>
-      <c r="C123" t="s">
-        <v>2957</v>
-      </c>
-      <c r="D123" t="s">
-        <v>27</v>
-      </c>
-      <c r="E123" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124"/>
-      <c r="B124" t="s">
-        <v>2958</v>
-      </c>
-      <c r="C124" t="s">
-        <v>2959</v>
-      </c>
-      <c r="D124" t="s">
-        <v>27</v>
-      </c>
-      <c r="E124" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125"/>
-      <c r="B125" t="s">
-        <v>2960</v>
-      </c>
-      <c r="C125" t="s">
-        <v>2961</v>
-      </c>
-      <c r="D125" t="s">
-        <v>27</v>
-      </c>
-      <c r="E125" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126"/>
-      <c r="B126" t="s">
-        <v>2962</v>
-      </c>
-      <c r="C126" t="s">
-        <v>2963</v>
-      </c>
-      <c r="D126" t="s">
-        <v>27</v>
-      </c>
-      <c r="E126" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127"/>
-      <c r="B127" t="s">
-        <v>2964</v>
-      </c>
-      <c r="C127" t="s">
-        <v>2965</v>
-      </c>
-      <c r="D127" t="s">
-        <v>27</v>
-      </c>
-      <c r="E127" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128"/>
-      <c r="B128" t="s">
-        <v>2966</v>
-      </c>
-      <c r="C128" t="s">
-        <v>2967</v>
-      </c>
-      <c r="D128" t="s">
-        <v>27</v>
-      </c>
-      <c r="E128" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129"/>
-      <c r="B129" t="s">
-        <v>235</v>
-      </c>
-      <c r="C129" t="s">
-        <v>236</v>
-      </c>
-      <c r="D129" t="s">
-        <v>27</v>
-      </c>
-      <c r="E129" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="s">
-        <v>2</v>
-      </c>
-      <c r="B131" t="s">
-        <v>214</v>
-      </c>
-      <c r="C131" t="s">
-        <v>4</v>
-      </c>
-      <c r="D131" t="s">
-        <v>5</v>
-      </c>
-      <c r="E131" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="s">
-        <v>2868</v>
-      </c>
-      <c r="B132" t="s">
-        <v>2972</v>
-      </c>
-      <c r="C132" t="s">
-        <v>2973</v>
-      </c>
-      <c r="D132" t="s">
-        <v>27</v>
-      </c>
-      <c r="E132" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133"/>
-      <c r="B133" t="s">
-        <v>2974</v>
-      </c>
-      <c r="C133" t="s">
-        <v>2975</v>
-      </c>
-      <c r="D133" t="s">
-        <v>27</v>
-      </c>
-      <c r="E133" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="s">
-        <v>2</v>
-      </c>
-      <c r="B135" t="s">
-        <v>214</v>
-      </c>
-      <c r="C135" t="s">
-        <v>4</v>
-      </c>
-      <c r="D135" t="s">
-        <v>5</v>
-      </c>
-      <c r="E135" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="s">
-        <v>53</v>
-      </c>
-      <c r="B136" t="s">
-        <v>237</v>
-      </c>
-      <c r="C136" t="s">
-        <v>238</v>
-      </c>
-      <c r="D136" t="s">
-        <v>27</v>
-      </c>
-      <c r="E136" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137"/>
-      <c r="B137" t="s">
-        <v>239</v>
-      </c>
-      <c r="C137" t="s">
-        <v>240</v>
-      </c>
-      <c r="D137" t="s">
-        <v>27</v>
-      </c>
-      <c r="E137" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138"/>
-      <c r="B138" t="s">
-        <v>235</v>
-      </c>
-      <c r="C138" t="s">
-        <v>236</v>
-      </c>
-      <c r="D138" t="s">
-        <v>27</v>
-      </c>
-      <c r="E138" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139"/>
-      <c r="B139" t="s">
-        <v>241</v>
-      </c>
-      <c r="C139" t="s">
-        <v>242</v>
-      </c>
-      <c r="D139" t="s">
-        <v>27</v>
-      </c>
-      <c r="E139" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="s">
-        <v>2</v>
-      </c>
-      <c r="B141" t="s">
-        <v>214</v>
-      </c>
-      <c r="C141" t="s">
-        <v>4</v>
-      </c>
-      <c r="D141" t="s">
-        <v>5</v>
-      </c>
-      <c r="E141" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="s">
-        <v>110</v>
-      </c>
-      <c r="B142" t="s">
-        <v>369</v>
-      </c>
-      <c r="C142" t="s">
-        <v>370</v>
-      </c>
-      <c r="D142" t="s">
-        <v>27</v>
-      </c>
-      <c r="E142" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143"/>
-      <c r="B143" t="s">
-        <v>371</v>
-      </c>
-      <c r="C143" t="s">
-        <v>372</v>
-      </c>
-      <c r="D143" t="s">
-        <v>27</v>
-      </c>
-      <c r="E143" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144"/>
-      <c r="B144" t="s">
-        <v>373</v>
-      </c>
-      <c r="C144" t="s">
-        <v>374</v>
-      </c>
-      <c r="D144" t="s">
-        <v>27</v>
-      </c>
-      <c r="E144" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145"/>
-      <c r="B145" t="s">
-        <v>241</v>
-      </c>
-      <c r="C145" t="s">
-        <v>242</v>
-      </c>
-      <c r="D145" t="s">
-        <v>27</v>
-      </c>
-      <c r="E145" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="s">
-        <v>2</v>
-      </c>
-      <c r="B147" t="s">
-        <v>214</v>
-      </c>
-      <c r="C147" t="s">
-        <v>4</v>
-      </c>
-      <c r="D147" t="s">
-        <v>5</v>
-      </c>
-      <c r="E147" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="s">
-        <v>2890</v>
-      </c>
-      <c r="B148" t="s">
-        <v>2982</v>
-      </c>
-      <c r="C148" t="s">
-        <v>2983</v>
-      </c>
-      <c r="D148" t="s">
-        <v>27</v>
-      </c>
-      <c r="E148" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149"/>
-      <c r="B149" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C149" t="s">
-        <v>1138</v>
-      </c>
-      <c r="D149" t="s">
-        <v>27</v>
-      </c>
-      <c r="E149" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150"/>
-      <c r="B150" t="s">
-        <v>2984</v>
-      </c>
-      <c r="C150" t="s">
-        <v>2985</v>
-      </c>
-      <c r="D150" t="s">
-        <v>27</v>
-      </c>
-      <c r="E150" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151"/>
-      <c r="B151" t="s">
-        <v>2986</v>
-      </c>
-      <c r="C151" t="s">
-        <v>2987</v>
-      </c>
-      <c r="D151" t="s">
-        <v>27</v>
-      </c>
-      <c r="E151" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152"/>
-      <c r="B152" t="s">
-        <v>2988</v>
-      </c>
-      <c r="C152" t="s">
-        <v>2989</v>
-      </c>
-      <c r="D152" t="s">
-        <v>27</v>
-      </c>
-      <c r="E152" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="s">
-        <v>2</v>
-      </c>
-      <c r="B154" t="s">
-        <v>214</v>
-      </c>
-      <c r="C154" t="s">
-        <v>4</v>
-      </c>
-      <c r="D154" t="s">
-        <v>5</v>
-      </c>
-      <c r="E154" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="s">
-        <v>4145</v>
-      </c>
-      <c r="B155" t="s">
-        <v>4155</v>
-      </c>
-      <c r="C155" t="s">
-        <v>4156</v>
-      </c>
-      <c r="D155" t="s">
-        <v>27</v>
-      </c>
-      <c r="E155" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156"/>
-      <c r="B156" t="s">
-        <v>2346</v>
-      </c>
-      <c r="C156" t="s">
-        <v>2347</v>
-      </c>
-      <c r="D156" t="s">
-        <v>27</v>
-      </c>
-      <c r="E156" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157"/>
-      <c r="B157" t="s">
-        <v>4157</v>
-      </c>
-      <c r="C157" t="s">
-        <v>4158</v>
-      </c>
-      <c r="D157" t="s">
-        <v>27</v>
-      </c>
-      <c r="E157" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158"/>
-      <c r="B158" t="s">
-        <v>4159</v>
-      </c>
-      <c r="C158" t="s">
-        <v>4160</v>
-      </c>
-      <c r="D158" t="s">
-        <v>27</v>
-      </c>
-      <c r="E158" t="s">
         <v>27</v>
       </c>
     </row>
@@ -63042,9 +62231,6 @@
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
-    <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
-    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -63111,13 +62297,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4161</v>
+        <v>4148</v>
       </c>
       <c r="B2" t="s">
-        <v>4162</v>
+        <v>4149</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4163</v>
+        <v>4150</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -63139,17 +62325,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4164</v>
+        <v>4151</v>
       </c>
       <c r="B3" t="s">
-        <v>4165</v>
+        <v>4152</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4166</v>
+        <v>4153</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -63165,13 +62351,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4167</v>
+        <v>4154</v>
       </c>
       <c r="B4" t="s">
-        <v>4168</v>
+        <v>4155</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>4097</v>
+        <v>4088</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
@@ -63191,17 +62377,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4169</v>
+        <v>4156</v>
       </c>
       <c r="B5" t="s">
-        <v>4170</v>
+        <v>4157</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4171</v>
+        <v>4158</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -63217,17 +62403,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4172</v>
+        <v>4159</v>
       </c>
       <c r="B6" t="s">
-        <v>4173</v>
+        <v>4160</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4174</v>
+        <v>4161</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -63243,7 +62429,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4175</v>
+        <v>4162</v>
       </c>
       <c r="B7" t="s">
         <v>3099</v>
@@ -63269,7 +62455,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4176</v>
+        <v>4163</v>
       </c>
       <c r="B8" t="s">
         <v>3111</v>
@@ -63295,7 +62481,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4177</v>
+        <v>4164</v>
       </c>
       <c r="B9" t="s">
         <v>3121</v>
@@ -63321,7 +62507,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4178</v>
+        <v>4165</v>
       </c>
       <c r="B10" t="s">
         <v>3129</v>
@@ -63347,7 +62533,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4179</v>
+        <v>4166</v>
       </c>
       <c r="B11" t="s">
         <v>3125</v>
@@ -63373,7 +62559,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4180</v>
+        <v>4167</v>
       </c>
       <c r="B12" t="s">
         <v>3096</v>
@@ -63399,7 +62585,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4181</v>
+        <v>4168</v>
       </c>
       <c r="B13" t="s">
         <v>196</v>
@@ -63425,7 +62611,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4182</v>
+        <v>4169</v>
       </c>
       <c r="B14" t="s">
         <v>3149</v>
@@ -63451,7 +62637,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4183</v>
+        <v>4170</v>
       </c>
       <c r="B15" t="s">
         <v>3087</v>
@@ -63477,7 +62663,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4184</v>
+        <v>4171</v>
       </c>
       <c r="B16" t="s">
         <v>3094</v>
@@ -63503,7 +62689,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4185</v>
+        <v>4172</v>
       </c>
       <c r="B17" t="s">
         <v>3152</v>
@@ -63529,10 +62715,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4186</v>
+        <v>4173</v>
       </c>
       <c r="B18" t="s">
-        <v>4187</v>
+        <v>4174</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3104</v>
@@ -64051,12 +63237,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4188</v>
+        <v>4175</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4189</v>
+        <v>4176</v>
       </c>
     </row>
   </sheetData>
@@ -66684,7 +65870,9 @@
       <c r="C94" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="D94"/>
+      <c r="D94" t="s">
+        <v>89</v>
+      </c>
       <c r="E94" t="s">
         <v>967</v>
       </c>
@@ -67326,7 +66514,9 @@
       <c r="C117" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="D117"/>
+      <c r="D117" t="s">
+        <v>89</v>
+      </c>
       <c r="E117" t="s">
         <v>1038</v>
       </c>
@@ -67592,7 +66782,9 @@
       <c r="C127" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="D127"/>
+      <c r="D127" t="s">
+        <v>89</v>
+      </c>
       <c r="E127" t="s">
         <v>1070</v>
       </c>

</xml_diff>

<commit_message>
#10214 - set ManyToOne relations of cached entities to lazy
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16473" uniqueCount="4181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16472" uniqueCount="4181">
   <si>
     <t>Field ID</t>
   </si>
@@ -12592,7 +12592,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.77.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -40637,9 +40637,7 @@
       <c r="F6" t="s" s="1">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
+      <c r="G6"/>
       <c r="H6"/>
       <c r="I6" t="s" s="1">
         <v>19</v>

</xml_diff>

<commit_message>
#9680: fixed test failings
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16478" uniqueCount="4184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16506" uniqueCount="4200">
   <si>
     <t>Field ID</t>
   </si>
@@ -11539,12 +11539,54 @@
     <t>Pfizer-BioNTech COVID-19 vaccine</t>
   </si>
   <si>
+    <t>MRNA_BIVALENT_BA_1_BIONTECH_PFIZER</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.1 (BioNTech/Pfizer)</t>
+  </si>
+  <si>
+    <t>MRNA_BIVALENT_BA_4_5_BIONTECH_PFIZER</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.4/5 (BioNTech/Pfizer)</t>
+  </si>
+  <si>
     <t>MRNA_1273</t>
   </si>
   <si>
     <t>Moderna COVID-19 Vaccine</t>
   </si>
   <si>
+    <t>MRNA_BIVALENT_BA_1_MODERNA</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.1 (Moderna)</t>
+  </si>
+  <si>
+    <t>MRNA_BIVALENT_BA_4_5_MODERNA</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.4/5 (Moderna)</t>
+  </si>
+  <si>
+    <t>VALNEVA</t>
+  </si>
+  <si>
+    <t>inactivated (Valneva)</t>
+  </si>
+  <si>
+    <t>NVX_COV_2373</t>
+  </si>
+  <si>
+    <t>Novavax COVID-19 vaccine</t>
+  </si>
+  <si>
+    <t>NUVAXOVID</t>
+  </si>
+  <si>
+    <t>protein-based, recombinant (Novavax)</t>
+  </si>
+  <si>
     <t>OXFORD_ASTRA_ZENECA</t>
   </si>
   <si>
@@ -11557,12 +11599,6 @@
     <t>Ad26.COV2.S</t>
   </si>
   <si>
-    <t>NVX_COV_2373</t>
-  </si>
-  <si>
-    <t>Novavax COVID-19 vaccine</t>
-  </si>
-  <si>
     <t>SANOFI_GSK</t>
   </si>
   <si>
@@ -11599,6 +11635,9 @@
     <t>Novavax</t>
   </si>
   <si>
+    <t>Valneva</t>
+  </si>
+  <si>
     <t>VACCINATION_CARD</t>
   </si>
   <si>
@@ -12445,7 +12484,16 @@
     <t>List of SampleReport</t>
   </si>
   <si>
-    <t>ExternalMessage.caze</t>
+    <t>ExternalMessage.surveillanceReport</t>
+  </si>
+  <si>
+    <t>surveillanceReport</t>
+  </si>
+  <si>
+    <t>SurveillanceReportReference</t>
+  </si>
+  <si>
+    <t>Linked Report</t>
   </si>
   <si>
     <t>ExternalMessage.externalMessageDetails</t>
@@ -14059,7 +14107,7 @@
 </file>
 
 <file path=xl/tables/table184.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="184" ref="A21:E29" displayName="VaccinationVaccine" name="VaccinationVaccine">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="184" ref="A21:E35" displayName="VaccinationVaccine" name="VaccinationVaccine">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14073,7 +14121,7 @@
 </file>
 
 <file path=xl/tables/table185.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="185" ref="A31:E39" displayName="VaccinationVaccineManufacturer" name="VaccinationVaccineManufacturer">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="185" ref="A37:E46" displayName="VaccinationVaccineManufacturer" name="VaccinationVaccineManufacturer">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14087,7 +14135,7 @@
 </file>
 
 <file path=xl/tables/table186.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="186" ref="A41:E45" displayName="VaccinationVaccinationInfoSource" name="VaccinationVaccinationInfoSource">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="186" ref="A48:E52" displayName="VaccinationVaccinationInfoSource" name="VaccinationVaccinationInfoSource">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14101,7 +14149,7 @@
 </file>
 
 <file path=xl/tables/table187.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="187" ref="A47:E50" displayName="VaccinationYesNoUnknown" name="VaccinationYesNoUnknown">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="187" ref="A54:E57" displayName="VaccinationYesNoUnknown" name="VaccinationYesNoUnknown">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14115,7 +14163,7 @@
 </file>
 
 <file path=xl/tables/table188.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="188" ref="A52:E56" displayName="VaccinationTrimester" name="VaccinationTrimester">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="188" ref="A59:E63" displayName="VaccinationTrimester" name="VaccinationTrimester">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -49698,7 +49746,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -50358,10 +50406,10 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>3839</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>3840</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -50373,10 +50421,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>235</v>
+        <v>3841</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>3842</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
@@ -50385,32 +50433,43 @@
         <v>27</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30"/>
+      <c r="B30" t="s">
+        <v>3843</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3844</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
+      <c r="A31"/>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>3845</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>3846</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>3797</v>
-      </c>
+      <c r="A32"/>
       <c r="B32" t="s">
-        <v>3839</v>
+        <v>3847</v>
       </c>
       <c r="C32" t="s">
-        <v>3840</v>
+        <v>3848</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -50422,10 +50481,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>3841</v>
+        <v>3849</v>
       </c>
       <c r="C33" t="s">
-        <v>3842</v>
+        <v>3850</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -50437,10 +50496,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>3843</v>
+        <v>241</v>
       </c>
       <c r="C34" t="s">
-        <v>3844</v>
+        <v>242</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -50452,10 +50511,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>3845</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
-        <v>3846</v>
+        <v>236</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
@@ -50464,43 +50523,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36"/>
-      <c r="B36" t="s">
-        <v>3847</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3848</v>
-      </c>
-      <c r="D36" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="37">
-      <c r="A37"/>
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
       <c r="B37" t="s">
-        <v>3837</v>
+        <v>214</v>
       </c>
       <c r="C37" t="s">
-        <v>3838</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38"/>
+      <c r="A38" t="s">
+        <v>3797</v>
+      </c>
       <c r="B38" t="s">
-        <v>241</v>
+        <v>3851</v>
       </c>
       <c r="C38" t="s">
-        <v>242</v>
+        <v>3852</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
@@ -50512,10 +50560,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>235</v>
+        <v>3853</v>
       </c>
       <c r="C39" t="s">
-        <v>236</v>
+        <v>3854</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -50524,32 +50572,43 @@
         <v>27</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40"/>
+      <c r="B40" t="s">
+        <v>3855</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3856</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>2</v>
-      </c>
+      <c r="A41"/>
       <c r="B41" t="s">
-        <v>214</v>
+        <v>3857</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>3858</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E41" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>3822</v>
-      </c>
+      <c r="A42"/>
       <c r="B42" t="s">
-        <v>3849</v>
+        <v>3859</v>
       </c>
       <c r="C42" t="s">
-        <v>3850</v>
+        <v>3860</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
@@ -50561,10 +50620,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>3851</v>
+        <v>3849</v>
       </c>
       <c r="C43" t="s">
-        <v>3852</v>
+        <v>3850</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
@@ -50576,10 +50635,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>3853</v>
+        <v>3839</v>
       </c>
       <c r="C44" t="s">
-        <v>3854</v>
+        <v>3861</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
@@ -50603,47 +50662,47 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
-        <v>214</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" t="s">
-        <v>224</v>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>749</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>1132</v>
+        <v>214</v>
       </c>
       <c r="C48" t="s">
-        <v>1133</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49"/>
+      <c r="A49" t="s">
+        <v>3822</v>
+      </c>
       <c r="B49" t="s">
-        <v>1134</v>
+        <v>3862</v>
       </c>
       <c r="C49" t="s">
-        <v>1135</v>
+        <v>3863</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -50655,74 +50714,74 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
+        <v>3864</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3865</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51"/>
+      <c r="B51" t="s">
+        <v>3866</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3867</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52"/>
+      <c r="B52" t="s">
         <v>241</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>242</v>
       </c>
-      <c r="D50" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
         <v>2</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>214</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>4</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>5</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E54" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>960</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1210</v>
-      </c>
-      <c r="D53" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54"/>
-      <c r="B54" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1212</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="55">
-      <c r="A55"/>
+      <c r="A55" t="s">
+        <v>749</v>
+      </c>
       <c r="B55" t="s">
-        <v>1213</v>
+        <v>1132</v>
       </c>
       <c r="C55" t="s">
-        <v>1214</v>
+        <v>1133</v>
       </c>
       <c r="D55" t="s">
         <v>27</v>
@@ -50734,15 +50793,109 @@
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57"/>
+      <c r="B57" t="s">
         <v>241</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>242</v>
       </c>
-      <c r="D56" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>960</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D60" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61"/>
+      <c r="B61" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62"/>
+      <c r="B62" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63"/>
+      <c r="B63" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63" t="s">
+        <v>242</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" t="s">
         <v>27</v>
       </c>
     </row>
@@ -50821,7 +50974,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3855</v>
+        <v>3868</v>
       </c>
       <c r="B2" t="s">
         <v>540</v>
@@ -50831,7 +50984,7 @@
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3856</v>
+        <v>3869</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -50849,7 +51002,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3857</v>
+        <v>3870</v>
       </c>
       <c r="B3" t="s">
         <v>709</v>
@@ -50875,7 +51028,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3858</v>
+        <v>3871</v>
       </c>
       <c r="B4" t="s">
         <v>712</v>
@@ -50901,7 +51054,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3859</v>
+        <v>3872</v>
       </c>
       <c r="B5" t="s">
         <v>3703</v>
@@ -50927,7 +51080,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3860</v>
+        <v>3873</v>
       </c>
       <c r="B6" t="s">
         <v>1063</v>
@@ -50953,7 +51106,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3861</v>
+        <v>3874</v>
       </c>
       <c r="B7" t="s">
         <v>678</v>
@@ -50979,7 +51132,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3862</v>
+        <v>3875</v>
       </c>
       <c r="B8" t="s">
         <v>685</v>
@@ -51007,7 +51160,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3863</v>
+        <v>3876</v>
       </c>
       <c r="B9" t="s">
         <v>681</v>
@@ -51033,7 +51186,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3864</v>
+        <v>3877</v>
       </c>
       <c r="B10" t="s">
         <v>688</v>
@@ -51061,7 +51214,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>3865</v>
+        <v>3878</v>
       </c>
       <c r="B11" t="s">
         <v>778</v>
@@ -51087,7 +51240,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3866</v>
+        <v>3879</v>
       </c>
       <c r="B12" t="s">
         <v>781</v>
@@ -51113,7 +51266,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3867</v>
+        <v>3880</v>
       </c>
       <c r="B13" t="s">
         <v>784</v>
@@ -51139,10 +51292,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>3868</v>
+        <v>3881</v>
       </c>
       <c r="B14" t="s">
-        <v>3869</v>
+        <v>3882</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>79</v>
@@ -51165,10 +51318,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3870</v>
+        <v>3883</v>
       </c>
       <c r="B15" t="s">
-        <v>3871</v>
+        <v>3884</v>
       </c>
       <c r="C15" t="s" s="1">
         <v>84</v>
@@ -51191,7 +51344,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>3872</v>
+        <v>3885</v>
       </c>
       <c r="B16" t="s">
         <v>883</v>
@@ -51217,7 +51370,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>3873</v>
+        <v>3886</v>
       </c>
       <c r="B17" t="s">
         <v>887</v>
@@ -51229,7 +51382,7 @@
         <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>3874</v>
+        <v>3887</v>
       </c>
       <c r="F17" t="s" s="1">
         <v>27</v>
@@ -51245,7 +51398,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>3875</v>
+        <v>3888</v>
       </c>
       <c r="B18" t="s">
         <v>2668</v>
@@ -51271,7 +51424,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>3876</v>
+        <v>3889</v>
       </c>
       <c r="B19" t="s">
         <v>196</v>
@@ -51297,10 +51450,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>3877</v>
+        <v>3890</v>
       </c>
       <c r="B20" t="s">
-        <v>3878</v>
+        <v>3891</v>
       </c>
       <c r="C20" t="s" s="1">
         <v>184</v>
@@ -51323,10 +51476,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>3879</v>
+        <v>3892</v>
       </c>
       <c r="B21" t="s">
-        <v>3880</v>
+        <v>3893</v>
       </c>
       <c r="C21" t="s" s="1">
         <v>184</v>
@@ -51349,17 +51502,17 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>3881</v>
+        <v>3894</v>
       </c>
       <c r="B22" t="s">
-        <v>3882</v>
+        <v>3895</v>
       </c>
       <c r="C22" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>3883</v>
+        <v>3896</v>
       </c>
       <c r="F22" t="s" s="1">
         <v>27</v>
@@ -51375,13 +51528,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>3884</v>
+        <v>3897</v>
       </c>
       <c r="B23" t="s">
-        <v>3885</v>
+        <v>3898</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>3886</v>
+        <v>3899</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
@@ -51401,7 +51554,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>3887</v>
+        <v>3900</v>
       </c>
       <c r="B24" t="s">
         <v>905</v>
@@ -51427,7 +51580,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>3888</v>
+        <v>3901</v>
       </c>
       <c r="B25" t="s">
         <v>909</v>
@@ -51455,7 +51608,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>3889</v>
+        <v>3902</v>
       </c>
       <c r="B26" t="s">
         <v>912</v>
@@ -51481,7 +51634,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>3890</v>
+        <v>3903</v>
       </c>
       <c r="B27" t="s">
         <v>915</v>
@@ -51507,7 +51660,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>3891</v>
+        <v>3904</v>
       </c>
       <c r="B28" t="s">
         <v>918</v>
@@ -51535,7 +51688,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>3892</v>
+        <v>3905</v>
       </c>
       <c r="B29" t="s">
         <v>921</v>
@@ -51561,7 +51714,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>3893</v>
+        <v>3906</v>
       </c>
       <c r="B30" t="s">
         <v>924</v>
@@ -51587,7 +51740,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>3894</v>
+        <v>3907</v>
       </c>
       <c r="B31" t="s">
         <v>927</v>
@@ -51613,7 +51766,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>3895</v>
+        <v>3908</v>
       </c>
       <c r="B32" t="s">
         <v>930</v>
@@ -51639,7 +51792,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>3896</v>
+        <v>3909</v>
       </c>
       <c r="B33" t="s">
         <v>933</v>
@@ -51665,7 +51818,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>3897</v>
+        <v>3910</v>
       </c>
       <c r="B34" t="s">
         <v>936</v>
@@ -51693,7 +51846,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>3898</v>
+        <v>3911</v>
       </c>
       <c r="B35" t="s">
         <v>939</v>
@@ -51719,7 +51872,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>3899</v>
+        <v>3912</v>
       </c>
       <c r="B36" t="s">
         <v>942</v>
@@ -51747,7 +51900,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>3900</v>
+        <v>3913</v>
       </c>
       <c r="B37" t="s">
         <v>944</v>
@@ -51773,7 +51926,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>3901</v>
+        <v>3914</v>
       </c>
       <c r="B38" t="s">
         <v>947</v>
@@ -51799,7 +51952,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>3902</v>
+        <v>3915</v>
       </c>
       <c r="B39" t="s">
         <v>950</v>
@@ -51825,7 +51978,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>3903</v>
+        <v>3916</v>
       </c>
       <c r="B40" t="s">
         <v>953</v>
@@ -51851,17 +52004,17 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>3904</v>
+        <v>3917</v>
       </c>
       <c r="B41" t="s">
-        <v>3905</v>
+        <v>3918</v>
       </c>
       <c r="C41" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>3906</v>
+        <v>3919</v>
       </c>
       <c r="F41" t="s" s="1">
         <v>27</v>
@@ -51877,7 +52030,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>3907</v>
+        <v>3920</v>
       </c>
       <c r="B42" t="s">
         <v>1065</v>
@@ -51903,7 +52056,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>3908</v>
+        <v>3921</v>
       </c>
       <c r="B43" t="s">
         <v>1069</v>
@@ -53247,17 +53400,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3909</v>
+        <v>3922</v>
       </c>
       <c r="B2" t="s">
-        <v>3910</v>
+        <v>3923</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3911</v>
+        <v>3924</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -53273,7 +53426,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3912</v>
+        <v>3925</v>
       </c>
       <c r="B3" t="s">
         <v>196</v>
@@ -53299,7 +53452,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3913</v>
+        <v>3926</v>
       </c>
       <c r="B4" t="s">
         <v>3703</v>
@@ -53309,7 +53462,7 @@
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -53393,17 +53546,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3915</v>
+        <v>3928</v>
       </c>
       <c r="B2" t="s">
-        <v>3910</v>
+        <v>3923</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3911</v>
+        <v>3924</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -53419,7 +53572,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3916</v>
+        <v>3929</v>
       </c>
       <c r="B3" t="s">
         <v>196</v>
@@ -53445,7 +53598,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3917</v>
+        <v>3930</v>
       </c>
       <c r="B4" t="s">
         <v>3703</v>
@@ -53455,7 +53608,7 @@
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -53471,7 +53624,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3918</v>
+        <v>3931</v>
       </c>
       <c r="B5" t="s">
         <v>583</v>
@@ -53481,7 +53634,7 @@
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>3919</v>
+        <v>3932</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -55482,17 +55635,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3920</v>
+        <v>3933</v>
       </c>
       <c r="B2" t="s">
-        <v>3910</v>
+        <v>3923</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3911</v>
+        <v>3924</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -55508,7 +55661,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3921</v>
+        <v>3934</v>
       </c>
       <c r="B3" t="s">
         <v>196</v>
@@ -55534,17 +55687,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3922</v>
+        <v>3935</v>
       </c>
       <c r="B4" t="s">
-        <v>3923</v>
+        <v>3936</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3924</v>
+        <v>3937</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -55560,17 +55713,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3925</v>
+        <v>3938</v>
       </c>
       <c r="B5" t="s">
-        <v>3926</v>
+        <v>3939</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>3927</v>
+        <v>3940</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -55586,7 +55739,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3928</v>
+        <v>3941</v>
       </c>
       <c r="B6" t="s">
         <v>3703</v>
@@ -55596,7 +55749,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -55612,7 +55765,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3929</v>
+        <v>3942</v>
       </c>
       <c r="B7" t="s">
         <v>587</v>
@@ -55706,17 +55859,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3930</v>
+        <v>3943</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -55732,17 +55885,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3933</v>
+        <v>3946</v>
       </c>
       <c r="B3" t="s">
-        <v>3934</v>
+        <v>3947</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>3935</v>
+        <v>3948</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -55758,17 +55911,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3936</v>
+        <v>3949</v>
       </c>
       <c r="B4" t="s">
-        <v>3937</v>
+        <v>3950</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>57</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3938</v>
+        <v>3951</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -55784,7 +55937,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3939</v>
+        <v>3952</v>
       </c>
       <c r="B5" t="s">
         <v>3703</v>
@@ -55794,7 +55947,7 @@
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -55810,7 +55963,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3940</v>
+        <v>3953</v>
       </c>
       <c r="B6" t="s">
         <v>891</v>
@@ -55836,17 +55989,17 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3941</v>
+        <v>3954</v>
       </c>
       <c r="B7" t="s">
-        <v>3942</v>
+        <v>3955</v>
       </c>
       <c r="C7" t="s" s="1">
-        <v>3943</v>
+        <v>3956</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>3944</v>
+        <v>3957</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -55862,7 +56015,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3945</v>
+        <v>3958</v>
       </c>
       <c r="B8" t="s">
         <v>591</v>
@@ -55956,17 +56109,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3946</v>
+        <v>3959</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -55982,17 +56135,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>3960</v>
+      </c>
+      <c r="B3" t="s">
         <v>3947</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3934</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>3935</v>
+        <v>3948</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -56008,17 +56161,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3948</v>
+        <v>3961</v>
       </c>
       <c r="B4" t="s">
-        <v>3937</v>
+        <v>3950</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>57</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3938</v>
+        <v>3951</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -56034,7 +56187,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3949</v>
+        <v>3962</v>
       </c>
       <c r="B5" t="s">
         <v>594</v>
@@ -56060,7 +56213,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3950</v>
+        <v>3963</v>
       </c>
       <c r="B6" t="s">
         <v>3703</v>
@@ -56070,7 +56223,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -56086,7 +56239,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3951</v>
+        <v>3964</v>
       </c>
       <c r="B7" t="s">
         <v>891</v>
@@ -56180,17 +56333,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3952</v>
+        <v>3965</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -56206,10 +56359,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3953</v>
+        <v>3966</v>
       </c>
       <c r="B3" t="s">
-        <v>3937</v>
+        <v>3950</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>57</v>
@@ -56232,7 +56385,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3954</v>
+        <v>3967</v>
       </c>
       <c r="B4" t="s">
         <v>594</v>
@@ -56258,7 +56411,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3955</v>
+        <v>3968</v>
       </c>
       <c r="B5" t="s">
         <v>597</v>
@@ -56284,7 +56437,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3956</v>
+        <v>3969</v>
       </c>
       <c r="B6" t="s">
         <v>3703</v>
@@ -56294,7 +56447,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -56310,7 +56463,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3957</v>
+        <v>3970</v>
       </c>
       <c r="B7" t="s">
         <v>891</v>
@@ -56404,17 +56557,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3958</v>
+        <v>3971</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -56430,7 +56583,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3959</v>
+        <v>3972</v>
       </c>
       <c r="B3" t="s">
         <v>594</v>
@@ -56456,7 +56609,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3960</v>
+        <v>3973</v>
       </c>
       <c r="B4" t="s">
         <v>597</v>
@@ -56482,7 +56635,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3961</v>
+        <v>3974</v>
       </c>
       <c r="B5" t="s">
         <v>600</v>
@@ -56508,7 +56661,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3962</v>
+        <v>3975</v>
       </c>
       <c r="B6" t="s">
         <v>604</v>
@@ -56534,7 +56687,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3963</v>
+        <v>3976</v>
       </c>
       <c r="B7" t="s">
         <v>624</v>
@@ -56560,7 +56713,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3964</v>
+        <v>3977</v>
       </c>
       <c r="B8" t="s">
         <v>627</v>
@@ -56586,7 +56739,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3965</v>
+        <v>3978</v>
       </c>
       <c r="B9" t="s">
         <v>630</v>
@@ -56612,7 +56765,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3966</v>
+        <v>3979</v>
       </c>
       <c r="B10" t="s">
         <v>560</v>
@@ -56638,7 +56791,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>3967</v>
+        <v>3980</v>
       </c>
       <c r="B11" t="s">
         <v>607</v>
@@ -56664,7 +56817,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3968</v>
+        <v>3981</v>
       </c>
       <c r="B12" t="s">
         <v>648</v>
@@ -56690,7 +56843,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3969</v>
+        <v>3982</v>
       </c>
       <c r="B13" t="s">
         <v>651</v>
@@ -56716,7 +56869,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>3970</v>
+        <v>3983</v>
       </c>
       <c r="B14" t="s">
         <v>654</v>
@@ -56742,7 +56895,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3971</v>
+        <v>3984</v>
       </c>
       <c r="B15" t="s">
         <v>657</v>
@@ -56768,7 +56921,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>3972</v>
+        <v>3985</v>
       </c>
       <c r="B16" t="s">
         <v>612</v>
@@ -56778,7 +56931,7 @@
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>3973</v>
+        <v>3986</v>
       </c>
       <c r="F16" t="s" s="1">
         <v>27</v>
@@ -56794,7 +56947,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>3974</v>
+        <v>3987</v>
       </c>
       <c r="B17" t="s">
         <v>616</v>
@@ -56804,7 +56957,7 @@
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>3975</v>
+        <v>3988</v>
       </c>
       <c r="F17" t="s" s="1">
         <v>27</v>
@@ -56820,10 +56973,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>3976</v>
+        <v>3989</v>
       </c>
       <c r="B18" t="s">
-        <v>3977</v>
+        <v>3990</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>93</v>
@@ -56846,17 +56999,17 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>3978</v>
+        <v>3991</v>
       </c>
       <c r="B19" t="s">
-        <v>3979</v>
+        <v>3992</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>3980</v>
+        <v>3993</v>
       </c>
       <c r="F19" t="s" s="1">
         <v>27</v>
@@ -56872,7 +57025,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>3981</v>
+        <v>3994</v>
       </c>
       <c r="B20" t="s">
         <v>3703</v>
@@ -56882,7 +57035,7 @@
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F20" t="s" s="1">
         <v>27</v>
@@ -56898,7 +57051,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>3982</v>
+        <v>3995</v>
       </c>
       <c r="B21" t="s">
         <v>891</v>
@@ -57977,17 +58130,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3983</v>
+        <v>3996</v>
       </c>
       <c r="B2" t="s">
-        <v>3984</v>
+        <v>3997</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>3985</v>
+        <v>3998</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3986</v>
+        <v>3999</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -58003,17 +58156,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3987</v>
+        <v>4000</v>
       </c>
       <c r="B3" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -58029,7 +58182,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3988</v>
+        <v>4001</v>
       </c>
       <c r="B4" t="s">
         <v>594</v>
@@ -58055,7 +58208,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3989</v>
+        <v>4002</v>
       </c>
       <c r="B5" t="s">
         <v>597</v>
@@ -58081,7 +58234,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3990</v>
+        <v>4003</v>
       </c>
       <c r="B6" t="s">
         <v>612</v>
@@ -58091,7 +58244,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3973</v>
+        <v>3986</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -58107,7 +58260,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3991</v>
+        <v>4004</v>
       </c>
       <c r="B7" t="s">
         <v>616</v>
@@ -58117,7 +58270,7 @@
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>3975</v>
+        <v>3988</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -58133,17 +58286,17 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3992</v>
+        <v>4005</v>
       </c>
       <c r="B8" t="s">
-        <v>3993</v>
+        <v>4006</v>
       </c>
       <c r="C8" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>3994</v>
+        <v>4007</v>
       </c>
       <c r="F8" t="s" s="1">
         <v>27</v>
@@ -58159,7 +58312,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3995</v>
+        <v>4008</v>
       </c>
       <c r="B9" t="s">
         <v>3703</v>
@@ -58169,7 +58322,7 @@
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F9" t="s" s="1">
         <v>27</v>
@@ -58185,7 +58338,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3996</v>
+        <v>4009</v>
       </c>
       <c r="B10" t="s">
         <v>891</v>
@@ -58228,13 +58381,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3985</v>
+        <v>3998</v>
       </c>
       <c r="B13" t="s">
-        <v>3997</v>
+        <v>4010</v>
       </c>
       <c r="C13" t="s">
-        <v>3998</v>
+        <v>4011</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -58246,10 +58399,10 @@
     <row r="14">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>3999</v>
+        <v>4012</v>
       </c>
       <c r="C14" t="s">
-        <v>4000</v>
+        <v>4013</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
@@ -58261,10 +58414,10 @@
     <row r="15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>4001</v>
+        <v>4014</v>
       </c>
       <c r="C15" t="s">
-        <v>4002</v>
+        <v>4015</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
@@ -58359,17 +58512,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4003</v>
+        <v>4016</v>
       </c>
       <c r="B2" t="s">
-        <v>3993</v>
+        <v>4006</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3994</v>
+        <v>4007</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -58385,17 +58538,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4004</v>
+        <v>4017</v>
       </c>
       <c r="B3" t="s">
-        <v>4005</v>
+        <v>4018</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4006</v>
+        <v>4019</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -58411,7 +58564,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4007</v>
+        <v>4020</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -58437,7 +58590,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4008</v>
+        <v>4021</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -58463,10 +58616,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4009</v>
+        <v>4022</v>
       </c>
       <c r="B6" t="s">
-        <v>4010</v>
+        <v>4023</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
@@ -58489,17 +58642,17 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4011</v>
+        <v>4024</v>
       </c>
       <c r="B7" t="s">
-        <v>4012</v>
+        <v>4025</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>4013</v>
+        <v>4026</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -58515,7 +58668,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4014</v>
+        <v>4027</v>
       </c>
       <c r="B8" t="s">
         <v>148</v>
@@ -58525,7 +58678,7 @@
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>4015</v>
+        <v>4028</v>
       </c>
       <c r="F8" t="s" s="1">
         <v>27</v>
@@ -58541,17 +58694,17 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4016</v>
+        <v>4029</v>
       </c>
       <c r="B9" t="s">
-        <v>4017</v>
+        <v>4030</v>
       </c>
       <c r="C9" t="s" s="1">
-        <v>4018</v>
+        <v>4031</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>4019</v>
+        <v>4032</v>
       </c>
       <c r="F9" t="s" s="1">
         <v>27</v>
@@ -58567,7 +58720,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4020</v>
+        <v>4033</v>
       </c>
       <c r="B10" t="s">
         <v>594</v>
@@ -58593,7 +58746,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4021</v>
+        <v>4034</v>
       </c>
       <c r="B11" t="s">
         <v>597</v>
@@ -58619,7 +58772,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4022</v>
+        <v>4035</v>
       </c>
       <c r="B12" t="s">
         <v>600</v>
@@ -58645,7 +58798,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4023</v>
+        <v>4036</v>
       </c>
       <c r="B13" t="s">
         <v>791</v>
@@ -58671,10 +58824,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4024</v>
+        <v>4037</v>
       </c>
       <c r="B14" t="s">
-        <v>4025</v>
+        <v>4038</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>97</v>
@@ -58697,7 +58850,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4026</v>
+        <v>4039</v>
       </c>
       <c r="B15" t="s">
         <v>883</v>
@@ -58707,7 +58860,7 @@
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>4027</v>
+        <v>4040</v>
       </c>
       <c r="F15" t="s" s="1">
         <v>27</v>
@@ -58723,17 +58876,17 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4028</v>
+        <v>4041</v>
       </c>
       <c r="B16" t="s">
-        <v>4029</v>
+        <v>4042</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>713</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>4030</v>
+        <v>4043</v>
       </c>
       <c r="F16" t="s" s="1">
         <v>27</v>
@@ -58749,20 +58902,20 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4031</v>
+        <v>4044</v>
       </c>
       <c r="B17" t="s">
-        <v>4032</v>
+        <v>4045</v>
       </c>
       <c r="C17" t="s" s="1">
         <v>123</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>4033</v>
+        <v>4046</v>
       </c>
       <c r="F17" t="s" s="1">
-        <v>4034</v>
+        <v>4047</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
@@ -58775,13 +58928,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4035</v>
+        <v>4048</v>
       </c>
       <c r="B18" t="s">
-        <v>4036</v>
+        <v>4049</v>
       </c>
       <c r="C18" t="s" s="1">
-        <v>4037</v>
+        <v>4050</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
@@ -58801,10 +58954,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4038</v>
+        <v>4051</v>
       </c>
       <c r="B19" t="s">
-        <v>4039</v>
+        <v>4052</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>184</v>
@@ -58827,13 +58980,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4040</v>
+        <v>4053</v>
       </c>
       <c r="B20" t="s">
-        <v>4041</v>
+        <v>4054</v>
       </c>
       <c r="C20" t="s" s="1">
-        <v>4042</v>
+        <v>4055</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
@@ -59856,13 +60009,13 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>4037</v>
+        <v>4050</v>
       </c>
       <c r="B91" t="s">
-        <v>4043</v>
+        <v>4056</v>
       </c>
       <c r="C91" t="s">
-        <v>4044</v>
+        <v>4057</v>
       </c>
       <c r="D91" t="s">
         <v>27</v>
@@ -59874,10 +60027,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>4045</v>
+        <v>4058</v>
       </c>
       <c r="C92" t="s">
-        <v>4046</v>
+        <v>4059</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -59889,10 +60042,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>4047</v>
+        <v>4060</v>
       </c>
       <c r="C93" t="s">
-        <v>4048</v>
+        <v>4061</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
@@ -59904,10 +60057,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>4049</v>
+        <v>4062</v>
       </c>
       <c r="C94" t="s">
-        <v>4050</v>
+        <v>4063</v>
       </c>
       <c r="D94" t="s">
         <v>27</v>
@@ -59919,10 +60072,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>4051</v>
+        <v>4064</v>
       </c>
       <c r="C95" t="s">
-        <v>4052</v>
+        <v>4065</v>
       </c>
       <c r="D95" t="s">
         <v>27</v>
@@ -59934,10 +60087,10 @@
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
-        <v>4053</v>
+        <v>4066</v>
       </c>
       <c r="C96" t="s">
-        <v>4054</v>
+        <v>4067</v>
       </c>
       <c r="D96" t="s">
         <v>27</v>
@@ -59949,10 +60102,10 @@
     <row r="97">
       <c r="A97"/>
       <c r="B97" t="s">
-        <v>4055</v>
+        <v>4068</v>
       </c>
       <c r="C97" t="s">
-        <v>4056</v>
+        <v>4069</v>
       </c>
       <c r="D97" t="s">
         <v>27</v>
@@ -59964,10 +60117,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>4057</v>
+        <v>4070</v>
       </c>
       <c r="C98" t="s">
-        <v>4058</v>
+        <v>4071</v>
       </c>
       <c r="D98" t="s">
         <v>27</v>
@@ -59979,10 +60132,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>4059</v>
+        <v>4072</v>
       </c>
       <c r="C99" t="s">
-        <v>4060</v>
+        <v>4073</v>
       </c>
       <c r="D99" t="s">
         <v>27</v>
@@ -59994,10 +60147,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>4061</v>
+        <v>4074</v>
       </c>
       <c r="C100" t="s">
-        <v>4062</v>
+        <v>4075</v>
       </c>
       <c r="D100" t="s">
         <v>27</v>
@@ -60009,10 +60162,10 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
-        <v>4063</v>
+        <v>4076</v>
       </c>
       <c r="C101" t="s">
-        <v>4064</v>
+        <v>4077</v>
       </c>
       <c r="D101" t="s">
         <v>27</v>
@@ -60024,10 +60177,10 @@
     <row r="102">
       <c r="A102"/>
       <c r="B102" t="s">
-        <v>4065</v>
+        <v>4078</v>
       </c>
       <c r="C102" t="s">
-        <v>4066</v>
+        <v>4079</v>
       </c>
       <c r="D102" t="s">
         <v>27</v>
@@ -60039,10 +60192,10 @@
     <row r="103">
       <c r="A103"/>
       <c r="B103" t="s">
-        <v>4067</v>
+        <v>4080</v>
       </c>
       <c r="C103" t="s">
-        <v>4068</v>
+        <v>4081</v>
       </c>
       <c r="D103" t="s">
         <v>27</v>
@@ -60054,10 +60207,10 @@
     <row r="104">
       <c r="A104"/>
       <c r="B104" t="s">
-        <v>4069</v>
+        <v>4082</v>
       </c>
       <c r="C104" t="s">
-        <v>4070</v>
+        <v>4083</v>
       </c>
       <c r="D104" t="s">
         <v>27</v>
@@ -60069,10 +60222,10 @@
     <row r="105">
       <c r="A105"/>
       <c r="B105" t="s">
-        <v>4071</v>
+        <v>4084</v>
       </c>
       <c r="C105" t="s">
-        <v>4072</v>
+        <v>4085</v>
       </c>
       <c r="D105" t="s">
         <v>27</v>
@@ -60084,10 +60237,10 @@
     <row r="106">
       <c r="A106"/>
       <c r="B106" t="s">
-        <v>4073</v>
+        <v>4086</v>
       </c>
       <c r="C106" t="s">
-        <v>4074</v>
+        <v>4087</v>
       </c>
       <c r="D106" t="s">
         <v>27</v>
@@ -60099,10 +60252,10 @@
     <row r="107">
       <c r="A107"/>
       <c r="B107" t="s">
-        <v>4075</v>
+        <v>4088</v>
       </c>
       <c r="C107" t="s">
-        <v>4076</v>
+        <v>4089</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -60130,7 +60283,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>4042</v>
+        <v>4055</v>
       </c>
       <c r="B110" t="s">
         <v>513</v>
@@ -60148,10 +60301,10 @@
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>4077</v>
+        <v>4090</v>
       </c>
       <c r="C111" t="s">
-        <v>4078</v>
+        <v>4091</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -60163,7 +60316,7 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>4079</v>
+        <v>4092</v>
       </c>
       <c r="C112" t="s">
         <v>595</v>
@@ -60178,7 +60331,7 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>4080</v>
+        <v>4093</v>
       </c>
       <c r="C113" t="s">
         <v>598</v>
@@ -60223,7 +60376,7 @@
     <row r="116">
       <c r="A116"/>
       <c r="B116" t="s">
-        <v>4081</v>
+        <v>4094</v>
       </c>
       <c r="C116" t="s">
         <v>644</v>
@@ -60253,10 +60406,10 @@
     <row r="118">
       <c r="A118"/>
       <c r="B118" t="s">
-        <v>4082</v>
+        <v>4095</v>
       </c>
       <c r="C118" t="s">
-        <v>4083</v>
+        <v>4096</v>
       </c>
       <c r="D118" t="s">
         <v>27</v>
@@ -60339,13 +60492,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4084</v>
+        <v>4097</v>
       </c>
       <c r="B2" t="s">
-        <v>3977</v>
+        <v>3990</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4085</v>
+        <v>4098</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -60365,7 +60518,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4086</v>
+        <v>4099</v>
       </c>
       <c r="B3" t="s">
         <v>678</v>
@@ -60391,17 +60544,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4087</v>
+        <v>4100</v>
       </c>
       <c r="B4" t="s">
-        <v>4088</v>
+        <v>4101</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>4089</v>
+        <v>4102</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -60417,17 +60570,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4090</v>
+        <v>4103</v>
       </c>
       <c r="B5" t="s">
-        <v>4091</v>
+        <v>4104</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4092</v>
+        <v>4105</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -60443,13 +60596,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4093</v>
+        <v>4106</v>
       </c>
       <c r="B6" t="s">
-        <v>4094</v>
+        <v>4107</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>4095</v>
+        <v>4108</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
@@ -60469,17 +60622,17 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4096</v>
+        <v>4109</v>
       </c>
       <c r="B7" t="s">
-        <v>4097</v>
+        <v>4110</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>4098</v>
+        <v>4111</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -60495,17 +60648,17 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4099</v>
+        <v>4112</v>
       </c>
       <c r="B8" t="s">
-        <v>4100</v>
+        <v>4113</v>
       </c>
       <c r="C8" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>4101</v>
+        <v>4114</v>
       </c>
       <c r="F8" t="s" s="1">
         <v>27</v>
@@ -60521,10 +60674,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4102</v>
+        <v>4115</v>
       </c>
       <c r="B9" t="s">
-        <v>4103</v>
+        <v>4116</v>
       </c>
       <c r="C9" t="s" s="1">
         <v>14</v>
@@ -60547,10 +60700,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4104</v>
+        <v>4117</v>
       </c>
       <c r="B10" t="s">
-        <v>4105</v>
+        <v>4118</v>
       </c>
       <c r="C10" t="s" s="1">
         <v>14</v>
@@ -60573,10 +60726,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4106</v>
+        <v>4119</v>
       </c>
       <c r="B11" t="s">
-        <v>4107</v>
+        <v>4120</v>
       </c>
       <c r="C11" t="s" s="1">
         <v>53</v>
@@ -60599,10 +60752,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4108</v>
+        <v>4121</v>
       </c>
       <c r="B12" t="s">
-        <v>4109</v>
+        <v>4122</v>
       </c>
       <c r="C12" t="s" s="1">
         <v>110</v>
@@ -60625,10 +60778,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4110</v>
+        <v>4123</v>
       </c>
       <c r="B13" t="s">
-        <v>4111</v>
+        <v>4124</v>
       </c>
       <c r="C13" t="s" s="1">
         <v>57</v>
@@ -60651,10 +60804,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4112</v>
+        <v>4125</v>
       </c>
       <c r="B14" t="s">
-        <v>4113</v>
+        <v>4126</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>57</v>
@@ -60677,10 +60830,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4114</v>
+        <v>4127</v>
       </c>
       <c r="B15" t="s">
-        <v>4115</v>
+        <v>4128</v>
       </c>
       <c r="C15" t="s" s="1">
         <v>57</v>
@@ -60703,10 +60856,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4116</v>
+        <v>4129</v>
       </c>
       <c r="B16" t="s">
-        <v>4117</v>
+        <v>4130</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>14</v>
@@ -60729,10 +60882,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4118</v>
+        <v>4131</v>
       </c>
       <c r="B17" t="s">
-        <v>4119</v>
+        <v>4132</v>
       </c>
       <c r="C17" t="s" s="1">
         <v>14</v>
@@ -60755,10 +60908,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4120</v>
+        <v>4133</v>
       </c>
       <c r="B18" t="s">
-        <v>4121</v>
+        <v>4134</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>14</v>
@@ -60781,10 +60934,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4122</v>
+        <v>4135</v>
       </c>
       <c r="B19" t="s">
-        <v>4123</v>
+        <v>4136</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>14</v>
@@ -60807,10 +60960,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4124</v>
+        <v>4137</v>
       </c>
       <c r="B20" t="s">
-        <v>4125</v>
+        <v>4138</v>
       </c>
       <c r="C20" t="s" s="1">
         <v>14</v>
@@ -60833,10 +60986,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4126</v>
+        <v>4139</v>
       </c>
       <c r="B21" t="s">
-        <v>4127</v>
+        <v>4140</v>
       </c>
       <c r="C21" t="s" s="1">
         <v>14</v>
@@ -60859,13 +61012,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>4128</v>
+        <v>4141</v>
       </c>
       <c r="B22" t="s">
-        <v>4129</v>
+        <v>4142</v>
       </c>
       <c r="C22" t="s" s="1">
-        <v>4130</v>
+        <v>4143</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
@@ -60885,17 +61038,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>4131</v>
+        <v>4144</v>
       </c>
       <c r="B23" t="s">
-        <v>1533</v>
+        <v>4145</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>1534</v>
+        <v>4146</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>4147</v>
       </c>
       <c r="F23" t="s" s="1">
         <v>27</v>
@@ -60911,10 +61064,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>4132</v>
+        <v>4148</v>
       </c>
       <c r="B24" t="s">
-        <v>4133</v>
+        <v>4149</v>
       </c>
       <c r="C24" t="s" s="1">
         <v>14</v>
@@ -60937,17 +61090,17 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>4134</v>
+        <v>4150</v>
       </c>
       <c r="B25" t="s">
-        <v>4135</v>
+        <v>4151</v>
       </c>
       <c r="C25" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>4136</v>
+        <v>4152</v>
       </c>
       <c r="F25" t="s" s="1">
         <v>27</v>
@@ -60963,17 +61116,17 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>4137</v>
+        <v>4153</v>
       </c>
       <c r="B26" t="s">
-        <v>4138</v>
+        <v>4154</v>
       </c>
       <c r="C26" t="s" s="1">
-        <v>4139</v>
+        <v>4155</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>4140</v>
+        <v>4156</v>
       </c>
       <c r="F26" t="s" s="1">
         <v>27</v>
@@ -60989,17 +61142,17 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>4141</v>
+        <v>4157</v>
       </c>
       <c r="B27" t="s">
-        <v>4142</v>
+        <v>4158</v>
       </c>
       <c r="C27" t="s" s="1">
         <v>713</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>4143</v>
+        <v>4159</v>
       </c>
       <c r="F27" t="s" s="1">
         <v>27</v>
@@ -61015,7 +61168,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4144</v>
+        <v>4160</v>
       </c>
       <c r="B28" t="s">
         <v>712</v>
@@ -61058,13 +61211,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4085</v>
+        <v>4098</v>
       </c>
       <c r="B31" t="s">
-        <v>4145</v>
+        <v>4161</v>
       </c>
       <c r="C31" t="s">
-        <v>4146</v>
+        <v>4162</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
@@ -61076,10 +61229,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>4147</v>
+        <v>4163</v>
       </c>
       <c r="C32" t="s">
-        <v>4148</v>
+        <v>4164</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -62199,13 +62352,13 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>4139</v>
+        <v>4155</v>
       </c>
       <c r="B110" t="s">
-        <v>4149</v>
+        <v>4165</v>
       </c>
       <c r="C110" t="s">
-        <v>4150</v>
+        <v>4166</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -62232,10 +62385,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>4151</v>
+        <v>4167</v>
       </c>
       <c r="C112" t="s">
-        <v>4152</v>
+        <v>4168</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
@@ -62247,10 +62400,10 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>4153</v>
+        <v>4169</v>
       </c>
       <c r="C113" t="s">
-        <v>4154</v>
+        <v>4170</v>
       </c>
       <c r="D113" t="s">
         <v>27</v>
@@ -62334,13 +62487,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4155</v>
+        <v>4171</v>
       </c>
       <c r="B2" t="s">
-        <v>4156</v>
+        <v>4172</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4157</v>
+        <v>4173</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -62362,17 +62515,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4158</v>
+        <v>4174</v>
       </c>
       <c r="B3" t="s">
-        <v>4159</v>
+        <v>4175</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4160</v>
+        <v>4176</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -62388,13 +62541,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4161</v>
+        <v>4177</v>
       </c>
       <c r="B4" t="s">
-        <v>4162</v>
+        <v>4178</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>4095</v>
+        <v>4108</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
@@ -62414,17 +62567,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4163</v>
+        <v>4179</v>
       </c>
       <c r="B5" t="s">
-        <v>4164</v>
+        <v>4180</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4165</v>
+        <v>4181</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -62440,17 +62593,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4166</v>
+        <v>4182</v>
       </c>
       <c r="B6" t="s">
-        <v>4167</v>
+        <v>4183</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4168</v>
+        <v>4184</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -62466,7 +62619,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4169</v>
+        <v>4185</v>
       </c>
       <c r="B7" t="s">
         <v>3103</v>
@@ -62492,7 +62645,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4170</v>
+        <v>4186</v>
       </c>
       <c r="B8" t="s">
         <v>3115</v>
@@ -62518,7 +62671,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4171</v>
+        <v>4187</v>
       </c>
       <c r="B9" t="s">
         <v>3125</v>
@@ -62544,7 +62697,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4172</v>
+        <v>4188</v>
       </c>
       <c r="B10" t="s">
         <v>3133</v>
@@ -62570,7 +62723,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4173</v>
+        <v>4189</v>
       </c>
       <c r="B11" t="s">
         <v>3129</v>
@@ -62596,7 +62749,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4174</v>
+        <v>4190</v>
       </c>
       <c r="B12" t="s">
         <v>3100</v>
@@ -62622,7 +62775,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4175</v>
+        <v>4191</v>
       </c>
       <c r="B13" t="s">
         <v>196</v>
@@ -62648,7 +62801,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4176</v>
+        <v>4192</v>
       </c>
       <c r="B14" t="s">
         <v>3153</v>
@@ -62674,7 +62827,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4177</v>
+        <v>4193</v>
       </c>
       <c r="B15" t="s">
         <v>3091</v>
@@ -62700,7 +62853,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4178</v>
+        <v>4194</v>
       </c>
       <c r="B16" t="s">
         <v>3098</v>
@@ -62726,7 +62879,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4179</v>
+        <v>4195</v>
       </c>
       <c r="B17" t="s">
         <v>3156</v>
@@ -62752,10 +62905,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4180</v>
+        <v>4196</v>
       </c>
       <c r="B18" t="s">
-        <v>4181</v>
+        <v>4197</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3108</v>
@@ -63274,12 +63427,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4182</v>
+        <v>4198</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4183</v>
+        <v>4199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change 9680 adjust the processing of external messages to create surveillance reports (#11082)
* #9680 rename method

... for better fitting the new generic use case.

* #9680 populate surveillance report

* #9680 rename method

* #9680 add some tests

incomplete, not all new functionility is properly tested yet.

* #9680: fixed some tests

* #9680: Create SurveillanceReport after processed an ExternalMessage

* #9680: Added UI part, fixed backend

* #9680: Added validation

* #9680: fixed problems

* #9680: migration

* #9680: Removed Case reference from ExternalMessage

* #9680: fixed test

* #9680: fixed test failings

* #9680: removed meaningless test

Co-authored-by: FredrikSchäferVitagroup <fredrik.schaefer@vitagroup.ag>
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16478" uniqueCount="4184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16506" uniqueCount="4200">
   <si>
     <t>Field ID</t>
   </si>
@@ -11539,12 +11539,54 @@
     <t>Pfizer-BioNTech COVID-19 vaccine</t>
   </si>
   <si>
+    <t>MRNA_BIVALENT_BA_1_BIONTECH_PFIZER</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.1 (BioNTech/Pfizer)</t>
+  </si>
+  <si>
+    <t>MRNA_BIVALENT_BA_4_5_BIONTECH_PFIZER</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.4/5 (BioNTech/Pfizer)</t>
+  </si>
+  <si>
     <t>MRNA_1273</t>
   </si>
   <si>
     <t>Moderna COVID-19 Vaccine</t>
   </si>
   <si>
+    <t>MRNA_BIVALENT_BA_1_MODERNA</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.1 (Moderna)</t>
+  </si>
+  <si>
+    <t>MRNA_BIVALENT_BA_4_5_MODERNA</t>
+  </si>
+  <si>
+    <t>mRNA/bivalent BA.4/5 (Moderna)</t>
+  </si>
+  <si>
+    <t>VALNEVA</t>
+  </si>
+  <si>
+    <t>inactivated (Valneva)</t>
+  </si>
+  <si>
+    <t>NVX_COV_2373</t>
+  </si>
+  <si>
+    <t>Novavax COVID-19 vaccine</t>
+  </si>
+  <si>
+    <t>NUVAXOVID</t>
+  </si>
+  <si>
+    <t>protein-based, recombinant (Novavax)</t>
+  </si>
+  <si>
     <t>OXFORD_ASTRA_ZENECA</t>
   </si>
   <si>
@@ -11557,12 +11599,6 @@
     <t>Ad26.COV2.S</t>
   </si>
   <si>
-    <t>NVX_COV_2373</t>
-  </si>
-  <si>
-    <t>Novavax COVID-19 vaccine</t>
-  </si>
-  <si>
     <t>SANOFI_GSK</t>
   </si>
   <si>
@@ -11599,6 +11635,9 @@
     <t>Novavax</t>
   </si>
   <si>
+    <t>Valneva</t>
+  </si>
+  <si>
     <t>VACCINATION_CARD</t>
   </si>
   <si>
@@ -12445,7 +12484,16 @@
     <t>List of SampleReport</t>
   </si>
   <si>
-    <t>ExternalMessage.caze</t>
+    <t>ExternalMessage.surveillanceReport</t>
+  </si>
+  <si>
+    <t>surveillanceReport</t>
+  </si>
+  <si>
+    <t>SurveillanceReportReference</t>
+  </si>
+  <si>
+    <t>Linked Report</t>
   </si>
   <si>
     <t>ExternalMessage.externalMessageDetails</t>
@@ -14059,7 +14107,7 @@
 </file>
 
 <file path=xl/tables/table184.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="184" ref="A21:E29" displayName="VaccinationVaccine" name="VaccinationVaccine">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="184" ref="A21:E35" displayName="VaccinationVaccine" name="VaccinationVaccine">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14073,7 +14121,7 @@
 </file>
 
 <file path=xl/tables/table185.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="185" ref="A31:E39" displayName="VaccinationVaccineManufacturer" name="VaccinationVaccineManufacturer">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="185" ref="A37:E46" displayName="VaccinationVaccineManufacturer" name="VaccinationVaccineManufacturer">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14087,7 +14135,7 @@
 </file>
 
 <file path=xl/tables/table186.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="186" ref="A41:E45" displayName="VaccinationVaccinationInfoSource" name="VaccinationVaccinationInfoSource">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="186" ref="A48:E52" displayName="VaccinationVaccinationInfoSource" name="VaccinationVaccinationInfoSource">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14101,7 +14149,7 @@
 </file>
 
 <file path=xl/tables/table187.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="187" ref="A47:E50" displayName="VaccinationYesNoUnknown" name="VaccinationYesNoUnknown">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="187" ref="A54:E57" displayName="VaccinationYesNoUnknown" name="VaccinationYesNoUnknown">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14115,7 +14163,7 @@
 </file>
 
 <file path=xl/tables/table188.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="188" ref="A52:E56" displayName="VaccinationTrimester" name="VaccinationTrimester">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="188" ref="A59:E63" displayName="VaccinationTrimester" name="VaccinationTrimester">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -49698,7 +49746,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -50358,10 +50406,10 @@
     <row r="28">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>3839</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>3840</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -50373,10 +50421,10 @@
     <row r="29">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>235</v>
+        <v>3841</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>3842</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
@@ -50385,32 +50433,43 @@
         <v>27</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30"/>
+      <c r="B30" t="s">
+        <v>3843</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3844</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
+      <c r="A31"/>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>3845</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>3846</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>3797</v>
-      </c>
+      <c r="A32"/>
       <c r="B32" t="s">
-        <v>3839</v>
+        <v>3847</v>
       </c>
       <c r="C32" t="s">
-        <v>3840</v>
+        <v>3848</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -50422,10 +50481,10 @@
     <row r="33">
       <c r="A33"/>
       <c r="B33" t="s">
-        <v>3841</v>
+        <v>3849</v>
       </c>
       <c r="C33" t="s">
-        <v>3842</v>
+        <v>3850</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -50437,10 +50496,10 @@
     <row r="34">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>3843</v>
+        <v>241</v>
       </c>
       <c r="C34" t="s">
-        <v>3844</v>
+        <v>242</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -50452,10 +50511,10 @@
     <row r="35">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>3845</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
-        <v>3846</v>
+        <v>236</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
@@ -50464,43 +50523,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36"/>
-      <c r="B36" t="s">
-        <v>3847</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3848</v>
-      </c>
-      <c r="D36" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="37">
-      <c r="A37"/>
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
       <c r="B37" t="s">
-        <v>3837</v>
+        <v>214</v>
       </c>
       <c r="C37" t="s">
-        <v>3838</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38"/>
+      <c r="A38" t="s">
+        <v>3797</v>
+      </c>
       <c r="B38" t="s">
-        <v>241</v>
+        <v>3851</v>
       </c>
       <c r="C38" t="s">
-        <v>242</v>
+        <v>3852</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
@@ -50512,10 +50560,10 @@
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>235</v>
+        <v>3853</v>
       </c>
       <c r="C39" t="s">
-        <v>236</v>
+        <v>3854</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -50524,32 +50572,43 @@
         <v>27</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40"/>
+      <c r="B40" t="s">
+        <v>3855</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3856</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>2</v>
-      </c>
+      <c r="A41"/>
       <c r="B41" t="s">
-        <v>214</v>
+        <v>3857</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>3858</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E41" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>3822</v>
-      </c>
+      <c r="A42"/>
       <c r="B42" t="s">
-        <v>3849</v>
+        <v>3859</v>
       </c>
       <c r="C42" t="s">
-        <v>3850</v>
+        <v>3860</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
@@ -50561,10 +50620,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>3851</v>
+        <v>3849</v>
       </c>
       <c r="C43" t="s">
-        <v>3852</v>
+        <v>3850</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
@@ -50576,10 +50635,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>3853</v>
+        <v>3839</v>
       </c>
       <c r="C44" t="s">
-        <v>3854</v>
+        <v>3861</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
@@ -50603,47 +50662,47 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
-        <v>214</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" t="s">
-        <v>224</v>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>749</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>1132</v>
+        <v>214</v>
       </c>
       <c r="C48" t="s">
-        <v>1133</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49"/>
+      <c r="A49" t="s">
+        <v>3822</v>
+      </c>
       <c r="B49" t="s">
-        <v>1134</v>
+        <v>3862</v>
       </c>
       <c r="C49" t="s">
-        <v>1135</v>
+        <v>3863</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -50655,74 +50714,74 @@
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
+        <v>3864</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3865</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51"/>
+      <c r="B51" t="s">
+        <v>3866</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3867</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52"/>
+      <c r="B52" t="s">
         <v>241</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>242</v>
       </c>
-      <c r="D50" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
         <v>2</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>214</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>4</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>5</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E54" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>960</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1210</v>
-      </c>
-      <c r="D53" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54"/>
-      <c r="B54" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1212</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="55">
-      <c r="A55"/>
+      <c r="A55" t="s">
+        <v>749</v>
+      </c>
       <c r="B55" t="s">
-        <v>1213</v>
+        <v>1132</v>
       </c>
       <c r="C55" t="s">
-        <v>1214</v>
+        <v>1133</v>
       </c>
       <c r="D55" t="s">
         <v>27</v>
@@ -50734,15 +50793,109 @@
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57"/>
+      <c r="B57" t="s">
         <v>241</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>242</v>
       </c>
-      <c r="D56" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>960</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D60" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61"/>
+      <c r="B61" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62"/>
+      <c r="B62" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63"/>
+      <c r="B63" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63" t="s">
+        <v>242</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" t="s">
         <v>27</v>
       </c>
     </row>
@@ -50821,7 +50974,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3855</v>
+        <v>3868</v>
       </c>
       <c r="B2" t="s">
         <v>540</v>
@@ -50831,7 +50984,7 @@
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3856</v>
+        <v>3869</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -50849,7 +51002,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3857</v>
+        <v>3870</v>
       </c>
       <c r="B3" t="s">
         <v>709</v>
@@ -50875,7 +51028,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3858</v>
+        <v>3871</v>
       </c>
       <c r="B4" t="s">
         <v>712</v>
@@ -50901,7 +51054,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3859</v>
+        <v>3872</v>
       </c>
       <c r="B5" t="s">
         <v>3703</v>
@@ -50927,7 +51080,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3860</v>
+        <v>3873</v>
       </c>
       <c r="B6" t="s">
         <v>1063</v>
@@ -50953,7 +51106,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3861</v>
+        <v>3874</v>
       </c>
       <c r="B7" t="s">
         <v>678</v>
@@ -50979,7 +51132,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3862</v>
+        <v>3875</v>
       </c>
       <c r="B8" t="s">
         <v>685</v>
@@ -51007,7 +51160,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3863</v>
+        <v>3876</v>
       </c>
       <c r="B9" t="s">
         <v>681</v>
@@ -51033,7 +51186,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3864</v>
+        <v>3877</v>
       </c>
       <c r="B10" t="s">
         <v>688</v>
@@ -51061,7 +51214,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>3865</v>
+        <v>3878</v>
       </c>
       <c r="B11" t="s">
         <v>778</v>
@@ -51087,7 +51240,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3866</v>
+        <v>3879</v>
       </c>
       <c r="B12" t="s">
         <v>781</v>
@@ -51113,7 +51266,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3867</v>
+        <v>3880</v>
       </c>
       <c r="B13" t="s">
         <v>784</v>
@@ -51139,10 +51292,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>3868</v>
+        <v>3881</v>
       </c>
       <c r="B14" t="s">
-        <v>3869</v>
+        <v>3882</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>79</v>
@@ -51165,10 +51318,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3870</v>
+        <v>3883</v>
       </c>
       <c r="B15" t="s">
-        <v>3871</v>
+        <v>3884</v>
       </c>
       <c r="C15" t="s" s="1">
         <v>84</v>
@@ -51191,7 +51344,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>3872</v>
+        <v>3885</v>
       </c>
       <c r="B16" t="s">
         <v>883</v>
@@ -51217,7 +51370,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>3873</v>
+        <v>3886</v>
       </c>
       <c r="B17" t="s">
         <v>887</v>
@@ -51229,7 +51382,7 @@
         <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>3874</v>
+        <v>3887</v>
       </c>
       <c r="F17" t="s" s="1">
         <v>27</v>
@@ -51245,7 +51398,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>3875</v>
+        <v>3888</v>
       </c>
       <c r="B18" t="s">
         <v>2668</v>
@@ -51271,7 +51424,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>3876</v>
+        <v>3889</v>
       </c>
       <c r="B19" t="s">
         <v>196</v>
@@ -51297,10 +51450,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>3877</v>
+        <v>3890</v>
       </c>
       <c r="B20" t="s">
-        <v>3878</v>
+        <v>3891</v>
       </c>
       <c r="C20" t="s" s="1">
         <v>184</v>
@@ -51323,10 +51476,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>3879</v>
+        <v>3892</v>
       </c>
       <c r="B21" t="s">
-        <v>3880</v>
+        <v>3893</v>
       </c>
       <c r="C21" t="s" s="1">
         <v>184</v>
@@ -51349,17 +51502,17 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>3881</v>
+        <v>3894</v>
       </c>
       <c r="B22" t="s">
-        <v>3882</v>
+        <v>3895</v>
       </c>
       <c r="C22" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>3883</v>
+        <v>3896</v>
       </c>
       <c r="F22" t="s" s="1">
         <v>27</v>
@@ -51375,13 +51528,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>3884</v>
+        <v>3897</v>
       </c>
       <c r="B23" t="s">
-        <v>3885</v>
+        <v>3898</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>3886</v>
+        <v>3899</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
@@ -51401,7 +51554,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>3887</v>
+        <v>3900</v>
       </c>
       <c r="B24" t="s">
         <v>905</v>
@@ -51427,7 +51580,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>3888</v>
+        <v>3901</v>
       </c>
       <c r="B25" t="s">
         <v>909</v>
@@ -51455,7 +51608,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>3889</v>
+        <v>3902</v>
       </c>
       <c r="B26" t="s">
         <v>912</v>
@@ -51481,7 +51634,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>3890</v>
+        <v>3903</v>
       </c>
       <c r="B27" t="s">
         <v>915</v>
@@ -51507,7 +51660,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>3891</v>
+        <v>3904</v>
       </c>
       <c r="B28" t="s">
         <v>918</v>
@@ -51535,7 +51688,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>3892</v>
+        <v>3905</v>
       </c>
       <c r="B29" t="s">
         <v>921</v>
@@ -51561,7 +51714,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>3893</v>
+        <v>3906</v>
       </c>
       <c r="B30" t="s">
         <v>924</v>
@@ -51587,7 +51740,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>3894</v>
+        <v>3907</v>
       </c>
       <c r="B31" t="s">
         <v>927</v>
@@ -51613,7 +51766,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>3895</v>
+        <v>3908</v>
       </c>
       <c r="B32" t="s">
         <v>930</v>
@@ -51639,7 +51792,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>3896</v>
+        <v>3909</v>
       </c>
       <c r="B33" t="s">
         <v>933</v>
@@ -51665,7 +51818,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>3897</v>
+        <v>3910</v>
       </c>
       <c r="B34" t="s">
         <v>936</v>
@@ -51693,7 +51846,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>3898</v>
+        <v>3911</v>
       </c>
       <c r="B35" t="s">
         <v>939</v>
@@ -51719,7 +51872,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>3899</v>
+        <v>3912</v>
       </c>
       <c r="B36" t="s">
         <v>942</v>
@@ -51747,7 +51900,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>3900</v>
+        <v>3913</v>
       </c>
       <c r="B37" t="s">
         <v>944</v>
@@ -51773,7 +51926,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>3901</v>
+        <v>3914</v>
       </c>
       <c r="B38" t="s">
         <v>947</v>
@@ -51799,7 +51952,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>3902</v>
+        <v>3915</v>
       </c>
       <c r="B39" t="s">
         <v>950</v>
@@ -51825,7 +51978,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>3903</v>
+        <v>3916</v>
       </c>
       <c r="B40" t="s">
         <v>953</v>
@@ -51851,17 +52004,17 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>3904</v>
+        <v>3917</v>
       </c>
       <c r="B41" t="s">
-        <v>3905</v>
+        <v>3918</v>
       </c>
       <c r="C41" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>3906</v>
+        <v>3919</v>
       </c>
       <c r="F41" t="s" s="1">
         <v>27</v>
@@ -51877,7 +52030,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>3907</v>
+        <v>3920</v>
       </c>
       <c r="B42" t="s">
         <v>1065</v>
@@ -51903,7 +52056,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>3908</v>
+        <v>3921</v>
       </c>
       <c r="B43" t="s">
         <v>1069</v>
@@ -53247,17 +53400,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3909</v>
+        <v>3922</v>
       </c>
       <c r="B2" t="s">
-        <v>3910</v>
+        <v>3923</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3911</v>
+        <v>3924</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -53273,7 +53426,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3912</v>
+        <v>3925</v>
       </c>
       <c r="B3" t="s">
         <v>196</v>
@@ -53299,7 +53452,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3913</v>
+        <v>3926</v>
       </c>
       <c r="B4" t="s">
         <v>3703</v>
@@ -53309,7 +53462,7 @@
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -53393,17 +53546,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3915</v>
+        <v>3928</v>
       </c>
       <c r="B2" t="s">
-        <v>3910</v>
+        <v>3923</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3911</v>
+        <v>3924</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -53419,7 +53572,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3916</v>
+        <v>3929</v>
       </c>
       <c r="B3" t="s">
         <v>196</v>
@@ -53445,7 +53598,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3917</v>
+        <v>3930</v>
       </c>
       <c r="B4" t="s">
         <v>3703</v>
@@ -53455,7 +53608,7 @@
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -53471,7 +53624,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3918</v>
+        <v>3931</v>
       </c>
       <c r="B5" t="s">
         <v>583</v>
@@ -53481,7 +53634,7 @@
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>3919</v>
+        <v>3932</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -55482,17 +55635,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3920</v>
+        <v>3933</v>
       </c>
       <c r="B2" t="s">
-        <v>3910</v>
+        <v>3923</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3911</v>
+        <v>3924</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -55508,7 +55661,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3921</v>
+        <v>3934</v>
       </c>
       <c r="B3" t="s">
         <v>196</v>
@@ -55534,17 +55687,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3922</v>
+        <v>3935</v>
       </c>
       <c r="B4" t="s">
-        <v>3923</v>
+        <v>3936</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3924</v>
+        <v>3937</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -55560,17 +55713,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3925</v>
+        <v>3938</v>
       </c>
       <c r="B5" t="s">
-        <v>3926</v>
+        <v>3939</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>3927</v>
+        <v>3940</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -55586,7 +55739,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3928</v>
+        <v>3941</v>
       </c>
       <c r="B6" t="s">
         <v>3703</v>
@@ -55596,7 +55749,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -55612,7 +55765,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3929</v>
+        <v>3942</v>
       </c>
       <c r="B7" t="s">
         <v>587</v>
@@ -55706,17 +55859,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3930</v>
+        <v>3943</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -55732,17 +55885,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3933</v>
+        <v>3946</v>
       </c>
       <c r="B3" t="s">
-        <v>3934</v>
+        <v>3947</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>3935</v>
+        <v>3948</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -55758,17 +55911,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3936</v>
+        <v>3949</v>
       </c>
       <c r="B4" t="s">
-        <v>3937</v>
+        <v>3950</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>57</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3938</v>
+        <v>3951</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -55784,7 +55937,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3939</v>
+        <v>3952</v>
       </c>
       <c r="B5" t="s">
         <v>3703</v>
@@ -55794,7 +55947,7 @@
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -55810,7 +55963,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3940</v>
+        <v>3953</v>
       </c>
       <c r="B6" t="s">
         <v>891</v>
@@ -55836,17 +55989,17 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3941</v>
+        <v>3954</v>
       </c>
       <c r="B7" t="s">
-        <v>3942</v>
+        <v>3955</v>
       </c>
       <c r="C7" t="s" s="1">
-        <v>3943</v>
+        <v>3956</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>3944</v>
+        <v>3957</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -55862,7 +56015,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3945</v>
+        <v>3958</v>
       </c>
       <c r="B8" t="s">
         <v>591</v>
@@ -55956,17 +56109,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3946</v>
+        <v>3959</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -55982,17 +56135,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>3960</v>
+      </c>
+      <c r="B3" t="s">
         <v>3947</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3934</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>3935</v>
+        <v>3948</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -56008,17 +56161,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3948</v>
+        <v>3961</v>
       </c>
       <c r="B4" t="s">
-        <v>3937</v>
+        <v>3950</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>57</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>3938</v>
+        <v>3951</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -56034,7 +56187,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3949</v>
+        <v>3962</v>
       </c>
       <c r="B5" t="s">
         <v>594</v>
@@ -56060,7 +56213,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3950</v>
+        <v>3963</v>
       </c>
       <c r="B6" t="s">
         <v>3703</v>
@@ -56070,7 +56223,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -56086,7 +56239,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3951</v>
+        <v>3964</v>
       </c>
       <c r="B7" t="s">
         <v>891</v>
@@ -56180,17 +56333,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3952</v>
+        <v>3965</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -56206,10 +56359,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3953</v>
+        <v>3966</v>
       </c>
       <c r="B3" t="s">
-        <v>3937</v>
+        <v>3950</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>57</v>
@@ -56232,7 +56385,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3954</v>
+        <v>3967</v>
       </c>
       <c r="B4" t="s">
         <v>594</v>
@@ -56258,7 +56411,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3955</v>
+        <v>3968</v>
       </c>
       <c r="B5" t="s">
         <v>597</v>
@@ -56284,7 +56437,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3956</v>
+        <v>3969</v>
       </c>
       <c r="B6" t="s">
         <v>3703</v>
@@ -56294,7 +56447,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -56310,7 +56463,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3957</v>
+        <v>3970</v>
       </c>
       <c r="B7" t="s">
         <v>891</v>
@@ -56404,17 +56557,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3958</v>
+        <v>3971</v>
       </c>
       <c r="B2" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -56430,7 +56583,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3959</v>
+        <v>3972</v>
       </c>
       <c r="B3" t="s">
         <v>594</v>
@@ -56456,7 +56609,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3960</v>
+        <v>3973</v>
       </c>
       <c r="B4" t="s">
         <v>597</v>
@@ -56482,7 +56635,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3961</v>
+        <v>3974</v>
       </c>
       <c r="B5" t="s">
         <v>600</v>
@@ -56508,7 +56661,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3962</v>
+        <v>3975</v>
       </c>
       <c r="B6" t="s">
         <v>604</v>
@@ -56534,7 +56687,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3963</v>
+        <v>3976</v>
       </c>
       <c r="B7" t="s">
         <v>624</v>
@@ -56560,7 +56713,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3964</v>
+        <v>3977</v>
       </c>
       <c r="B8" t="s">
         <v>627</v>
@@ -56586,7 +56739,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3965</v>
+        <v>3978</v>
       </c>
       <c r="B9" t="s">
         <v>630</v>
@@ -56612,7 +56765,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3966</v>
+        <v>3979</v>
       </c>
       <c r="B10" t="s">
         <v>560</v>
@@ -56638,7 +56791,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>3967</v>
+        <v>3980</v>
       </c>
       <c r="B11" t="s">
         <v>607</v>
@@ -56664,7 +56817,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3968</v>
+        <v>3981</v>
       </c>
       <c r="B12" t="s">
         <v>648</v>
@@ -56690,7 +56843,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3969</v>
+        <v>3982</v>
       </c>
       <c r="B13" t="s">
         <v>651</v>
@@ -56716,7 +56869,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>3970</v>
+        <v>3983</v>
       </c>
       <c r="B14" t="s">
         <v>654</v>
@@ -56742,7 +56895,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3971</v>
+        <v>3984</v>
       </c>
       <c r="B15" t="s">
         <v>657</v>
@@ -56768,7 +56921,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>3972</v>
+        <v>3985</v>
       </c>
       <c r="B16" t="s">
         <v>612</v>
@@ -56778,7 +56931,7 @@
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>3973</v>
+        <v>3986</v>
       </c>
       <c r="F16" t="s" s="1">
         <v>27</v>
@@ -56794,7 +56947,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>3974</v>
+        <v>3987</v>
       </c>
       <c r="B17" t="s">
         <v>616</v>
@@ -56804,7 +56957,7 @@
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>3975</v>
+        <v>3988</v>
       </c>
       <c r="F17" t="s" s="1">
         <v>27</v>
@@ -56820,10 +56973,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>3976</v>
+        <v>3989</v>
       </c>
       <c r="B18" t="s">
-        <v>3977</v>
+        <v>3990</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>93</v>
@@ -56846,17 +56999,17 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>3978</v>
+        <v>3991</v>
       </c>
       <c r="B19" t="s">
-        <v>3979</v>
+        <v>3992</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>3980</v>
+        <v>3993</v>
       </c>
       <c r="F19" t="s" s="1">
         <v>27</v>
@@ -56872,7 +57025,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>3981</v>
+        <v>3994</v>
       </c>
       <c r="B20" t="s">
         <v>3703</v>
@@ -56882,7 +57035,7 @@
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F20" t="s" s="1">
         <v>27</v>
@@ -56898,7 +57051,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>3982</v>
+        <v>3995</v>
       </c>
       <c r="B21" t="s">
         <v>891</v>
@@ -57977,17 +58130,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3983</v>
+        <v>3996</v>
       </c>
       <c r="B2" t="s">
-        <v>3984</v>
+        <v>3997</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>3985</v>
+        <v>3998</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3986</v>
+        <v>3999</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -58003,17 +58156,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3987</v>
+        <v>4000</v>
       </c>
       <c r="B3" t="s">
-        <v>3931</v>
+        <v>3944</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>3932</v>
+        <v>3945</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -58029,7 +58182,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3988</v>
+        <v>4001</v>
       </c>
       <c r="B4" t="s">
         <v>594</v>
@@ -58055,7 +58208,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3989</v>
+        <v>4002</v>
       </c>
       <c r="B5" t="s">
         <v>597</v>
@@ -58081,7 +58234,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3990</v>
+        <v>4003</v>
       </c>
       <c r="B6" t="s">
         <v>612</v>
@@ -58091,7 +58244,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>3973</v>
+        <v>3986</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -58107,7 +58260,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3991</v>
+        <v>4004</v>
       </c>
       <c r="B7" t="s">
         <v>616</v>
@@ -58117,7 +58270,7 @@
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>3975</v>
+        <v>3988</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -58133,17 +58286,17 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>3992</v>
+        <v>4005</v>
       </c>
       <c r="B8" t="s">
-        <v>3993</v>
+        <v>4006</v>
       </c>
       <c r="C8" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>3994</v>
+        <v>4007</v>
       </c>
       <c r="F8" t="s" s="1">
         <v>27</v>
@@ -58159,7 +58312,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3995</v>
+        <v>4008</v>
       </c>
       <c r="B9" t="s">
         <v>3703</v>
@@ -58169,7 +58322,7 @@
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>3914</v>
+        <v>3927</v>
       </c>
       <c r="F9" t="s" s="1">
         <v>27</v>
@@ -58185,7 +58338,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3996</v>
+        <v>4009</v>
       </c>
       <c r="B10" t="s">
         <v>891</v>
@@ -58228,13 +58381,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3985</v>
+        <v>3998</v>
       </c>
       <c r="B13" t="s">
-        <v>3997</v>
+        <v>4010</v>
       </c>
       <c r="C13" t="s">
-        <v>3998</v>
+        <v>4011</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -58246,10 +58399,10 @@
     <row r="14">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>3999</v>
+        <v>4012</v>
       </c>
       <c r="C14" t="s">
-        <v>4000</v>
+        <v>4013</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
@@ -58261,10 +58414,10 @@
     <row r="15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>4001</v>
+        <v>4014</v>
       </c>
       <c r="C15" t="s">
-        <v>4002</v>
+        <v>4015</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
@@ -58359,17 +58512,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4003</v>
+        <v>4016</v>
       </c>
       <c r="B2" t="s">
-        <v>3993</v>
+        <v>4006</v>
       </c>
       <c r="C2" t="s" s="1">
         <v>184</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>3994</v>
+        <v>4007</v>
       </c>
       <c r="F2" t="s" s="1">
         <v>27</v>
@@ -58385,17 +58538,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4004</v>
+        <v>4017</v>
       </c>
       <c r="B3" t="s">
-        <v>4005</v>
+        <v>4018</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4006</v>
+        <v>4019</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -58411,7 +58564,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4007</v>
+        <v>4020</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -58437,7 +58590,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4008</v>
+        <v>4021</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -58463,10 +58616,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4009</v>
+        <v>4022</v>
       </c>
       <c r="B6" t="s">
-        <v>4010</v>
+        <v>4023</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
@@ -58489,17 +58642,17 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4011</v>
+        <v>4024</v>
       </c>
       <c r="B7" t="s">
-        <v>4012</v>
+        <v>4025</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>4013</v>
+        <v>4026</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -58515,7 +58668,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4014</v>
+        <v>4027</v>
       </c>
       <c r="B8" t="s">
         <v>148</v>
@@ -58525,7 +58678,7 @@
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>4015</v>
+        <v>4028</v>
       </c>
       <c r="F8" t="s" s="1">
         <v>27</v>
@@ -58541,17 +58694,17 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4016</v>
+        <v>4029</v>
       </c>
       <c r="B9" t="s">
-        <v>4017</v>
+        <v>4030</v>
       </c>
       <c r="C9" t="s" s="1">
-        <v>4018</v>
+        <v>4031</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>4019</v>
+        <v>4032</v>
       </c>
       <c r="F9" t="s" s="1">
         <v>27</v>
@@ -58567,7 +58720,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4020</v>
+        <v>4033</v>
       </c>
       <c r="B10" t="s">
         <v>594</v>
@@ -58593,7 +58746,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4021</v>
+        <v>4034</v>
       </c>
       <c r="B11" t="s">
         <v>597</v>
@@ -58619,7 +58772,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4022</v>
+        <v>4035</v>
       </c>
       <c r="B12" t="s">
         <v>600</v>
@@ -58645,7 +58798,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4023</v>
+        <v>4036</v>
       </c>
       <c r="B13" t="s">
         <v>791</v>
@@ -58671,10 +58824,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4024</v>
+        <v>4037</v>
       </c>
       <c r="B14" t="s">
-        <v>4025</v>
+        <v>4038</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>97</v>
@@ -58697,7 +58850,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4026</v>
+        <v>4039</v>
       </c>
       <c r="B15" t="s">
         <v>883</v>
@@ -58707,7 +58860,7 @@
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>4027</v>
+        <v>4040</v>
       </c>
       <c r="F15" t="s" s="1">
         <v>27</v>
@@ -58723,17 +58876,17 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4028</v>
+        <v>4041</v>
       </c>
       <c r="B16" t="s">
-        <v>4029</v>
+        <v>4042</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>713</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>4030</v>
+        <v>4043</v>
       </c>
       <c r="F16" t="s" s="1">
         <v>27</v>
@@ -58749,20 +58902,20 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4031</v>
+        <v>4044</v>
       </c>
       <c r="B17" t="s">
-        <v>4032</v>
+        <v>4045</v>
       </c>
       <c r="C17" t="s" s="1">
         <v>123</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>4033</v>
+        <v>4046</v>
       </c>
       <c r="F17" t="s" s="1">
-        <v>4034</v>
+        <v>4047</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
@@ -58775,13 +58928,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4035</v>
+        <v>4048</v>
       </c>
       <c r="B18" t="s">
-        <v>4036</v>
+        <v>4049</v>
       </c>
       <c r="C18" t="s" s="1">
-        <v>4037</v>
+        <v>4050</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
@@ -58801,10 +58954,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4038</v>
+        <v>4051</v>
       </c>
       <c r="B19" t="s">
-        <v>4039</v>
+        <v>4052</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>184</v>
@@ -58827,13 +58980,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4040</v>
+        <v>4053</v>
       </c>
       <c r="B20" t="s">
-        <v>4041</v>
+        <v>4054</v>
       </c>
       <c r="C20" t="s" s="1">
-        <v>4042</v>
+        <v>4055</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
@@ -59856,13 +60009,13 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>4037</v>
+        <v>4050</v>
       </c>
       <c r="B91" t="s">
-        <v>4043</v>
+        <v>4056</v>
       </c>
       <c r="C91" t="s">
-        <v>4044</v>
+        <v>4057</v>
       </c>
       <c r="D91" t="s">
         <v>27</v>
@@ -59874,10 +60027,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>4045</v>
+        <v>4058</v>
       </c>
       <c r="C92" t="s">
-        <v>4046</v>
+        <v>4059</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -59889,10 +60042,10 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>4047</v>
+        <v>4060</v>
       </c>
       <c r="C93" t="s">
-        <v>4048</v>
+        <v>4061</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
@@ -59904,10 +60057,10 @@
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>4049</v>
+        <v>4062</v>
       </c>
       <c r="C94" t="s">
-        <v>4050</v>
+        <v>4063</v>
       </c>
       <c r="D94" t="s">
         <v>27</v>
@@ -59919,10 +60072,10 @@
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
-        <v>4051</v>
+        <v>4064</v>
       </c>
       <c r="C95" t="s">
-        <v>4052</v>
+        <v>4065</v>
       </c>
       <c r="D95" t="s">
         <v>27</v>
@@ -59934,10 +60087,10 @@
     <row r="96">
       <c r="A96"/>
       <c r="B96" t="s">
-        <v>4053</v>
+        <v>4066</v>
       </c>
       <c r="C96" t="s">
-        <v>4054</v>
+        <v>4067</v>
       </c>
       <c r="D96" t="s">
         <v>27</v>
@@ -59949,10 +60102,10 @@
     <row r="97">
       <c r="A97"/>
       <c r="B97" t="s">
-        <v>4055</v>
+        <v>4068</v>
       </c>
       <c r="C97" t="s">
-        <v>4056</v>
+        <v>4069</v>
       </c>
       <c r="D97" t="s">
         <v>27</v>
@@ -59964,10 +60117,10 @@
     <row r="98">
       <c r="A98"/>
       <c r="B98" t="s">
-        <v>4057</v>
+        <v>4070</v>
       </c>
       <c r="C98" t="s">
-        <v>4058</v>
+        <v>4071</v>
       </c>
       <c r="D98" t="s">
         <v>27</v>
@@ -59979,10 +60132,10 @@
     <row r="99">
       <c r="A99"/>
       <c r="B99" t="s">
-        <v>4059</v>
+        <v>4072</v>
       </c>
       <c r="C99" t="s">
-        <v>4060</v>
+        <v>4073</v>
       </c>
       <c r="D99" t="s">
         <v>27</v>
@@ -59994,10 +60147,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>4061</v>
+        <v>4074</v>
       </c>
       <c r="C100" t="s">
-        <v>4062</v>
+        <v>4075</v>
       </c>
       <c r="D100" t="s">
         <v>27</v>
@@ -60009,10 +60162,10 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
-        <v>4063</v>
+        <v>4076</v>
       </c>
       <c r="C101" t="s">
-        <v>4064</v>
+        <v>4077</v>
       </c>
       <c r="D101" t="s">
         <v>27</v>
@@ -60024,10 +60177,10 @@
     <row r="102">
       <c r="A102"/>
       <c r="B102" t="s">
-        <v>4065</v>
+        <v>4078</v>
       </c>
       <c r="C102" t="s">
-        <v>4066</v>
+        <v>4079</v>
       </c>
       <c r="D102" t="s">
         <v>27</v>
@@ -60039,10 +60192,10 @@
     <row r="103">
       <c r="A103"/>
       <c r="B103" t="s">
-        <v>4067</v>
+        <v>4080</v>
       </c>
       <c r="C103" t="s">
-        <v>4068</v>
+        <v>4081</v>
       </c>
       <c r="D103" t="s">
         <v>27</v>
@@ -60054,10 +60207,10 @@
     <row r="104">
       <c r="A104"/>
       <c r="B104" t="s">
-        <v>4069</v>
+        <v>4082</v>
       </c>
       <c r="C104" t="s">
-        <v>4070</v>
+        <v>4083</v>
       </c>
       <c r="D104" t="s">
         <v>27</v>
@@ -60069,10 +60222,10 @@
     <row r="105">
       <c r="A105"/>
       <c r="B105" t="s">
-        <v>4071</v>
+        <v>4084</v>
       </c>
       <c r="C105" t="s">
-        <v>4072</v>
+        <v>4085</v>
       </c>
       <c r="D105" t="s">
         <v>27</v>
@@ -60084,10 +60237,10 @@
     <row r="106">
       <c r="A106"/>
       <c r="B106" t="s">
-        <v>4073</v>
+        <v>4086</v>
       </c>
       <c r="C106" t="s">
-        <v>4074</v>
+        <v>4087</v>
       </c>
       <c r="D106" t="s">
         <v>27</v>
@@ -60099,10 +60252,10 @@
     <row r="107">
       <c r="A107"/>
       <c r="B107" t="s">
-        <v>4075</v>
+        <v>4088</v>
       </c>
       <c r="C107" t="s">
-        <v>4076</v>
+        <v>4089</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -60130,7 +60283,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>4042</v>
+        <v>4055</v>
       </c>
       <c r="B110" t="s">
         <v>513</v>
@@ -60148,10 +60301,10 @@
     <row r="111">
       <c r="A111"/>
       <c r="B111" t="s">
-        <v>4077</v>
+        <v>4090</v>
       </c>
       <c r="C111" t="s">
-        <v>4078</v>
+        <v>4091</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -60163,7 +60316,7 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>4079</v>
+        <v>4092</v>
       </c>
       <c r="C112" t="s">
         <v>595</v>
@@ -60178,7 +60331,7 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>4080</v>
+        <v>4093</v>
       </c>
       <c r="C113" t="s">
         <v>598</v>
@@ -60223,7 +60376,7 @@
     <row r="116">
       <c r="A116"/>
       <c r="B116" t="s">
-        <v>4081</v>
+        <v>4094</v>
       </c>
       <c r="C116" t="s">
         <v>644</v>
@@ -60253,10 +60406,10 @@
     <row r="118">
       <c r="A118"/>
       <c r="B118" t="s">
-        <v>4082</v>
+        <v>4095</v>
       </c>
       <c r="C118" t="s">
-        <v>4083</v>
+        <v>4096</v>
       </c>
       <c r="D118" t="s">
         <v>27</v>
@@ -60339,13 +60492,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4084</v>
+        <v>4097</v>
       </c>
       <c r="B2" t="s">
-        <v>3977</v>
+        <v>3990</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4085</v>
+        <v>4098</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -60365,7 +60518,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4086</v>
+        <v>4099</v>
       </c>
       <c r="B3" t="s">
         <v>678</v>
@@ -60391,17 +60544,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4087</v>
+        <v>4100</v>
       </c>
       <c r="B4" t="s">
-        <v>4088</v>
+        <v>4101</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>75</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>4089</v>
+        <v>4102</v>
       </c>
       <c r="F4" t="s" s="1">
         <v>27</v>
@@ -60417,17 +60570,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4090</v>
+        <v>4103</v>
       </c>
       <c r="B5" t="s">
-        <v>4091</v>
+        <v>4104</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4092</v>
+        <v>4105</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -60443,13 +60596,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4093</v>
+        <v>4106</v>
       </c>
       <c r="B6" t="s">
-        <v>4094</v>
+        <v>4107</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>4095</v>
+        <v>4108</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
@@ -60469,17 +60622,17 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4096</v>
+        <v>4109</v>
       </c>
       <c r="B7" t="s">
-        <v>4097</v>
+        <v>4110</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>4098</v>
+        <v>4111</v>
       </c>
       <c r="F7" t="s" s="1">
         <v>27</v>
@@ -60495,17 +60648,17 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4099</v>
+        <v>4112</v>
       </c>
       <c r="B8" t="s">
-        <v>4100</v>
+        <v>4113</v>
       </c>
       <c r="C8" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>4101</v>
+        <v>4114</v>
       </c>
       <c r="F8" t="s" s="1">
         <v>27</v>
@@ -60521,10 +60674,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4102</v>
+        <v>4115</v>
       </c>
       <c r="B9" t="s">
-        <v>4103</v>
+        <v>4116</v>
       </c>
       <c r="C9" t="s" s="1">
         <v>14</v>
@@ -60547,10 +60700,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4104</v>
+        <v>4117</v>
       </c>
       <c r="B10" t="s">
-        <v>4105</v>
+        <v>4118</v>
       </c>
       <c r="C10" t="s" s="1">
         <v>14</v>
@@ -60573,10 +60726,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4106</v>
+        <v>4119</v>
       </c>
       <c r="B11" t="s">
-        <v>4107</v>
+        <v>4120</v>
       </c>
       <c r="C11" t="s" s="1">
         <v>53</v>
@@ -60599,10 +60752,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4108</v>
+        <v>4121</v>
       </c>
       <c r="B12" t="s">
-        <v>4109</v>
+        <v>4122</v>
       </c>
       <c r="C12" t="s" s="1">
         <v>110</v>
@@ -60625,10 +60778,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4110</v>
+        <v>4123</v>
       </c>
       <c r="B13" t="s">
-        <v>4111</v>
+        <v>4124</v>
       </c>
       <c r="C13" t="s" s="1">
         <v>57</v>
@@ -60651,10 +60804,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4112</v>
+        <v>4125</v>
       </c>
       <c r="B14" t="s">
-        <v>4113</v>
+        <v>4126</v>
       </c>
       <c r="C14" t="s" s="1">
         <v>57</v>
@@ -60677,10 +60830,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4114</v>
+        <v>4127</v>
       </c>
       <c r="B15" t="s">
-        <v>4115</v>
+        <v>4128</v>
       </c>
       <c r="C15" t="s" s="1">
         <v>57</v>
@@ -60703,10 +60856,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4116</v>
+        <v>4129</v>
       </c>
       <c r="B16" t="s">
-        <v>4117</v>
+        <v>4130</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>14</v>
@@ -60729,10 +60882,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4118</v>
+        <v>4131</v>
       </c>
       <c r="B17" t="s">
-        <v>4119</v>
+        <v>4132</v>
       </c>
       <c r="C17" t="s" s="1">
         <v>14</v>
@@ -60755,10 +60908,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4120</v>
+        <v>4133</v>
       </c>
       <c r="B18" t="s">
-        <v>4121</v>
+        <v>4134</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>14</v>
@@ -60781,10 +60934,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>4122</v>
+        <v>4135</v>
       </c>
       <c r="B19" t="s">
-        <v>4123</v>
+        <v>4136</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>14</v>
@@ -60807,10 +60960,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4124</v>
+        <v>4137</v>
       </c>
       <c r="B20" t="s">
-        <v>4125</v>
+        <v>4138</v>
       </c>
       <c r="C20" t="s" s="1">
         <v>14</v>
@@ -60833,10 +60986,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4126</v>
+        <v>4139</v>
       </c>
       <c r="B21" t="s">
-        <v>4127</v>
+        <v>4140</v>
       </c>
       <c r="C21" t="s" s="1">
         <v>14</v>
@@ -60859,13 +61012,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>4128</v>
+        <v>4141</v>
       </c>
       <c r="B22" t="s">
-        <v>4129</v>
+        <v>4142</v>
       </c>
       <c r="C22" t="s" s="1">
-        <v>4130</v>
+        <v>4143</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
@@ -60885,17 +61038,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>4131</v>
+        <v>4144</v>
       </c>
       <c r="B23" t="s">
-        <v>1533</v>
+        <v>4145</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>1534</v>
+        <v>4146</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>4147</v>
       </c>
       <c r="F23" t="s" s="1">
         <v>27</v>
@@ -60911,10 +61064,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>4132</v>
+        <v>4148</v>
       </c>
       <c r="B24" t="s">
-        <v>4133</v>
+        <v>4149</v>
       </c>
       <c r="C24" t="s" s="1">
         <v>14</v>
@@ -60937,17 +61090,17 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>4134</v>
+        <v>4150</v>
       </c>
       <c r="B25" t="s">
-        <v>4135</v>
+        <v>4151</v>
       </c>
       <c r="C25" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>4136</v>
+        <v>4152</v>
       </c>
       <c r="F25" t="s" s="1">
         <v>27</v>
@@ -60963,17 +61116,17 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>4137</v>
+        <v>4153</v>
       </c>
       <c r="B26" t="s">
-        <v>4138</v>
+        <v>4154</v>
       </c>
       <c r="C26" t="s" s="1">
-        <v>4139</v>
+        <v>4155</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>4140</v>
+        <v>4156</v>
       </c>
       <c r="F26" t="s" s="1">
         <v>27</v>
@@ -60989,17 +61142,17 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>4141</v>
+        <v>4157</v>
       </c>
       <c r="B27" t="s">
-        <v>4142</v>
+        <v>4158</v>
       </c>
       <c r="C27" t="s" s="1">
         <v>713</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>4143</v>
+        <v>4159</v>
       </c>
       <c r="F27" t="s" s="1">
         <v>27</v>
@@ -61015,7 +61168,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4144</v>
+        <v>4160</v>
       </c>
       <c r="B28" t="s">
         <v>712</v>
@@ -61058,13 +61211,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4085</v>
+        <v>4098</v>
       </c>
       <c r="B31" t="s">
-        <v>4145</v>
+        <v>4161</v>
       </c>
       <c r="C31" t="s">
-        <v>4146</v>
+        <v>4162</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
@@ -61076,10 +61229,10 @@
     <row r="32">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>4147</v>
+        <v>4163</v>
       </c>
       <c r="C32" t="s">
-        <v>4148</v>
+        <v>4164</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -62199,13 +62352,13 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>4139</v>
+        <v>4155</v>
       </c>
       <c r="B110" t="s">
-        <v>4149</v>
+        <v>4165</v>
       </c>
       <c r="C110" t="s">
-        <v>4150</v>
+        <v>4166</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -62232,10 +62385,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>4151</v>
+        <v>4167</v>
       </c>
       <c r="C112" t="s">
-        <v>4152</v>
+        <v>4168</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
@@ -62247,10 +62400,10 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>4153</v>
+        <v>4169</v>
       </c>
       <c r="C113" t="s">
-        <v>4154</v>
+        <v>4170</v>
       </c>
       <c r="D113" t="s">
         <v>27</v>
@@ -62334,13 +62487,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4155</v>
+        <v>4171</v>
       </c>
       <c r="B2" t="s">
-        <v>4156</v>
+        <v>4172</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4157</v>
+        <v>4173</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -62362,17 +62515,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4158</v>
+        <v>4174</v>
       </c>
       <c r="B3" t="s">
-        <v>4159</v>
+        <v>4175</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4160</v>
+        <v>4176</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -62388,13 +62541,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4161</v>
+        <v>4177</v>
       </c>
       <c r="B4" t="s">
-        <v>4162</v>
+        <v>4178</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>4095</v>
+        <v>4108</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
@@ -62414,17 +62567,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4163</v>
+        <v>4179</v>
       </c>
       <c r="B5" t="s">
-        <v>4164</v>
+        <v>4180</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4165</v>
+        <v>4181</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -62440,17 +62593,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4166</v>
+        <v>4182</v>
       </c>
       <c r="B6" t="s">
-        <v>4167</v>
+        <v>4183</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4168</v>
+        <v>4184</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -62466,7 +62619,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4169</v>
+        <v>4185</v>
       </c>
       <c r="B7" t="s">
         <v>3103</v>
@@ -62492,7 +62645,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4170</v>
+        <v>4186</v>
       </c>
       <c r="B8" t="s">
         <v>3115</v>
@@ -62518,7 +62671,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4171</v>
+        <v>4187</v>
       </c>
       <c r="B9" t="s">
         <v>3125</v>
@@ -62544,7 +62697,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4172</v>
+        <v>4188</v>
       </c>
       <c r="B10" t="s">
         <v>3133</v>
@@ -62570,7 +62723,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4173</v>
+        <v>4189</v>
       </c>
       <c r="B11" t="s">
         <v>3129</v>
@@ -62596,7 +62749,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4174</v>
+        <v>4190</v>
       </c>
       <c r="B12" t="s">
         <v>3100</v>
@@ -62622,7 +62775,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4175</v>
+        <v>4191</v>
       </c>
       <c r="B13" t="s">
         <v>196</v>
@@ -62648,7 +62801,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4176</v>
+        <v>4192</v>
       </c>
       <c r="B14" t="s">
         <v>3153</v>
@@ -62674,7 +62827,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4177</v>
+        <v>4193</v>
       </c>
       <c r="B15" t="s">
         <v>3091</v>
@@ -62700,7 +62853,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4178</v>
+        <v>4194</v>
       </c>
       <c r="B16" t="s">
         <v>3098</v>
@@ -62726,7 +62879,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4179</v>
+        <v>4195</v>
       </c>
       <c r="B17" t="s">
         <v>3156</v>
@@ -62752,10 +62905,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4180</v>
+        <v>4196</v>
       </c>
       <c r="B18" t="s">
-        <v>4181</v>
+        <v>4197</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3108</v>
@@ -63274,12 +63427,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4182</v>
+        <v>4198</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4183</v>
+        <v>4199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature 10826 add field for notification bundle id and map it (#11097)
* #10825: Added field to ExternalMessage

* #10825: Added test
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_Data_Dictionary.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16506" uniqueCount="4200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16512" uniqueCount="4203">
   <si>
     <t>Field ID</t>
   </si>
@@ -12511,6 +12511,15 @@
     <t>Report ID</t>
   </si>
   <si>
+    <t>ExternalMessage.reportMessageId</t>
+  </si>
+  <si>
+    <t>reportMessageId</t>
+  </si>
+  <si>
+    <t>Report Message ID</t>
+  </si>
+  <si>
     <t>ExternalMessage.status</t>
   </si>
   <si>
@@ -12649,7 +12658,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.77.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -14594,7 +14603,7 @@
 </file>
 
 <file path=xl/tables/table210.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A1:L28" displayName="Message" name="Message">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="210" ref="A1:L29" displayName="Message" name="Message">
   <autoFilter/>
   <tableColumns count="12">
     <tableColumn id="1" name="Field ID"/>
@@ -14615,7 +14624,7 @@
 </file>
 
 <file path=xl/tables/table211.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A30:E32" displayName="MessageExternalMessageType" name="MessageExternalMessageType">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="211" ref="A31:E33" displayName="MessageExternalMessageType" name="MessageExternalMessageType">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14629,7 +14638,7 @@
 </file>
 
 <file path=xl/tables/table212.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A34:E95" displayName="MessageDisease" name="MessageDisease">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="212" ref="A35:E96" displayName="MessageDisease" name="MessageDisease">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14643,7 +14652,7 @@
 </file>
 
 <file path=xl/tables/table213.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A97:E101" displayName="MessageSex" name="MessageSex">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="213" ref="A98:E102" displayName="MessageSex" name="MessageSex">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14657,7 +14666,7 @@
 </file>
 
 <file path=xl/tables/table214.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A103:E107" displayName="MessagePresentCondition" name="MessagePresentCondition">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="214" ref="A104:E108" displayName="MessagePresentCondition" name="MessagePresentCondition">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -14671,7 +14680,7 @@
 </file>
 
 <file path=xl/tables/table215.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A109:E113" displayName="MessageExternalMessageStatus" name="MessageExternalMessageStatus">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="215" ref="A110:E114" displayName="MessageExternalMessageStatus" name="MessageExternalMessageStatus">
   <autoFilter/>
   <tableColumns count="5">
     <tableColumn id="1" name="Type"/>
@@ -60432,7 +60441,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L113"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -61122,11 +61131,11 @@
         <v>4154</v>
       </c>
       <c r="C26" t="s" s="1">
-        <v>4155</v>
+        <v>14</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>4156</v>
+        <v>4155</v>
       </c>
       <c r="F26" t="s" s="1">
         <v>27</v>
@@ -61142,13 +61151,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>4156</v>
+      </c>
+      <c r="B27" t="s">
         <v>4157</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s" s="1">
         <v>4158</v>
-      </c>
-      <c r="C27" t="s" s="1">
-        <v>713</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
@@ -61171,14 +61180,14 @@
         <v>4160</v>
       </c>
       <c r="B28" t="s">
-        <v>712</v>
+        <v>4161</v>
       </c>
       <c r="C28" t="s" s="1">
         <v>713</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>714</v>
+        <v>4162</v>
       </c>
       <c r="F28" t="s" s="1">
         <v>27</v>
@@ -61192,47 +61201,58 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
-        <v>214</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>224</v>
-      </c>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>4163</v>
+      </c>
+      <c r="B29" t="s">
+        <v>712</v>
+      </c>
+      <c r="C29" t="s" s="1">
+        <v>713</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29" t="s">
+        <v>714</v>
+      </c>
+      <c r="F29" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
         <v>4098</v>
       </c>
-      <c r="B31" t="s">
-        <v>4161</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4162</v>
-      </c>
-      <c r="D31" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32"/>
       <c r="B32" t="s">
-        <v>4163</v>
+        <v>4164</v>
       </c>
       <c r="C32" t="s">
-        <v>4164</v>
+        <v>4165</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -61241,137 +61261,137 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>214</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" t="s">
-        <v>224</v>
+    <row r="33">
+      <c r="A33"/>
+      <c r="B33" t="s">
+        <v>4166</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4167</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>214</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
         <v>123</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>379</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>380</v>
       </c>
-      <c r="D35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36"/>
-      <c r="B36" t="s">
-        <v>381</v>
-      </c>
-      <c r="C36" t="s">
-        <v>382</v>
-      </c>
-      <c r="D36" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="37">
       <c r="A37"/>
       <c r="B37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C37" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C38" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
       </c>
       <c r="E38" t="s">
-        <v>387</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39">
       <c r="A39"/>
       <c r="B39" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C39" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
       </c>
       <c r="E39" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C40" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
       </c>
       <c r="E40" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="41">
       <c r="A41"/>
       <c r="B41" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C41" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D41" t="s">
         <v>27</v>
       </c>
       <c r="E41" t="s">
-        <v>27</v>
+        <v>391</v>
       </c>
     </row>
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C42" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
@@ -61383,10 +61403,10 @@
     <row r="43">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C43" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
@@ -61398,10 +61418,10 @@
     <row r="44">
       <c r="A44"/>
       <c r="B44" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C44" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
@@ -61413,85 +61433,85 @@
     <row r="45">
       <c r="A45"/>
       <c r="B45" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C45" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D45" t="s">
         <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>403</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C46" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>403</v>
       </c>
     </row>
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C47" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>408</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C48" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="49">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C49" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>27</v>
+        <v>411</v>
       </c>
     </row>
     <row r="50">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
@@ -61503,40 +61523,40 @@
     <row r="51">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C51" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
       </c>
       <c r="E51" t="s">
-        <v>418</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C52" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D52" t="s">
         <v>27</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>418</v>
       </c>
     </row>
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C53" t="s">
-        <v>186</v>
+        <v>420</v>
       </c>
       <c r="D53" t="s">
         <v>27</v>
@@ -61548,10 +61568,10 @@
     <row r="54">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C54" t="s">
-        <v>423</v>
+        <v>186</v>
       </c>
       <c r="D54" t="s">
         <v>27</v>
@@ -61563,10 +61583,10 @@
     <row r="55">
       <c r="A55"/>
       <c r="B55" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C55" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D55" t="s">
         <v>27</v>
@@ -61578,10 +61598,10 @@
     <row r="56">
       <c r="A56"/>
       <c r="B56" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C56" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
@@ -61593,10 +61613,10 @@
     <row r="57">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C57" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D57" t="s">
         <v>27</v>
@@ -61608,10 +61628,10 @@
     <row r="58">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C58" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D58" t="s">
         <v>27</v>
@@ -61623,10 +61643,10 @@
     <row r="59">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C59" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D59" t="s">
         <v>27</v>
@@ -61638,10 +61658,10 @@
     <row r="60">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C60" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D60" t="s">
         <v>27</v>
@@ -61653,10 +61673,10 @@
     <row r="61">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C61" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D61" t="s">
         <v>27</v>
@@ -61668,10 +61688,10 @@
     <row r="62">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D62" t="s">
         <v>27</v>
@@ -61683,10 +61703,10 @@
     <row r="63">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C63" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D63" t="s">
         <v>27</v>
@@ -61698,10 +61718,10 @@
     <row r="64">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C64" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D64" t="s">
         <v>27</v>
@@ -61713,10 +61733,10 @@
     <row r="65">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C65" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
@@ -61728,10 +61748,10 @@
     <row r="66">
       <c r="A66"/>
       <c r="B66" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C66" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D66" t="s">
         <v>27</v>
@@ -61743,10 +61763,10 @@
     <row r="67">
       <c r="A67"/>
       <c r="B67" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C67" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D67" t="s">
         <v>27</v>
@@ -61758,10 +61778,10 @@
     <row r="68">
       <c r="A68"/>
       <c r="B68" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C68" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D68" t="s">
         <v>27</v>
@@ -61773,10 +61793,10 @@
     <row r="69">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C69" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D69" t="s">
         <v>27</v>
@@ -61788,10 +61808,10 @@
     <row r="70">
       <c r="A70"/>
       <c r="B70" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C70" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D70" t="s">
         <v>27</v>
@@ -61803,10 +61823,10 @@
     <row r="71">
       <c r="A71"/>
       <c r="B71" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C71" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D71" t="s">
         <v>27</v>
@@ -61818,10 +61838,10 @@
     <row r="72">
       <c r="A72"/>
       <c r="B72" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C72" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
@@ -61833,10 +61853,10 @@
     <row r="73">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C73" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D73" t="s">
         <v>27</v>
@@ -61848,10 +61868,10 @@
     <row r="74">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C74" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D74" t="s">
         <v>27</v>
@@ -61863,10 +61883,10 @@
     <row r="75">
       <c r="A75"/>
       <c r="B75" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C75" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D75" t="s">
         <v>27</v>
@@ -61878,10 +61898,10 @@
     <row r="76">
       <c r="A76"/>
       <c r="B76" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C76" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D76" t="s">
         <v>27</v>
@@ -61893,10 +61913,10 @@
     <row r="77">
       <c r="A77"/>
       <c r="B77" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C77" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D77" t="s">
         <v>27</v>
@@ -61908,10 +61928,10 @@
     <row r="78">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C78" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D78" t="s">
         <v>27</v>
@@ -61923,10 +61943,10 @@
     <row r="79">
       <c r="A79"/>
       <c r="B79" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C79" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D79" t="s">
         <v>27</v>
@@ -61938,10 +61958,10 @@
     <row r="80">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C80" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D80" t="s">
         <v>27</v>
@@ -61953,10 +61973,10 @@
     <row r="81">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C81" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D81" t="s">
         <v>27</v>
@@ -61968,55 +61988,55 @@
     <row r="82">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C82" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
       </c>
       <c r="E82" t="s">
-        <v>479</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C83" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
       </c>
       <c r="E83" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="84">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C84" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D84" t="s">
         <v>27</v>
       </c>
       <c r="E84" t="s">
-        <v>27</v>
+        <v>482</v>
       </c>
     </row>
     <row r="85">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C85" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D85" t="s">
         <v>27</v>
@@ -62028,10 +62048,10 @@
     <row r="86">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C86" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D86" t="s">
         <v>27</v>
@@ -62043,10 +62063,10 @@
     <row r="87">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C87" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D87" t="s">
         <v>27</v>
@@ -62058,10 +62078,10 @@
     <row r="88">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C88" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D88" t="s">
         <v>27</v>
@@ -62073,40 +62093,40 @@
     <row r="89">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C89" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D89" t="s">
         <v>27</v>
       </c>
       <c r="E89" t="s">
-        <v>493</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C90" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D90" t="s">
         <v>27</v>
       </c>
       <c r="E90" t="s">
-        <v>27</v>
+        <v>493</v>
       </c>
     </row>
     <row r="91">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C91" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D91" t="s">
         <v>27</v>
@@ -62118,10 +62138,10 @@
     <row r="92">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C92" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -62133,89 +62153,89 @@
     <row r="93">
       <c r="A93"/>
       <c r="B93" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C93" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
       </c>
       <c r="E93" t="s">
-        <v>501</v>
+        <v>27</v>
       </c>
     </row>
     <row r="94">
       <c r="A94"/>
       <c r="B94" t="s">
-        <v>235</v>
+        <v>501</v>
       </c>
       <c r="C94" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D94" t="s">
         <v>27</v>
       </c>
       <c r="E94" t="s">
-        <v>236</v>
+        <v>501</v>
       </c>
     </row>
     <row r="95">
       <c r="A95"/>
       <c r="B95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C95" t="s">
+        <v>503</v>
+      </c>
+      <c r="D95" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96"/>
+      <c r="B96" t="s">
         <v>504</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>505</v>
       </c>
-      <c r="D95" t="s">
-        <v>27</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="D96" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>2</v>
-      </c>
-      <c r="B97" t="s">
-        <v>214</v>
-      </c>
-      <c r="C97" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" t="s">
-        <v>5</v>
-      </c>
-      <c r="E97" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" t="s">
+        <v>214</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
         <v>53</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>237</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>238</v>
-      </c>
-      <c r="D98" t="s">
-        <v>27</v>
-      </c>
-      <c r="E98" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99"/>
-      <c r="B99" t="s">
-        <v>239</v>
-      </c>
-      <c r="C99" t="s">
-        <v>240</v>
       </c>
       <c r="D99" t="s">
         <v>27</v>
@@ -62227,10 +62247,10 @@
     <row r="100">
       <c r="A100"/>
       <c r="B100" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C100" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D100" t="s">
         <v>27</v>
@@ -62242,59 +62262,59 @@
     <row r="101">
       <c r="A101"/>
       <c r="B101" t="s">
+        <v>235</v>
+      </c>
+      <c r="C101" t="s">
+        <v>236</v>
+      </c>
+      <c r="D101" t="s">
+        <v>27</v>
+      </c>
+      <c r="E101" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102"/>
+      <c r="B102" t="s">
         <v>241</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>242</v>
       </c>
-      <c r="D101" t="s">
-        <v>27</v>
-      </c>
-      <c r="E101" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" t="s">
-        <v>214</v>
-      </c>
-      <c r="C103" t="s">
-        <v>4</v>
-      </c>
-      <c r="D103" t="s">
-        <v>5</v>
-      </c>
-      <c r="E103" t="s">
-        <v>224</v>
+      <c r="D102" t="s">
+        <v>27</v>
+      </c>
+      <c r="E102" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" t="s">
+        <v>214</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
         <v>110</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>369</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>370</v>
-      </c>
-      <c r="D104" t="s">
-        <v>27</v>
-      </c>
-      <c r="E104" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105"/>
-      <c r="B105" t="s">
-        <v>371</v>
-      </c>
-      <c r="C105" t="s">
-        <v>372</v>
       </c>
       <c r="D105" t="s">
         <v>27</v>
@@ -62306,10 +62326,10 @@
     <row r="106">
       <c r="A106"/>
       <c r="B106" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C106" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D106" t="s">
         <v>27</v>
@@ -62321,59 +62341,59 @@
     <row r="107">
       <c r="A107"/>
       <c r="B107" t="s">
+        <v>373</v>
+      </c>
+      <c r="C107" t="s">
+        <v>374</v>
+      </c>
+      <c r="D107" t="s">
+        <v>27</v>
+      </c>
+      <c r="E107" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108"/>
+      <c r="B108" t="s">
         <v>241</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>242</v>
       </c>
-      <c r="D107" t="s">
-        <v>27</v>
-      </c>
-      <c r="E107" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" t="s">
-        <v>214</v>
-      </c>
-      <c r="C109" t="s">
-        <v>4</v>
-      </c>
-      <c r="D109" t="s">
-        <v>5</v>
-      </c>
-      <c r="E109" t="s">
-        <v>224</v>
+      <c r="D108" t="s">
+        <v>27</v>
+      </c>
+      <c r="E108" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>4155</v>
+        <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>4165</v>
+        <v>214</v>
       </c>
       <c r="C110" t="s">
-        <v>4166</v>
+        <v>4</v>
       </c>
       <c r="D110" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E110" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111"/>
+      <c r="A111" t="s">
+        <v>4158</v>
+      </c>
       <c r="B111" t="s">
-        <v>2350</v>
+        <v>4168</v>
       </c>
       <c r="C111" t="s">
-        <v>2351</v>
+        <v>4169</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -62385,10 +62405,10 @@
     <row r="112">
       <c r="A112"/>
       <c r="B112" t="s">
-        <v>4167</v>
+        <v>2350</v>
       </c>
       <c r="C112" t="s">
-        <v>4168</v>
+        <v>2351</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
@@ -62400,15 +62420,30 @@
     <row r="113">
       <c r="A113"/>
       <c r="B113" t="s">
-        <v>4169</v>
+        <v>4170</v>
       </c>
       <c r="C113" t="s">
-        <v>4170</v>
+        <v>4171</v>
       </c>
       <c r="D113" t="s">
         <v>27</v>
       </c>
       <c r="E113" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114"/>
+      <c r="B114" t="s">
+        <v>4172</v>
+      </c>
+      <c r="C114" t="s">
+        <v>4173</v>
+      </c>
+      <c r="D114" t="s">
+        <v>27</v>
+      </c>
+      <c r="E114" t="s">
         <v>27</v>
       </c>
     </row>
@@ -62487,13 +62522,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4171</v>
+        <v>4174</v>
       </c>
       <c r="B2" t="s">
-        <v>4172</v>
+        <v>4175</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>4173</v>
+        <v>4176</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
@@ -62515,17 +62550,17 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4174</v>
+        <v>4177</v>
       </c>
       <c r="B3" t="s">
-        <v>4175</v>
+        <v>4178</v>
       </c>
       <c r="C3" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>4176</v>
+        <v>4179</v>
       </c>
       <c r="F3" t="s" s="1">
         <v>27</v>
@@ -62541,10 +62576,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4177</v>
+        <v>4180</v>
       </c>
       <c r="B4" t="s">
-        <v>4178</v>
+        <v>4181</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>4108</v>
@@ -62567,17 +62602,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4179</v>
+        <v>4182</v>
       </c>
       <c r="B5" t="s">
-        <v>4180</v>
+        <v>4183</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>4181</v>
+        <v>4184</v>
       </c>
       <c r="F5" t="s" s="1">
         <v>27</v>
@@ -62593,17 +62628,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4182</v>
+        <v>4185</v>
       </c>
       <c r="B6" t="s">
-        <v>4183</v>
+        <v>4186</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>4184</v>
+        <v>4187</v>
       </c>
       <c r="F6" t="s" s="1">
         <v>27</v>
@@ -62619,7 +62654,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4185</v>
+        <v>4188</v>
       </c>
       <c r="B7" t="s">
         <v>3103</v>
@@ -62645,7 +62680,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4186</v>
+        <v>4189</v>
       </c>
       <c r="B8" t="s">
         <v>3115</v>
@@ -62671,7 +62706,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4187</v>
+        <v>4190</v>
       </c>
       <c r="B9" t="s">
         <v>3125</v>
@@ -62697,7 +62732,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4188</v>
+        <v>4191</v>
       </c>
       <c r="B10" t="s">
         <v>3133</v>
@@ -62723,7 +62758,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4189</v>
+        <v>4192</v>
       </c>
       <c r="B11" t="s">
         <v>3129</v>
@@ -62749,7 +62784,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4190</v>
+        <v>4193</v>
       </c>
       <c r="B12" t="s">
         <v>3100</v>
@@ -62775,7 +62810,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4191</v>
+        <v>4194</v>
       </c>
       <c r="B13" t="s">
         <v>196</v>
@@ -62801,7 +62836,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4192</v>
+        <v>4195</v>
       </c>
       <c r="B14" t="s">
         <v>3153</v>
@@ -62827,7 +62862,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4193</v>
+        <v>4196</v>
       </c>
       <c r="B15" t="s">
         <v>3091</v>
@@ -62853,7 +62888,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4194</v>
+        <v>4197</v>
       </c>
       <c r="B16" t="s">
         <v>3098</v>
@@ -62879,7 +62914,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4195</v>
+        <v>4198</v>
       </c>
       <c r="B17" t="s">
         <v>3156</v>
@@ -62905,10 +62940,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4196</v>
+        <v>4199</v>
       </c>
       <c r="B18" t="s">
-        <v>4197</v>
+        <v>4200</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>3108</v>
@@ -63427,12 +63462,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4198</v>
+        <v>4201</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4199</v>
+        <v>4202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>